<commit_message>
Create api Family_Balance and update excellsheet
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="292">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -857,13 +857,66 @@
   </si>
   <si>
     <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"tradedt\": \"20170125\",\r\n \"Buy\": 81000.0,\r\n \"BuyAmount\": 8280173.70,\r\n \"Sell\": 81000.0,\r\n \"SellAmount\": 8300976.30,\r\n \"Net\": 0.0,\r\n \"NetAmount\": -20802.60\r\n }\r\n]" }</t>
+  </si>
+  <si>
+    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"01/04/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": 63814.00,\r\n \"Particular\": \"Opening Balance\",\r\n \"Debitflag\": \"D\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"O\",\r\n \"Common\": \"\",\r\n \"Ldate\": \"2019-04-01T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"03/04/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -6508.00,\r\n \"Particular\": \"ByBill For BW2019003\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019003\",\r\n \"Ldate\": \"2019-04-03T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019003/20190403\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"08/04/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -726.00,\r\n \"Particular\": \"ByBill For BW2019006\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019006\",\r\n \"Ldate\": \"2019-04-08T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019006/20190408\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"16/04/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -6459.00,\r\n \"Particular\": \"ByBill For BW2019012\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019012\",\r\n \"Ldate\": \"2019-04-16T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019012/20190416\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"13/05/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": 307.00,\r\n \"Particular\": \"Debit Balance of DP Services (1202870000086521)\",\r\n \"Debitflag\": \"D\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"J\",\r\n \"Common\": \"DPBT\",\r\n \"Ldate\": \"2019-05-13T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"17/05/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": 3913.00,\r\n \"Particular\": \"ToBill For BW2019031\",\r\n \"Debitflag\": \"D\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019031\",\r\n \"Ldate\": \"2019-05-17T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019031/20190517\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"04/06/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -8437.00,\r\n \"Particular\": \"ByBill For BW2019043\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019043\",\r\n \"Ldate\": \"2019-06-04T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019043/20190604\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"07/06/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -15868.00,\r\n \"Particular\": \"ByBill For BW2019045\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019045\",\r\n \"Ldate\": \"2019-06-07T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019045/20190607\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"10/06/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -11271.00,\r\n \"Particular\": \"ByBill For BW2019046\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019046\",\r\n \"Ldate\": \"2019-06-10T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019046/20190610\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"11/06/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -1712.00,\r\n \"Particular\": \"ByBill For BW2019047\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019047\",\r\n \"Ldate\": \"2019-06-11T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019047/20190611\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"12/06/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -4439.00,\r\n \"Particular\": \"ByBill For BW2019048\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019048\",\r\n \"Ldate\": \"2019-06-12T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019048/20190612\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"13/06/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -4040.00,\r\n \"Particular\": \"ByBill For BW2019049\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019049\",\r\n \"Ldate\": \"2019-06-13T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019049/20190613\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"17/06/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -21.00,\r\n \"Particular\": \"ByBill For BW2019051\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019051\",\r\n \"Ldate\": \"2019-06-17T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019051/20190617\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"19/06/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -38404.00,\r\n \"Particular\": \"ByBill For BW2019053\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019053\",\r\n \"Ldate\": \"2019-06-19T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019053/20190619\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"21/06/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -1238.00,\r\n \"Particular\": \"ByBill For BW2019055\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"B\",\r\n \"Common\": \"BW2019055\",\r\n \"Ldate\": \"2019-06-21T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"B/C/BW2019055/20190621\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"04/07/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -67000.00,\r\n \"Particular\": \"ON ACCOUNT\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"001115\",\r\n \"Documenttype\": \"R\",\r\n \"Common\": \"\",\r\n \"Ldate\": \"2019-07-04T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"16/07/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": 98089.00,\r\n \"Particular\": \"AMT PAID THRU NEFT\",\r\n \"Debitflag\": \"D\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"P\",\r\n \"Common\": \"Payout Execution\",\r\n \"Ldate\": \"2019-07-16T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"24/07/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": -25.00,\r\n \"Particular\": \"Dividend @ Rs.0.25 on 100 Shares of SOUTHBANK\",\r\n \"Debitflag\": \"C\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"J\",\r\n \"Common\": \"Dividend\",\r\n \"Ldate\": \"2019-07-24T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"30/07/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": 25.00,\r\n \"Particular\": \"AMT PAID THRU NEFT\",\r\n \"Debitflag\": \"D\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"P\",\r\n \"Common\": \"Payout Execution\",\r\n \"Ldate\": \"2019-07-30T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"\"\r\n },\r\n {\r\n \"Type\": \"Trading\",\r\n \"ClientCode\": \"MG040 \",\r\n \"Date\": \"08/08/2019 \",\r\n \"ExchSeg\": \"BSE-Cash \",\r\n \"Amount\": 42.00,\r\n \"Particular\": \"Debit Balance of DP Services (1202870000086521)\",\r\n \"Debitflag\": \"D\",\r\n \"Chequeno\": \"\",\r\n \"Documenttype\": \"J\",\r\n \"Common\": \"DPBT\",\r\n \"Ldate\": \"2019-08-08T00:00:00\",\r\n \"CESCD\": \"ABC \",\r\n \"LookUp\": \"\"\r\n }\r\n]" }</t>
+  </si>
+  <si>
+    <r>
+      <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematActNo\": \"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>1202870000086521</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>\"\r\n }\r\n]" }</t>
+    </r>
+  </si>
+  <si>
+    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE748C01020\",\r\n \"CompanyName\": \"3I INFOTECH LIMITED-NEW RS 10-AFTER CONSOLIDATION\",\r\n \"ISINName\": \"3I INFOTECH RS 10\",\r\n \"Quantity\": 1000.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 4.36,\r\n \"Value\": 4360.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE00PV01013\",\r\n \"CompanyName\": \"AHLADA ENGINEERS LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"AHLADA ENGINEERS-EQ\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 88.55,\r\n \"Value\": 265.65\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE00PV01013\",\r\n \"CompanyName\": \"AHLADA ENGINEERS LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"AHLADA ENGINEERS-EQ\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 88.55,\r\n \"Value\": 265.65\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE031B01049\",\r\n \"CompanyName\": \"AJANTA PHARMA LIMITED # NEW EQUITY SHARE WITH FACE VALUE RS.2/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"AJANTA PHAR-EQ\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1680.25,\r\n \"Value\": 1680.25\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE093B01015\",\r\n \"CompanyName\": \"ALPS INDUSTRIES LIMITED EQUITY SHARES\",\r\n \"ISINName\": \"ALPS INDUSTRIES EQTY\",\r\n \"Quantity\": 200.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 0.99,\r\n \"Value\": 198.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE079A01024\",\r\n \"CompanyName\": \"AMBUJA CEMENTS LIMITED-NEW EQUITY SHARES OF RS.2/- AFTER SPLIT\",\r\n \"ISINName\": \"AMBUJA CEMENTS EQ\",\r\n \"Quantity\": 106.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 252.90,\r\n \"Value\": 26807.40\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE437A01024\",\r\n \"CompanyName\": \"APOLLO HOSPITALS ENTERPRISE LIMITED-NEW EQUITY SHARES OF RS.5/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"APOLLO HOSPIT-EQ5/-\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 2441.15,\r\n \"Value\": 2441.15\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE208A01029\",\r\n \"CompanyName\": \"ASHOK LEYLAND LIMITED- EQUITY SHARES OF RS 1/- EACH AFTER SUBDIVISION\",\r\n \"ISINName\": \"ASHOK LEYLAND-RE.1/-\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 95.35,\r\n \"Value\": 286.05\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE208A01029\",\r\n \"CompanyName\": \"ASHOK LEYLAND LIMITED- EQUITY SHARES OF RS 1/- EACH AFTER SUBDIVISION\",\r\n \"ISINName\": \"ASHOK LEYLAND-RE.1/-\",\r\n \"Quantity\": 50.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 95.35,\r\n \"Value\": 4767.50\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE442H01029\",\r\n \"CompanyName\": \"ASHOKA BUILDCON LIMITED # NEW EQUITY SHARES OF RS.5/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"ASHOKA BUILD EQ 5/-\",\r\n \"Quantity\": 30.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 95.45,\r\n \"Value\": 2863.50\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE871C01038\",\r\n \"CompanyName\": \"AVANTI FEEDS LIMITED#NEW EQUITY SHARES FACE VALUE RE. 1/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"AVANTI FEEDS-EQ1/-\",\r\n \"Quantity\": 2.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 531.95,\r\n \"Value\": 1063.90\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE192R01011\",\r\n \"CompanyName\": \"AVENUE SUPERMARTS LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"AVENUE SUPER-EQ\",\r\n \"Quantity\": 14.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 2622.40,\r\n \"Value\": 36713.60\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE296A01024\",\r\n \"CompanyName\": \"BAJAJ FINANCE LIMITED # NEW EQ SH WITH FV RS.2/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"BAJAJ FINANCE-EQ\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 4843.00,\r\n \"Value\": 4843.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE787D01026\",\r\n \"CompanyName\": \"BALKRISHNA INDUSTRIES LIMITED- NEW EQUITY SHARES OF RS. 2/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"BALKRISHNA IND RS.2\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1667.10,\r\n \"Value\": 1667.10\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE545U01014\",\r\n \"CompanyName\": \"BANDHAN BANK LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"BANDHAN BANK-EQ\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 399.90,\r\n \"Value\": 1199.70\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE545U01014\",\r\n \"CompanyName\": \"BANDHAN BANK LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"BANDHAN BANK-EQ\",\r\n \"Quantity\": 48.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 399.90,\r\n \"Value\": 19195.20\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE028A01039\",\r\n \"CompanyName\": \"BANK OF BARODA # NEW EQ SH WITH FV RS.2/- AFTER SUB-DIV\",\r\n \"ISINName\": \"BANK OF BARODA-EQ\",\r\n \"Quantity\": 16.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 65.60,\r\n \"Value\": 1049.60\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE166C01025\",\r\n \"CompanyName\": \"BELLARY STEELS AND ALLOYS LIMITED - EQUITY SHARES OF RE.1/- EACH AFTER SPLIT\",\r\n \"ISINName\": \"BELLARY STEEL-EQ RE1\",\r\n \"Quantity\": 1000.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 1.91,\r\n \"Value\": 1910.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE052T01013\",\r\n \"CompanyName\": \"BEST AGROLIFE LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"BEST AGROLIFE-EQ\",\r\n \"Quantity\": 24.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 478.30,\r\n \"Value\": 11479.20\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE354C01027\",\r\n \"CompanyName\": \"BHAGERIA INDUSTRIES LIMITED # NEW EQ SH WITH FV RE 5/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"BHAGERIA INDUSTRI-EQ\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 150.05,\r\n \"Value\": 150.05\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE257A01026\",\r\n \"CompanyName\": \"BHARAT HEAVY ELECTRICALS LIMITED - NEW EQUITY SHARES OF RS.2/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"BHARAT HEAVY - EQ 2\",\r\n \"Quantity\": 23.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 36.55,\r\n \"Value\": 840.65\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE029A01011\",\r\n \"CompanyName\": \"BHARAT PETROLEUM CORPORATION LTD EQUITY SHARES\",\r\n \"ISINName\": \"BPCL EQUITY\",\r\n \"Quantity\": 2.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 395.20,\r\n \"Value\": 790.40\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE216A01030\",\r\n \"CompanyName\": \"BRITANNIA INDUSTRIES LIMITED#NEW EQUITY SHARES FACE VALUE RE. 1/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"BRITANNIA IND-EQ1/-\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 3627.35,\r\n \"Value\": 10882.05\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE07T201019\",\r\n \"CompanyName\": \"BURGER KING INDIA LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"BURGER KING INDIA-EQ\",\r\n \"Quantity\": 709.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 0.00,\r\n \"Value\": 0.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE476A01014\",\r\n \"CompanyName\": \"CANARA BANK-EQUITY SHARES\",\r\n \"ISINName\": \"CANARA BANK-EQ\",\r\n \"Quantity\": 9.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 128.10,\r\n \"Value\": 1152.90\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE736A01011\",\r\n \"CompanyName\": \"CENTRAL DEPOSITORY SERVICES (INDIA) LIMITED -EQUITY SHARES\",\r\n \"ISINName\": \"CDSL EQUITY\",\r\n \"Quantity\": 71.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 525.65,\r\n \"Value\": 37321.15\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE736A01011\",\r\n \"CompanyName\": \"CENTRAL DEPOSITORY SERVICES (INDIA) LIMITED -EQUITY SHARES\",\r\n \"ISINName\": \"CDSL EQUITY\",\r\n \"Quantity\": 329.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 525.65,\r\n \"Value\": 172938.85\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE522F01014\",\r\n \"CompanyName\": \"COAL INDIA LIMITED - EQUITY SHARES\",\r\n \"ISINName\": \"COAL INDIA LTD-EQ\",\r\n \"Quantity\": 6.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 134.75,\r\n \"Value\": 808.50\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE522F01014\",\r\n \"CompanyName\": \"COAL INDIA LIMITED - EQUITY SHARES\",\r\n \"ISINName\": \"COAL INDIA LTD-EQ\",\r\n \"Quantity\": 15.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 134.75,\r\n \"Value\": 2021.25\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE259A01022\",\r\n \"CompanyName\": \"COLGATE-PALMOLIVE (INDIA) LIMITED - NEW EQUITY SHARES OF RE. 1/- AFTER CAPITAL REDUCTION\",\r\n \"ISINName\": \"COLGATE PALM-EQ RE 1\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1567.60,\r\n \"Value\": 1567.60\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE016A01026\",\r\n \"CompanyName\": \"DABUR INDIA LIMITED - EQUITY SHARES (FV RE.1/-)\",\r\n \"ISINName\": \"DABUR INDIA (RE.1/-)\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 502.05,\r\n \"Value\": 502.05\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE500A01029\",\r\n \"CompanyName\": \"DCW LTD - EQUITY SHARES OF RS.2 AFTER SPLIT\",\r\n \"ISINName\": \"DCW LTD - EQ RS 2\",\r\n \"Quantity\": 100.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 18.81,\r\n \"Value\": 1881.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE288B01029\",\r\n \"CompanyName\": \"DEEPAK NITRITE LTD#FULLY PAID UP EQ SH WITH F.V. OF RS.2/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"DEEPAK NITR-EQ\",\r\n \"Quantity\": 2.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 859.80,\r\n \"Value\": 1719.60\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE989C01012\",\r\n \"CompanyName\": \"DIAMOND POWER INFRASTRUCTURE LIMITED - EQUITY SHARES\",\r\n \"ISINName\": \"DIAMOND POWER EQ\",\r\n \"Quantity\": 445.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 0.76,\r\n \"Value\": 338.20\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE016M01021\",\r\n \"CompanyName\": \"DILIGENT MEDIA CORPORATION LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"DILIGENT MEDIA-EQ\",\r\n \"Quantity\": 500.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 0.44,\r\n \"Value\": 220.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE042A01014\",\r\n \"CompanyName\": \"ESCORTS LIMITED EQUITY SHARES - TRF CUM DEMAT 0005\",\r\n \"ISINName\": \"ESCORTS LIMITED EQ\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1389.25,\r\n \"Value\": 1389.25\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE302A01020\",\r\n \"CompanyName\": \"EXIDE INDUSTRIES LIMITED - NEW EQUITY SHARES OF RE. 1/- AFTER SPLIT\",\r\n \"ISINName\": \"EXIDE - EQ RE 1/-\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 192.75,\r\n \"Value\": 578.25\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE129A01019\",\r\n \"CompanyName\": \"GAIL (INDIA) LTD [FORMERLY GAS AUTHORITY OF INDIA LTD]\",\r\n \"ISINName\": \"GAIL (INDIA) LTD-EQ\",\r\n \"Quantity\": 9.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 122.55,\r\n \"Value\": 1102.95\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE181G01025\",\r\n \"CompanyName\": \"GAMMON INFRASTRUCTURE PROJECTS LIMITED -NEW EQUITY SHARES OF RS. 2/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"GAMMON INFRA - EQ\",\r\n \"Quantity\": 27900.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 0.96,\r\n \"Value\": 26784.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE289B01019\",\r\n \"CompanyName\": \"GIC HOUSING FINANCE LIMITED EQUITY SHARES\",\r\n \"ISINName\": \"GIC HOU FINAN\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 116.35,\r\n \"Value\": 349.05\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE776C01039\",\r\n \"CompanyName\": \"GMR INFRASTRUCTURE LIMITED - NEW EQUITY SHARES OF RE. 1/- AFTER SPLIT\",\r\n \"ISINName\": \"GMR INFRA - EQ RE 1\",\r\n \"Quantity\": 125.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 27.50,\r\n \"Value\": 3437.50\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE101D01020\",\r\n \"CompanyName\": \"GRANULES INDIA LIMITED # NEW EQUITY SHARE WITH FACE VALUE RS.1/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"GRANULES INDIA-EQ\",\r\n \"Quantity\": 15.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 391.50,\r\n \"Value\": 5872.50\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE419U01012\",\r\n \"CompanyName\": \"HAPPIEST MINDS TECHNOLOGIES LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"HAPPIEST MINDS TE-EQ\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 322.70,\r\n \"Value\": 968.10\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE860A01027\",\r\n \"CompanyName\": \"HCL TECHNOLOGIES LIMITED - EQUITY SHARES - FV RS.2/-\",\r\n \"ISINName\": \"HCL TECH (FV RS.2/-)\",\r\n \"Quantity\": 6.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 870.50,\r\n \"Value\": 5223.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE127D01025\",\r\n \"CompanyName\": \"HDFC ASSET MANAGEMENT COMPANY LIMITED#NEW EQUITY SHARES FV Rs. 5/- AFTER SUBDIVISION\",\r\n \"ISINName\": \"HDFC ASSET-EQ5/-\",\r\n \"Quantity\": 2.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 2811.05,\r\n \"Value\": 5622.10\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE040A01034\",\r\n \"CompanyName\": \"HDFC BANK LIMITED#NEW EQUITY SHARES WITH FACE VALUE RE. 1/- AFTER SUBDIVISION\",\r\n \"ISINName\": \"HDFC BANK-EQ1/-\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1405.85,\r\n \"Value\": 1405.85\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE782E01017\",\r\n \"CompanyName\": \"HESTER BIOSCIENCES LIMITED - EQUITY SHARES\",\r\n \"ISINName\": \"HESTER BIOSCIENCES\",\r\n \"Quantity\": 21.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1760.00,\r\n \"Value\": 36960.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE093A01033\",\r\n \"CompanyName\": \"HEXAWARE TECHNOLOGIES LIMITED EQ- RS 2/- (AFTER SPLIT)\",\r\n \"ISINName\": \"HEXAWARE TECH RS 2/-\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 470.75,\r\n \"Value\": 1412.25\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE094A01015\",\r\n \"CompanyName\": \"HINDUSTAN PETROLEUM CORPORATION LIMITED-EQUITY SHARES\",\r\n \"ISINName\": \"HPCL EQUITY\",\r\n \"Quantity\": 8.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 218.30,\r\n \"Value\": 1746.40\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE267A01025\",\r\n \"CompanyName\": \"HINDUSTAN ZINC LIMITED-NEW EQUITY SHARES OF RS-2/-AFTER SUB-DIVISION\",\r\n \"ISINName\": \"HIND ZINC EQ-RS 2/-\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 243.00,\r\n \"Value\": 729.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE267A01025\",\r\n \"CompanyName\": \"HINDUSTAN ZINC LIMITED-NEW EQUITY SHARES OF RS-2/-AFTER SUB-DIVISION\",\r\n \"ISINName\": \"HIND ZINC EQ-RS 2/-\",\r\n \"Quantity\": 6.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 243.00,\r\n \"Value\": 1458.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE001A01036\",\r\n \"CompanyName\": \"HOUSING DEVELOPMENT FINANCE CORPORATION LIMITED-NEW EQUITY SHARES OF RS. 2/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"HDFC LTD-EQ 2/-\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 2305.20,\r\n \"Value\": 2305.20\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE090A01021\",\r\n \"CompanyName\": \"ICICI BANK LIMITED # NEW EQ SH WITH FV RS.2/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"ICICI BANK-EQ\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 511.30,\r\n \"Value\": 511.30\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE092T01019\",\r\n \"CompanyName\": \"IDFC FIRST BANK LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"IDFC FIRST BANK-EQ\",\r\n \"Quantity\": 305.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 38.65,\r\n \"Value\": 11788.25\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE043D01016\",\r\n \"CompanyName\": \"IDFC LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"IDFC LIMITED-EQ\",\r\n \"Quantity\": 1175.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 39.95,\r\n \"Value\": 46941.25\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE969D01012\",\r\n \"CompanyName\": \"IND BANK HOUSING LTD - EQUITY SHARES\",\r\n \"ISINName\": \"IND BANK HOUSING LTD\",\r\n \"Quantity\": 30.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 24.65,\r\n \"Value\": 739.50\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE353K01014\",\r\n \"CompanyName\": \"INDIA TOURISM DEVELOPMENT CORPORATION LIMITED - EQUITY SHARES\",\r\n \"ISINName\": \"INDIA TOURISM - EQ\",\r\n \"Quantity\": 30.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 287.00,\r\n \"Value\": 8610.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE242A01010\",\r\n \"CompanyName\": \"INDIAN OIL CORPORATION LIMITED EQUITY SHARES\",\r\n \"ISINName\": \"INDIAN OIL CORP EQ\",\r\n \"Quantity\": 12.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 93.95,\r\n \"Value\": 1127.40\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE565A01014\",\r\n \"CompanyName\": \"INDIAN OVERSEAS BANK LIMITED EQUITY SHARES\",\r\n \"ISINName\": \"INDIAN OVERSEAS BANK\",\r\n \"Quantity\": 200.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 11.70,\r\n \"Value\": 2340.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE203G01027\",\r\n \"CompanyName\": \"INDRAPRASTHA GAS LIMITED#NEW EQUITY SHARES FV RS. 2/- AFTER SUBDIVISION\",\r\n \"ISINName\": \"INDRAPRASTHA-EQ2/-\",\r\n \"Quantity\": 7.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 483.00,\r\n \"Value\": 3381.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE121J01017\",\r\n \"CompanyName\": \"INDUS TOWERS LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"INDUS TOWERS LTD-EQ\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 246.40,\r\n \"Value\": 739.20\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE009A01021\",\r\n \"CompanyName\": \"INFOSYS LIMITED - EQUITY SHARES OF RS 5/- EACH\",\r\n \"ISINName\": \"INFOSYS LTD-EQ 5/-\",\r\n \"Quantity\": 12.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1175.15,\r\n \"Value\": 14101.80\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE154A01025\",\r\n \"CompanyName\": \"ITC LIMITED - EQUITY SHARES OF RE.1/- AFTER SPLIT\",\r\n \"ISINName\": \"ITC LIMITED -EQ RE.1\",\r\n \"Quantity\": 9.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 205.35,\r\n \"Value\": 1848.15\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE019A01038\",\r\n \"CompanyName\": \"JSW STEEL LIMITED#EQUITY SHARES WITH FACE VALUE RE. 1/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"JSW STEEL-EQTY\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 361.85,\r\n \"Value\": 361.85\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE430G01026\",\r\n \"CompanyName\": \"JVL AGRO INDUSTRIES LIMITED-NEW EQUITY SHARES OF RE. 1/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"JVL AGRO IND-EQ 1/-\",\r\n \"Quantity\": 300.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 0.69,\r\n \"Value\": 207.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE415I01015\",\r\n \"CompanyName\": \"KIRI INDUSTRIES LIMITED - EQUITY SHARES\",\r\n \"ISINName\": \"KIRI INDUSTRIES-EQ\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 481.85,\r\n \"Value\": 481.85\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE775B01025\",\r\n \"CompanyName\": \"KWALITY LIMITED# EQUITY SHARES\",\r\n \"ISINName\": \"KWALITY-EQ 1/-\",\r\n \"Quantity\": 1500.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 3.35,\r\n \"Value\": 5025.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE498L01015\",\r\n \"CompanyName\": \"L&amp;T FINANCE HOLDINGS LIMITED-EQUITY SHARES\",\r\n \"ISINName\": \"L&amp;T FINANCE HOLD-EQ\",\r\n \"Quantity\": 119.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 92.00,\r\n \"Value\": 10948.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE010V01017\",\r\n \"CompanyName\": \"L&amp;T TECHNOLOGY SERVICES LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"L&amp;T TECHNOLOGY-EQ\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1840.05,\r\n \"Value\": 5520.15\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE018A01030\",\r\n \"CompanyName\": \"LARSEN &amp; TOUBRO LIMITED-EQUITY SHARES OF RS.2/- EACH\",\r\n \"ISINName\": \"LARSEN &amp; TOUBR-EQ2/-\",\r\n \"Quantity\": 4.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1181.10,\r\n \"Value\": 4724.40\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE947Q01028\",\r\n \"CompanyName\": \"LAURUS LABS LIMITED#NEW EQUITY SHARES WITH FACE VALUE RS. 2/- AFTER SUBDIVISION\",\r\n \"ISINName\": \"LAURUS LABS-EQ2/-\",\r\n \"Quantity\": 25.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 328.70,\r\n \"Value\": 8217.50\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE115A01026\",\r\n \"CompanyName\": \"LIC HOUSING FINANCE LTD-NEW EQUITY SHARES OF RS.2/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"LIC HSG FIN RS-2-EQ\",\r\n \"Quantity\": 15.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 357.10,\r\n \"Value\": 5356.50\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE326A01037\",\r\n \"CompanyName\": \"LUPIN LIMITED-NEW EQUITY SHARES OF RS. 2/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"LUPIN LIMITED-EQ2/-\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 950.70,\r\n \"Value\": 2852.10\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE326A01037\",\r\n \"CompanyName\": \"LUPIN LIMITED-NEW EQUITY SHARES OF RS. 2/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"LUPIN LIMITED-EQ2/-\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 950.70,\r\n \"Value\": 950.70\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE150G01020\",\r\n \"CompanyName\": \"LUX INDUSTRIES LIMITED # NEW EQ SH WITH FV RS.2/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"LUX INDUSTRIES-EQ\",\r\n \"Quantity\": 11.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1590.75,\r\n \"Value\": 17498.25\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE378D01032\",\r\n \"CompanyName\": \"MADHUCON PROJECTS LIMITED - NEW EQUITY SHARES OF RE.1/- AFTER SPLIT\",\r\n \"ISINName\": \"MADHUCON PROJ EQ 1\",\r\n \"Quantity\": 2000.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 4.44,\r\n \"Value\": 8880.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE002S01010\",\r\n \"CompanyName\": \"MAHANAGAR GAS LIMITED # EQUITY SHARES\",\r\n \"ISINName\": \"MAHANAGAR GAS-EQ\",\r\n \"Quantity\": 2.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1037.55,\r\n \"Value\": 2075.10\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE101A01026\",\r\n \"CompanyName\": \"MAHINDRA &amp; MAHINDRA EQUITY SHARES - EQUITY SHARES OF RS 5/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"MAH &amp; MAH EQ RS 5/-\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 754.85,\r\n \"Value\": 754.85\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE774D01024\",\r\n \"CompanyName\": \"MAHINDRA &amp; MAHINDRA FINANCIAL SERVICES LIMITED # NEW EQUITY SHARES OF RS. 2/- AFTER SUB DIVISION\",\r\n \"ISINName\": \"MAH &amp; MAH FIN EQ 2/-\",\r\n \"Quantity\": 13.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 176.05,\r\n \"Value\": 2288.65\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE585B01010\",\r\n \"CompanyName\": \"MARUTI SUZUKI INDIA LIMITED-EQUITY SHARES\",\r\n \"ISINName\": \"MARUTI SUZUKI IND-EQ\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 7707.75,\r\n \"Value\": 7707.75\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE018I01017\",\r\n \"CompanyName\": \"MINDTREE LIMITED-FORMERLY MINDTREE CONSULTING PVT LTD-EQUITY SHARES\",\r\n \"ISINName\": \"MINDTREE LIMITED-EQ\",\r\n \"Quantity\": 6.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1456.30,\r\n \"Value\": 8737.80\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE083A01026\",\r\n \"CompanyName\": \"MOREPEN LABORATORIES LIMITED - EQUITY SHARES - FV RS.2/-\",\r\n \"ISINName\": \"MOREPEN LAB(RS.2/-)\",\r\n \"Quantity\": 6.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 32.15,\r\n \"Value\": 192.90\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE775A01035\",\r\n \"CompanyName\": \"MOTHERSON SUMI SYSTEMS LTD- RE 1/- AFTER SUB DIVISION OF SHARES-EQUITY SHARES\",\r\n \"ISINName\": \"MOTHERSON SUMI-RE1/-\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 157.60,\r\n \"Value\": 472.80\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE139A01034\",\r\n \"CompanyName\": \"NATIONAL ALUMINIUM COMPANY LIMITED-NEW EQUITY SHARES OF RS-5/-AFTER SUB-DIVISION\",\r\n \"ISINName\": \"NALCO EQ-RS 5/-\",\r\n \"Quantity\": 37.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 42.10,\r\n \"Value\": 1557.70\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE794A01010\",\r\n \"CompanyName\": \"NEULAND LABORATORIES LIMITED EQUITY SHARES\",\r\n \"ISINName\": \"NEULAND LABS EQUITY\",\r\n \"Quantity\": 15.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 1114.55,\r\n \"Value\": 16718.25\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE937C01029\",\r\n \"CompanyName\": \"NILA INFRASTRUCTURES LIMITED - EQUITY SHARES OF RE.1/- AFTER SPLIT\",\r\n \"ISINName\": \"NILA INFRASTRU RE 1/\",\r\n \"Quantity\": 900.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 5.80,\r\n \"Value\": 5220.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE589A01014\",\r\n \"CompanyName\": \"NLC INDIA LIMITED # EQTY SHARES\",\r\n \"ISINName\": \"NLC INDIA LIMITED-EQ\",\r\n \"Quantity\": 1880.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 54.50,\r\n \"Value\": 102460.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE584A01023\",\r\n \"CompanyName\": \"NMDC LIMITED - EQUITY SHARES OF RE. 1/- AFTER SPLIT\",\r\n \"ISINName\": \"NMDC LIMITED-EQ RE 1\",\r\n \"Quantity\": 21.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 107.10,\r\n \"Value\": 2249.10\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE584A01023\",\r\n \"CompanyName\": \"NMDC LIMITED - EQUITY SHARES OF RE. 1/- AFTER SPLIT\",\r\n \"ISINName\": \"NMDC LIMITED-EQ RE 1\",\r\n \"Quantity\": 3.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 107.10,\r\n \"Value\": 321.30\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE733E01010\",\r\n \"CompanyName\": \"NTPC LIMITED-EQUITY SHARES\",\r\n \"ISINName\": \"NTPC LTD\",\r\n \"Quantity\": 28.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 98.25,\r\n \"Value\": 2751.00\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE213A01029\",\r\n \"CompanyName\": \"OIL &amp; NATURAL GAS CORPORATION LIMITED-NEW EQUITY SHARES OF RS-5/- AFTER SUB-DIVISION\",\r\n \"ISINName\": \"ONGC-EQ-RS.5/-\",\r\n \"Quantity\": 39.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 91.15,\r\n \"Value\": 3554.85\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE881D01027\",\r\n \"CompanyName\": \"ORACLE FINANCIAL SERVICES SOFTWARE LIMITED - EQUITY SHARES-RS.5/-\",\r\n \"ISINName\": \"ORACLE FINANC RS.5/-\",\r\n \"Quantity\": 1.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 3158.55,\r\n \"Value\": 3158.55\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE347G01014\",\r\n \"CompanyName\": \"PETRONET LNG LIMITED-EQUITY SHARES\",\r\n \"ISINName\": \"PETRONET LNG LTD-EQ\",\r\n \"Quantity\": 2.000,\r\n \"BalanceType\": \"Beneficiary\",\r\n \"Rate\": 257.70,\r\n \"Value\": 515.40\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"1202870000086521\",\r\n \"ISIN\": \"INE140A01024\",\r\n \"CompanyName\": \"PIRAMAL ENTERPRISES LIMITED # NEW RS 2- AFTER SPLIT\",\r\n \"ISINName\": \"PIRAMAL ENTER - EQ\",\r\n \"Quantity\": 2.000,\r\n \"BalanceType\": \"Pledge\",\r\n \"Rate\": 1465.65,\r\n \"Value\": 2931.30\r\n },\r\n {\r\n \"ClientCode\": \"MG040 \",\r\n \"DematAc\": \"12028700</t>
+  </si>
+  <si>
+    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"name\": \"20220212\"\r\n }\r\n]" }</t>
+  </si>
+  <si>
+    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"CESCd\": \"ABC\",\r\n \"exchange\": \"BSE \",\r\n \"segment\": \"Cash \"\r\n },\r\n {\r\n \"CESCd\": \"ANC\",\r\n \"exchange\": \"NSE \",\r\n \"segment\": \"Cash \"\r\n },\r\n {\r\n \"CESCd\": \"AMC\",\r\n \"exchange\": \"MCX \",\r\n \"segment\": \"Cash \"\r\n },\r\n {\r\n \"CESCd\": \"ABF\",\r\n \"exchange\": \"BSE \",\r\n \"segment\": \"F&amp;O \"\r\n },\r\n {\r\n \"CESCd\": \"ANF\",\r\n \"exchange\": \"NSE \",\r\n \"segment\": \"F&amp;O \"\r\n },\r\n {\r\n \"CESCd\": \"AMF\",\r\n \"exchange\": \"MCX \",\r\n \"segment\": \"F&amp;O \"\r\n },\r\n {\r\n \"CESCd\": \"ANK\",\r\n \"exchange\": \"NSE \",\r\n \"segment\": \"FX \"\r\n },\r\n {\r\n \"CESCd\": \"AMK\",\r\n \"exchange\": \"MCX \",\r\n \"segment\": \"FX \"\r\n }\r\n]" }</t>
+  </si>
+  <si>
+    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"type\": \"N\",\r\n \"description\": \"N - Normal \"\r\n },\r\n {\r\n \"type\": \"Q\",\r\n \"description\": \"Q - Normal (T+1) \"\r\n },\r\n {\r\n \"type\": \"U\",\r\n \"description\": \"U - T2T (T+1) \"\r\n },\r\n {\r\n \"type\": \"Z\",\r\n \"description\": \"Z - T2T \"\r\n },\r\n {\r\n \"type\": \"A\",\r\n \"description\": \"A - Auction Nomal \"\r\n },\r\n {\r\n \"type\": \"B\",\r\n \"description\": \"B - Objection Physical \"\r\n },\r\n {\r\n \"type\": \"T\",\r\n \"description\": \"Buy Beck \"\r\n },\r\n {\r\n \"type\": \"C\",\r\n \"description\": \"C - F&amp;O Physical Stock \"\r\n },\r\n {\r\n \"type\": \"D\",\r\n \"description\": \"D-BuyBack \"\r\n },\r\n {\r\n \"type\": \"E\",\r\n \"description\": \"E - F&amp;O Physical Auction \"\r\n },\r\n {\r\n \"type\": \"G\",\r\n \"description\": \"G - Close - Out ( Internal ) \"\r\n },\r\n {\r\n \"type\": \"H\",\r\n \"description\": \"H - OFS \"\r\n },\r\n {\r\n \"type\": \"I\",\r\n \"description\": \"I - ITP \"\r\n },\r\n {\r\n \"type\": \"L\",\r\n \"description\": \"L - SLBM \"\r\n },\r\n {\r\n \"type\": \"O\",\r\n \"description\": \"O - Limited Physical \"\r\n },\r\n {\r\n \"type\": \"P\",\r\n \"description\": \"P - Periodic \"\r\n },\r\n {\r\n \"type\": \"R\",\r\n \"description\": \"R - SLBM-Return \"\r\n },\r\n {\r\n \"type\": \"S\",\r\n \"description\": \"S - Spot \"\r\n },\r\n {\r\n \"type\": \"W\",\r\n \"description\": \"W - Rolling (old) \"\r\n },\r\n {\r\n \"type\": \"X\",\r\n \"description\": \"X - NSE-CloseOut \"\r\n }\r\n]" }</t>
+  </si>
+  <si>
+    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006065295.0,\r\n \"TradeID\": 2393678.0,\r\n \"TradeTime\": \"14:10:13\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 202.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 529.00,\r\n \"Brokerage\": 8.0800,\r\n \"BuyValue\": 106866.0800,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006065295.0,\r\n \"TradeID\": 2393676.0,\r\n \"TradeTime\": \"14:10:13\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 3.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 529.00,\r\n \"Brokerage\": 0.1200,\r\n \"BuyValue\": 1587.1200,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006065295.0,\r\n \"TradeID\": 2393673.0,\r\n \"TradeTime\": \"14:10:13\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 5.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 529.00,\r\n \"Brokerage\": 0.2000,\r\n \"BuyValue\": 2645.2000,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006065295.0,\r\n \"TradeID\": 2393672.0,\r\n \"TradeTime\": \"14:10:13\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 787.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 528.95,\r\n \"Brokerage\": 31.4800,\r\n \"BuyValue\": 416315.1300,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006065295.0,\r\n \"TradeID\": 2393677.0,\r\n \"TradeTime\": \"14:10:13\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 1.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 529.00,\r\n \"Brokerage\": 0.0400,\r\n \"BuyValue\": 529.0400,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006065295.0,\r\n \"TradeID\": 2393675.0,\r\n \"TradeTime\": \"14:10:13\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 1.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 529.00,\r\n \"Brokerage\": 0.0400,\r\n \"BuyValue\": 529.0400,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006065295.0,\r\n \"TradeID\": 2393674.0,\r\n \"TradeTime\": \"14:10:13\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 1.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 529.00,\r\n \"Brokerage\": 0.0400,\r\n \"BuyValue\": 529.0400,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394634.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 1.0,\r\n \"MarketRate\": 530.70,\r\n \"Brokerage\": 0.0400,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 530.6600,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394636.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 24.0,\r\n \"MarketRate\": 530.50,\r\n \"Brokerage\": 0.9600,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 12731.0400,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394638.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 64.0,\r\n \"MarketRate\": 530.40,\r\n \"Brokerage\": 2.5600,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 33943.0400,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394640.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 38.0,\r\n \"MarketRate\": 530.30,\r\n \"Brokerage\": 1.5200,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 20149.8800,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394642.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 64.0,\r\n \"MarketRate\": 530.20,\r\n \"Brokerage\": 2.5600,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 33930.2400,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394644.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 375.0,\r\n \"MarketRate\": 530.05,\r\n \"Brokerage\": 15.0000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 198753.7500,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394646.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 1.0,\r\n \"MarketRate\": 530.00,\r\n \"Brokerage\": 0.0400,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 529.9600,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394648.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 10.0,\r\n \"MarketRate\": 530.00,\r\n \"Brokerage\": 0.4000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 5299.6000,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394650.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 229.0,\r\n \"MarketRate\": 530.00,\r\n \"Brokerage\": 9.1600,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 121360.8400,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394635.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 1.0,\r\n \"MarketRate\": 530.70,\r\n \"Brokerage\": 0.0400,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 530.6600,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394637.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 48.0,\r\n \"MarketRate\": 530.45,\r\n \"Brokerage\": 1.9200,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 25459.6800,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394639.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 5.0,\r\n \"MarketRate\": 530.35,\r\n \"Brokerage\": 0.2000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 2651.5500,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394641.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 64.0,\r\n \"MarketRate\": 530.30,\r\n \"Brokerage\": 2.5600,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 33936.6400,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394643.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 64.0,\r\n \"MarketRate\": 530.10,\r\n \"Brokerage\": 2.5600,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 33923.8400,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394645.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 10.0,\r\n \"MarketRate\": 530.00,\r\n \"Brokerage\": 0.4000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 5299.6000,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394647.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 1.0,\r\n \"MarketRate\": 530.00,\r\n \"Brokerage\": 0.0400,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 529.9600,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"541153 \",\r\n \"OrderID\": 1000000006067401.0,\r\n \"TradeID\": 2394649.0,\r\n \"TradeTime\": \"14:10:18\",\r\n \"ScripName\": \"BANDHANBNK\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 1.0,\r\n \"MarketRate\": 530.00,\r\n \"Brokerage\": 0.0400,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 529.9600,\r\n \"Ordr\": \"BANDHANBNKb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828401.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 100.0,\r\n \"MarketRate\": 167.55,\r\n \"Brokerage\": 1.0000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 16754.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828403.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 1.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 0.0100,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 167.4900,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828405.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 50.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 0.5000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 8374.5000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828407.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 58.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 0.5800,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 9714.4200,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828398.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 250.0,\r\n \"MarketRate\": 167.65,\r\n \"Brokerage\": 2.5000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 41910.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828400.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 12.0,\r\n \"MarketRate\": 167.60,\r\n \"Brokerage\": 0.1200,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 2011.0800,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828402.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 250.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 2.5000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 41872.5000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828404.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 1.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 0.0100,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 167.4900,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828406.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 1.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 0.0100,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 167.4900,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828397.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 98.0,\r\n \"MarketRate\": 167.70,\r\n \"Brokerage\": 0.9800,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 16433.6200,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2828399.0,\r\n \"TradeTime\": \"14:55:37\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 120.0,\r\n \"MarketRate\": 167.60,\r\n \"Brokerage\": 1.2000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 20110.8000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2831116.0,\r\n \"TradeTime\": \"14:55:54\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 139.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 1.3900,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 23281.1100,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2831119.0,\r\n \"TradeTime\": \"14:55:54\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 13.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 0.1300,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 2177.3700,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2831118.0,\r\n \"TradeTime\": \"14:55:54\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 60.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 0.6000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 10049.4000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2833325.0,\r\n \"TradeTime\": \"14:56:03\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 427.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 4.2700,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 71518.2300,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007117195.0,\r\n \"TradeID\": 2836218.0,\r\n \"TradeTime\": \"14:56:19\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 3420.0,\r\n \"MarketRate\": 167.50,\r\n \"Brokerage\": 34.2000,\r\n \"BuyValue\": 0.0000,\r\n \"SellValue\": 572815.8000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007150633.0,\r\n \"TradeID\": 2844958.0,\r\n \"TradeTime\": \"14:57:01\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 500.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 167.05,\r\n \"Brokerage\": 5.0000,\r\n \"BuyValue\": 83530.0000,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007150633.0,\r\n \"TradeID\": 2844966.0,\r\n \"TradeTime\": \"14:57:01\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 500.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 167.05,\r\n \"Brokerage\": 5.0000,\r\n \"BuyValue\": 83530.0000,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007150633.0,\r\n \"TradeID\": 2844973.0,\r\n \"TradeTime\": \"14:57:01\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 500.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 167.05,\r\n \"Brokerage\": 5.0000,\r\n \"BuyValue\": 83530.0000,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007150633.0,\r\n \"TradeID\": 2844978.0,\r\n \"TradeTime\": \"14:57:01\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 20.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 167.05,\r\n \"Brokerage\": 0.2000,\r\n \"BuyValue\": 3341.2000,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007150633.0,\r\n \"TradeID\": 2844954.0,\r\n \"TradeTime\": \"14:57:01\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 500.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 167.05,\r\n \"Brokerage\": 5.0000,\r\n \"BuyValue\": 83530.0000,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007150633.0,\r\n \"TradeID\": 2844962.0,\r\n \"TradeTime\": \"14:57:01\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 500.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 167.05,\r\n \"Brokerage\": 5.0000,\r\n \"BuyValue\": 83530.0000,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007150633.0,\r\n \"TradeID\": 2844970.0,\r\n \"TradeTime\": \"14:57:01\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 500.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 167.05,\r\n \"Brokerage\": 5.0000,\r\n \"BuyValue\": 83530.0000,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007150633.0,\r\n \"TradeID\": 2844976.0,\r\n \"TradeTime\": \"14:57:01\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 101.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 167.05,\r\n \"Brokerage\": 1.0100,\r\n \"BuyValue\": 16873.0600,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007243483.0,\r\n \"TradeID\": 2892661.0,\r\n \"TradeTime\": \"15:00:16\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 136.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 170.00,\r\n \"Brokerage\": 1.3600,\r\n \"BuyValue\": 23121.3600,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007243483.0,\r\n \"TradeID\": 2892914.0,\r\n \"TradeTime\": \"15:00:17\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 112.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 170.00,\r\n \"Brokerage\": 1.1200,\r\n \"BuyValue\": 19041.1200,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"506197 \",\r\n \"OrderID\": 1000000007243483.0,\r\n \"TradeID\": 2893828.0,\r\n \"TradeTime\": \"15:00:19\",\r\n \"ScripName\": \"BLISSGVS\",\r\n \"Buy\": 1631.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 170.00,\r\n \"Brokerage\": 16.3100,\r\n \"BuyValue\": 277286.3100,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"BLISSGVSb\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": null,\r\n \"ScripCode\": null,\r\n \"OrderID\": null,\r\n \"TradeID\": null,\r\n \"TradeTime\": null,\r\n \"ScripName\": \"Net Item Amount (Sale-Buy) :\",\r\n \"Buy\": null,\r\n \"Sell\": null,\r\n \"MarketRate\": null,\r\n \"Brokerage\": null,\r\n \"BuyValue\": null,\r\n \"SellValue\": null,\r\n \"Ordr\": null,\r\n \"tdDt\": null,\r\n \"NetValue\": \"-2252.00\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"Charges\",\r\n \"OrderID\": 0.0,\r\n \"TradeID\": 0.0,\r\n \"TradeTime\": \"Charges \",\r\n \"ScripName\": \"Central GST @ 9%\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 0.00,\r\n \"Brokerage\": 0.0000,\r\n \"BuyValue\": 24.2100,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"zzz\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"Charges\",\r\n \"OrderID\": 0.0,\r\n \"TradeID\": 0.0,\r\n \"TradeTime\": \"Charges \",\r\n \"ScripName\": \"SEBI FEES\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 0.00,\r\n \"Brokerage\": 0.0000,\r\n \"BuyValue\": 4.1100,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"zzz\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"Charges\",\r\n \"OrderID\": 0.0,\r\n \"TradeID\": 0.0,\r\n \"TradeTime\": \"Charges \",\r\n \"ScripName\": \"Stamp Duty on Trading\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 0.00,\r\n \"Brokerage\": 0.0000,\r\n \"BuyValue\": 54.7500,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"zzz\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"Charges\",\r\n \"OrderID\": 0.0,\r\n \"TradeID\": 0.0,\r\n \"TradeTime\": \"Charges \",\r\n \"ScripName\": \"State GST @ 9%\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 0.00,\r\n \"Brokerage\": 0.0000,\r\n \"BuyValue\": 24.2100,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"zzz\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"Charges\",\r\n \"OrderID\": 0.0,\r\n \"TradeID\": 0.0,\r\n \"TradeTime\": \"Charges \",\r\n \"ScripName\": \"STT\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 0.00,\r\n \"Brokerage\": 0.0000,\r\n \"BuyValue\": 342.0000,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"zzz\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": \"NN2019061\",\r\n \"ScripCode\": \"Charges\",\r\n \"OrderID\": 0.0,\r\n \"TradeID\": 0.0,\r\n \"TradeTime\": \"Charges \",\r\n \"ScripName\": \"TOCharge\",\r\n \"Buy\": 0.0,\r\n \"Sell\": 0.0,\r\n \"MarketRate\": 0.00,\r\n \"Brokerage\": 0.0000,\r\n \"BuyValue\": 88.9700,\r\n \"SellValue\": 0.0000,\r\n \"Ordr\": \"zzz\",\r\n \"tdDt\": \"20190328\",\r\n \"NetValue\": \"\"\r\n },\r\n {\r\n \"Stlmnt\": null,\r\n \"ScripCode\": null,\r\n \"OrderID\": null,\r\n \"TradeID\": null,\r\n \"TradeTime\": null,\r\n \"ScripName\": \"Due To Us :\",\r\n \"Buy\": null,\r\n \"Sell\": null,\r\n \"MarketRate\": null,\r\n \"Brokerage\": null,\r\n \"BuyValue\": null,\r\n \"SellValue\": null,\r\n \"Ordr\": null,\r\n \"tdDt\": null,\r\n \"NetValue\": \"-2766.00\"\r\n }\r\n]" }</t>
+  </si>
+  <si>
+    <t>NN2019061</t>
+  </si>
+  <si>
+    <t>0 - Cumulative                                         1 - Confirmation</t>
+  </si>
+  <si>
+    <t>"20201001"</t>
+  </si>
+  <si>
+    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"SorORder\": 1,\r\n \"type\": \"Equity : BW2020128\",\r\n \"stlmnt\": \"BW2020128\",\r\n \"scripcode\": \"543232 \",\r\n \"scripname\": \"CAMS\",\r\n \"buy\": 3.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 1412.5000,\r\n \"netrate\": 1414.2000,\r\n \"netamount\": 4242.60,\r\n \"brokerage\": 1.7000,\r\n \"lookup\": \"BW2020128/543232\"\r\n },\r\n {\r\n \"SorORder\": 1,\r\n \"type\": \"Equity : NN2020190\",\r\n \"stlmnt\": \"NN2020190\",\r\n \"scripcode\": \"543233 \",\r\n \"scripname\": \"CHEMCON\",\r\n \"buy\": 3.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 584.8000,\r\n \"netrate\": 585.5100,\r\n \"netamount\": 1756.53,\r\n \"brokerage\": 0.7100,\r\n \"lookup\": \"NN2020190/543233\"\r\n },\r\n {\r\n \"SorORder\": 1,\r\n \"type\": \"Equity : NN2020190\",\r\n \"stlmnt\": \"NN2020190\",\r\n \"scripcode\": \"533519 \",\r\n \"scripname\": \"LTFH\",\r\n \"buy\": 30.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 64.5000,\r\n \"netrate\": 64.5800,\r\n \"netamount\": 1937.40,\r\n \"brokerage\": 0.0800,\r\n \"lookup\": \"NN2020190/533519\"\r\n },\r\n {\r\n \"SorORder\": 1,\r\n \"type\": \"Equity : NN2020190\",\r\n \"stlmnt\": \"NN2020190\",\r\n \"scripcode\": \"521064 \",\r\n \"scripname\": \"TRIDENT\",\r\n \"buy\": 0.0,\r\n \"sell\": 9.0,\r\n \"marketrate\": 8.0000,\r\n \"netrate\": 7.9900,\r\n \"netamount\": -71.91,\r\n \"brokerage\": 0.0100,\r\n \"lookup\": \"NN2020190/521064\"\r\n },\r\n {\r\n \"SorORder\": 2,\r\n \"type\": \"NSE F&amp;O\",\r\n \"stlmnt\": \" \",\r\n \"scripcode\": \"IGL \",\r\n \"scripname\": \"FUTSTK IGL 29-OCT-2020\",\r\n \"buy\": 1375.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 398.9500,\r\n \"netrate\": 398.9769,\r\n \"netamount\": 548593.24,\r\n \"brokerage\": 0.0269,\r\n \"lookup\": \"N/F/158372 \"\r\n },\r\n {\r\n \"SorORder\": 2,\r\n \"type\": \"NSE F&amp;O\",\r\n \"stlmnt\": \" \",\r\n \"scripcode\": \"IGL \",\r\n \"scripname\": \"FUTSTK IGL 29-OCT-2020\",\r\n \"buy\": 0.0,\r\n \"sell\": 1375.0,\r\n \"marketrate\": 400.0000,\r\n \"netrate\": 399.9730,\r\n \"netamount\": -549962.88,\r\n \"brokerage\": 0.0270,\r\n \"lookup\": \"N/F/158372 \"\r\n },\r\n {\r\n \"SorORder\": 2,\r\n \"type\": \"NSE F&amp;O\",\r\n \"stlmnt\": \" \",\r\n \"scripcode\": \"IGL \",\r\n \"scripname\": \"FUTSTK IGL 29-OCT-2020\",\r\n \"buy\": 1375.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 397.8000,\r\n \"netrate\": 397.8269,\r\n \"netamount\": 547011.99,\r\n \"brokerage\": 0.0269,\r\n \"lookup\": \"N/F/158372 \"\r\n },\r\n {\r\n \"SorORder\": 2,\r\n \"type\": \"NSE F&amp;O\",\r\n \"stlmnt\": \" \",\r\n \"scripcode\": \"IGL \",\r\n \"scripname\": \"FUTSTK IGL 29-OCT-2020\",\r\n \"buy\": 0.0,\r\n \"sell\": 1375.0,\r\n \"marketrate\": 397.2000,\r\n \"netrate\": 397.1732,\r\n \"netamount\": -546113.15,\r\n \"brokerage\": 0.0268,\r\n \"lookup\": \"N/F/158372 \"\r\n },\r\n {\r\n \"SorORder\": 2,\r\n \"type\": \"NSE F&amp;O\",\r\n \"stlmnt\": \" \",\r\n \"scripcode\": \"NIFTY \",\r\n \"scripname\": \"OPTIDX NIFTY 01-OCT-2020 11300.00 PE\",\r\n \"buy\": 300.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 7.9500,\r\n \"netrate\": 8.3500,\r\n \"netamount\": 2505.00,\r\n \"brokerage\": 0.4000,\r\n \"lookup\": \"N/F/158453 \"\r\n },\r\n {\r\n \"SorORder\": 2,\r\n \"type\": \"NSE F&amp;O\",\r\n \"stlmnt\": \" \",\r\n \"scripcode\": \"NIFTY \",\r\n \"scripname\": \"OPTIDX NIFTY 01-OCT-2020 11300.00 PE\",\r\n \"buy\": 300.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 8.2000,\r\n \"netrate\": 8.6000,\r\n \"netamount\": 2580.00,\r\n \"brokerage\": 0.4000,\r\n \"lookup\": \"N/F/158453 \"\r\n },\r\n {\r\n \"SorORder\": 2,\r\n \"type\": \"NSE F&amp;O\",\r\n \"stlmnt\": \" \",\r\n \"scripcode\": \"NIFTY \",\r\n \"scripname\": \"OPTIDX NIFTY 01-OCT-2020 11350.00 PE\",\r\n \"buy\": 75.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 23.6000,\r\n \"netrate\": 24.0000,\r\n \"netamount\": 1800.00,\r\n \"brokerage\": 0.4000,\r\n \"lookup\": \"N/F/159062 \"\r\n },\r\n {\r\n \"SorORder\": 2,\r\n \"type\": \"NSE F&amp;O\",\r\n \"stlmnt\": \" \",\r\n \"scripcode\": \"NIFTY \",\r\n \"scripname\": \"OPTIDX NIFTY 01-OCT-2020 11350.00 PE\",\r\n \"buy\": 225.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 19.8500,\r\n \"netrate\": 20.2500,\r\n \"netamount\": 4556.25,\r\n \"brokerage\": 0.4000,\r\n \"lookup\": \"N/F/159062 \"\r\n },\r\n {\r\n \"SorORder\": 2,\r\n \"type\": \"NSE F&amp;O\",\r\n \"stlmnt\": \" \",\r\n \"scripcode\": \"NIFTY \",\r\n \"scripname\": \"OPTIDX NIFTY 01-OCT-2020 11350.00 PE\",\r\n \"buy\": 225.0,\r\n \"sell\": 0.0,\r\n \"marketrate\": 19.9500,\r\n \"netrate\": 20.3500,\r\n \"netamount\": 4578.75,\r\n \"brokerage\": 0.4000,\r\n \"lookup\": \"N/F/159062 \"\r\n }\r\n]" }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -905,8 +958,20 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -916,6 +981,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -932,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -979,6 +1050,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1285,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="C93" workbookViewId="0">
+      <selection activeCell="F281" sqref="F281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1630,7 +1713,7 @@
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D29" s="9"/>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>33</v>
       </c>
@@ -1651,6 +1734,9 @@
       </c>
       <c r="H30" s="17" t="s">
         <v>171</v>
+      </c>
+      <c r="I30" s="26" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
@@ -1968,7 +2054,7 @@
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D70" s="9"/>
     </row>
-    <row r="71" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>38</v>
       </c>
@@ -1978,11 +2064,14 @@
       <c r="D71" s="9" t="s">
         <v>256</v>
       </c>
+      <c r="I71" s="7" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D72" s="9"/>
     </row>
-    <row r="73" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>38</v>
       </c>
@@ -1997,6 +2086,12 @@
       </c>
       <c r="F73" t="s">
         <v>23</v>
+      </c>
+      <c r="H73" s="27">
+        <v>1202870000086520</v>
+      </c>
+      <c r="I73" s="26" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
@@ -2031,7 +2126,7 @@
     <row r="77" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D77" s="9"/>
     </row>
-    <row r="78" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
         <v>38</v>
       </c>
@@ -2040,6 +2135,9 @@
       </c>
       <c r="D78" s="9" t="s">
         <v>260</v>
+      </c>
+      <c r="I78" s="26" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
@@ -2095,7 +2193,7 @@
     <row r="83" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D83" s="9"/>
     </row>
-    <row r="84" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B84" t="s">
         <v>26</v>
       </c>
@@ -2105,11 +2203,14 @@
       <c r="D84" s="9" t="s">
         <v>261</v>
       </c>
+      <c r="I84" s="26" t="s">
+        <v>285</v>
+      </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D85" s="9"/>
     </row>
-    <row r="86" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B86" t="s">
         <v>26</v>
       </c>
@@ -2121,6 +2222,15 @@
       </c>
       <c r="E86" t="s">
         <v>263</v>
+      </c>
+      <c r="F86" t="s">
+        <v>23</v>
+      </c>
+      <c r="H86" t="s">
+        <v>28</v>
+      </c>
+      <c r="I86" s="26" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
@@ -2165,7 +2275,7 @@
     <row r="90" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D90" s="9"/>
     </row>
-    <row r="91" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B91" t="s">
         <v>26</v>
       </c>
@@ -2181,11 +2291,18 @@
       <c r="F91" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H91" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="I91" s="26" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D92" s="9"/>
-    </row>
-    <row r="93" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H92" s="8"/>
+    </row>
+    <row r="93" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
         <v>26</v>
       </c>
@@ -2200,6 +2317,12 @@
       </c>
       <c r="F93" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="H93" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="I93" s="26" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
@@ -2210,9 +2333,13 @@
       <c r="F94" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H94" s="8">
+        <v>20190328</v>
+      </c>
     </row>
     <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D95" s="9"/>
+      <c r="H95" s="8"/>
     </row>
     <row r="96" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B96" t="s">
@@ -2227,23 +2354,38 @@
       <c r="E96" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F96" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H96" s="29"/>
+    </row>
+    <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D97" s="9"/>
       <c r="E97" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F97" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H97" s="29"/>
+    </row>
+    <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D98" s="9"/>
       <c r="E98" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F98" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H98" s="29">
+        <v>20190328</v>
+      </c>
+    </row>
+    <row r="99" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D99" s="9"/>
-    </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H99" s="29"/>
+    </row>
+    <row r="100" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B100" t="s">
         <v>26</v>
       </c>
@@ -2256,17 +2398,26 @@
       <c r="E100" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F100" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H100" s="29"/>
+    </row>
+    <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D101" s="9"/>
       <c r="E101" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F101" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H101" s="29"/>
+    </row>
+    <row r="102" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D102" s="9"/>
-    </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H102" s="8"/>
+    </row>
+    <row r="103" spans="2:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>20</v>
       </c>
@@ -2279,17 +2430,32 @@
       <c r="E103" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F103" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H103" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="I103" s="31" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D104" s="9"/>
       <c r="E104" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F104" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H104" s="14" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D105" s="9"/>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B106" t="s">
         <v>20</v>
       </c>
@@ -2302,38 +2468,62 @@
       <c r="E106" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F106" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H106" s="28"/>
+    </row>
+    <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D107" s="9"/>
       <c r="E107" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F107" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H107" s="28"/>
+    </row>
+    <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F108" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H108" s="28"/>
+    </row>
+    <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D109" s="9"/>
       <c r="E109" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F109" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H109" s="28"/>
+    </row>
+    <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D110" s="9"/>
       <c r="E110" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F110" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H110" s="28"/>
+    </row>
+    <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D111" s="9"/>
       <c r="E111" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="F111" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H111" s="28"/>
+    </row>
+    <row r="112" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D112" s="9"/>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
create api family_position, family_holding, family_retainedStoke
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="309">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -952,6 +952,15 @@
   </si>
   <si>
     <t>Family_Balance</t>
+  </si>
+  <si>
+    <t>Family_RetainedStoke</t>
+  </si>
+  <si>
+    <t>Family_Holding</t>
+  </si>
+  <si>
+    <t>Family_Position</t>
   </si>
 </sst>
 </file>
@@ -1408,10 +1417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I321"/>
+  <dimension ref="A1:I334"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
-      <selection activeCell="A189" sqref="A189"/>
+    <sheetView tabSelected="1" topLeftCell="A178" workbookViewId="0">
+      <selection activeCell="C201" sqref="C201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3458,131 +3467,116 @@
     <row r="192" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D192" s="9"/>
     </row>
-    <row r="193" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="193" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B193" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C193" t="s">
-        <v>244</v>
-      </c>
-      <c r="D193" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E193" t="s">
-        <v>15</v>
-      </c>
-      <c r="F193" t="s">
-        <v>9</v>
-      </c>
-      <c r="G193" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H193" s="6">
-        <v>20210401</v>
-      </c>
-      <c r="I193" s="7" t="s">
-        <v>109</v>
+        <v>243</v>
+      </c>
+      <c r="D193" t="s">
+        <v>306</v>
+      </c>
+      <c r="H193" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="194" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D194" s="9"/>
-      <c r="E194" t="s">
-        <v>17</v>
-      </c>
-      <c r="F194" t="s">
-        <v>9</v>
-      </c>
-      <c r="G194" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H194" s="6">
-        <v>20220112</v>
+      <c r="E194" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F194" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H194" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D195" s="9"/>
-      <c r="E195" t="s">
-        <v>110</v>
-      </c>
-      <c r="F195" t="s">
-        <v>9</v>
-      </c>
-      <c r="H195" s="6">
-        <v>0</v>
+      <c r="H195" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="196" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D196" s="9"/>
-      <c r="H196" s="6"/>
-    </row>
-    <row r="197" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="H196" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="197" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B197" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="C197" t="s">
-        <v>244</v>
-      </c>
-      <c r="D197" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="H197" s="6"/>
-      <c r="I197" s="7" t="s">
-        <v>112</v>
+        <v>243</v>
+      </c>
+      <c r="D197" t="s">
+        <v>307</v>
+      </c>
+      <c r="H197" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="198" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D198" s="9"/>
-      <c r="H198" s="6"/>
+      <c r="E198" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H198" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="199" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D199" s="9"/>
-      <c r="H199" s="6"/>
-    </row>
-    <row r="200" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B200" t="s">
-        <v>107</v>
-      </c>
-      <c r="C200" t="s">
-        <v>244</v>
-      </c>
-      <c r="D200" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="H200" s="6"/>
-      <c r="I200" s="7" t="s">
-        <v>114</v>
+      <c r="H199" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="200" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H200" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D201" s="9"/>
-      <c r="H201" s="6"/>
+      <c r="B201" t="s">
+        <v>90</v>
+      </c>
+      <c r="C201" t="s">
+        <v>243</v>
+      </c>
+      <c r="D201" t="s">
+        <v>308</v>
+      </c>
+      <c r="H201" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="202" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D202" s="9"/>
-      <c r="H202" s="6"/>
-    </row>
-    <row r="203" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B203" t="s">
-        <v>107</v>
-      </c>
-      <c r="C203" t="s">
-        <v>244</v>
-      </c>
-      <c r="D203" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H203" s="6"/>
-      <c r="I203" s="7" t="s">
-        <v>116</v>
+      <c r="E202" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H202" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="203" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D203" s="9"/>
+      <c r="H203" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D204" s="9"/>
-      <c r="H204" s="6"/>
+      <c r="H204" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D205" s="9"/>
-      <c r="H205" s="6"/>
     </row>
     <row r="206" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B206" t="s">
@@ -3592,817 +3586,769 @@
         <v>244</v>
       </c>
       <c r="D206" s="9" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="E206" t="s">
-        <v>118</v>
+        <v>15</v>
       </c>
       <c r="F206" t="s">
-        <v>119</v>
-      </c>
-      <c r="H206" s="6" t="b">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="G206" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H206" s="6">
+        <v>20210401</v>
       </c>
       <c r="I206" s="7" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="207" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D207" s="9"/>
       <c r="E207" t="s">
-        <v>121</v>
+        <v>17</v>
       </c>
       <c r="F207" t="s">
-        <v>119</v>
-      </c>
-      <c r="H207" s="6" t="b">
-        <v>1</v>
+        <v>9</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H207" s="6">
+        <v>20220112</v>
       </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D208" s="9"/>
-      <c r="H208" s="6"/>
-    </row>
-    <row r="209" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B209" t="s">
+      <c r="E208" t="s">
+        <v>110</v>
+      </c>
+      <c r="F208" t="s">
+        <v>9</v>
+      </c>
+      <c r="H208" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D209" s="9"/>
+      <c r="H209" s="6"/>
+    </row>
+    <row r="210" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B210" t="s">
         <v>107</v>
       </c>
-      <c r="C209" t="s">
+      <c r="C210" t="s">
         <v>244</v>
       </c>
-      <c r="D209" s="9" t="s">
+      <c r="D210" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="H210" s="6"/>
+      <c r="I210" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="211" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D211" s="9"/>
+      <c r="H211" s="6"/>
+    </row>
+    <row r="212" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D212" s="9"/>
+      <c r="H212" s="6"/>
+    </row>
+    <row r="213" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B213" t="s">
+        <v>107</v>
+      </c>
+      <c r="C213" t="s">
+        <v>244</v>
+      </c>
+      <c r="D213" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H213" s="6"/>
+      <c r="I213" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="214" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D214" s="9"/>
+      <c r="H214" s="6"/>
+    </row>
+    <row r="215" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D215" s="9"/>
+      <c r="H215" s="6"/>
+    </row>
+    <row r="216" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B216" t="s">
+        <v>107</v>
+      </c>
+      <c r="C216" t="s">
+        <v>244</v>
+      </c>
+      <c r="D216" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="H216" s="6"/>
+      <c r="I216" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="217" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D217" s="9"/>
+      <c r="H217" s="6"/>
+    </row>
+    <row r="218" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D218" s="9"/>
+      <c r="H218" s="6"/>
+    </row>
+    <row r="219" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B219" t="s">
+        <v>107</v>
+      </c>
+      <c r="C219" t="s">
+        <v>244</v>
+      </c>
+      <c r="D219" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E219" t="s">
+        <v>118</v>
+      </c>
+      <c r="F219" t="s">
+        <v>119</v>
+      </c>
+      <c r="H219" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I219" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="220" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D220" s="9"/>
+      <c r="E220" t="s">
+        <v>121</v>
+      </c>
+      <c r="F220" t="s">
+        <v>119</v>
+      </c>
+      <c r="H220" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D221" s="9"/>
+      <c r="H221" s="6"/>
+    </row>
+    <row r="222" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B222" t="s">
+        <v>107</v>
+      </c>
+      <c r="C222" t="s">
+        <v>244</v>
+      </c>
+      <c r="D222" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E209" t="s">
+      <c r="E222" t="s">
         <v>123</v>
       </c>
-      <c r="F209" t="s">
+      <c r="F222" t="s">
         <v>21</v>
       </c>
-      <c r="H209" s="6">
+      <c r="H222" s="6">
         <v>3</v>
       </c>
-      <c r="I209" s="7" t="s">
+      <c r="I222" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="210" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D210" s="9"/>
-    </row>
-    <row r="211" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B211" s="1" t="s">
+    <row r="223" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D223" s="9"/>
+    </row>
+    <row r="224" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B224" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C211" t="s">
+      <c r="C224" t="s">
         <v>278</v>
       </c>
-      <c r="D211" s="10" t="s">
+      <c r="D224" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E211" s="1"/>
-      <c r="F211" s="10"/>
-      <c r="G211" s="1"/>
-      <c r="H211" s="3"/>
-      <c r="I211" s="7" t="s">
+      <c r="E224" s="1"/>
+      <c r="F224" s="10"/>
+      <c r="G224" s="1"/>
+      <c r="H224" s="3"/>
+      <c r="I224" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="212" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B212" s="1"/>
-      <c r="C212" s="1"/>
-      <c r="D212" s="10"/>
-      <c r="E212" s="1"/>
-      <c r="F212" s="1"/>
-      <c r="G212" s="1"/>
-      <c r="H212" s="3"/>
-      <c r="I212" s="13"/>
-    </row>
-    <row r="213" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B213" s="1" t="s">
+    <row r="225" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B225" s="1"/>
+      <c r="C225" s="1"/>
+      <c r="D225" s="10"/>
+      <c r="E225" s="1"/>
+      <c r="F225" s="1"/>
+      <c r="G225" s="1"/>
+      <c r="H225" s="3"/>
+      <c r="I225" s="13"/>
+    </row>
+    <row r="226" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B226" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C213" t="s">
+      <c r="C226" t="s">
         <v>278</v>
       </c>
-      <c r="D213" s="10" t="s">
+      <c r="D226" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E213" s="1"/>
-      <c r="F213" s="10"/>
-      <c r="G213" s="1"/>
-      <c r="H213" s="3"/>
-      <c r="I213" s="7" t="s">
+      <c r="E226" s="1"/>
+      <c r="F226" s="10"/>
+      <c r="G226" s="1"/>
+      <c r="H226" s="3"/>
+      <c r="I226" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="214" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B214" s="1"/>
-      <c r="C214" s="1"/>
-      <c r="D214" s="10"/>
-      <c r="E214" s="1"/>
-      <c r="F214" s="1"/>
-      <c r="G214" s="1"/>
-      <c r="H214" s="3"/>
-      <c r="I214" s="13"/>
-    </row>
-    <row r="215" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B215" s="1" t="s">
+    <row r="227" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B227" s="1"/>
+      <c r="C227" s="1"/>
+      <c r="D227" s="10"/>
+      <c r="E227" s="1"/>
+      <c r="F227" s="1"/>
+      <c r="G227" s="1"/>
+      <c r="H227" s="3"/>
+      <c r="I227" s="13"/>
+    </row>
+    <row r="228" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B228" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C215" t="s">
+      <c r="C228" t="s">
         <v>278</v>
       </c>
-      <c r="D215" s="10" t="s">
+      <c r="D228" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E215" s="11" t="s">
+      <c r="E228" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F215" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G215" s="1"/>
-      <c r="H215" s="3" t="s">
+      <c r="F228" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G228" s="1"/>
+      <c r="H228" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I215" s="7" t="s">
+      <c r="I228" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="216" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B216" s="1"/>
-      <c r="C216" s="1"/>
-      <c r="D216" s="10"/>
-      <c r="E216" s="11"/>
-      <c r="F216" s="10"/>
-      <c r="G216" s="1"/>
-      <c r="H216" s="3"/>
-      <c r="I216" s="13"/>
-    </row>
-    <row r="217" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B217" s="1" t="s">
+    <row r="229" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B229" s="1"/>
+      <c r="C229" s="1"/>
+      <c r="D229" s="10"/>
+      <c r="E229" s="11"/>
+      <c r="F229" s="10"/>
+      <c r="G229" s="1"/>
+      <c r="H229" s="3"/>
+      <c r="I229" s="13"/>
+    </row>
+    <row r="230" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B230" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C217" t="s">
+      <c r="C230" t="s">
         <v>278</v>
       </c>
-      <c r="D217" s="10" t="s">
+      <c r="D230" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E217" s="11"/>
-      <c r="F217" s="10"/>
-      <c r="G217" s="1"/>
-      <c r="H217" s="3"/>
-      <c r="I217" s="7" t="s">
+      <c r="E230" s="11"/>
+      <c r="F230" s="10"/>
+      <c r="G230" s="1"/>
+      <c r="H230" s="3"/>
+      <c r="I230" s="7" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="218" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B218" s="1"/>
-      <c r="C218" s="1"/>
-      <c r="D218" s="10"/>
-      <c r="E218" s="11"/>
-      <c r="F218" s="10"/>
-      <c r="G218" s="1"/>
-      <c r="H218" s="3"/>
-      <c r="I218" s="13"/>
-    </row>
-    <row r="219" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B219" s="1" t="s">
+    <row r="231" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B231" s="1"/>
+      <c r="C231" s="1"/>
+      <c r="D231" s="10"/>
+      <c r="E231" s="11"/>
+      <c r="F231" s="10"/>
+      <c r="G231" s="1"/>
+      <c r="H231" s="3"/>
+      <c r="I231" s="13"/>
+    </row>
+    <row r="232" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B232" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C219" t="s">
+      <c r="C232" t="s">
         <v>278</v>
       </c>
-      <c r="D219" s="10" t="s">
+      <c r="D232" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E219" s="11" t="s">
+      <c r="E232" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F219" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G219" s="1"/>
-      <c r="H219" s="3" t="s">
+      <c r="F232" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G232" s="1"/>
+      <c r="H232" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="I219" s="7" t="s">
+      <c r="I232" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="220" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B220" s="1"/>
-      <c r="C220" s="1"/>
-      <c r="D220" s="10"/>
-      <c r="E220" s="11" t="s">
+    <row r="233" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B233" s="1"/>
+      <c r="C233" s="1"/>
+      <c r="D233" s="10"/>
+      <c r="E233" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="F220" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G220" s="1"/>
-      <c r="H220" s="3" t="b">
+      <c r="F233" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G233" s="1"/>
+      <c r="H233" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="I220" s="13"/>
-    </row>
-    <row r="221" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B221" s="1"/>
-      <c r="C221" s="1"/>
-      <c r="D221" s="10"/>
-      <c r="E221" s="11" t="s">
+      <c r="I233" s="13"/>
+    </row>
+    <row r="234" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B234" s="1"/>
+      <c r="C234" s="1"/>
+      <c r="D234" s="10"/>
+      <c r="E234" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F221" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G221" s="1"/>
-      <c r="H221" s="3">
+      <c r="F234" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G234" s="1"/>
+      <c r="H234" s="3">
         <v>43590</v>
       </c>
-      <c r="I221" s="13"/>
-    </row>
-    <row r="222" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B222" s="1"/>
-      <c r="C222" s="1"/>
-      <c r="D222" s="10"/>
-      <c r="E222" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F222" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G222" s="1"/>
-      <c r="H222" s="3">
-        <v>532667</v>
-      </c>
-      <c r="I222" s="13"/>
-    </row>
-    <row r="223" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B223" s="1"/>
-      <c r="C223" s="1"/>
-      <c r="D223" s="10"/>
-      <c r="E223" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F223" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G223" s="1"/>
-      <c r="H223" s="3">
-        <v>198</v>
-      </c>
-      <c r="I223" s="13"/>
-    </row>
-    <row r="224" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D224" s="9"/>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D225" s="9"/>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B226" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D226" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="E226" t="s">
-        <v>15</v>
-      </c>
-      <c r="F226" t="s">
-        <v>9</v>
-      </c>
-      <c r="H226" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="I226" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D227" s="9"/>
-      <c r="E227" t="s">
-        <v>17</v>
-      </c>
-      <c r="F227" t="s">
-        <v>9</v>
-      </c>
-      <c r="H227" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="I227" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D228" s="9"/>
-      <c r="I228" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D229" s="9"/>
-      <c r="I229" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D230" s="9"/>
-      <c r="I230" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D231" s="9"/>
-      <c r="I231" s="19" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D232" s="9"/>
-      <c r="I232" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D233" s="9"/>
-    </row>
-    <row r="234" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A234" s="1">
-        <v>36</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D234" s="10" t="s">
-        <v>238</v>
-      </c>
-      <c r="E234" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F234" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G234" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H234" s="15">
-        <v>20200401</v>
-      </c>
-      <c r="I234" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="235" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="1"/>
+      <c r="I234" s="13"/>
+    </row>
+    <row r="235" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
       <c r="D235" s="10"/>
-      <c r="E235" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F235" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G235" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H235" s="6">
-        <v>20210331</v>
-      </c>
-      <c r="I235" s="1"/>
-    </row>
-    <row r="236" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A236" s="1"/>
+      <c r="E235" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F235" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G235" s="1"/>
+      <c r="H235" s="3">
+        <v>532667</v>
+      </c>
+      <c r="I235" s="13"/>
+    </row>
+    <row r="236" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
       <c r="D236" s="10"/>
-      <c r="E236" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F236" s="1" t="s">
+      <c r="E236" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F236" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G236" s="1"/>
       <c r="H236" s="3">
-        <v>533271</v>
+        <v>198</v>
       </c>
       <c r="I236" s="13"/>
     </row>
-    <row r="237" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A237" s="1"/>
-      <c r="B237" s="1"/>
-      <c r="C237" s="1"/>
-      <c r="D237" s="10"/>
-      <c r="E237" s="1"/>
-      <c r="F237" s="1"/>
-      <c r="G237" s="1"/>
-      <c r="H237" s="3"/>
-      <c r="I237" s="13"/>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B238" s="1" t="s">
+    <row r="237" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D237" s="9"/>
+    </row>
+    <row r="238" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D238" s="9"/>
+    </row>
+    <row r="239" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B239" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C238" s="1" t="s">
+      <c r="C239" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D238" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="E238" t="s">
-        <v>27</v>
-      </c>
-      <c r="F238" t="s">
-        <v>9</v>
-      </c>
-      <c r="H238" t="s">
-        <v>232</v>
-      </c>
-      <c r="I238" t="s">
+      <c r="D239" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="E239" t="s">
+        <v>15</v>
+      </c>
+      <c r="F239" t="s">
+        <v>9</v>
+      </c>
+      <c r="H239" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="I239" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D239" s="9"/>
-      <c r="E239" t="s">
-        <v>48</v>
-      </c>
-      <c r="F239" t="s">
-        <v>9</v>
-      </c>
-      <c r="H239" t="s">
-        <v>233</v>
-      </c>
-      <c r="I239" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D240" s="9"/>
       <c r="E240" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F240" t="s">
         <v>9</v>
       </c>
       <c r="H240" s="17" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I240" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="241" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D241" s="9"/>
+      <c r="I241" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="241" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D241" s="9"/>
-      <c r="E241" t="s">
-        <v>17</v>
-      </c>
-      <c r="F241" t="s">
-        <v>9</v>
-      </c>
-      <c r="H241" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="I241" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="242" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D242" s="9"/>
       <c r="I242" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="243" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D243" s="9"/>
+      <c r="I243" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="243" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D243" s="9"/>
-      <c r="I243" s="19" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="244" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D244" s="9"/>
       <c r="I244" s="19" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="245" spans="2:9" x14ac:dyDescent="0.3">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="245" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D245" s="9"/>
       <c r="I245" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="246" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D246" s="9"/>
     </row>
-    <row r="247" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A247" s="1">
+        <v>36</v>
+      </c>
       <c r="B247" s="1" t="s">
         <v>239</v>
       </c>
       <c r="C247" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D247" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="E247" t="s">
+      <c r="D247" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="E247" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F247" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G247" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H247" s="15">
+        <v>20200401</v>
+      </c>
+      <c r="I247" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="248" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A248" s="1"/>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
+      <c r="D248" s="10"/>
+      <c r="E248" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F248" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G248" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H248" s="6">
+        <v>20210331</v>
+      </c>
+      <c r="I248" s="1"/>
+    </row>
+    <row r="249" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A249" s="1"/>
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="10"/>
+      <c r="E249" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F249" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G249" s="1"/>
+      <c r="H249" s="3">
+        <v>533271</v>
+      </c>
+      <c r="I249" s="13"/>
+    </row>
+    <row r="250" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A250" s="1"/>
+      <c r="B250" s="1"/>
+      <c r="C250" s="1"/>
+      <c r="D250" s="10"/>
+      <c r="E250" s="1"/>
+      <c r="F250" s="1"/>
+      <c r="G250" s="1"/>
+      <c r="H250" s="3"/>
+      <c r="I250" s="13"/>
+    </row>
+    <row r="251" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B251" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C251" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D251" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E251" t="s">
         <v>27</v>
       </c>
-      <c r="F247" t="s">
-        <v>9</v>
-      </c>
-      <c r="H247" t="s">
-        <v>236</v>
-      </c>
-      <c r="I247" t="s">
+      <c r="F251" t="s">
+        <v>9</v>
+      </c>
+      <c r="H251" t="s">
+        <v>232</v>
+      </c>
+      <c r="I251" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="248" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D248" s="9"/>
-      <c r="E248" t="s">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D252" s="9"/>
+      <c r="E252" t="s">
+        <v>48</v>
+      </c>
+      <c r="F252" t="s">
+        <v>9</v>
+      </c>
+      <c r="H252" t="s">
+        <v>233</v>
+      </c>
+      <c r="I252" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="253" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D253" s="9"/>
+      <c r="E253" t="s">
         <v>15</v>
       </c>
-      <c r="F248" t="s">
-        <v>9</v>
-      </c>
-      <c r="H248" s="17" t="s">
+      <c r="F253" t="s">
+        <v>9</v>
+      </c>
+      <c r="H253" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="I248" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="249" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D249" s="9"/>
-      <c r="E249" t="s">
+      <c r="I253" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="254" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D254" s="9"/>
+      <c r="E254" t="s">
         <v>17</v>
       </c>
-      <c r="F249" t="s">
-        <v>9</v>
-      </c>
-      <c r="H249" s="17" t="s">
+      <c r="F254" t="s">
+        <v>9</v>
+      </c>
+      <c r="H254" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="I249" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="250" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D250" s="9"/>
-      <c r="I250" t="s">
+      <c r="I254" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="251" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D251" s="9"/>
-      <c r="I251" t="s">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D255" s="9"/>
+      <c r="I255" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="252" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D252" s="9"/>
-      <c r="I252" s="25" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="253" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D253" s="9"/>
-      <c r="E253" s="24"/>
-      <c r="H253" s="18"/>
-      <c r="I253" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="254" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D254" s="9"/>
-    </row>
-    <row r="255" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B255" t="s">
-        <v>128</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D255" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E255" t="s">
-        <v>15</v>
-      </c>
-      <c r="F255" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G255" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H255" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I255" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="256" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D256" s="9"/>
-      <c r="E256" t="s">
-        <v>17</v>
-      </c>
-      <c r="F256" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G256" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H256" s="8">
-        <v>20210331</v>
+      <c r="I256" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="257" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D257" s="9"/>
-      <c r="F257" s="9"/>
-      <c r="H257" s="8"/>
-    </row>
-    <row r="258" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B258" t="s">
-        <v>128</v>
-      </c>
-      <c r="C258" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D258" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E258" t="s">
-        <v>15</v>
-      </c>
-      <c r="F258" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G258" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H258" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I258" s="7" t="s">
-        <v>132</v>
+      <c r="I257" s="19" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="258" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D258" s="9"/>
+      <c r="I258" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="259" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D259" s="9"/>
-      <c r="E259" t="s">
-        <v>17</v>
-      </c>
-      <c r="F259" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G259" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H259" s="8">
-        <v>20210331</v>
-      </c>
     </row>
     <row r="260" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D260" s="9"/>
+      <c r="B260" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C260" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D260" s="9" t="s">
+        <v>241</v>
+      </c>
       <c r="E260" t="s">
-        <v>133</v>
-      </c>
-      <c r="F260" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H260" s="8" t="s">
-        <v>134</v>
+        <v>27</v>
+      </c>
+      <c r="F260" t="s">
+        <v>9</v>
+      </c>
+      <c r="H260" t="s">
+        <v>236</v>
+      </c>
+      <c r="I260" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="261" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D261" s="9"/>
       <c r="E261" t="s">
-        <v>135</v>
-      </c>
-      <c r="F261" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H261" s="8" t="s">
-        <v>134</v>
+        <v>15</v>
+      </c>
+      <c r="F261" t="s">
+        <v>9</v>
+      </c>
+      <c r="H261" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="I261" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="262" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D262" s="9"/>
       <c r="E262" t="s">
-        <v>136</v>
-      </c>
-      <c r="F262" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H262" s="8" t="s">
-        <v>134</v>
+        <v>17</v>
+      </c>
+      <c r="F262" t="s">
+        <v>9</v>
+      </c>
+      <c r="H262" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="I262" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="263" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D263" s="9"/>
-      <c r="E263" t="s">
-        <v>137</v>
-      </c>
-      <c r="F263" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H263" s="8" t="s">
-        <v>138</v>
+      <c r="I263" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="264" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D264" s="9"/>
-      <c r="H264" s="8"/>
-    </row>
-    <row r="265" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B265" t="s">
-        <v>128</v>
-      </c>
-      <c r="C265" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D265" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="E265" t="s">
-        <v>15</v>
-      </c>
-      <c r="F265" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G265" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H265" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I265" s="7" t="s">
-        <v>140</v>
+      <c r="I264" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="265" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D265" s="9"/>
+      <c r="I265" s="25" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="266" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D266" s="9"/>
-      <c r="E266" t="s">
-        <v>17</v>
-      </c>
-      <c r="F266" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G266" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H266" s="8">
-        <v>20210331</v>
+      <c r="E266" s="24"/>
+      <c r="H266" s="18"/>
+      <c r="I266" s="18" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="267" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D267" s="9"/>
-      <c r="E267" t="s">
-        <v>141</v>
-      </c>
-      <c r="F267" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H267" s="8" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="268" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D268" s="9"/>
+    </row>
+    <row r="268" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B268" t="s">
+        <v>128</v>
+      </c>
+      <c r="C268" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D268" s="9" t="s">
+        <v>129</v>
+      </c>
       <c r="E268" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="F268" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H268" s="8" t="s">
-        <v>28</v>
+      <c r="G268" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H268" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I268" s="7" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="269" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D269" s="9"/>
       <c r="E269" t="s">
-        <v>144</v>
+        <v>17</v>
       </c>
       <c r="F269" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="G269" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="H269" s="8">
-        <v>512573</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="270" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D270" s="9"/>
+      <c r="F270" s="9"/>
       <c r="H270" s="8"/>
     </row>
     <row r="271" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4413,7 +4359,7 @@
         <v>245</v>
       </c>
       <c r="D271" s="9" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="E271" t="s">
         <v>15</v>
@@ -4428,7 +4374,7 @@
         <v>20200401</v>
       </c>
       <c r="I271" s="7" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="272" spans="2:9" x14ac:dyDescent="0.3">
@@ -4448,59 +4394,50 @@
     </row>
     <row r="273" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D273" s="9"/>
-      <c r="H273" s="8"/>
-    </row>
-    <row r="274" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B274" t="s">
-        <v>128</v>
-      </c>
-      <c r="C274" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D274" s="9" t="s">
-        <v>147</v>
-      </c>
+      <c r="E273" t="s">
+        <v>133</v>
+      </c>
+      <c r="F273" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="H273" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="274" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D274" s="9"/>
       <c r="E274" t="s">
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="F274" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G274" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H274" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I274" s="7" t="s">
-        <v>148</v>
+        <v>119</v>
+      </c>
+      <c r="H274" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="275" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D275" s="9"/>
       <c r="E275" t="s">
-        <v>17</v>
+        <v>136</v>
       </c>
       <c r="F275" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G275" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H275" s="8">
-        <v>20210331</v>
+        <v>119</v>
+      </c>
+      <c r="H275" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="276" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D276" s="9"/>
       <c r="E276" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="F276" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H276" s="8">
-        <v>500425</v>
+      <c r="H276" s="8" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="277" spans="2:9" x14ac:dyDescent="0.3">
@@ -4515,10 +4452,10 @@
         <v>245</v>
       </c>
       <c r="D278" s="9" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
       <c r="E278" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="F278" s="9" t="s">
         <v>23</v>
@@ -4526,395 +4463,578 @@
       <c r="G278" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H278" s="16">
-        <v>20220228</v>
+      <c r="H278" s="8">
+        <v>20200401</v>
       </c>
       <c r="I278" s="7" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="279" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D279" s="9"/>
       <c r="E279" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="F279" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H279" s="8" t="s">
-        <v>152</v>
+      <c r="G279" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H279" s="8">
+        <v>20210331</v>
       </c>
     </row>
     <row r="280" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D280" s="9"/>
       <c r="E280" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="F280" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H280" s="8" t="s">
-        <v>25</v>
+        <v>142</v>
       </c>
     </row>
     <row r="281" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D281" s="9"/>
       <c r="E281" t="s">
-        <v>35</v>
+        <v>143</v>
       </c>
       <c r="F281" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H281" s="8" t="s">
-        <v>153</v>
+        <v>28</v>
       </c>
     </row>
     <row r="282" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D282" s="9"/>
       <c r="E282" t="s">
-        <v>75</v>
+        <v>144</v>
       </c>
       <c r="F282" s="9" t="s">
-        <v>154</v>
+        <v>23</v>
       </c>
       <c r="H282" s="8">
-        <v>4</v>
+        <v>512573</v>
       </c>
     </row>
     <row r="283" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D283" s="9"/>
-      <c r="E283" t="s">
-        <v>155</v>
-      </c>
-      <c r="F283" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="H283" s="8">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="284" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D284" s="9"/>
+      <c r="H283" s="8"/>
+    </row>
+    <row r="284" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B284" t="s">
+        <v>128</v>
+      </c>
+      <c r="C284" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D284" s="9" t="s">
+        <v>145</v>
+      </c>
       <c r="E284" t="s">
-        <v>156</v>
+        <v>15</v>
       </c>
       <c r="F284" s="9" t="s">
-        <v>154</v>
+        <v>23</v>
+      </c>
+      <c r="G284" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H284" s="8">
-        <v>1.1000000000000001</v>
+        <v>20200401</v>
+      </c>
+      <c r="I284" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="285" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D285" s="9"/>
       <c r="E285" t="s">
-        <v>157</v>
+        <v>17</v>
       </c>
       <c r="F285" s="9" t="s">
-        <v>154</v>
+        <v>23</v>
+      </c>
+      <c r="G285" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H285" s="8">
-        <v>3.2</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="286" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D286" s="9"/>
-      <c r="E286" t="s">
-        <v>158</v>
-      </c>
-      <c r="F286" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="H286" s="8">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="287" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D287" s="9"/>
+      <c r="H286" s="8"/>
+    </row>
+    <row r="287" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B287" t="s">
+        <v>128</v>
+      </c>
+      <c r="C287" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D287" s="9" t="s">
+        <v>147</v>
+      </c>
       <c r="E287" t="s">
-        <v>159</v>
+        <v>15</v>
       </c>
       <c r="F287" s="9" t="s">
-        <v>154</v>
+        <v>23</v>
+      </c>
+      <c r="G287" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H287" s="8">
-        <v>0.2</v>
+        <v>20200401</v>
+      </c>
+      <c r="I287" s="7" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="288" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D288" s="9"/>
       <c r="E288" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
       <c r="F288" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="G288" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="H288" s="8">
-        <v>500820</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="289" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D289" s="9"/>
-    </row>
-    <row r="290" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B290" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D290" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E290" s="1"/>
-      <c r="F290" s="1"/>
-      <c r="G290" s="1"/>
-      <c r="H290" s="3"/>
-      <c r="I290" s="13" t="s">
-        <v>78</v>
-      </c>
+      <c r="E289" t="s">
+        <v>149</v>
+      </c>
+      <c r="F289" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H289" s="8">
+        <v>500425</v>
+      </c>
+    </row>
+    <row r="290" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D290" s="9"/>
+      <c r="H290" s="8"/>
     </row>
     <row r="291" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B291" s="1"/>
-      <c r="C291" s="1"/>
-      <c r="D291" s="10"/>
-      <c r="E291" s="1"/>
-      <c r="F291" s="1"/>
-      <c r="G291" s="1"/>
-      <c r="H291" s="12"/>
-      <c r="I291" s="13"/>
-    </row>
-    <row r="292" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B292" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C292" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D292" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E292" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F292" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G292" s="1"/>
-      <c r="H292" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I292" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="293" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B293" s="1"/>
-      <c r="C293" s="1"/>
-      <c r="D293" s="10"/>
-      <c r="E293" s="1"/>
-      <c r="F293" s="1"/>
-      <c r="G293" s="1"/>
-      <c r="H293" s="3"/>
-      <c r="I293" s="13"/>
-    </row>
-    <row r="294" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B294" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C294" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D294" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="E294" s="1"/>
-      <c r="F294" s="1"/>
-      <c r="G294" s="1"/>
-      <c r="H294" s="3"/>
-      <c r="I294" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="295" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B295" s="1"/>
-      <c r="C295" s="1"/>
-      <c r="D295" s="10"/>
-      <c r="E295" s="1"/>
-      <c r="F295" s="1"/>
-      <c r="G295" s="1"/>
-      <c r="H295" s="3"/>
-      <c r="I295" s="13"/>
-    </row>
-    <row r="296" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B296" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C296" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D296" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E296" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F296" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G296" s="1"/>
-      <c r="H296" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I296" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="297" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B297" s="1"/>
-      <c r="C297" s="1"/>
-      <c r="D297" s="10"/>
-      <c r="E297" s="1"/>
-      <c r="F297" s="1"/>
-      <c r="G297" s="1"/>
-      <c r="H297" s="3"/>
-      <c r="I297" s="13"/>
-    </row>
-    <row r="298" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B298" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C298" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D298" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="E298" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="F298" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G298" s="1"/>
-      <c r="H298" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I298" s="7" t="s">
-        <v>87</v>
+      <c r="B291" t="s">
+        <v>128</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D291" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E291" t="s">
+        <v>22</v>
+      </c>
+      <c r="F291" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G291" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H291" s="16">
+        <v>20220228</v>
+      </c>
+      <c r="I291" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="292" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D292" s="9"/>
+      <c r="E292" t="s">
+        <v>37</v>
+      </c>
+      <c r="F292" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H292" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="293" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D293" s="9"/>
+      <c r="E293" t="s">
+        <v>24</v>
+      </c>
+      <c r="F293" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H293" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="294" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D294" s="9"/>
+      <c r="E294" t="s">
+        <v>35</v>
+      </c>
+      <c r="F294" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H294" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="295" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D295" s="9"/>
+      <c r="E295" t="s">
+        <v>75</v>
+      </c>
+      <c r="F295" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H295" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="296" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D296" s="9"/>
+      <c r="E296" t="s">
+        <v>155</v>
+      </c>
+      <c r="F296" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H296" s="8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="297" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D297" s="9"/>
+      <c r="E297" t="s">
+        <v>156</v>
+      </c>
+      <c r="F297" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H297" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="298" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D298" s="9"/>
+      <c r="E298" t="s">
+        <v>157</v>
+      </c>
+      <c r="F298" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H298" s="8">
+        <v>3.2</v>
       </c>
     </row>
     <row r="299" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B299" s="1"/>
-      <c r="C299" s="1"/>
-      <c r="D299" s="10"/>
-      <c r="E299" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F299" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G299" s="1"/>
-      <c r="H299" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I299" s="1"/>
+      <c r="D299" s="9"/>
+      <c r="E299" t="s">
+        <v>158</v>
+      </c>
+      <c r="F299" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H299" s="8">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="300" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B300" s="1"/>
-      <c r="C300" s="1"/>
-      <c r="D300" s="10"/>
-      <c r="E300" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F300" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G300" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H300" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I300" s="1"/>
+      <c r="D300" s="9"/>
+      <c r="E300" t="s">
+        <v>159</v>
+      </c>
+      <c r="F300" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="H300" s="8">
+        <v>0.2</v>
+      </c>
     </row>
     <row r="301" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B301" s="1"/>
-      <c r="C301" s="1"/>
-      <c r="D301" s="10"/>
-      <c r="E301" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F301" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G301" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H301" s="3">
-        <v>20200331</v>
-      </c>
-      <c r="I301" s="1"/>
+      <c r="D301" s="9"/>
+      <c r="E301" t="s">
+        <v>149</v>
+      </c>
+      <c r="F301" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H301" s="8">
+        <v>500820</v>
+      </c>
     </row>
     <row r="302" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D302" s="9"/>
     </row>
-    <row r="303" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D303" s="9"/>
-    </row>
-    <row r="304" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D304" s="9"/>
-    </row>
-    <row r="305" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D305" s="9"/>
-    </row>
-    <row r="306" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D306" s="9"/>
-    </row>
-    <row r="307" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D307" s="9"/>
-    </row>
-    <row r="308" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D308" s="9"/>
-    </row>
-    <row r="309" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D309" s="9"/>
-    </row>
-    <row r="310" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D310" s="9"/>
-    </row>
-    <row r="311" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D311" s="9"/>
-    </row>
-    <row r="312" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D312" s="9"/>
-    </row>
-    <row r="313" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D313" s="9"/>
-    </row>
-    <row r="314" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D314" s="9"/>
-    </row>
-    <row r="315" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="303" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B303" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D303" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E303" s="1"/>
+      <c r="F303" s="1"/>
+      <c r="G303" s="1"/>
+      <c r="H303" s="3"/>
+      <c r="I303" s="13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="304" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B304" s="1"/>
+      <c r="C304" s="1"/>
+      <c r="D304" s="10"/>
+      <c r="E304" s="1"/>
+      <c r="F304" s="1"/>
+      <c r="G304" s="1"/>
+      <c r="H304" s="12"/>
+      <c r="I304" s="13"/>
+    </row>
+    <row r="305" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B305" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C305" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D305" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E305" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F305" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G305" s="1"/>
+      <c r="H305" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I305" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="306" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B306" s="1"/>
+      <c r="C306" s="1"/>
+      <c r="D306" s="10"/>
+      <c r="E306" s="1"/>
+      <c r="F306" s="1"/>
+      <c r="G306" s="1"/>
+      <c r="H306" s="3"/>
+      <c r="I306" s="13"/>
+    </row>
+    <row r="307" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B307" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C307" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D307" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E307" s="1"/>
+      <c r="F307" s="1"/>
+      <c r="G307" s="1"/>
+      <c r="H307" s="3"/>
+      <c r="I307" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="308" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B308" s="1"/>
+      <c r="C308" s="1"/>
+      <c r="D308" s="10"/>
+      <c r="E308" s="1"/>
+      <c r="F308" s="1"/>
+      <c r="G308" s="1"/>
+      <c r="H308" s="3"/>
+      <c r="I308" s="13"/>
+    </row>
+    <row r="309" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B309" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D309" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E309" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F309" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G309" s="1"/>
+      <c r="H309" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I309" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="310" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B310" s="1"/>
+      <c r="C310" s="1"/>
+      <c r="D310" s="10"/>
+      <c r="E310" s="1"/>
+      <c r="F310" s="1"/>
+      <c r="G310" s="1"/>
+      <c r="H310" s="3"/>
+      <c r="I310" s="13"/>
+    </row>
+    <row r="311" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B311" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C311" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D311" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E311" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F311" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G311" s="1"/>
+      <c r="H311" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I311" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="312" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B312" s="1"/>
+      <c r="C312" s="1"/>
+      <c r="D312" s="10"/>
+      <c r="E312" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F312" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G312" s="1"/>
+      <c r="H312" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="I312" s="1"/>
+    </row>
+    <row r="313" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B313" s="1"/>
+      <c r="C313" s="1"/>
+      <c r="D313" s="10"/>
+      <c r="E313" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F313" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G313" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H313" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I313" s="1"/>
+    </row>
+    <row r="314" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B314" s="1"/>
+      <c r="C314" s="1"/>
+      <c r="D314" s="10"/>
+      <c r="E314" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F314" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G314" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H314" s="3">
+        <v>20200331</v>
+      </c>
+      <c r="I314" s="1"/>
+    </row>
+    <row r="315" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D315" s="9"/>
     </row>
-    <row r="316" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="316" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D316" s="9"/>
     </row>
-    <row r="317" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D317" s="9"/>
     </row>
-    <row r="318" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="318" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D318" s="9"/>
     </row>
-    <row r="319" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="319" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D319" s="9"/>
     </row>
-    <row r="320" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D320" s="9"/>
     </row>
     <row r="321" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D321" s="9"/>
+    </row>
+    <row r="322" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D322" s="9"/>
+    </row>
+    <row r="323" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D323" s="9"/>
+    </row>
+    <row r="324" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D324" s="9"/>
+    </row>
+    <row r="325" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D325" s="9"/>
+    </row>
+    <row r="326" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D326" s="9"/>
+    </row>
+    <row r="327" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D327" s="9"/>
+    </row>
+    <row r="328" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D328" s="9"/>
+    </row>
+    <row r="329" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D329" s="9"/>
+    </row>
+    <row r="330" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D330" s="9"/>
+    </row>
+    <row r="331" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D331" s="9"/>
+    </row>
+    <row r="332" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D332" s="9"/>
+    </row>
+    <row r="333" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D333" s="9"/>
+    </row>
+    <row r="334" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D334" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
create api Margin and update document
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="856" uniqueCount="325">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -1014,6 +1014,9 @@
   </si>
   <si>
     <t>Family_Transaction_DetailsJson</t>
+  </si>
+  <si>
+    <t>[ { "ExchSeg": "MCX-COMM", "fm_TotalMrgn": 29007.75, "Collected": 89799.23, "TotalShort": 0.00, "TotalShortPER": 0.00, "Tmp_NFiller4": 0.00, "Tmp_PeakMargin": 0.00, "Tmp_NFiller5": 0.00, "PeakShort": 0.00, "Tmp_HighestShortFall": 0.00, "ShortPenalty": 0.00 } ]</t>
   </si>
 </sst>
 </file>
@@ -1479,10 +1482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I371"/>
+  <dimension ref="A1:I372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A238" workbookViewId="0">
-      <selection activeCell="D251" sqref="D251"/>
+    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
+      <selection activeCell="F275" sqref="F275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4450,116 +4453,118 @@
     <row r="274" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D274" s="9"/>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D275" s="9"/>
+    <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B275" t="s">
+        <v>62</v>
+      </c>
+      <c r="C275" t="s">
+        <v>278</v>
+      </c>
+      <c r="D275" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E275" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="F275" t="s">
+        <v>9</v>
+      </c>
+      <c r="H275" s="8">
+        <v>20191101</v>
+      </c>
+      <c r="I275" s="26" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B276" s="1" t="s">
+      <c r="D276" s="9"/>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B277" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C276" s="1" t="s">
+      <c r="C277" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D276" s="9" t="s">
+      <c r="D277" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="E276" t="s">
+      <c r="E277" t="s">
         <v>15</v>
       </c>
-      <c r="F276" t="s">
-        <v>9</v>
-      </c>
-      <c r="H276" s="17" t="s">
+      <c r="F277" t="s">
+        <v>9</v>
+      </c>
+      <c r="H277" s="17" t="s">
         <v>171</v>
       </c>
-      <c r="I276" t="s">
+      <c r="I277" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D277" s="9"/>
-      <c r="E277" t="s">
-        <v>17</v>
-      </c>
-      <c r="F277" t="s">
-        <v>9</v>
-      </c>
-      <c r="H277" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="I277" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D278" s="9"/>
+      <c r="E278" t="s">
+        <v>17</v>
+      </c>
+      <c r="F278" t="s">
+        <v>9</v>
+      </c>
+      <c r="H278" s="17" t="s">
+        <v>173</v>
+      </c>
       <c r="I278" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D279" s="9"/>
       <c r="I279" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D280" s="9"/>
       <c r="I280" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D281" s="9"/>
-      <c r="I281" s="19" t="s">
-        <v>230</v>
+      <c r="I281" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D282" s="9"/>
-      <c r="I282" t="s">
-        <v>188</v>
+      <c r="I282" s="19" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D283" s="9"/>
-    </row>
-    <row r="284" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A284" s="1">
+      <c r="I283" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D284" s="9"/>
+    </row>
+    <row r="285" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A285" s="1">
         <v>36</v>
       </c>
-      <c r="B284" s="1" t="s">
+      <c r="B285" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C284" s="1" t="s">
+      <c r="C285" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D284" s="10" t="s">
+      <c r="D285" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="E284" s="1" t="s">
+      <c r="E285" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F284" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G284" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H284" s="15">
-        <v>20200401</v>
-      </c>
-      <c r="I284" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="285" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A285" s="1"/>
-      <c r="B285" s="1"/>
-      <c r="C285" s="1"/>
-      <c r="D285" s="10"/>
-      <c r="E285" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="F285" s="1" t="s">
         <v>9</v>
@@ -4567,246 +4572,249 @@
       <c r="G285" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H285" s="6">
-        <v>20210331</v>
-      </c>
-      <c r="I285" s="1"/>
-    </row>
-    <row r="286" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H285" s="15">
+        <v>20200401</v>
+      </c>
+      <c r="I285" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A286" s="1"/>
       <c r="B286" s="1"/>
       <c r="C286" s="1"/>
       <c r="D286" s="10"/>
       <c r="E286" s="1" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="F286" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G286" s="1"/>
-      <c r="H286" s="3">
-        <v>533271</v>
-      </c>
-      <c r="I286" s="13"/>
+      <c r="G286" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H286" s="6">
+        <v>20210331</v>
+      </c>
+      <c r="I286" s="1"/>
     </row>
     <row r="287" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A287" s="1"/>
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
       <c r="D287" s="10"/>
-      <c r="E287" s="1"/>
-      <c r="F287" s="1"/>
+      <c r="E287" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F287" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G287" s="1"/>
-      <c r="H287" s="3"/>
+      <c r="H287" s="3">
+        <v>533271</v>
+      </c>
       <c r="I287" s="13"/>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B288" s="1" t="s">
+    <row r="288" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A288" s="1"/>
+      <c r="B288" s="1"/>
+      <c r="C288" s="1"/>
+      <c r="D288" s="10"/>
+      <c r="E288" s="1"/>
+      <c r="F288" s="1"/>
+      <c r="G288" s="1"/>
+      <c r="H288" s="3"/>
+      <c r="I288" s="13"/>
+    </row>
+    <row r="289" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B289" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C288" s="1" t="s">
+      <c r="C289" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D288" s="9" t="s">
+      <c r="D289" s="9" t="s">
         <v>240</v>
       </c>
-      <c r="E288" t="s">
+      <c r="E289" t="s">
         <v>27</v>
       </c>
-      <c r="F288" t="s">
-        <v>9</v>
-      </c>
-      <c r="H288" t="s">
+      <c r="F289" t="s">
+        <v>9</v>
+      </c>
+      <c r="H289" t="s">
         <v>232</v>
       </c>
-      <c r="I288" t="s">
+      <c r="I289" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="289" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D289" s="9"/>
-      <c r="E289" t="s">
-        <v>48</v>
-      </c>
-      <c r="F289" t="s">
-        <v>9</v>
-      </c>
-      <c r="H289" t="s">
-        <v>233</v>
-      </c>
-      <c r="I289" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="290" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D290" s="9"/>
       <c r="E290" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="F290" t="s">
         <v>9</v>
       </c>
-      <c r="H290" s="17" t="s">
-        <v>171</v>
+      <c r="H290" t="s">
+        <v>233</v>
       </c>
       <c r="I290" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="291" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D291" s="9"/>
       <c r="E291" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F291" t="s">
         <v>9</v>
       </c>
       <c r="H291" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I291" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="292" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D292" s="9"/>
+      <c r="E292" t="s">
+        <v>17</v>
+      </c>
+      <c r="F292" t="s">
+        <v>9</v>
+      </c>
+      <c r="H292" s="17" t="s">
+        <v>173</v>
+      </c>
       <c r="I292" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="293" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D293" s="9"/>
-      <c r="I293" s="19" t="s">
-        <v>234</v>
+      <c r="I293" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="294" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D294" s="9"/>
       <c r="I294" s="19" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="295" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D295" s="9"/>
-      <c r="I295" t="s">
-        <v>188</v>
+      <c r="I295" s="19" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="296" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D296" s="9"/>
+      <c r="I296" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="297" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B297" s="1" t="s">
+      <c r="D297" s="9"/>
+    </row>
+    <row r="298" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B298" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C297" s="1" t="s">
+      <c r="C298" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D297" s="9" t="s">
+      <c r="D298" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="E297" t="s">
+      <c r="E298" t="s">
         <v>27</v>
       </c>
-      <c r="F297" t="s">
-        <v>9</v>
-      </c>
-      <c r="H297" t="s">
+      <c r="F298" t="s">
+        <v>9</v>
+      </c>
+      <c r="H298" t="s">
         <v>236</v>
       </c>
-      <c r="I297" t="s">
+      <c r="I298" t="s">
         <v>164</v>
-      </c>
-    </row>
-    <row r="298" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D298" s="9"/>
-      <c r="E298" t="s">
-        <v>15</v>
-      </c>
-      <c r="F298" t="s">
-        <v>9</v>
-      </c>
-      <c r="H298" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="I298" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="299" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D299" s="9"/>
       <c r="E299" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F299" t="s">
         <v>9</v>
       </c>
       <c r="H299" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I299" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="300" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D300" s="9"/>
+      <c r="E300" t="s">
+        <v>17</v>
+      </c>
+      <c r="F300" t="s">
+        <v>9</v>
+      </c>
+      <c r="H300" s="17" t="s">
+        <v>173</v>
+      </c>
       <c r="I300" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="301" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D301" s="9"/>
       <c r="I301" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="302" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D302" s="9"/>
-      <c r="I302" s="25" t="s">
-        <v>237</v>
+      <c r="I302" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="303" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D303" s="9"/>
-      <c r="E303" s="24"/>
-      <c r="H303" s="18"/>
-      <c r="I303" s="18" t="s">
-        <v>188</v>
+      <c r="I303" s="25" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="304" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D304" s="9"/>
-    </row>
-    <row r="305" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B305" t="s">
+      <c r="E304" s="24"/>
+      <c r="H304" s="18"/>
+      <c r="I304" s="18" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="305" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D305" s="9"/>
+    </row>
+    <row r="306" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B306" t="s">
         <v>128</v>
       </c>
-      <c r="C305" s="1" t="s">
+      <c r="C306" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D305" s="9" t="s">
+      <c r="D306" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="E305" t="s">
+      <c r="E306" t="s">
         <v>15</v>
-      </c>
-      <c r="F305" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G305" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H305" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I305" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="306" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D306" s="9"/>
-      <c r="E306" t="s">
-        <v>17</v>
       </c>
       <c r="F306" s="9" t="s">
         <v>23</v>
@@ -4815,44 +4823,44 @@
         <v>16</v>
       </c>
       <c r="H306" s="8">
-        <v>20210331</v>
+        <v>20200401</v>
+      </c>
+      <c r="I306" s="7" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D307" s="9"/>
-      <c r="F307" s="9"/>
-      <c r="H307" s="8"/>
-    </row>
-    <row r="308" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B308" t="s">
+      <c r="E307" t="s">
+        <v>17</v>
+      </c>
+      <c r="F307" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G307" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H307" s="8">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="308" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D308" s="9"/>
+      <c r="F308" s="9"/>
+      <c r="H308" s="8"/>
+    </row>
+    <row r="309" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B309" t="s">
         <v>128</v>
       </c>
-      <c r="C308" s="1" t="s">
+      <c r="C309" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D308" s="9" t="s">
+      <c r="D309" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="E308" t="s">
+      <c r="E309" t="s">
         <v>15</v>
-      </c>
-      <c r="F308" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G308" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H308" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I308" s="7" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="309" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D309" s="9"/>
-      <c r="E309" t="s">
-        <v>17</v>
       </c>
       <c r="F309" s="9" t="s">
         <v>23</v>
@@ -4861,25 +4869,31 @@
         <v>16</v>
       </c>
       <c r="H309" s="8">
-        <v>20210331</v>
+        <v>20200401</v>
+      </c>
+      <c r="I309" s="7" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D310" s="9"/>
       <c r="E310" t="s">
-        <v>133</v>
+        <v>17</v>
       </c>
       <c r="F310" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H310" s="8" t="s">
-        <v>134</v>
+        <v>23</v>
+      </c>
+      <c r="G310" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H310" s="8">
+        <v>20210331</v>
       </c>
     </row>
     <row r="311" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D311" s="9"/>
       <c r="E311" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F311" s="9" t="s">
         <v>119</v>
@@ -4891,7 +4905,7 @@
     <row r="312" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D312" s="9"/>
       <c r="E312" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F312" s="9" t="s">
         <v>119</v>
@@ -4903,49 +4917,43 @@
     <row r="313" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D313" s="9"/>
       <c r="E313" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F313" s="9" t="s">
-        <v>23</v>
+        <v>119</v>
       </c>
       <c r="H313" s="8" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="314" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D314" s="9"/>
-      <c r="H314" s="8"/>
-    </row>
-    <row r="315" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B315" t="s">
+      <c r="E314" t="s">
+        <v>137</v>
+      </c>
+      <c r="F314" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H314" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="315" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D315" s="9"/>
+      <c r="H315" s="8"/>
+    </row>
+    <row r="316" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B316" t="s">
         <v>128</v>
       </c>
-      <c r="C315" s="1" t="s">
+      <c r="C316" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D315" s="9" t="s">
+      <c r="D316" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="E315" t="s">
+      <c r="E316" t="s">
         <v>15</v>
-      </c>
-      <c r="F315" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G315" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H315" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I315" s="7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="316" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D316" s="9"/>
-      <c r="E316" t="s">
-        <v>17</v>
       </c>
       <c r="F316" s="9" t="s">
         <v>23</v>
@@ -4954,79 +4962,79 @@
         <v>16</v>
       </c>
       <c r="H316" s="8">
-        <v>20210331</v>
+        <v>20200401</v>
+      </c>
+      <c r="I316" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D317" s="9"/>
       <c r="E317" t="s">
-        <v>141</v>
+        <v>17</v>
       </c>
       <c r="F317" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H317" s="8" t="s">
-        <v>142</v>
+      <c r="G317" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H317" s="8">
+        <v>20210331</v>
       </c>
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D318" s="9"/>
       <c r="E318" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F318" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H318" s="8" t="s">
-        <v>28</v>
+        <v>142</v>
       </c>
     </row>
     <row r="319" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D319" s="9"/>
       <c r="E319" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F319" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H319" s="8">
-        <v>512573</v>
+      <c r="H319" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="320" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D320" s="9"/>
-      <c r="H320" s="8"/>
-    </row>
-    <row r="321" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B321" t="s">
+      <c r="E320" t="s">
+        <v>144</v>
+      </c>
+      <c r="F320" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H320" s="8">
+        <v>512573</v>
+      </c>
+    </row>
+    <row r="321" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D321" s="9"/>
+      <c r="H321" s="8"/>
+    </row>
+    <row r="322" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B322" t="s">
         <v>128</v>
       </c>
-      <c r="C321" s="1" t="s">
+      <c r="C322" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D321" s="9" t="s">
+      <c r="D322" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="E321" t="s">
+      <c r="E322" t="s">
         <v>15</v>
-      </c>
-      <c r="F321" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G321" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H321" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I321" s="7" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="322" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D322" s="9"/>
-      <c r="E322" t="s">
-        <v>17</v>
       </c>
       <c r="F322" s="9" t="s">
         <v>23</v>
@@ -5035,43 +5043,43 @@
         <v>16</v>
       </c>
       <c r="H322" s="8">
-        <v>20210331</v>
+        <v>20200401</v>
+      </c>
+      <c r="I322" s="7" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D323" s="9"/>
-      <c r="H323" s="8"/>
-    </row>
-    <row r="324" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B324" t="s">
+      <c r="E323" t="s">
+        <v>17</v>
+      </c>
+      <c r="F323" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G323" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H323" s="8">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="324" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D324" s="9"/>
+      <c r="H324" s="8"/>
+    </row>
+    <row r="325" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B325" t="s">
         <v>128</v>
       </c>
-      <c r="C324" s="1" t="s">
+      <c r="C325" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D324" s="9" t="s">
+      <c r="D325" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="E324" t="s">
+      <c r="E325" t="s">
         <v>15</v>
-      </c>
-      <c r="F324" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G324" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H324" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I324" s="7" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="325" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D325" s="9"/>
-      <c r="E325" t="s">
-        <v>17</v>
       </c>
       <c r="F325" s="9" t="s">
         <v>23</v>
@@ -5080,353 +5088,353 @@
         <v>16</v>
       </c>
       <c r="H325" s="8">
-        <v>20210331</v>
+        <v>20200401</v>
+      </c>
+      <c r="I325" s="7" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="326" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D326" s="9"/>
       <c r="E326" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
       <c r="F326" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="G326" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="H326" s="8">
-        <v>500425</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="327" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D327" s="9"/>
-      <c r="H327" s="8"/>
-    </row>
-    <row r="328" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B328" t="s">
+      <c r="E327" t="s">
+        <v>149</v>
+      </c>
+      <c r="F327" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H327" s="8">
+        <v>500425</v>
+      </c>
+    </row>
+    <row r="328" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D328" s="9"/>
+      <c r="H328" s="8"/>
+    </row>
+    <row r="329" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B329" t="s">
         <v>128</v>
       </c>
-      <c r="C328" s="1" t="s">
+      <c r="C329" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D328" s="9" t="s">
+      <c r="D329" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="E328" t="s">
+      <c r="E329" t="s">
         <v>22</v>
-      </c>
-      <c r="F328" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G328" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H328" s="16">
-        <v>20220228</v>
-      </c>
-      <c r="I328" s="7" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="329" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D329" s="9"/>
-      <c r="E329" t="s">
-        <v>37</v>
       </c>
       <c r="F329" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H329" s="8" t="s">
-        <v>152</v>
+      <c r="G329" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H329" s="16">
+        <v>20220228</v>
+      </c>
+      <c r="I329" s="7" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="330" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D330" s="9"/>
       <c r="E330" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F330" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H330" s="8" t="s">
-        <v>25</v>
+        <v>152</v>
       </c>
     </row>
     <row r="331" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D331" s="9"/>
       <c r="E331" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="F331" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H331" s="8" t="s">
-        <v>153</v>
+        <v>25</v>
       </c>
     </row>
     <row r="332" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D332" s="9"/>
       <c r="E332" t="s">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="F332" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="H332" s="8">
-        <v>4</v>
+        <v>23</v>
+      </c>
+      <c r="H332" s="8" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="333" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D333" s="9"/>
       <c r="E333" t="s">
-        <v>155</v>
+        <v>75</v>
       </c>
       <c r="F333" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H333" s="8">
-        <v>48</v>
+        <v>4</v>
       </c>
     </row>
     <row r="334" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D334" s="9"/>
       <c r="E334" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F334" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H334" s="8">
-        <v>1.1000000000000001</v>
+        <v>48</v>
       </c>
     </row>
     <row r="335" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D335" s="9"/>
       <c r="E335" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F335" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H335" s="8">
-        <v>3.2</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="336" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D336" s="9"/>
       <c r="E336" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F336" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H336" s="8">
-        <v>0.11</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="337" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D337" s="9"/>
       <c r="E337" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F337" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H337" s="8">
-        <v>0.2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="338" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D338" s="9"/>
       <c r="E338" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="F338" s="9" t="s">
-        <v>23</v>
+        <v>154</v>
       </c>
       <c r="H338" s="8">
-        <v>500820</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="339" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D339" s="9"/>
-    </row>
-    <row r="340" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B340" s="1" t="s">
+      <c r="E339" t="s">
+        <v>149</v>
+      </c>
+      <c r="F339" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H339" s="8">
+        <v>500820</v>
+      </c>
+    </row>
+    <row r="340" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D340" s="9"/>
+    </row>
+    <row r="341" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B341" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C340" s="1" t="s">
+      <c r="C341" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D340" s="10" t="s">
+      <c r="D341" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E340" s="1"/>
-      <c r="F340" s="1"/>
-      <c r="G340" s="1"/>
-      <c r="H340" s="3"/>
-      <c r="I340" s="13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="341" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B341" s="1"/>
-      <c r="C341" s="1"/>
-      <c r="D341" s="10"/>
       <c r="E341" s="1"/>
       <c r="F341" s="1"/>
       <c r="G341" s="1"/>
-      <c r="H341" s="12"/>
-      <c r="I341" s="13"/>
+      <c r="H341" s="3"/>
+      <c r="I341" s="13" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="342" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B342" s="1" t="s">
+      <c r="B342" s="1"/>
+      <c r="C342" s="1"/>
+      <c r="D342" s="10"/>
+      <c r="E342" s="1"/>
+      <c r="F342" s="1"/>
+      <c r="G342" s="1"/>
+      <c r="H342" s="12"/>
+      <c r="I342" s="13"/>
+    </row>
+    <row r="343" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B343" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C342" s="1" t="s">
+      <c r="C343" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D342" s="10" t="s">
+      <c r="D343" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E342" s="1" t="s">
+      <c r="E343" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F342" s="10" t="s">
+      <c r="F343" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G342" s="1"/>
-      <c r="H342" s="3" t="s">
+      <c r="G343" s="1"/>
+      <c r="H343" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I342" s="7" t="s">
+      <c r="I343" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="343" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B343" s="1"/>
-      <c r="C343" s="1"/>
-      <c r="D343" s="10"/>
-      <c r="E343" s="1"/>
-      <c r="F343" s="1"/>
-      <c r="G343" s="1"/>
-      <c r="H343" s="3"/>
-      <c r="I343" s="13"/>
-    </row>
     <row r="344" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B344" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C344" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D344" s="10" t="s">
-        <v>83</v>
-      </c>
+      <c r="B344" s="1"/>
+      <c r="C344" s="1"/>
+      <c r="D344" s="10"/>
       <c r="E344" s="1"/>
       <c r="F344" s="1"/>
       <c r="G344" s="1"/>
       <c r="H344" s="3"/>
-      <c r="I344" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="I344" s="13"/>
     </row>
     <row r="345" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B345" s="1"/>
-      <c r="C345" s="1"/>
-      <c r="D345" s="10"/>
+      <c r="B345" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C345" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D345" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="E345" s="1"/>
       <c r="F345" s="1"/>
       <c r="G345" s="1"/>
       <c r="H345" s="3"/>
-      <c r="I345" s="13"/>
+      <c r="I345" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="346" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B346" s="1" t="s">
+      <c r="B346" s="1"/>
+      <c r="C346" s="1"/>
+      <c r="D346" s="10"/>
+      <c r="E346" s="1"/>
+      <c r="F346" s="1"/>
+      <c r="G346" s="1"/>
+      <c r="H346" s="3"/>
+      <c r="I346" s="13"/>
+    </row>
+    <row r="347" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B347" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C346" s="1" t="s">
+      <c r="C347" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D346" s="10" t="s">
+      <c r="D347" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E346" s="1" t="s">
+      <c r="E347" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F346" s="10" t="s">
+      <c r="F347" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G346" s="1"/>
-      <c r="H346" s="3" t="s">
+      <c r="G347" s="1"/>
+      <c r="H347" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I346" s="7" t="s">
+      <c r="I347" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="347" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B347" s="1"/>
-      <c r="C347" s="1"/>
-      <c r="D347" s="10"/>
-      <c r="E347" s="1"/>
-      <c r="F347" s="1"/>
-      <c r="G347" s="1"/>
-      <c r="H347" s="3"/>
-      <c r="I347" s="13"/>
-    </row>
     <row r="348" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B348" s="1" t="s">
+      <c r="B348" s="1"/>
+      <c r="C348" s="1"/>
+      <c r="D348" s="10"/>
+      <c r="E348" s="1"/>
+      <c r="F348" s="1"/>
+      <c r="G348" s="1"/>
+      <c r="H348" s="3"/>
+      <c r="I348" s="13"/>
+    </row>
+    <row r="349" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B349" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C348" s="1" t="s">
+      <c r="C349" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D348" s="10" t="s">
+      <c r="D349" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="E348" s="1" t="s">
+      <c r="E349" s="1" t="s">
         <v>86</v>
-      </c>
-      <c r="F348" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G348" s="1"/>
-      <c r="H348" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I348" s="7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="349" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B349" s="1"/>
-      <c r="C349" s="1"/>
-      <c r="D349" s="10"/>
-      <c r="E349" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F349" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G349" s="1"/>
       <c r="H349" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="I349" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="I349" s="7" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="350" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B350" s="1"/>
       <c r="C350" s="1"/>
       <c r="D350" s="10"/>
       <c r="E350" s="1" t="s">
-        <v>15</v>
+        <v>88</v>
       </c>
       <c r="F350" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G350" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="G350" s="1"/>
       <c r="H350" s="3" t="s">
-        <v>14</v>
+        <v>89</v>
       </c>
       <c r="I350" s="1"/>
     </row>
@@ -5435,7 +5443,7 @@
       <c r="C351" s="1"/>
       <c r="D351" s="10"/>
       <c r="E351" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F351" s="1" t="s">
         <v>9</v>
@@ -5443,13 +5451,28 @@
       <c r="G351" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H351" s="3">
+      <c r="H351" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I351" s="1"/>
+    </row>
+    <row r="352" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B352" s="1"/>
+      <c r="C352" s="1"/>
+      <c r="D352" s="10"/>
+      <c r="E352" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F352" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G352" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H352" s="3">
         <v>20200331</v>
       </c>
-      <c r="I351" s="1"/>
-    </row>
-    <row r="352" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D352" s="9"/>
+      <c r="I352" s="1"/>
     </row>
     <row r="353" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D353" s="9"/>
@@ -5507,6 +5530,9 @@
     </row>
     <row r="371" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D371" s="9"/>
+    </row>
+    <row r="372" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D372" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change output response of margin api
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -1016,7 +1017,7 @@
     <t>Family_Transaction_DetailsJson</t>
   </si>
   <si>
-    <t>[ { "ExchSeg": "MCX-COMM", "fm_TotalMrgn": 29007.75, "Collected": 89799.23, "TotalShort": 0.00, "TotalShortPER": 0.00, "Tmp_NFiller4": 0.00, "Tmp_PeakMargin": 0.00, "Tmp_NFiller5": 0.00, "PeakShort": 0.00, "Tmp_HighestShortFall": 0.00, "ShortPenalty": 0.00 } ]</t>
+    <t>[ { "exchSeg": "MCX-COMM", "eoD_Margin_Required": 29007.75, "eoD_Margin_Available": 89799.23, "eoD_ShortFall_Amount": 0, "eoD_ShortFall_Per": 0, "peak_Margin_Required": 0, "peak_Margin_To_Be_Collected": 0, "peak_Margin_Available": 29007.75, "peak_Margin_Shortfall": 0, "peak_Margin_Highest_Shortfall": 0 } ]</t>
   </si>
 </sst>
 </file>
@@ -1482,10 +1483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I372"/>
+  <dimension ref="A1:I371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="F275" sqref="F275"/>
+    <sheetView tabSelected="1" topLeftCell="C258" workbookViewId="0">
+      <selection activeCell="H276" sqref="H276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3124,148 +3125,159 @@
       </c>
       <c r="I159" s="1"/>
     </row>
-    <row r="160" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="D160" s="10"/>
+    <row r="160" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D160" s="9"/>
       <c r="E160" s="1" t="s">
         <v>17</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G160" s="1"/>
       <c r="H160" s="3">
         <v>20210101</v>
       </c>
-      <c r="I160" s="13"/>
-    </row>
-    <row r="161" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D161" s="9"/>
-    </row>
-    <row r="162" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B162" t="s">
+    </row>
+    <row r="161" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B161" t="s">
         <v>50</v>
       </c>
-      <c r="C162" t="s">
+      <c r="C161" t="s">
         <v>277</v>
       </c>
-      <c r="D162" s="10" t="s">
+      <c r="D161" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E162" s="1"/>
-      <c r="F162" s="1"/>
-      <c r="G162" s="1"/>
-      <c r="H162" s="3"/>
-      <c r="I162" s="7" t="s">
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="3"/>
+      <c r="I161" s="7" t="s">
         <v>61</v>
       </c>
+    </row>
+    <row r="162" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D162" s="9"/>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D163" s="9"/>
     </row>
-    <row r="164" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D164" s="9"/>
-    </row>
-    <row r="165" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B165" s="1" t="s">
+    <row r="164" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B164" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C165" t="s">
+      <c r="C164" t="s">
         <v>243</v>
       </c>
-      <c r="D165" s="10" t="s">
+      <c r="D164" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E165" s="1"/>
-      <c r="F165" s="1"/>
-      <c r="G165" s="1"/>
-      <c r="H165" s="3"/>
-      <c r="I165" s="7" t="s">
+      <c r="E164" s="1"/>
+      <c r="F164" s="1"/>
+      <c r="G164" s="1"/>
+      <c r="H164" s="3"/>
+      <c r="I164" s="7" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="166" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D166" s="9"/>
-    </row>
-    <row r="167" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B167" s="1" t="s">
+    <row r="165" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D165" s="9"/>
+    </row>
+    <row r="166" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B166" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C167" t="s">
+      <c r="C166" t="s">
         <v>243</v>
       </c>
-      <c r="D167" s="10" t="s">
+      <c r="D166" s="10" t="s">
         <v>93</v>
       </c>
+      <c r="E166" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G166" s="1"/>
+      <c r="H166" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="I166" s="7" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="10"/>
       <c r="E167" s="1" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F167" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G167" s="1"/>
       <c r="H167" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="I167" s="7" t="s">
-        <v>96</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="I167" s="1"/>
     </row>
     <row r="168" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B168" s="1"/>
-      <c r="C168" s="1"/>
-      <c r="D168" s="10"/>
-      <c r="E168" s="1" t="s">
+      <c r="D168" s="9"/>
+    </row>
+    <row r="169" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B169" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C169" t="s">
+        <v>243</v>
+      </c>
+      <c r="D169" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="E169" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F169" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G169" s="1"/>
+      <c r="H169" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I169" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="170" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B170" s="1"/>
+      <c r="C170" s="1"/>
+      <c r="D170" s="10"/>
+      <c r="E170" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G168" s="1"/>
-      <c r="H168" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="I168" s="1"/>
-    </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D169" s="9"/>
-    </row>
-    <row r="170" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B170" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C170" t="s">
-        <v>243</v>
-      </c>
-      <c r="D170" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="E170" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="F170" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G170" s="1"/>
       <c r="H170" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I170" s="7" t="s">
-        <v>100</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="I170" s="1"/>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
       <c r="D171" s="10"/>
       <c r="E171" s="1" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G171" s="1"/>
       <c r="H171" s="3" t="s">
-        <v>98</v>
+        <v>36</v>
       </c>
       <c r="I171" s="1"/>
     </row>
@@ -3274,14 +3286,16 @@
       <c r="C172" s="1"/>
       <c r="D172" s="10"/>
       <c r="E172" s="1" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G172" s="1"/>
-      <c r="H172" s="3" t="s">
-        <v>36</v>
+      <c r="G172" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H172" s="3">
+        <v>20200401</v>
       </c>
       <c r="I172" s="1"/>
     </row>
@@ -3290,7 +3304,7 @@
       <c r="C173" s="1"/>
       <c r="D173" s="10"/>
       <c r="E173" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>9</v>
@@ -3299,68 +3313,68 @@
         <v>16</v>
       </c>
       <c r="H173" s="3">
-        <v>20200401</v>
+        <v>20210331</v>
       </c>
       <c r="I173" s="1"/>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B174" s="1"/>
-      <c r="C174" s="1"/>
-      <c r="D174" s="10"/>
-      <c r="E174" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F174" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G174" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H174" s="3">
-        <v>20210331</v>
-      </c>
-      <c r="I174" s="1"/>
-    </row>
-    <row r="175" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D175" s="9"/>
-    </row>
-    <row r="176" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B176" s="1" t="s">
+      <c r="D174" s="9"/>
+    </row>
+    <row r="175" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B175" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C176" t="s">
+      <c r="C175" t="s">
         <v>243</v>
       </c>
-      <c r="D176" s="10" t="s">
+      <c r="D175" s="10" t="s">
         <v>102</v>
       </c>
+      <c r="E175" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F175" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G175" s="1"/>
+      <c r="H175" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="I175" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="176" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B176" s="1"/>
+      <c r="C176" s="1"/>
+      <c r="D176" s="10"/>
       <c r="E176" s="1" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G176" s="1"/>
       <c r="H176" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="I176" s="7" t="s">
-        <v>104</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="I176" s="1"/>
     </row>
     <row r="177" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
       <c r="D177" s="10"/>
       <c r="E177" s="1" t="s">
-        <v>105</v>
+        <v>15</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G177" s="1"/>
-      <c r="H177" s="3" t="s">
-        <v>106</v>
+      <c r="G177" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H177" s="3">
+        <v>20200401</v>
       </c>
       <c r="I177" s="1"/>
     </row>
@@ -3369,7 +3383,7 @@
       <c r="C178" s="1"/>
       <c r="D178" s="10"/>
       <c r="E178" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>9</v>
@@ -3378,290 +3392,289 @@
         <v>16</v>
       </c>
       <c r="H178" s="3">
-        <v>20200401</v>
+        <v>20210331</v>
       </c>
       <c r="I178" s="1"/>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B179" s="1"/>
-      <c r="C179" s="1"/>
-      <c r="D179" s="10"/>
-      <c r="E179" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G179" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H179" s="3">
-        <v>20210331</v>
-      </c>
-      <c r="I179" s="1"/>
-    </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D180" s="9"/>
-      <c r="F180" s="10" t="s">
+      <c r="D179" s="9"/>
+      <c r="F179" s="10" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="181" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B181" s="1" t="s">
+    <row r="180" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B180" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C180" t="s">
         <v>243</v>
       </c>
-      <c r="D181" s="10" t="s">
+      <c r="D180" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="I181" s="26" t="s">
+      <c r="I180" s="26" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D182" s="9"/>
-    </row>
-    <row r="183" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B183" s="1" t="s">
+    <row r="181" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D181" s="9"/>
+    </row>
+    <row r="182" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B182" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C183" t="s">
+      <c r="C182" t="s">
         <v>243</v>
       </c>
-      <c r="D183" s="10" t="s">
+      <c r="D182" s="10" t="s">
         <v>294</v>
       </c>
+      <c r="E182" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F182" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H182" t="s">
+        <v>297</v>
+      </c>
+      <c r="I182" s="26" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D183" s="9"/>
       <c r="E183" s="11" t="s">
-        <v>295</v>
+        <v>11</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H183" t="s">
-        <v>297</v>
-      </c>
-      <c r="I183" s="26" t="s">
-        <v>298</v>
+      <c r="H183">
+        <v>1234</v>
       </c>
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D184" s="9"/>
-      <c r="E184" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F184" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H184">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D185" s="9"/>
-    </row>
-    <row r="186" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B186" t="s">
+    </row>
+    <row r="185" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B185" t="s">
         <v>90</v>
       </c>
-      <c r="C186" t="s">
+      <c r="C185" t="s">
         <v>243</v>
       </c>
-      <c r="D186" s="10" t="s">
+      <c r="D185" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="E186" s="11" t="s">
+      <c r="E185" s="11" t="s">
         <v>295</v>
       </c>
-      <c r="F186" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H186" t="s">
+      <c r="F185" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H185" t="s">
         <v>297</v>
       </c>
-      <c r="I186" s="26" t="s">
+      <c r="I185" s="26" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="186" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D186" s="9"/>
+    </row>
+    <row r="187" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D187" s="9"/>
+      <c r="H187" t="s">
+        <v>301</v>
+      </c>
+      <c r="I187" s="26"/>
     </row>
     <row r="188" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D188" s="9"/>
+      <c r="B188" t="s">
+        <v>90</v>
+      </c>
+      <c r="C188" t="s">
+        <v>243</v>
+      </c>
+      <c r="D188" s="10" t="s">
+        <v>305</v>
+      </c>
+      <c r="E188" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H188" t="s">
-        <v>301</v>
-      </c>
-      <c r="I188" s="26"/>
-    </row>
-    <row r="189" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B189" t="s">
-        <v>90</v>
-      </c>
-      <c r="C189" t="s">
-        <v>243</v>
-      </c>
-      <c r="D189" s="10" t="s">
-        <v>305</v>
-      </c>
-      <c r="E189" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="I188" s="26" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="189" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D189" s="9"/>
       <c r="H189" t="s">
-        <v>302</v>
-      </c>
-      <c r="I189" s="26" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D190" s="9"/>
       <c r="H190" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="191" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D191" s="9"/>
-      <c r="H191" t="s">
-        <v>304</v>
-      </c>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D192" s="9"/>
+      <c r="B192" t="s">
+        <v>90</v>
+      </c>
+      <c r="C192" t="s">
+        <v>243</v>
+      </c>
+      <c r="D192" t="s">
+        <v>306</v>
+      </c>
+      <c r="H192" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="193" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B193" t="s">
-        <v>90</v>
-      </c>
-      <c r="C193" t="s">
-        <v>243</v>
-      </c>
-      <c r="D193" t="s">
-        <v>306</v>
+      <c r="E193" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F193" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H193" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="194" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E194" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="F194" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H194" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="195" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H195" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="197" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B197" t="s">
+        <v>90</v>
+      </c>
+      <c r="C197" t="s">
+        <v>243</v>
+      </c>
+      <c r="D197" t="s">
+        <v>307</v>
+      </c>
+      <c r="H197" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="198" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E198" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F198" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H198" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="199" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H199" t="s">
         <v>303</v>
-      </c>
-    </row>
-    <row r="196" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H196" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="198" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B198" t="s">
-        <v>90</v>
-      </c>
-      <c r="C198" t="s">
-        <v>243</v>
-      </c>
-      <c r="D198" t="s">
-        <v>307</v>
-      </c>
-      <c r="H198" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="199" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="E199" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="F199" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H199" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="200" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H200" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="201" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H201" t="s">
         <v>304</v>
       </c>
     </row>
+    <row r="202" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B202" t="s">
+        <v>90</v>
+      </c>
+      <c r="C202" t="s">
+        <v>243</v>
+      </c>
+      <c r="D202" t="s">
+        <v>308</v>
+      </c>
+      <c r="H202" t="s">
+        <v>301</v>
+      </c>
+    </row>
     <row r="203" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B203" t="s">
-        <v>90</v>
-      </c>
-      <c r="C203" t="s">
-        <v>243</v>
-      </c>
-      <c r="D203" t="s">
-        <v>308</v>
+      <c r="D203" s="9"/>
+      <c r="E203" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F203" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="H203" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="204" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D204" s="9"/>
-      <c r="E204" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="F204" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H204" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="205" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D205" s="9"/>
       <c r="H205" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="206" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D206" s="9"/>
-      <c r="H206" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="207" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D207" s="9"/>
-    </row>
-    <row r="208" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B208" s="8" t="s">
+    </row>
+    <row r="207" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B207" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C208" s="8" t="s">
+      <c r="C207" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="D208" s="32" t="s">
+      <c r="D207" s="32" t="s">
         <v>309</v>
       </c>
+      <c r="E207" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="F207" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G207" s="8"/>
+      <c r="H207" s="18" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="208" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B208" s="8"/>
+      <c r="C208" s="8"/>
+      <c r="D208" s="32"/>
       <c r="E208" s="8" t="s">
-        <v>310</v>
+        <v>15</v>
       </c>
       <c r="F208" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G208" s="8"/>
-      <c r="H208" s="18" t="s">
-        <v>312</v>
+      <c r="G208" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H208" s="3">
+        <v>20200401</v>
       </c>
     </row>
     <row r="209" spans="2:9" x14ac:dyDescent="0.3">
@@ -3669,7 +3682,7 @@
       <c r="C209" s="8"/>
       <c r="D209" s="32"/>
       <c r="E209" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F209" s="8" t="s">
         <v>23</v>
@@ -3678,7 +3691,7 @@
         <v>16</v>
       </c>
       <c r="H209" s="3">
-        <v>20200401</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="210" spans="2:9" x14ac:dyDescent="0.3">
@@ -3686,89 +3699,87 @@
       <c r="C210" s="8"/>
       <c r="D210" s="32"/>
       <c r="E210" s="8" t="s">
-        <v>17</v>
+        <v>311</v>
       </c>
       <c r="F210" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G210" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H210" s="3">
-        <v>20210331</v>
+      <c r="G210" s="8"/>
+      <c r="H210" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="211" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B211" s="8"/>
       <c r="C211" s="8"/>
       <c r="D211" s="32"/>
-      <c r="E211" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="F211" s="8" t="s">
-        <v>23</v>
-      </c>
+      <c r="E211" s="8"/>
+      <c r="F211" s="8"/>
       <c r="G211" s="8"/>
-      <c r="H211" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="212" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B212" s="8"/>
-      <c r="C212" s="8"/>
-      <c r="D212" s="32"/>
-      <c r="E212" s="8"/>
-      <c r="F212" s="8"/>
-      <c r="G212" s="8"/>
-    </row>
-    <row r="213" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="212" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="D212" s="9"/>
+      <c r="H212" s="18" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="213" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D213" s="9"/>
-      <c r="H213" s="18" t="s">
-        <v>313</v>
-      </c>
     </row>
     <row r="214" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D214" s="9"/>
     </row>
     <row r="215" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D215" s="9"/>
-    </row>
-    <row r="216" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B216" s="8" t="s">
+      <c r="B215" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C216" s="8" t="s">
+      <c r="C215" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="D216" s="32" t="s">
+      <c r="D215" s="32" t="s">
         <v>314</v>
       </c>
-      <c r="E216" s="33" t="s">
+      <c r="E215" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F216" s="32" t="s">
+      <c r="F215" s="32" t="s">
         <v>23</v>
       </c>
+      <c r="G215" s="8"/>
+      <c r="H215" s="32" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="216" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D216" s="9"/>
+      <c r="E216" s="8"/>
+      <c r="F216" s="8" t="s">
+        <v>127</v>
+      </c>
       <c r="G216" s="8"/>
-      <c r="H216" s="32" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="217" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H216" s="18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="217" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D217" s="9"/>
-      <c r="E217" s="8"/>
+      <c r="E217" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="F217" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G217" s="8"/>
-      <c r="H217" s="18" t="s">
-        <v>316</v>
+        <v>23</v>
+      </c>
+      <c r="G217" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H217" s="3">
+        <v>20200401</v>
       </c>
     </row>
     <row r="218" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D218" s="9"/>
       <c r="E218" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F218" s="8" t="s">
         <v>23</v>
@@ -3777,155 +3788,155 @@
         <v>16</v>
       </c>
       <c r="H218" s="3">
-        <v>20200401</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="219" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D219" s="9"/>
-      <c r="E219" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F219" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G219" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H219" s="3">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="220" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D220" s="9"/>
-      <c r="E220" s="8"/>
-      <c r="F220" s="8"/>
-      <c r="G220" s="1"/>
-      <c r="H220" s="3"/>
-    </row>
-    <row r="221" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B221" s="8" t="s">
+      <c r="E219" s="8"/>
+      <c r="F219" s="8"/>
+      <c r="G219" s="1"/>
+      <c r="H219" s="3"/>
+    </row>
+    <row r="220" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B220" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C221" s="8" t="s">
+      <c r="C220" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="D221" s="9" t="s">
+      <c r="D220" s="9" t="s">
         <v>317</v>
       </c>
+      <c r="H220" t="s">
+        <v>301</v>
+      </c>
+      <c r="I220" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="221" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D221" s="9"/>
+      <c r="E221" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F221" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H221" t="s">
-        <v>301</v>
-      </c>
-      <c r="I221" s="7" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
     </row>
     <row r="222" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D222" s="9"/>
-      <c r="E222" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="F222" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H222" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="223" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D223" s="9"/>
       <c r="H223" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="224" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D224" s="9"/>
-      <c r="H224" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="225" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D225" s="9"/>
-      <c r="E225" s="8"/>
-      <c r="F225" s="8"/>
-      <c r="G225" s="1"/>
-      <c r="H225" s="3"/>
-    </row>
-    <row r="226" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B226" s="8" t="s">
+      <c r="E224" s="8"/>
+      <c r="F224" s="8"/>
+      <c r="G224" s="1"/>
+      <c r="H224" s="3"/>
+    </row>
+    <row r="225" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B225" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C226" s="8" t="s">
+      <c r="C225" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="D226" s="9" t="s">
+      <c r="D225" s="9" t="s">
         <v>319</v>
       </c>
+      <c r="H225" t="s">
+        <v>301</v>
+      </c>
+      <c r="I225" s="7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="226" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D226" s="9"/>
+      <c r="E226" s="11" t="s">
+        <v>295</v>
+      </c>
+      <c r="F226" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H226" t="s">
-        <v>301</v>
-      </c>
-      <c r="I226" s="7" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D227" s="9"/>
-      <c r="E227" s="11" t="s">
-        <v>295</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="H227" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D228" s="9"/>
       <c r="H228" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D229" s="9"/>
-      <c r="H229" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="230" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D230" s="9"/>
-      <c r="E230" s="8"/>
-      <c r="F230" s="8"/>
-      <c r="G230" s="1"/>
-      <c r="H230" s="3"/>
-    </row>
-    <row r="231" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
-      <c r="B231" s="8" t="s">
+      <c r="E229" s="8"/>
+      <c r="F229" s="8"/>
+      <c r="G229" s="1"/>
+      <c r="H229" s="3"/>
+    </row>
+    <row r="230" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
+      <c r="B230" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C231" s="8" t="s">
+      <c r="C230" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="D231" s="34" t="s">
+      <c r="D230" s="34" t="s">
         <v>321</v>
       </c>
+      <c r="E230" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="F230" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G230" s="8"/>
+      <c r="H230" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="I230" s="7" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="231" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D231" s="9"/>
       <c r="E231" s="8" t="s">
-        <v>310</v>
+        <v>15</v>
       </c>
       <c r="F231" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G231" s="8"/>
-      <c r="H231" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="I231" s="7" t="s">
-        <v>322</v>
+      <c r="G231" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H231" s="3">
+        <v>20200401</v>
       </c>
     </row>
     <row r="232" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D232" s="9"/>
       <c r="E232" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F232" s="8" t="s">
         <v>23</v>
@@ -3934,92 +3945,92 @@
         <v>16</v>
       </c>
       <c r="H232" s="3">
-        <v>20200401</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="233" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D233" s="9"/>
       <c r="E233" s="8" t="s">
-        <v>17</v>
+        <v>311</v>
       </c>
       <c r="F233" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G233" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H233" s="3">
-        <v>20210331</v>
+      <c r="G233" s="8"/>
+      <c r="H233" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="234" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D234" s="9"/>
-      <c r="E234" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="F234" s="8" t="s">
+      <c r="E234" s="8"/>
+      <c r="F234" s="8"/>
+      <c r="G234" s="8"/>
+    </row>
+    <row r="235" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="D235" s="9"/>
+      <c r="H235" s="18" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="236" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D236" s="9"/>
+      <c r="E236" s="8"/>
+      <c r="F236" s="8"/>
+      <c r="G236" s="1"/>
+      <c r="H236" s="3"/>
+    </row>
+    <row r="237" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B237" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="C237" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="D237" s="32" t="s">
+        <v>323</v>
+      </c>
+      <c r="E237" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="F237" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="G234" s="8"/>
-      <c r="H234" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="235" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D235" s="9"/>
-      <c r="E235" s="8"/>
-      <c r="F235" s="8"/>
-      <c r="G235" s="8"/>
-    </row>
-    <row r="236" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="D236" s="9"/>
-      <c r="H236" s="18" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="237" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D237" s="9"/>
-      <c r="E237" s="8"/>
-      <c r="F237" s="8"/>
-      <c r="G237" s="1"/>
-      <c r="H237" s="3"/>
-    </row>
-    <row r="238" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B238" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C238" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="D238" s="32" t="s">
-        <v>323</v>
-      </c>
-      <c r="E238" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F238" s="32" t="s">
+      <c r="G237" s="8"/>
+      <c r="H237" s="32" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="238" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D238" s="9"/>
+      <c r="E238" s="8"/>
+      <c r="F238" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G238" s="8"/>
+      <c r="H238" s="18" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="239" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D239" s="9"/>
+      <c r="E239" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F239" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G238" s="8"/>
-      <c r="H238" s="32" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="239" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D239" s="9"/>
-      <c r="E239" s="8"/>
-      <c r="F239" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G239" s="8"/>
-      <c r="H239" s="18" t="s">
-        <v>316</v>
+      <c r="G239" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H239" s="3">
+        <v>20200401</v>
       </c>
     </row>
     <row r="240" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D240" s="9"/>
       <c r="E240" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F240" s="8" t="s">
         <v>23</v>
@@ -4028,43 +4039,46 @@
         <v>16</v>
       </c>
       <c r="H240" s="3">
-        <v>20200401</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="241" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D241" s="9"/>
-      <c r="E241" s="8" t="s">
+      <c r="E241" s="8"/>
+      <c r="F241" s="8"/>
+      <c r="G241" s="1"/>
+      <c r="H241" s="3"/>
+    </row>
+    <row r="242" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B242" t="s">
+        <v>107</v>
+      </c>
+      <c r="C242" t="s">
+        <v>244</v>
+      </c>
+      <c r="D242" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E242" t="s">
+        <v>15</v>
+      </c>
+      <c r="F242" t="s">
+        <v>9</v>
+      </c>
+      <c r="G242" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H242" s="6">
+        <v>20210401</v>
+      </c>
+      <c r="I242" s="7" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="243" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D243" s="9"/>
+      <c r="E243" t="s">
         <v>17</v>
-      </c>
-      <c r="F241" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G241" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H241" s="3">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="242" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D242" s="9"/>
-      <c r="E242" s="8"/>
-      <c r="F242" s="8"/>
-      <c r="G242" s="1"/>
-      <c r="H242" s="3"/>
-    </row>
-    <row r="243" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B243" t="s">
-        <v>107</v>
-      </c>
-      <c r="C243" t="s">
-        <v>244</v>
-      </c>
-      <c r="D243" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="E243" t="s">
-        <v>15</v>
       </c>
       <c r="F243" t="s">
         <v>9</v>
@@ -4073,332 +4087,330 @@
         <v>16</v>
       </c>
       <c r="H243" s="6">
-        <v>20210401</v>
-      </c>
-      <c r="I243" s="7" t="s">
-        <v>109</v>
+        <v>20220112</v>
       </c>
     </row>
     <row r="244" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D244" s="9"/>
       <c r="E244" t="s">
-        <v>17</v>
+        <v>110</v>
       </c>
       <c r="F244" t="s">
         <v>9</v>
       </c>
-      <c r="G244" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="H244" s="6">
-        <v>20220112</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D245" s="9"/>
-      <c r="E245" t="s">
-        <v>110</v>
-      </c>
-      <c r="F245" t="s">
-        <v>9</v>
-      </c>
-      <c r="H245" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="246" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D246" s="9"/>
+      <c r="H245" s="6"/>
+    </row>
+    <row r="246" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B246" t="s">
+        <v>107</v>
+      </c>
+      <c r="C246" t="s">
+        <v>244</v>
+      </c>
+      <c r="D246" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="H246" s="6"/>
-    </row>
-    <row r="247" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B247" t="s">
-        <v>107</v>
-      </c>
-      <c r="C247" t="s">
-        <v>244</v>
-      </c>
-      <c r="D247" s="9" t="s">
-        <v>111</v>
-      </c>
+      <c r="I246" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="247" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D247" s="9"/>
       <c r="H247" s="6"/>
-      <c r="I247" s="7" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="248" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D248" s="9"/>
       <c r="H248" s="6"/>
     </row>
-    <row r="249" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D249" s="9"/>
+    <row r="249" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B249" t="s">
+        <v>107</v>
+      </c>
+      <c r="C249" t="s">
+        <v>244</v>
+      </c>
+      <c r="D249" s="9" t="s">
+        <v>113</v>
+      </c>
       <c r="H249" s="6"/>
-    </row>
-    <row r="250" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B250" t="s">
-        <v>107</v>
-      </c>
-      <c r="C250" t="s">
-        <v>244</v>
-      </c>
-      <c r="D250" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="I249" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="250" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D250" s="9"/>
       <c r="H250" s="6"/>
-      <c r="I250" s="7" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="251" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D251" s="9"/>
       <c r="H251" s="6"/>
     </row>
-    <row r="252" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D252" s="9"/>
+    <row r="252" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B252" t="s">
+        <v>107</v>
+      </c>
+      <c r="C252" t="s">
+        <v>244</v>
+      </c>
+      <c r="D252" s="9" t="s">
+        <v>115</v>
+      </c>
       <c r="H252" s="6"/>
-    </row>
-    <row r="253" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B253" t="s">
-        <v>107</v>
-      </c>
-      <c r="C253" t="s">
-        <v>244</v>
-      </c>
-      <c r="D253" s="9" t="s">
-        <v>115</v>
-      </c>
+      <c r="I252" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="253" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D253" s="9"/>
       <c r="H253" s="6"/>
-      <c r="I253" s="7" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="254" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D254" s="9"/>
       <c r="H254" s="6"/>
     </row>
-    <row r="255" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D255" s="9"/>
-      <c r="H255" s="6"/>
-    </row>
-    <row r="256" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B256" t="s">
+    <row r="255" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B255" t="s">
         <v>107</v>
       </c>
-      <c r="C256" t="s">
+      <c r="C255" t="s">
         <v>244</v>
       </c>
-      <c r="D256" s="9" t="s">
+      <c r="D255" s="9" t="s">
         <v>117</v>
       </c>
+      <c r="E255" t="s">
+        <v>118</v>
+      </c>
+      <c r="F255" t="s">
+        <v>119</v>
+      </c>
+      <c r="H255" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I255" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="256" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D256" s="9"/>
       <c r="E256" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="F256" t="s">
         <v>119</v>
       </c>
       <c r="H256" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I256" s="7" t="s">
-        <v>120</v>
+        <v>1</v>
       </c>
     </row>
     <row r="257" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D257" s="9"/>
-      <c r="E257" t="s">
-        <v>121</v>
-      </c>
-      <c r="F257" t="s">
-        <v>119</v>
-      </c>
-      <c r="H257" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="258" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D258" s="9"/>
-      <c r="H258" s="6"/>
-    </row>
-    <row r="259" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B259" t="s">
+      <c r="H257" s="6"/>
+    </row>
+    <row r="258" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B258" t="s">
         <v>107</v>
       </c>
-      <c r="C259" t="s">
+      <c r="C258" t="s">
         <v>244</v>
       </c>
-      <c r="D259" s="9" t="s">
+      <c r="D258" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="E259" t="s">
+      <c r="E258" t="s">
         <v>123</v>
       </c>
-      <c r="F259" t="s">
+      <c r="F258" t="s">
         <v>21</v>
       </c>
-      <c r="H259" s="6">
+      <c r="H258" s="6">
         <v>3</v>
       </c>
-      <c r="I259" s="7" t="s">
+      <c r="I258" s="7" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="260" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D260" s="9"/>
+    <row r="259" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D259" s="9"/>
+    </row>
+    <row r="260" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B260" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C260" t="s">
+        <v>278</v>
+      </c>
+      <c r="D260" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="E260" s="1"/>
+      <c r="F260" s="10"/>
+      <c r="G260" s="1"/>
+      <c r="H260" s="3"/>
+      <c r="I260" s="7" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="261" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B261" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C261" t="s">
-        <v>278</v>
-      </c>
-      <c r="D261" s="10" t="s">
-        <v>63</v>
-      </c>
+      <c r="B261" s="1"/>
+      <c r="C261" s="1"/>
+      <c r="D261" s="10"/>
       <c r="E261" s="1"/>
-      <c r="F261" s="10"/>
+      <c r="F261" s="1"/>
       <c r="G261" s="1"/>
       <c r="H261" s="3"/>
-      <c r="I261" s="7" t="s">
-        <v>64</v>
-      </c>
+      <c r="I261" s="13"/>
     </row>
     <row r="262" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B262" s="1"/>
-      <c r="C262" s="1"/>
-      <c r="D262" s="10"/>
+      <c r="B262" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C262" t="s">
+        <v>278</v>
+      </c>
+      <c r="D262" s="10" t="s">
+        <v>65</v>
+      </c>
       <c r="E262" s="1"/>
-      <c r="F262" s="1"/>
+      <c r="F262" s="10"/>
       <c r="G262" s="1"/>
       <c r="H262" s="3"/>
-      <c r="I262" s="13"/>
+      <c r="I262" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="263" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B263" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C263" t="s">
-        <v>278</v>
-      </c>
-      <c r="D263" s="10" t="s">
-        <v>65</v>
-      </c>
+      <c r="B263" s="1"/>
+      <c r="C263" s="1"/>
+      <c r="D263" s="10"/>
       <c r="E263" s="1"/>
-      <c r="F263" s="10"/>
+      <c r="F263" s="1"/>
       <c r="G263" s="1"/>
       <c r="H263" s="3"/>
-      <c r="I263" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="I263" s="13"/>
     </row>
     <row r="264" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B264" s="1"/>
-      <c r="C264" s="1"/>
-      <c r="D264" s="10"/>
-      <c r="E264" s="1"/>
-      <c r="F264" s="1"/>
+      <c r="B264" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C264" t="s">
+        <v>278</v>
+      </c>
+      <c r="D264" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="E264" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F264" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="G264" s="1"/>
-      <c r="H264" s="3"/>
-      <c r="I264" s="13"/>
+      <c r="H264" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I264" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="265" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B265" s="1" t="s">
+      <c r="B265" s="1"/>
+      <c r="C265" s="1"/>
+      <c r="D265" s="10"/>
+      <c r="E265" s="11"/>
+      <c r="F265" s="10"/>
+      <c r="G265" s="1"/>
+      <c r="H265" s="3"/>
+      <c r="I265" s="13"/>
+    </row>
+    <row r="266" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B266" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C265" t="s">
+      <c r="C266" t="s">
         <v>278</v>
       </c>
-      <c r="D265" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E265" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F265" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G265" s="1"/>
-      <c r="H265" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I265" s="7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="266" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B266" s="1"/>
-      <c r="C266" s="1"/>
-      <c r="D266" s="10"/>
+      <c r="D266" s="10" t="s">
+        <v>70</v>
+      </c>
       <c r="E266" s="11"/>
       <c r="F266" s="10"/>
       <c r="G266" s="1"/>
       <c r="H266" s="3"/>
-      <c r="I266" s="13"/>
+      <c r="I266" s="7" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="267" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B267" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C267" t="s">
-        <v>278</v>
-      </c>
-      <c r="D267" s="10" t="s">
-        <v>70</v>
-      </c>
+      <c r="B267" s="1"/>
+      <c r="C267" s="1"/>
+      <c r="D267" s="10"/>
       <c r="E267" s="11"/>
       <c r="F267" s="10"/>
       <c r="G267" s="1"/>
       <c r="H267" s="3"/>
-      <c r="I267" s="7" t="s">
-        <v>71</v>
-      </c>
+      <c r="I267" s="13"/>
     </row>
     <row r="268" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B268" s="1"/>
-      <c r="C268" s="1"/>
-      <c r="D268" s="10"/>
-      <c r="E268" s="11"/>
-      <c r="F268" s="10"/>
+      <c r="B268" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C268" t="s">
+        <v>278</v>
+      </c>
+      <c r="D268" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E268" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F268" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="G268" s="1"/>
-      <c r="H268" s="3"/>
-      <c r="I268" s="13"/>
+      <c r="H268" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I268" s="7" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="269" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B269" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C269" t="s">
-        <v>278</v>
-      </c>
-      <c r="D269" s="10" t="s">
-        <v>72</v>
-      </c>
+      <c r="B269" s="1"/>
+      <c r="C269" s="1"/>
+      <c r="D269" s="10"/>
       <c r="E269" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="F269" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G269" s="1"/>
-      <c r="H269" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I269" s="7" t="s">
-        <v>43</v>
-      </c>
+      <c r="H269" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I269" s="13"/>
     </row>
     <row r="270" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B270" s="1"/>
       <c r="C270" s="1"/>
       <c r="D270" s="10"/>
       <c r="E270" s="11" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F270" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G270" s="1"/>
-      <c r="H270" s="3" t="b">
-        <v>1</v>
+      <c r="H270" s="3">
+        <v>43590</v>
       </c>
       <c r="I270" s="13"/>
     </row>
@@ -4407,14 +4419,14 @@
       <c r="C271" s="1"/>
       <c r="D271" s="10"/>
       <c r="E271" s="11" t="s">
-        <v>74</v>
+        <v>44</v>
       </c>
       <c r="F271" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G271" s="1"/>
       <c r="H271" s="3">
-        <v>43590</v>
+        <v>532667</v>
       </c>
       <c r="I271" s="13"/>
     </row>
@@ -4423,148 +4435,153 @@
       <c r="C272" s="1"/>
       <c r="D272" s="10"/>
       <c r="E272" s="11" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="F272" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G272" s="1"/>
       <c r="H272" s="3">
-        <v>532667</v>
+        <v>198</v>
       </c>
       <c r="I272" s="13"/>
     </row>
-    <row r="273" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B273" s="1"/>
-      <c r="C273" s="1"/>
-      <c r="D273" s="10"/>
-      <c r="E273" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F273" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G273" s="1"/>
-      <c r="H273" s="3">
-        <v>198</v>
-      </c>
-      <c r="I273" s="13"/>
-    </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D274" s="9"/>
-    </row>
-    <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B275" t="s">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D273" s="9"/>
+    </row>
+    <row r="274" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B274" t="s">
         <v>62</v>
       </c>
-      <c r="C275" t="s">
+      <c r="C274" t="s">
         <v>278</v>
       </c>
-      <c r="D275" s="9" t="s">
+      <c r="D274" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E275" s="11" t="s">
+      <c r="E274" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F275" t="s">
-        <v>9</v>
-      </c>
-      <c r="H275" s="8">
+      <c r="F274" t="s">
+        <v>9</v>
+      </c>
+      <c r="H274" s="8">
         <v>20191101</v>
       </c>
-      <c r="I275" s="26" t="s">
+      <c r="I274" s="7" t="s">
         <v>324</v>
       </c>
     </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D275" s="9"/>
+    </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D276" s="9"/>
+      <c r="B276" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C276" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D276" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="E276" t="s">
+        <v>15</v>
+      </c>
+      <c r="F276" t="s">
+        <v>9</v>
+      </c>
+      <c r="H276" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="I276" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B277" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C277" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D277" s="9" t="s">
-        <v>231</v>
-      </c>
+      <c r="D277" s="9"/>
       <c r="E277" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F277" t="s">
         <v>9</v>
       </c>
       <c r="H277" s="17" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I277" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D278" s="9"/>
-      <c r="E278" t="s">
-        <v>17</v>
-      </c>
-      <c r="F278" t="s">
-        <v>9</v>
-      </c>
-      <c r="H278" s="17" t="s">
-        <v>173</v>
-      </c>
       <c r="I278" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D279" s="9"/>
       <c r="I279" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D280" s="9"/>
       <c r="I280" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D281" s="9"/>
-      <c r="I281" t="s">
-        <v>172</v>
+      <c r="I281" s="19" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D282" s="9"/>
-      <c r="I282" s="19" t="s">
-        <v>230</v>
+      <c r="I282" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D283" s="9"/>
-      <c r="I283" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D284" s="9"/>
-    </row>
-    <row r="285" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A285" s="1">
+    </row>
+    <row r="284" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A284" s="1">
         <v>36</v>
       </c>
-      <c r="B285" s="1" t="s">
+      <c r="B284" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C285" s="1" t="s">
+      <c r="C284" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D285" s="10" t="s">
+      <c r="D284" s="10" t="s">
         <v>238</v>
       </c>
+      <c r="E284" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F284" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G284" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H284" s="15">
+        <v>20200401</v>
+      </c>
+      <c r="I284" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A285" s="1"/>
+      <c r="B285" s="1"/>
+      <c r="C285" s="1"/>
+      <c r="D285" s="10"/>
       <c r="E285" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F285" s="1" t="s">
         <v>9</v>
@@ -4572,249 +4589,246 @@
       <c r="G285" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H285" s="15">
-        <v>20200401</v>
-      </c>
-      <c r="I285" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="286" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H285" s="6">
+        <v>20210331</v>
+      </c>
+      <c r="I285" s="1"/>
+    </row>
+    <row r="286" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A286" s="1"/>
       <c r="B286" s="1"/>
       <c r="C286" s="1"/>
       <c r="D286" s="10"/>
       <c r="E286" s="1" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="F286" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G286" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H286" s="6">
-        <v>20210331</v>
-      </c>
-      <c r="I286" s="1"/>
+      <c r="G286" s="1"/>
+      <c r="H286" s="3">
+        <v>533271</v>
+      </c>
+      <c r="I286" s="13"/>
     </row>
     <row r="287" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A287" s="1"/>
       <c r="B287" s="1"/>
       <c r="C287" s="1"/>
       <c r="D287" s="10"/>
-      <c r="E287" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F287" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E287" s="1"/>
+      <c r="F287" s="1"/>
       <c r="G287" s="1"/>
-      <c r="H287" s="3">
-        <v>533271</v>
-      </c>
+      <c r="H287" s="3"/>
       <c r="I287" s="13"/>
     </row>
-    <row r="288" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A288" s="1"/>
-      <c r="B288" s="1"/>
-      <c r="C288" s="1"/>
-      <c r="D288" s="10"/>
-      <c r="E288" s="1"/>
-      <c r="F288" s="1"/>
-      <c r="G288" s="1"/>
-      <c r="H288" s="3"/>
-      <c r="I288" s="13"/>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B288" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D288" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E288" t="s">
+        <v>27</v>
+      </c>
+      <c r="F288" t="s">
+        <v>9</v>
+      </c>
+      <c r="H288" t="s">
+        <v>232</v>
+      </c>
+      <c r="I288" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="289" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B289" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C289" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D289" s="9" t="s">
-        <v>240</v>
-      </c>
+      <c r="D289" s="9"/>
       <c r="E289" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F289" t="s">
         <v>9</v>
       </c>
       <c r="H289" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="I289" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="290" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D290" s="9"/>
       <c r="E290" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="F290" t="s">
         <v>9</v>
       </c>
-      <c r="H290" t="s">
-        <v>233</v>
+      <c r="H290" s="17" t="s">
+        <v>171</v>
       </c>
       <c r="I290" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="291" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D291" s="9"/>
       <c r="E291" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F291" t="s">
         <v>9</v>
       </c>
       <c r="H291" s="17" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I291" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="292" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D292" s="9"/>
-      <c r="E292" t="s">
-        <v>17</v>
-      </c>
-      <c r="F292" t="s">
-        <v>9</v>
-      </c>
-      <c r="H292" s="17" t="s">
-        <v>173</v>
-      </c>
       <c r="I292" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="293" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D293" s="9"/>
-      <c r="I293" t="s">
-        <v>172</v>
+      <c r="I293" s="19" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="294" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D294" s="9"/>
       <c r="I294" s="19" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="295" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D295" s="9"/>
-      <c r="I295" s="19" t="s">
-        <v>235</v>
+      <c r="I295" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="296" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D296" s="9"/>
-      <c r="I296" t="s">
-        <v>188</v>
-      </c>
     </row>
     <row r="297" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D297" s="9"/>
+      <c r="B297" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C297" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D297" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="E297" t="s">
+        <v>27</v>
+      </c>
+      <c r="F297" t="s">
+        <v>9</v>
+      </c>
+      <c r="H297" t="s">
+        <v>236</v>
+      </c>
+      <c r="I297" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="298" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B298" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="C298" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D298" s="9" t="s">
-        <v>241</v>
-      </c>
+      <c r="D298" s="9"/>
       <c r="E298" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F298" t="s">
         <v>9</v>
       </c>
-      <c r="H298" t="s">
-        <v>236</v>
+      <c r="H298" s="17" t="s">
+        <v>171</v>
       </c>
       <c r="I298" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="299" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D299" s="9"/>
       <c r="E299" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F299" t="s">
         <v>9</v>
       </c>
       <c r="H299" s="17" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="I299" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
     </row>
     <row r="300" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D300" s="9"/>
-      <c r="E300" t="s">
-        <v>17</v>
-      </c>
-      <c r="F300" t="s">
-        <v>9</v>
-      </c>
-      <c r="H300" s="17" t="s">
-        <v>173</v>
-      </c>
       <c r="I300" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="301" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D301" s="9"/>
       <c r="I301" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
     </row>
     <row r="302" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D302" s="9"/>
-      <c r="I302" t="s">
-        <v>172</v>
+      <c r="I302" s="25" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="303" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D303" s="9"/>
-      <c r="I303" s="25" t="s">
-        <v>237</v>
+      <c r="E303" s="24"/>
+      <c r="H303" s="18"/>
+      <c r="I303" s="18" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="304" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D304" s="9"/>
-      <c r="E304" s="24"/>
-      <c r="H304" s="18"/>
-      <c r="I304" s="18" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="305" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D305" s="9"/>
-    </row>
-    <row r="306" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B306" t="s">
+    </row>
+    <row r="305" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B305" t="s">
         <v>128</v>
       </c>
-      <c r="C306" s="1" t="s">
+      <c r="C305" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D306" s="9" t="s">
+      <c r="D305" s="9" t="s">
         <v>129</v>
       </c>
+      <c r="E305" t="s">
+        <v>15</v>
+      </c>
+      <c r="F305" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G305" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H305" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I305" s="7" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="306" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D306" s="9"/>
       <c r="E306" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F306" s="9" t="s">
         <v>23</v>
@@ -4823,44 +4837,44 @@
         <v>16</v>
       </c>
       <c r="H306" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I306" s="7" t="s">
-        <v>130</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D307" s="9"/>
-      <c r="E307" t="s">
+      <c r="F307" s="9"/>
+      <c r="H307" s="8"/>
+    </row>
+    <row r="308" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B308" t="s">
+        <v>128</v>
+      </c>
+      <c r="C308" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D308" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E308" t="s">
+        <v>15</v>
+      </c>
+      <c r="F308" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G308" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H308" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I308" s="7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="309" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D309" s="9"/>
+      <c r="E309" t="s">
         <v>17</v>
-      </c>
-      <c r="F307" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G307" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H307" s="8">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="308" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D308" s="9"/>
-      <c r="F308" s="9"/>
-      <c r="H308" s="8"/>
-    </row>
-    <row r="309" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B309" t="s">
-        <v>128</v>
-      </c>
-      <c r="C309" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D309" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E309" t="s">
-        <v>15</v>
       </c>
       <c r="F309" s="9" t="s">
         <v>23</v>
@@ -4869,31 +4883,25 @@
         <v>16</v>
       </c>
       <c r="H309" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I309" s="7" t="s">
-        <v>132</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D310" s="9"/>
       <c r="E310" t="s">
-        <v>17</v>
+        <v>133</v>
       </c>
       <c r="F310" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G310" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H310" s="8">
-        <v>20210331</v>
+        <v>119</v>
+      </c>
+      <c r="H310" s="8" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="311" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D311" s="9"/>
       <c r="E311" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="F311" s="9" t="s">
         <v>119</v>
@@ -4905,7 +4913,7 @@
     <row r="312" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D312" s="9"/>
       <c r="E312" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F312" s="9" t="s">
         <v>119</v>
@@ -4917,43 +4925,49 @@
     <row r="313" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D313" s="9"/>
       <c r="E313" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F313" s="9" t="s">
-        <v>119</v>
+        <v>23</v>
       </c>
       <c r="H313" s="8" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="314" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D314" s="9"/>
-      <c r="E314" t="s">
-        <v>137</v>
-      </c>
-      <c r="F314" s="9" t="s">
+      <c r="H314" s="8"/>
+    </row>
+    <row r="315" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B315" t="s">
+        <v>128</v>
+      </c>
+      <c r="C315" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D315" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E315" t="s">
+        <v>15</v>
+      </c>
+      <c r="F315" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H314" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="315" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D315" s="9"/>
-      <c r="H315" s="8"/>
-    </row>
-    <row r="316" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B316" t="s">
-        <v>128</v>
-      </c>
-      <c r="C316" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D316" s="9" t="s">
-        <v>139</v>
-      </c>
+      <c r="G315" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H315" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I315" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="316" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D316" s="9"/>
       <c r="E316" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F316" s="9" t="s">
         <v>23</v>
@@ -4962,79 +4976,79 @@
         <v>16</v>
       </c>
       <c r="H316" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I316" s="7" t="s">
-        <v>140</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D317" s="9"/>
       <c r="E317" t="s">
-        <v>17</v>
+        <v>141</v>
       </c>
       <c r="F317" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G317" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H317" s="8">
-        <v>20210331</v>
+      <c r="H317" s="8" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D318" s="9"/>
       <c r="E318" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="F318" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H318" s="8" t="s">
-        <v>142</v>
+        <v>28</v>
       </c>
     </row>
     <row r="319" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D319" s="9"/>
       <c r="E319" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F319" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H319" s="8" t="s">
-        <v>28</v>
+      <c r="H319" s="8">
+        <v>512573</v>
       </c>
     </row>
     <row r="320" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D320" s="9"/>
-      <c r="E320" t="s">
-        <v>144</v>
-      </c>
-      <c r="F320" s="9" t="s">
+      <c r="H320" s="8"/>
+    </row>
+    <row r="321" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B321" t="s">
+        <v>128</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D321" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="E321" t="s">
+        <v>15</v>
+      </c>
+      <c r="F321" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H320" s="8">
-        <v>512573</v>
-      </c>
-    </row>
-    <row r="321" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D321" s="9"/>
-      <c r="H321" s="8"/>
-    </row>
-    <row r="322" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B322" t="s">
-        <v>128</v>
-      </c>
-      <c r="C322" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D322" s="9" t="s">
-        <v>145</v>
-      </c>
+      <c r="G321" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H321" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I321" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="322" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D322" s="9"/>
       <c r="E322" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F322" s="9" t="s">
         <v>23</v>
@@ -5043,43 +5057,43 @@
         <v>16</v>
       </c>
       <c r="H322" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I322" s="7" t="s">
-        <v>146</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D323" s="9"/>
-      <c r="E323" t="s">
+      <c r="H323" s="8"/>
+    </row>
+    <row r="324" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B324" t="s">
+        <v>128</v>
+      </c>
+      <c r="C324" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D324" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="E324" t="s">
+        <v>15</v>
+      </c>
+      <c r="F324" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G324" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H324" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I324" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="325" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D325" s="9"/>
+      <c r="E325" t="s">
         <v>17</v>
-      </c>
-      <c r="F323" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G323" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H323" s="8">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="324" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D324" s="9"/>
-      <c r="H324" s="8"/>
-    </row>
-    <row r="325" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B325" t="s">
-        <v>128</v>
-      </c>
-      <c r="C325" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D325" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E325" t="s">
-        <v>15</v>
       </c>
       <c r="F325" s="9" t="s">
         <v>23</v>
@@ -5088,353 +5102,353 @@
         <v>16</v>
       </c>
       <c r="H325" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I325" s="7" t="s">
-        <v>148</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="326" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D326" s="9"/>
       <c r="E326" t="s">
-        <v>17</v>
+        <v>149</v>
       </c>
       <c r="F326" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G326" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="H326" s="8">
-        <v>20210331</v>
+        <v>500425</v>
       </c>
     </row>
     <row r="327" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D327" s="9"/>
-      <c r="E327" t="s">
-        <v>149</v>
-      </c>
-      <c r="F327" s="9" t="s">
+      <c r="H327" s="8"/>
+    </row>
+    <row r="328" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B328" t="s">
+        <v>128</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="D328" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="E328" t="s">
+        <v>22</v>
+      </c>
+      <c r="F328" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H327" s="8">
-        <v>500425</v>
-      </c>
-    </row>
-    <row r="328" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D328" s="9"/>
-      <c r="H328" s="8"/>
-    </row>
-    <row r="329" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B329" t="s">
-        <v>128</v>
-      </c>
-      <c r="C329" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D329" s="9" t="s">
-        <v>150</v>
-      </c>
+      <c r="G328" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H328" s="16">
+        <v>20220228</v>
+      </c>
+      <c r="I328" s="7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="329" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D329" s="9"/>
       <c r="E329" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="F329" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G329" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H329" s="16">
-        <v>20220228</v>
-      </c>
-      <c r="I329" s="7" t="s">
-        <v>151</v>
+      <c r="H329" s="8" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="330" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D330" s="9"/>
       <c r="E330" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F330" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H330" s="8" t="s">
-        <v>152</v>
+        <v>25</v>
       </c>
     </row>
     <row r="331" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D331" s="9"/>
       <c r="E331" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="F331" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H331" s="8" t="s">
-        <v>25</v>
+        <v>153</v>
       </c>
     </row>
     <row r="332" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D332" s="9"/>
       <c r="E332" t="s">
-        <v>35</v>
+        <v>75</v>
       </c>
       <c r="F332" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H332" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
+      </c>
+      <c r="H332" s="8">
+        <v>4</v>
       </c>
     </row>
     <row r="333" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D333" s="9"/>
       <c r="E333" t="s">
-        <v>75</v>
+        <v>155</v>
       </c>
       <c r="F333" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H333" s="8">
-        <v>4</v>
+        <v>48</v>
       </c>
     </row>
     <row r="334" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D334" s="9"/>
       <c r="E334" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F334" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H334" s="8">
-        <v>48</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="335" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D335" s="9"/>
       <c r="E335" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F335" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H335" s="8">
-        <v>1.1000000000000001</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="336" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D336" s="9"/>
       <c r="E336" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F336" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H336" s="8">
-        <v>3.2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="337" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D337" s="9"/>
       <c r="E337" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F337" s="9" t="s">
         <v>154</v>
       </c>
       <c r="H337" s="8">
-        <v>0.11</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="338" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D338" s="9"/>
       <c r="E338" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="F338" s="9" t="s">
-        <v>154</v>
+        <v>23</v>
       </c>
       <c r="H338" s="8">
-        <v>0.2</v>
+        <v>500820</v>
       </c>
     </row>
     <row r="339" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D339" s="9"/>
-      <c r="E339" t="s">
-        <v>149</v>
-      </c>
-      <c r="F339" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H339" s="8">
-        <v>500820</v>
-      </c>
-    </row>
-    <row r="340" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D340" s="9"/>
+    </row>
+    <row r="340" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B340" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D340" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E340" s="1"/>
+      <c r="F340" s="1"/>
+      <c r="G340" s="1"/>
+      <c r="H340" s="3"/>
+      <c r="I340" s="13" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="341" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B341" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C341" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D341" s="10" t="s">
-        <v>77</v>
-      </c>
+      <c r="B341" s="1"/>
+      <c r="C341" s="1"/>
+      <c r="D341" s="10"/>
       <c r="E341" s="1"/>
       <c r="F341" s="1"/>
       <c r="G341" s="1"/>
-      <c r="H341" s="3"/>
-      <c r="I341" s="13" t="s">
-        <v>78</v>
-      </c>
+      <c r="H341" s="12"/>
+      <c r="I341" s="13"/>
     </row>
     <row r="342" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B342" s="1"/>
-      <c r="C342" s="1"/>
-      <c r="D342" s="10"/>
-      <c r="E342" s="1"/>
-      <c r="F342" s="1"/>
+      <c r="B342" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C342" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D342" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="E342" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F342" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="G342" s="1"/>
-      <c r="H342" s="12"/>
-      <c r="I342" s="13"/>
+      <c r="H342" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I342" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="343" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B343" s="1" t="s">
+      <c r="B343" s="1"/>
+      <c r="C343" s="1"/>
+      <c r="D343" s="10"/>
+      <c r="E343" s="1"/>
+      <c r="F343" s="1"/>
+      <c r="G343" s="1"/>
+      <c r="H343" s="3"/>
+      <c r="I343" s="13"/>
+    </row>
+    <row r="344" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B344" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C343" s="1" t="s">
+      <c r="C344" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D343" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="E343" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F343" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G343" s="1"/>
-      <c r="H343" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I343" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="344" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B344" s="1"/>
-      <c r="C344" s="1"/>
-      <c r="D344" s="10"/>
+      <c r="D344" s="10" t="s">
+        <v>83</v>
+      </c>
       <c r="E344" s="1"/>
       <c r="F344" s="1"/>
       <c r="G344" s="1"/>
       <c r="H344" s="3"/>
-      <c r="I344" s="13"/>
+      <c r="I344" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="345" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B345" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C345" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D345" s="10" t="s">
-        <v>83</v>
-      </c>
+      <c r="B345" s="1"/>
+      <c r="C345" s="1"/>
+      <c r="D345" s="10"/>
       <c r="E345" s="1"/>
       <c r="F345" s="1"/>
       <c r="G345" s="1"/>
       <c r="H345" s="3"/>
-      <c r="I345" s="7" t="s">
-        <v>40</v>
-      </c>
+      <c r="I345" s="13"/>
     </row>
     <row r="346" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B346" s="1"/>
-      <c r="C346" s="1"/>
-      <c r="D346" s="10"/>
-      <c r="E346" s="1"/>
-      <c r="F346" s="1"/>
+      <c r="B346" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D346" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E346" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F346" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="G346" s="1"/>
-      <c r="H346" s="3"/>
-      <c r="I346" s="13"/>
+      <c r="H346" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="I346" s="7" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="347" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B347" s="1" t="s">
+      <c r="B347" s="1"/>
+      <c r="C347" s="1"/>
+      <c r="D347" s="10"/>
+      <c r="E347" s="1"/>
+      <c r="F347" s="1"/>
+      <c r="G347" s="1"/>
+      <c r="H347" s="3"/>
+      <c r="I347" s="13"/>
+    </row>
+    <row r="348" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B348" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C347" s="1" t="s">
+      <c r="C348" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="D347" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="E347" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="F347" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G347" s="1"/>
-      <c r="H347" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="I347" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="348" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B348" s="1"/>
-      <c r="C348" s="1"/>
-      <c r="D348" s="10"/>
-      <c r="E348" s="1"/>
-      <c r="F348" s="1"/>
+      <c r="D348" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="E348" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F348" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G348" s="1"/>
-      <c r="H348" s="3"/>
-      <c r="I348" s="13"/>
-    </row>
-    <row r="349" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B349" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C349" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="D349" s="10" t="s">
-        <v>85</v>
-      </c>
+      <c r="H348" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I348" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="349" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B349" s="1"/>
+      <c r="C349" s="1"/>
+      <c r="D349" s="10"/>
       <c r="E349" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="F349" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G349" s="1"/>
       <c r="H349" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I349" s="7" t="s">
-        <v>87</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="I349" s="1"/>
     </row>
     <row r="350" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B350" s="1"/>
       <c r="C350" s="1"/>
       <c r="D350" s="10"/>
       <c r="E350" s="1" t="s">
-        <v>88</v>
+        <v>15</v>
       </c>
       <c r="F350" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G350" s="1"/>
+      <c r="G350" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H350" s="3" t="s">
-        <v>89</v>
+        <v>14</v>
       </c>
       <c r="I350" s="1"/>
     </row>
@@ -5443,7 +5457,7 @@
       <c r="C351" s="1"/>
       <c r="D351" s="10"/>
       <c r="E351" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F351" s="1" t="s">
         <v>9</v>
@@ -5451,28 +5465,13 @@
       <c r="G351" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H351" s="3" t="s">
-        <v>14</v>
+      <c r="H351" s="3">
+        <v>20200331</v>
       </c>
       <c r="I351" s="1"/>
     </row>
     <row r="352" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B352" s="1"/>
-      <c r="C352" s="1"/>
-      <c r="D352" s="10"/>
-      <c r="E352" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F352" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G352" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H352" s="3">
-        <v>20200331</v>
-      </c>
-      <c r="I352" s="1"/>
+      <c r="D352" s="9"/>
     </row>
     <row r="353" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D353" s="9"/>
@@ -5530,12 +5529,27 @@
     </row>
     <row r="371" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D371" s="9"/>
-    </row>
-    <row r="372" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D372" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="B5:E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Change api name Request_Get_PledgeForMargin and change output json
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -215,9 +215,6 @@
     <t>GetDropdownData</t>
   </si>
   <si>
-    <t>GetMarginPledgeData</t>
-  </si>
-  <si>
     <t>DPIDValue</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
   </si>
   <si>
     <t>GetCurrentPledgeRequest</t>
-  </si>
-  <si>
-    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"Column1\": 43598.0\r\n }\r\n]" }</t>
   </si>
   <si>
     <t>AddPledgeRequest</t>
@@ -1024,6 +1018,12 @@
   </si>
   <si>
     <t>{ "fileName": "15444_CombineContract_20210101.pdf", "fileData": "JVBERi0xLjQKJeLjz9MKMiAwIG9iago8PC9GaWx0ZXIvRmxhdGVEZWNvZGUvTGVuZ3RoIDg3MjQ+PnN0cmVhbQp4nO1dXXfcuJF99zn+D3jZ7EzioUgQBEk/rSTLdu9KsmPJSTZxzh66RVmdobqV/rCtf78AiAKqQDbFHsUnemgnmUxdN75u3cIXq9n/fJ4lMsozyVis/lMkkUwLJniUcZbHSVRkBZvePj+Y3H7h7NXi+R+fPzu6fP7s4PV8fcRKdnn9/FlSFlEuCiZLVTgT7PLq+bOfjt+dX344PL5k5+8uT9jxxzN2efgXNjn/07vJ8Qn79NPHgxVLE7a4Zm8uLtnhdP3p55/Z5T+ePztRtc+fPxOxajpjsiijtJDs9vmzTIpIcA81AOUOau3C2nlgl2wKRXRnyygrCl8LQCVztWq7TJhr2NpT3zuLNBYRDjEmd1USs3A1cNezJkByBhXaoQV8qBouvCfOmTSeaN0mlROFKFs/vKqrZjb/wt5dX8+m9Uv29pC9npwwfiCPz9jH08kblly+fvfh1enpxYeTF68/vGBnH8+ODifs/eScvVTNqj8Je//23fmJMjmXWZLEpXeV70LRdqGUUSxT2om2cTZ5paqIzZ9eX+dllBQJ8bWFsK8t5LxmbB7Y4in62vasCRDufG2HFvDR+jph+j/LL8+fxewNoU0WUZmbEOFxHJVcOKgByH+qtaW1i8A2IeIg3X5e+FosBIV8D127vsfBGBBreJBAAbFyQprtVxMghSPNDixgQ9VwvWdpBEsXWlCgKj+1kwklTyIuYGJfzNfLarpm5wszIQgV7SSa22GWmHHBRZRKTHiLcN8vY6e+28Q2hDvIE04gKMQ9ebZZz7frmye8hYrAS4ETJeY8FEMTQlCqCPRUBryHbPNY0V0KyrdeHifzrws9gSq+84MkLSVP6ARqBiox5W4i85y7uc5Cbi60naY2XS0953SeZf3TMpm8XO+Qyg0kAk8FjkyJ0ANBNCEEpUSgKRmQvn0ezdQ2JuetXpMo5h5qAMod1NqFtdPAFm2XLWTaF74WgDLmanVdtg37LgcRi6YIHNLcV4lNgecI27MmQFI3R8DQKB+dmXTP0zaexsylUvU8tfuiy2V1VbNX1bpmTG+NkgP1XzULoOjukaseu9o6Yz/IPMoTQfxgIN+71s79WIjdjh8g5AcCZczVCpxCw8gP0D082WsocF7o3IK4IlBJE0JWSCnVGWLFq3ZP1zi6hsWbFpEZCFLv0cXJoE7NYEtMfJaoxSHmmPgW8r5o7cz1m9rtth4gTzyFMuZqhaUOGkbEQ/cQ8QYqAneF7swJ84EumhAC6RSBtMoepe4JG0vYsFYLERVpScV6PizWdrwF4V4XLwn1BvHeaO3UU09sewS1EKKeQBlztbptWduuZ951Du3lDCQDf4X+zDDzoTCaEALtyEBbRVeqe7pG0jUo1CxNokTv97FQz7BQfYn2doWXUVpqktXWI83aAsz8+Xh8fHDczOr5mh0vrvRRIcmEEH1VtY2neaYOGUFdF/V63dS3uhZ9vOu75rExpkrHKaelz8/13iWOk+0D0CNVhKmtk9q4t3ug3nbg8+oAwPWyhQq8+vM5mxyyt2+HxiajUs8oqBga2qv18NBku3KiwnHW3Zlt62oamwOQKSfP//SRTU4O2Tk7fTfQ30z7IqNlL06OJuxD/WW2Uuft9Wwxf8gl6riTaXJxJZPzv+oLvFxmae+lHQxZCzHbpWg4ah5HnLcFk+zPpydvD9m7V5cn7PByYNiyVKfihBR+vVlvljX7HXt3Z8Y8ZsCo+I7jHV3SdblQ4xVKWUkcxYm0VyKb5bKeT++HVWWbxAV3ojgry6hIEjtLnB22d7Nye1/V30c8y2nB4zN9CzvQz4JHQZEkETzuayYn3VPMyNgO7Ky6qZbV6kYpd4DLMlHuD0oenx29f6CHeWGmHlJscp5Jwctsezft1Jmp7uqNDZo69Z/3h+fs/J2aNU/eXKhzpv5ztvg8a8xEyr+rP3lRDpAAtStFJ2Ue1n5yW80aVVP1+fv3/9L/iKaL7w9XppaRsux09ZXhR/VKTVJ5HPu/sNP/5MrcsvNY7aF679mzTEY5F3rRToWIUu0CCzUA+U+1trS2DOxcL3IAmXVPlr4WWBoZVAorI7SLVsrgNI3O7/i4DbsJYskSHd+hX02ASDi+w8ACNtrFeg5dLzFNcN2AaIIbCVebPW+5xoidd05psuye0lj/5Qm5YoDeIZ5aKA/IDbiXmKrQh00IgZvzQAZlly44SWK67DEX02VPwo4uu+d3dBE775wULF3kpMD6D+2CqCo456Ljde8FFQudhPyGldXn7ZSKAXHiybJHGUQWnLQQWXAYAwj2ndAatfPObrUli+5WWf+5kROygoMWPuH13ouw0EfIbZitXmcXgRh6tAUbakxXu93HbNkDgWPLHhgcW8TOyTEDsUUOI6z/7ILJCjf7+JTRezRnoY+Q2xBZ/c6WgRiKgKzuMq7CVahPCdVWYRekw6Zhf6qaTb1iszmbzK9m1Zx92NzV9Soa2mbpe8ssLaKsgL30bHlwVl1Vty8eLMaLKM0Lu0izA/bnmt1UX2u2vpmt2FV1z64W85p9vmf3i82SLZZX9ZJV8yumtn4GqabTxUatauubml0vmmbxTT/NVvuK+aqa6h3iCm0V1IyuDnP4nz33/FmSRaUiWIkpUZuxQj87tlADUOqg1oZSeWCbRxMO4jJK4tzXAlDJXK3aTphrtzX96mcBv/hZAFYyWx0xc7z42V41AeLSCWBYARfhHf+eo16O4DQf7mTV/CWF/mQRJbmNkXdaymOl2Q42J7znwpwJMe8Gkp53Y+eed2K3vAOEeCdQyVytlndo1/HuOueIbxFJXRV6MsPch5JoQghUIwNV5V2N7skaRdY2sSapXhpSqlbzJGq0WvWoySTByzgqJeG/hXyPWrtwI6B2+2AdIM8/hUrmam3JdO16/m3fPP3GRSX1WOjQnNAfKKMJIRBPScXVM53umXqYqa06VT3Owln1op5ulrP1/YFLQ7mqV9PlzFwWjdWv4SJPsFvSWE/h2Cst4j/U2n6xoLbxioO8VyhUMldryzE065ziuua80jqupH4M3Vxgr4R6aUIIJFVSySFGnID3VI2gapuCecmjPBDw0eb+YKxO2yGT6SNVm5KyKAj7GvL9a83Ek0/slnyAEPkEKhlUarmHVh35rmuO/BYR1F2hN8l+LJRFE0KgHBEoq2ei3VM1gqptOk0Trg63gVD/uKnmazXTjharoUEQD+SqCzk5OrQQ6qWx/b6G2q0LAEIuIFDJXK2WUGjX+wA6531gEE7c1nFqQnwQqKMJIRAQDwQmeuS6J2sMWVsFK9KIG2KQYN8sF6sV+1CtR+9j26EX2Asi0Rd7CfZCC/l+trZw46B2m6wIkPcChUrmarWHV2jXewE6571gEEkdF/qVHCRCgTQhBBqSgcaKHsnuyRpD1lbJ6udO+mEc2QwsF7/Wy+rLaMW2I5fECSKP8pjsx1rIf6q1/Z6c2q0TAEJOIFDJXK3WCdCuv5+BzvkLmsQ+N8F+C90qsBNCfTQhBBLKAonJrmL3ZI0ia5tiRZJHSXhPcF6vd5pizcDJ8UGUqgcZ2Za1kN+XGVv6lYLarQsAQi4gUMlcrZZPaNe7wPbNe8B4qaROC31KDsChOJoQAv2UVF89J609Uw8ztVWqGWwdkFSPm8VKPyvYSa6GGbIvy4SCCrLItZC//25tH3TUNl5wkPcChUrmam05de16L0DnvBsMwonjQr9Ksi8LBdKEEGiIBxrr2cTuyRpF1jbRZnFqvg7YmV8vF+uqGavYduTkMjzLVNygBxcNQP5Tre0vOajdOgEg5AQClczVap0A7TonuM45J7RIRv0WupUscqE+mhACCWWBxHqeHOzJGkXWVsWqjxYy2MN+qG9/GS1WPWhJFrlMP/uXhH6D+JBq7dQPgNgt/QAh+glUMler5dI269mHrnn2M/yRfneSy8RQF00IWelIqizZsxmg5ZBQi65Qiy1C7dqhUJOOToNxdsx/bQ2PGslWkWZlFKcFFenJ912TBOJM7UXMd9ELhej7YIs0Fikdok29TzEmp6bJzwDEdD6FGhwiGFRoTMmgRWuiR98WQc++LUKeZAtqpvjht+1VEyDuO+gwqICHToLAnp+Qn+HvpKjTv76winPzMKFd6ze3n8enCBhKBCbeZUh45l0OhYXcY2M7CGqL7sPmtPuwWTCa7yF9aoZ3APTOO8AgnPgs8ChyORKBd0CfbjhVlegKdM/TQzwNCrUookLftGGhXs5ux+cGQCIC4l+IiKcJ4d9AvpOtnXr+id3yDxDin0CCuVqBf2jY80/zJCTJzyBeC72aYR+E8mhCiPsEDaKwvKvXPWGjCRsUbpKo/YUJg988xbbDl8QVkOCDXAEpQNBRyHiAgRBbdPMk0m6ehGA0XUn6zCLkCugecoWBssCBoYNT4opAKU0IgZiyQGyyR7t7wsYSNqzdjLdXAb951rVZNd4PLt/H+8FlBFnIZTrYUVBbdPMj0m5+hGA0e0n6RCPkB5zzI0mqEXFe6NycuCFQSRNC3OcaYaH17GF/OFv+GPpvzcp6DFNEryPTqTyfkKzj6XTZPBZy6Qu2R9QW3aSHtJv0IBjNPJIuSchrj6brSJImRBQbKrrA4gud3YQQ93lCWC+IlW5K1Y+iCz36/3emVD2KqsHpkpdpVCbBdHlRN6MvTV1uDHIB5O0gH9jEHnAB5C+AC4gtulkPaTfrQTCSgiR9upBXLE3ckSRhiMg8DANyng0F0oQQ9xlDRGM98+UPpwsp9t+ZXPUoqnaYMF2mC+ITsnAQn5CnA21CMgL0idiim8KQdlMYBKM5RdKn/yABkkQcSRKAsGw7qibn1NDfTQhxnwFEJNNzpv/xhD2VdKlHkTU4aaZqj1noJD88ab6vl+zjfLbeOWPKO8Il43hHuHQdC7mkBDsUaotuKkPaTWUQjKYWSZ8FhJRL8nEkyQMieg/jgRxWQ500IcR9IhCRWtGj3B9O2FPJmnoUWcPKLaR5HeKjlOsSX5AjICkHOQLSdsARkKIAjiC26CY2pN3EBsFoipH02UDoApvk5UiSD0T0HsaDwMoNddKEEPcJQURqPWf7H0/YU8meehRZD7zyj5vXgD5OuTYNBvkBEnSQHyCFB3oKeQowEmKLbnZD2s1uEIymG0mfGYSEi5N0JMkNImoPo4Gc7UOVNCHEfXIQFlrP6eqHs/VE0qgew9SwZqWabYvkkZqFNBjvBpei493gkngs5FIV7EioLboJDmk3wUEwmnAkfW4QEi3J0pEkOwhLPQwFSXa4oUqaEOI+PYgIrWeH++MJeyq5VI8i64FnrMo1MtgnfPrpqL5eLGt2Wn+d1Sv8KwMjE6uQRyBnB3kEsnrAI5CoAB4htuimP6Td9Afhc4VAwiRJSZJsIS9hmtkjWX9gkA1DKJgmhLjPFyKa63mQ9eMJeyrJVY8ia/iNgCKNklJSCVfLX1c7Z1ghJ9hUJ+QDyIWCXkKuFIyC2IJkWCHREkgwmrclGcnskiTHCmk2Ix/qDwRyFRsKpAkh7rKssMRk0qPYH03W00hHewxRw2rN9KvfArVObwbeSGfeCSNK3Qz8nEB1N1tXDTtTKq/X7G/uHZJ/V/9+ccLOF8vbqvm7fcFZXS11SvfbxWal38ymP+DA0/VVxD79xM6PTxme5rvvj4tUD5go8kgNwL7fMVfEJUW6vVQh2hfV41JJ+jITL/lAqSQR5g2fpBjPlYfIryZ0iqk+qqlg59ZyFSVJRou9nZyy09ntbF1fbS/JS9XPsOTR5n57iTRVbQkZdHHg82pIUm8NCBM8y6KM/BxMp5z6vAyZSNQOdaiQ/uqKvr4NGlM723ywXKbLdfpoig0UknGU5YGPz/tevCeKLOIlnmcAQfMMQDBjtHYa2GSe0RsfUZJJuYUyN8+0tpuUwfSpc4D41DlAbB4c1EhMnDoHHWsCxL03H0YWsDHtf4GVjdI8j1L4TanxUYpL7RCluJiN0p436HaidMfWIEpxsd2iFJccF6WkiyOilDBhojQbE6WkmdFRShtT4VakY6K0p9iIKMWl+qNUv9pY7dlQlFoER6mFXLwZuwjskkSp1jv8ChWOZdYf+jhAgpBBQYpjCmogFvkJKuhWEyDud4JgXAEXwzGquptku4YoKrRDhKJSNkB7XvnaCdDd2oL4RKV2C09UcFx04v6NCE5Mgo7NYtQKihsZHZqkKWXEo9bPbqkRgYkK9celFCabFsWlRXBcWshFmLHTwM5IXBqNCxKXBkKrJ4l2HBVBnKDAxIHEXY3ExL86Ax1rAsSvnnZkARvDkZlJJbCdQxOX2iE2cTEbnD1vp+4E546tQXTiYruFJy45Lj5JF0cEKGHCROio1ZM0MzpEaWM6ikatnj3FRgQpLtUfpZmIZE5WT4vgKLWQizdjF9Qm3+wycs9LEqQmAhLWH/o4QIKQQUGKY4q7GrGZ43dL2341FPC/sgfjCrgYjlGhjhc7b3BRoR0iFJWyAZqPCNDd2oL4RKV2C09UcFx0ogID840LTkwCV3qOR62emITRoUmaUrIcLqbf7Ku3ppRwGadKcyNCE5Xqj0whIpGT9dMiODIt5ILM2CKw6fppVE7XTwNJ1h/vOC6CSEGhiUOJuxqJSdZP27EmQISLTTuygI3p8I8CilREXIW8/54bIP57boDY7+G0ZknMPEFf3WmbRt/caYEEvuYGXYMGfU+DviO28OC4q5CYmCzbp4YisnRk2SEFLEyDbwHu2QnYIdelY0QFGY2IN5vyCAjkgUEfiJ2jDDRMHUUgWcwR4Vp9UuRtk9aeo8cIzOYrYvJsRqNjz+ZrOfawnaNMsQyzR5DEpUk6+qDdJ0XfVontWXqMyCBlANEHSQUAwZNS6ASxc/SMViD6KJK4TAW3S4F2nxR920S2Z+lxIrObR8QebC+BPdh+AnvYtuyRfSzZswJ7vTvhJ0beVontOeoXWOcbl7k623N1vEhllMHvFx4xdFJlk4vJ+cvJ+UmW5YdxEicJY+xCv2o8fEFTJ1855ergLGjdSe+Ph/mDHzcbHFRAHxiTKBs6ZtoLBC6jNLW/1abvZwspBn77Dm4QcCl1rOfFy2zotg6uEHCxLCkTdaQdaMzdIezYGlwi4GLn1dfZnL1uNovlbF6zyXxdL+fmhxGrhp2OuFjAlY27WcAlBu483NUC/jyXSsvlqLsFSk7E+ajLBdpYVkTJYDm498PF8lKFQTrgCHe5QBzRe7vARRSrwaBJyCJ4ErKQm0+MLQJbkknIBHRGZiEDodsFMrXhKSCYFNAshGcN7mokZoanIduxJkD87YIdWcDG8M2ffmMBl7sGLi61Q+DiYm3g9k1JncDdsTUIXFzs0YGLKxsXuLjEwBWnC1z8eRW42chLQUpOxAcv3l3g0sZU4A6Xc9eCpLVC6q8gDjyMcKFLXNEbuqrrRUb2DxbBoWshF4TaloFJtw8mBkjgGoSz/ukAB00QRihwcZxxVyMxcdzabjUB4sLWjipg4qFLQX0lmwl87WURdO1lEbjEMmZGTf9GoMQ2neF7L4Pk7t7L9g1a9F0NOo/IwqPjrkJiklnO9qoJkMzRZQcV8NDZkO75CfkZedrxxLnrJ88cXFBZxN1f2T5QG32Tl5BHodzdelkqXLNPi75t8tqz9DiRwfUTog9uqIA/uMEC/oiNvnWbEf4IlPt7LyAQGn5aBG6V2Z6nxwnNXUF5At0tlYXcLZbtBLXRd14EJpBCub/7gu0KNPy0CNwmtD1PjxWa3Uoi/mCzCfzBZhT4IzY9eyL+CJSz/m3xU6Nvq8z2LG0TWfe1gkWUpHo/oY6W3N6AnPyRDR9q3eVhLIo3caK/M77r5SFub9TlIS6gj5VJVKKjbxBBXhZpmUZClGizDojfrANid97GzKjF8V7dcOteBewQzno2/+h0MO1oFekBu4+7ComZID1Ar5oAATnAkAIWwqDZsxOwQ19zNEJUsLIg3mDxAQgWJ9sHanKyonnuKMRZ/zqZPDH6tolrz9LjRNYuLJg9u/Q49uzSBOwRk5P1DLFHIHRxRVbJJ0beVontOeoXWPfnMEWU5eowVmZRnuTBD7OwzhsFmLLar6Ju/S7rw8s3aUyUPFN9xcv3mB8tSPM0itOyfVWPiNLcIQ0giYNam7e2SAK7fYgLUJFGXCS+FoBS5mo1tmDQrjW9twHx3nZFrOugRmwSb9uONQGSOHfDyCgbnZDYs9TPkguKB15HpPtOaSxUiPOU8Ggg/6nWlr4zxG55BAjxSKCUuVqBFGgYEQndQ0waSATsh96hZAZubkIIlCACpfTJbk/YWMK2/75babI11MejNIYZ+eJk9Pxohl1iF2SpgoTELmihwkGtXboBULtdDwHyLqBQylytlkzXMHIBdA+5wEB54LjQsZK4IFBIE0IgojwQWdmjWVwQa1Z2NSv7NdtjdzQrupoNh9q1//W1PGpEI2dNO9tKHhVphtcei+C1x0IugIwtAzvvhF2ad8IuLVj/ikZ8QlcCtPbgpQLViE2crAUdawLEPW51I6NsdFboH8XS01ihfztLO7xj2M2uiEuY/BGZsD5Ak6Bv6BGx827U5N2oKfyqQ6ImJZoLJn+86vRtvZyQqe4CXzchJP2qQ+TSp70fTthTWqYfRdgD7w+M2wONzKIk5vYtP4fvz/7ncufl2rvCrZreFW5htZBbeO1AqJ2T5dprl0IF698E9KxhZXfdCBfWMCIk0W6glCaEpF+uidjKHu3+cMKe0v7mUYQNv9AqjiNpSEPavXx3eXiqTv3n9brvtVLu1iBOVZyomM1EVJSFLVt9rz43NftaNZuaLa7ZRb38OpvWK32LAD/+zv7Ajm+q5Rf6dsJuXOlcNU7r5/pLnz35eEc46VNPLEOF0MKb8cjmcIIXWwSrp0WcDIyZBHZKxGPY50Q8BkLiIZKU2GHBKojWXbxMclclMTled23PmgDxJ+N2ZJSL/gzONC8iXupsEhHJ0v7I5PvqfjI/UP9cbNbs3edm9sU8DxrICJQ6q0TSWrp3P92EwCSKk/KhYsitgkeC02nBQtixFnI+MrYM7IJ4VnPE6TxqoJL1ykUiVinNyK3IC9xVR0yy57S9agLE76bssAIutmTmKmrLQn0qFZEobLy8W9/USxWiX1YDrtSJ1IKWS5R3BrzIdep1OlQEeTDlEefEgS2C/dcizhHGDG0amIYLGpgGEqxfFBLTFxCKPIgZ565KYpLAtD1rAoQ7F7Yjo1xsCcwyUX+pPsT1tSr8Enw9Xy+rhr25uGT/xcr/GHKjCi39qwC4OFftDSXacv1S8HywDPKk+ps4kcSVFsK+tJBzi7HzwC6JMzUtSUGcaSAUi1ghEhFJmUWeRMRzVx0x8duloFdNgOTOkXZYARfbXCmjLFMBkogozuFXftbVut7FkbjwWEcOlEGOVFNFkSTEkRbCjrSQc4mxeWAL4kjDSkocaSAUlUQeEhMZUIt8ibnnrkpi4tf5Qc+aAPFRaYcW8LF9YpV6JGqXVMBrKi5Ojibs9cnJxcPzKi4WR/HAS7/cvLq9CHJirLoV02i0EHaihZw7jF0ENo1GzUZMo9EQxPqVITF/AaPIh5hycAixYhKPtl9NgLj31cDAAja2uzBN9G9+pZGUPh5v79irzXrgWxnWh6RcHg1+5cH6cKCI9yFXU76IyeIIEPIhQOCN1k4DmwaioYMGooEy1q8MiRkMOEVOxKRzVyUxcSBCz5oAcW8Gg6EFfGzxYqq8qDZUaqWKhLTfNby4vHx4KiUlRPmAA9updKgM8mCRREmZEw9aCHvQQs5jxi6ITS7lNRFpWWL/GW5YvyYkZi7g0nuPkG1dgQ3dIPKd6VNDbN1nqMwOKeBhOvz1E563vwTlr0cBQdejAMH1TmungZ3hS6G2eXS1BJB016Ouw7Zd3+FgCIgwPEZUIzbxi3ygY02AeLnDyCgb4SXynqUtLI3LqcX02dtIzJ+9sHSt2IsY1wliZ/j6BvNHIOmuQR0Z0PDTInCrzPY8PU5obh72BLqp2kJuIredoHZGpn9PIIUk619S5FMjcJvQ9jzthbYX2r9baN0HAO3DBp6nkfu+db1m1e1iM1+zD/W0nn3VTwM+/fTLp5/ZAXtf3bfmH5R5dM+Om1k9Xw89AVAdSUn9okzNGyyHngCoQmZQY0q5Pb/5oQ4uU3VuzuCHlPSty/kiUlUdHh4eH6nu8FP+10vVef3n4vCYHS+u9M9ylGWeqOL4EUc1v2LLuqn0i1VW9XSznK1n9Ur9a/s4JFKVvG+qac3eXbOLzd1dc6/qOatuqmW1ulkvqwe7qn/d1Pb0Q31bLX99+WAR9X/6YY8p87ff//7v7HJZXalOVcua1d9VJ3VnrzY1Wy/YfDH/5Wq2mprnNPpBzsLd76u//lYtr1Y67fPLbH5wdnl2cFGv1019q9zJFku2MBfIV/Xn2Tp6sFf6wim1vXpVr6tZs9LtrXXffvk2W9WsMXmnbHVTNQ37XLO75eLr7Er1VfVlWf9zU69GNJPwKIYXeqhxz1fVVA9mxZjutfo3Vd9sztj6ZrZi04W+QJ2uFQ3rmk03t+zzTLXtevBl8bVe6hLGz6vN53/U6sOKNjVwxj5smnr1Qim8/qWpvq3MZz7UXzZN1bao7ePZcqqAZTtWVWpZr+5UJbOvNTv5rmiff1FDVgP8djOb3rRsrNhN9fXBgarztE4da8+5Xnm6UVczO1ooD+qmJ/OrWcWul4tbNfTZrfG9/v+ITdZ2vFWzWuhBB8NU6q6/Vsrhh9O1Gq0dNBrni1ezZTsihZ8v1rPr2dT+zZuN8l8zm5vngrP5tNlc6V+00QF3qhhTwfE7x9BDA07UIVRy7m/YDt4Y77RihBEeMHuT6v6upeTjXCv6sl4qmhbLe/L3s9Vqo3xsyCHcXN5gJ1k5qsng9q6pZmbqWy2ajR7qC3a4VFGwbANHN3h4d1c3el5QYef/5rqaPjhONbELSJhWNLffvMLVm2t/Q+mHw+NPP0dM93NqJll2W92z6k51tVJqmqnBzWsV9qs1m5pCL1S0utBrJadnheqrwswDXRNqHYX+54p9qz+vZuv6wQBM8iTiCTw5bOpKBfbXmSrKvn37Fn1e1TPtp2iquNbp5UcXJ+yF/ptb9TeRCkwNnl2cTF68MAXmYYHzi5OH+5DGUVraK1JNjhL4soYIbGYrM1uvF9Nf1XxoI6WNgcVcTdAqBq7qqlmzz/fsWnVcu1MxeqfmOvW/lQntlf5XRRVEgZKn+RyPzdPwk+NjMhV8+um16ruNbjVKPezfsbPjv7wwg7rVafez+bX+TShTm2HswWHyOEoKe4t4s17fvTw40Jyt1IQcqalL0Xmg//3/rqp1dVCt10oTV4vp6iBJRcxzHpdJHhfR3ZWq8fmzbTy9qu8WqzZo3lfL9Ww6u9OzwW/i6+L47cmrj6cnbDJ5we7URKKnl+v64diPy6gsrEPVfPLr82dbxqsm89XBzHxpEc1EeowPtVGWUW6fVr7SYavW6Tg5UP/V33Vg1ZqdfTw7OpwMVFNK8woXVNH/LjZq5r+uZuub603T3L8Y2ATpO5WUFWWU5Xa915IxS/dds1mpuWt6M180iy96lj89fT/QkayIYl6wvNS3NHaT8/7w3Gxy/BZn8LfE9C/jmESTKM/sov3fh5eTc/Z2cnZ2eHl6eMou3h6+9TX8P7ZH9EcKZW5kc3RyZWFtCmVuZG9iago1IDAgb2JqCjw8L1R5cGUvRm9udERlc2NyaXB0b3IvRm9udE5hbWUvQXJpYWwvRmxhZ3MgMzIvRm9udEJCb3hbLTI1MCAtMjIxIDExOTAgMTAwMF0vTWlzc2luZ1dpZHRoIDI3Mi9TdGVtViA4MC9TdGVtSCA4MC9JdGFsaWNBbmdsZSAwL0NhcEhlaWdodCA5MDUvWEhlaWdodCA0NTMvQXNjZW50IDkwNS9EZXNjZW50IC0yMTIvTGVhZGluZyAxNTAvTWF4V2lkdGggOTkyL0F2Z1dpZHRoIDQ0MT4+CmVuZG9iago0IDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50Ti9CYXNlRm9udC9BcmlhbC9GaXJzdENoYXIgMzIvTGFzdENoYXIgMjU1L0ZvbnREZXNjcmlwdG9yIDUgMCBSL0VuY29kaW5nL1dpbkFuc2lFbmNvZGluZy9XaWR0aHNbMjc4IDI3OCAzNTUgNTU2IDU1NiA4ODkgNjY3IDE5MSAzMzMgMzMzIDM4OSA1ODQgMjc4IDMzMyAyNzggMjc4IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiAyNzggMjc4IDU4NCA1ODQgNTg0IDU1NiAxMDE1IDY2NyA2NjcgNzIyIDcyMiA2NjcgNjExIDc3OCA3MjIgMjc4IDUwMCA2NjcgNTU2IDgzMyA3MjIgNzc4IDY2NyA3NzggNzIyIDY2NyA2MTEgNzIyIDY2NyA5NDQgNjY3IDY2NyA2MTEgMjc4IDI3OCAyNzggNDY5IDU1NiAzMzMgNTU2IDU1NiA1MDAgNTU2IDU1NiAyNzggNTU2IDU1NiAyMjIgMjIyIDUwMCAyMjIgODMzIDU1NiA1NTYgNTU2IDU1NiAzMzMgNTAwIDI3OCA1NTYgNTAwIDcyMiA1MDAgNTAwIDUwMCAzMzQgMjYwIDMzNCA1ODQgNzUwIDU1NiA3NTAgMjIyIDU1NiAzMzMgMTAwMCA1NTYgNTU2IDMzMyAxMDAwIDY2NyAzMzMgMTAwMCA3NTAgNjExIDc1MCA3NTAgMjIyIDIyMiAzMzMgMzMzIDM1MCA1NTYgMTAwMCAzMzMgMTAwMCA1MDAgMzMzIDk0NCA3NTAgNTAwIDY2NyAyNzggMzMzIDU1NiA1NTYgNTU2IDU1NiAyNjAgNTU2IDMzMyA3MzcgMzcwIDU1NiA1ODQgMzMzIDczNyA1NTIgNDAwIDU0OSAzMzMgMzMzIDMzMyA1NzYgNTM3IDI3OCAzMzMgMzMzIDM2NSA1NTYgODM0IDgzNCA4MzQgNjExIDY2NyA2NjcgNjY3IDY2NyA2NjcgNjY3IDEwMDAgNzIyIDY2NyA2NjcgNjY3IDY2NyAyNzggMjc4IDI3OCAyNzggNzIyIDcyMiA3NzggNzc4IDc3OCA3NzggNzc4IDU4NCA3NzggNzIyIDcyMiA3MjIgNzIyIDY2NyA2NjcgNjExIDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDg4OSA1MDAgNTU2IDU1NiA1NTYgNTU2IDI3OCAyNzggMjc4IDI3OCA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTQ5IDYxMSA1NTYgNTU2IDU1NiA1NTYgNTAwIDU1NiA1MDBdPj4KZW5kb2JqCjcgMCBvYmoKPDwvVHlwZS9Gb250RGVzY3JpcHRvci9Gb250TmFtZS9BcmlhbCxCb2xkL0ZsYWdzIDE2NDE2L0ZvbnRCQm94Wy0yNTAgLTIxMiAxMTIwIDEwMDBdL01pc3NpbmdXaWR0aCAzMTEvU3RlbVYgMTUzL1N0ZW1IIDE1My9JdGFsaWNBbmdsZSAwL0NhcEhlaWdodCA5MDUvWEhlaWdodCA0NTMvQXNjZW50IDkwNS9EZXNjZW50IC0yMTIvTGVhZGluZyAxNTAvTWF4V2lkdGggOTMzL0F2Z1dpZHRoIDQ3OT4+CmVuZG9iago2IDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50Qi9CYXNlRm9udC9BcmlhbCxCb2xkL0ZpcnN0Q2hhciAzMi9MYXN0Q2hhciAyNTUvRm9udERlc2NyaXB0b3IgNyAwIFIvRW5jb2RpbmcvV2luQW5zaUVuY29kaW5nL1dpZHRoc1syNzggMzMzIDQ3NCA1NTYgNTU2IDg4OSA3MjIgMjM4IDMzMyAzMzMgMzg5IDU4NCAyNzggMzMzIDI3OCAyNzggNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDMzMyAzMzMgNTg0IDU4NCA1ODQgNjExIDk3NSA3MjIgNzIyIDcyMiA3MjIgNjY3IDYxMSA3NzggNzIyIDI3OCA1NTYgNzIyIDYxMSA4MzMgNzIyIDc3OCA2NjcgNzc4IDcyMiA2NjcgNjExIDcyMiA2NjcgOTQ0IDY2NyA2NjcgNjExIDMzMyAyNzggMzMzIDU4NCA1NTYgMzMzIDU1NiA2MTEgNTU2IDYxMSA1NTYgMzMzIDYxMSA2MTEgMjc4IDI3OCA1NTYgMjc4IDg4OSA2MTEgNjExIDYxMSA2MTEgMzg5IDU1NiAzMzMgNjExIDU1NiA3NzggNTU2IDU1NiA1MDAgMzg5IDI4MCAzODkgNTg0IDc1MCA1NTYgNzUwIDI3OCA1NTYgNTAwIDEwMDAgNTU2IDU1NiAzMzMgMTAwMCA2NjcgMzMzIDEwMDAgNzUwIDYxMSA3NTAgNzUwIDI3OCAyNzggNTAwIDUwMCAzNTAgNTU2IDEwMDAgMzMzIDEwMDAgNTU2IDMzMyA5NDQgNzUwIDUwMCA2NjcgMjc4IDMzMyA1NTYgNTU2IDU1NiA1NTYgMjgwIDU1NiAzMzMgNzM3IDM3MCA1NTYgNTg0IDMzMyA3MzcgNTUyIDQwMCA1NDkgMzMzIDMzMyAzMzMgNTc2IDU1NiAyNzggMzMzIDMzMyAzNjUgNTU2IDgzNCA4MzQgODM0IDYxMSA3MjIgNzIyIDcyMiA3MjIgNzIyIDcyMiAxMDAwIDcyMiA2NjcgNjY3IDY2NyA2NjcgMjc4IDI3OCAyNzggMjc4IDcyMiA3MjIgNzc4IDc3OCA3NzggNzc4IDc3OCA1ODQgNzc4IDcyMiA3MjIgNzIyIDcyMiA2NjcgNjY3IDYxMSA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA4ODkgNTU2IDU1NiA1NTYgNTU2IDU1NiAyNzggMjc4IDI3OCAyNzggNjExIDYxMSA2MTEgNjExIDYxMSA2MTEgNjExIDU0OSA2MTEgNjExIDYxMSA2MTEgNjExIDU1NiA2MTEgNTU2XT4+CmVuZG9iago5IDAgb2JqCjw8L1R5cGUvRm9udERlc2NyaXB0b3IvRm9udE5hbWUvQ291cmllck5ldyxJdGFsaWMvRmxhZ3MgOTgvRm9udEJCb3hbLTI1MCAtMzAwIDcyMCAxMDAwXS9NaXNzaW5nV2lkdGggNjAwL1N0ZW1WIDEwOS9TdGVtSCAxMDkvSXRhbGljQW5nbGUgLTExL0NhcEhlaWdodCA4MzMvWEhlaWdodCA0MTcvQXNjZW50IDgzMy9EZXNjZW50IC0zMDAvTGVhZGluZyAxMzMvTWF4V2lkdGggNjAwL0F2Z1dpZHRoIDYwMD4+CmVuZG9iago4IDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50MS9CYXNlRm9udC9Db3VyaWVyTmV3LEl0YWxpYy9GaXJzdENoYXIgMzIvTGFzdENoYXIgMjU1L0ZvbnREZXNjcmlwdG9yIDkgMCBSL0VuY29kaW5nL1dpbkFuc2lFbmNvZGluZy9XaWR0aHNbNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMF0+PgplbmRvYmoKMTEgMCBvYmoKPDwvVHlwZS9Gb250RGVzY3JpcHRvci9Gb250TmFtZS9UaW1lc05ld1JvbWFuL0ZsYWdzIDM0L0ZvbnRCQm94Wy0yNTAgLTIxNiAxMjAwIDEwMDBdL01pc3NpbmdXaWR0aCAzMzMvU3RlbVYgNzMvU3RlbUggNzMvSXRhbGljQW5nbGUgMC9DYXBIZWlnaHQgODkxL1hIZWlnaHQgNDQ2L0FzY2VudCA4OTEvRGVzY2VudCAtMjE2L0xlYWRpbmcgMTQ5L01heFdpZHRoIDEwMDAvQXZnV2lkdGggNDAxPj4KZW5kb2JqCjEwIDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50Mi9CYXNlRm9udC9UaW1lc05ld1JvbWFuL0ZpcnN0Q2hhciAzMi9MYXN0Q2hhciAyNTUvRm9udERlc2NyaXB0b3IgMTEgMCBSL0VuY29kaW5nL1dpbkFuc2lFbmNvZGluZy9XaWR0aHNbMjUwIDMzMyA0MDggNTAwIDUwMCA4MzMgNzc4IDE4MCAzMzMgMzMzIDUwMCA1NjQgMjUwIDMzMyAyNTAgMjc4IDUwMCA1MDAgNTAwIDUwMCA1MDAgNTAwIDUwMCA1MDAgNTAwIDUwMCAyNzggMjc4IDU2NCA1NjQgNTY0IDQ0NCA5MjEgNzIyIDY2NyA2NjcgNzIyIDYxMSA1NTYgNzIyIDcyMiAzMzMgMzg5IDcyMiA2MTEgODg5IDcyMiA3MjIgNTU2IDcyMiA2NjcgNTU2IDYxMSA3MjIgNzIyIDk0NCA3MjIgNzIyIDYxMSAzMzMgMjc4IDMzMyA0NjkgNTAwIDMzMyA0NDQgNTAwIDQ0NCA1MDAgNDQ0IDMzMyA1MDAgNTAwIDI3OCAyNzggNTAwIDI3OCA3NzggNTAwIDUwMCA1MDAgNTAwIDMzMyAzODkgMjc4IDUwMCA1MDAgNzIyIDUwMCA1MDAgNDQ0IDQ4MCAyMDAgNDgwIDU0MSA3NzggNTAwIDc3OCAzMzMgNTAwIDQ0NCAxMDAwIDUwMCA1MDAgMzMzIDEwMDAgNTU2IDMzMyA4ODkgNzc4IDYxMSA3NzggNzc4IDMzMyAzMzMgNDQ0IDQ0NCAzNTAgNTAwIDEwMDAgMzMzIDk4MCAzODkgMzMzIDcyMiA3NzggNDQ0IDcyMiAyNTAgMzMzIDUwMCA1MDAgNTAwIDUwMCAyMDAgNTAwIDMzMyA3NjAgMjc2IDUwMCA1NjQgMzMzIDc2MCA1MDAgNDAwIDU0OSAzMDAgMzAwIDMzMyA1NzYgNDUzIDI1MCAzMzMgMzAwIDMxMCA1MDAgNzUwIDc1MCA3NTAgNDQ0IDcyMiA3MjIgNzIyIDcyMiA3MjIgNzIyIDg4OSA2NjcgNjExIDYxMSA2MTEgNjExIDMzMyAzMzMgMzMzIDMzMyA3MjIgNzIyIDcyMiA3MjIgNzIyIDcyMiA3MjIgNTY0IDcyMiA3MjIgNzIyIDcyMiA3MjIgNzIyIDU1NiA1MDAgNDQ0IDQ0NCA0NDQgNDQ0IDQ0NCA0NDQgNjY3IDQ0NCA0NDQgNDQ0IDQ0NCA0NDQgMjc4IDI3OCAyNzggMjc4IDUwMCA1MDAgNTAwIDUwMCA1MDAgNTAwIDUwMCA1NDkgNTAwIDUwMCA1MDAgNTAwIDUwMCA1MDAgNTAwIDUwMF0+PgplbmRvYmoKMTMgMCBvYmoKPDwvVHlwZS9Gb250RGVzY3JpcHRvci9Gb250TmFtZS9BcmlhbCxCb2xkSXRhbGljL0ZsYWdzIDE2NDgwL0ZvbnRCQm94Wy0yNTAgLTIxMiAxMTIwIDEwMDBdL01pc3NpbmdXaWR0aCAzMTEvU3RlbVYgMTUzL1N0ZW1IIDE1My9JdGFsaWNBbmdsZSAtMTEvQ2FwSGVpZ2h0IDkwNS9YSGVpZ2h0IDQ1My9Bc2NlbnQgOTA1L0Rlc2NlbnQgLTIxMi9MZWFkaW5nIDE1MC9NYXhXaWR0aCA5MzMvQXZnV2lkdGggNDc5Pj4KZW5kb2JqCjEyIDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50My9CYXNlRm9udC9BcmlhbCxCb2xkSXRhbGljL0ZpcnN0Q2hhciAzMi9MYXN0Q2hhciAyNTUvRm9udERlc2NyaXB0b3IgMTMgMCBSL0VuY29kaW5nL1dpbkFuc2lFbmNvZGluZy9XaWR0aHNbMjc4IDMzMyA0NzQgNTU2IDU1NiA4ODkgNzIyIDIzOCAzMzMgMzMzIDM4OSA1ODQgMjc4IDMzMyAyNzggMjc4IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiAzMzMgMzMzIDU4NCA1ODQgNTg0IDYxMSA5NzUgNzIyIDcyMiA3MjIgNzIyIDY2NyA2MTEgNzc4IDcyMiAyNzggNTU2IDcyMiA2MTEgODMzIDcyMiA3NzggNjY3IDc3OCA3MjIgNjY3IDYxMSA3MjIgNjY3IDk0NCA2NjcgNjY3IDYxMSAzMzMgMjc4IDMzMyA1ODQgNTU2IDMzMyA1NTYgNjExIDU1NiA2MTEgNTU2IDMzMyA2MTEgNjExIDI3OCAyNzggNTU2IDI3OCA4ODkgNjExIDYxMSA2MTEgNjExIDM4OSA1NTYgMzMzIDYxMSA1NTYgNzc4IDU1NiA1NTYgNTAwIDM4OSAyODAgMzg5IDU4NCA3NTAgNTU2IDc1MCAyNzggNTU2IDUwMCAxMDAwIDU1NiA1NTYgMzMzIDEwMDAgNjY3IDMzMyAxMDAwIDc1MCA2MTEgNzUwIDc1MCAyNzggMjc4IDUwMCA1MDAgMzUwIDU1NiAxMDAwIDMzMyAxMDAwIDU1NiAzMzMgOTQ0IDc1MCA1MDAgNjY3IDI3OCAzMzMgNTU2IDU1NiA1NTYgNTU2IDI4MCA1NTYgMzMzIDczNyAzNzAgNTU2IDU4NCAzMzMgNzM3IDU1MiA0MDAgNTQ5IDMzMyAzMzMgMzMzIDU3NiA1NTYgMjc4IDMzMyAzMzMgMzY1IDU1NiA4MzQgODM0IDgzNCA2MTEgNzIyIDcyMiA3MjIgNzIyIDcyMiA3MjIgMTAwMCA3MjIgNjY3IDY2NyA2NjcgNjY3IDI3OCAyNzggMjc4IDI3OCA3MjIgNzIyIDc3OCA3NzggNzc4IDc3OCA3NzggNTg0IDc3OCA3MjIgNzIyIDcyMiA3MjIgNjY3IDY2NyA2MTEgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgODg5IDU1NiA1NTYgNTU2IDU1NiA1NTYgMjc4IDI3OCAyNzggMjc4IDYxMSA2MTEgNjExIDYxMSA2MTEgNjExIDYxMSA1NDkgNjExIDYxMSA2MTEgNjExIDYxMSA1NTYgNjExIDU1Nl0+PgplbmRvYmoKMTUgMCBvYmoKPDwvTGVuZ3RoIDQ4Pj5zdHJlYW0KAAAAAAA/AD8AAD8/PwAAPwA/Pz8APz8/wMDAAAD/AP8AAP///wAA/wD///8A////CmVuZHN0cmVhbQplbmRvYmoKMTQgMCBvYmoKPDwvVHlwZS9YT2JqZWN0L1N1YnR5cGUvSW1hZ2UvTmFtZS9JbWcxL1dpZHRoIDg4L0hlaWdodCAxOS9CaXRzUGVyQ29tcG9uZW50IDQvQ29sb3JTcGFjZVsvSW5kZXhlZC9EZXZpY2VSR0IgMTUgMTUgMCBSXS9MZW5ndGggODM2Pj5zdHJlYW0K////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////f///////////////P/////////////////////////////////d4d394P3c/93d39z8//394dz8/+I//////////////////////////////P3c/f3d4eHh3Pz/3P/ePd3h4d3+P//////////////8I//////////////////////////////+P//+P//////////////////////CP///////////////////////////////////////////////wj///P//wjwAAAH/wd3cP93/3D/AHd39wd3D/cHdw/3f/+A//8Hd3j/////CPP/8/+Aj/cGZmD/D//wj3f3D/8I///4//8I+P//CPd//wcP/w////////8AAADz93cP92BgYP8P93D/cHdw/wB3//P3dw/z93d/93/3fwj/B3f//////wj/8PP//wj3ZmYA/w//+P93//D/CP//93//j/eP/4/3f4D/8P8I////////AHcH8/d3D/PwAAD/F3dw/3B3AP8Adwfz93cP8/d3D/d/CP/3jwB3A/j/////////////////93//////////////////////////////////////////////////////////cP////////////////////////////////////////////////////////9w////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////8KZW5kc3RyZWFtCmVuZG9iagoxNiAwIG9iago8PC9UeXBlL1hPYmplY3QvU3VidHlwZS9JbWFnZS9GaWx0ZXJbL0RDVERlY29kZV0vV2lkdGggMTAyNC9IZWlnaHQgMTU3L0NvbG9yU3BhY2UvRGV2aWNlUkdCL0JpdHNQZXJDb21wb25lbnQgOC9MZW5ndGggMjk5NzcvTmFtZS9JbWcyPj5zdHJlYW0K/9j/4AAQSkZJRgABAgECWAJYAAD/4QdBRXhpZgAATU0AKgAAAAgABwESAAMAAAABAAEAAAEaAAUAAAABAAAAYgEbAAUAAAABAAAAagEoAAMAAAABAAIAAAExAAIAAAAUAAAAcgEyAAIAAAAUAAAAhodpAAQAAAABAAAAnAAAAMgAAAJYAAAAAQAAAlgAAAABQWRvYmUgUGhvdG9zaG9wIDcuMAAyMDIxOjA0OjAyIDExOjI1OjA4AAAAAAOgAQADAAAAAf//AACgAgAEAAAAAQAABACgAwAEAAAAAQAAAJ0AAAAAAAAABgEDAAMAAAABAAYAAAEaAAUAAAABAAABFgEbAAUAAAABAAABHgEoAAMAAAABAAIAAAIBAAQAAAABAAABJgICAAQAAAABAAAGEwAAAAAAAABIAAAAAQAAAEgAAAAB/9j/4AAQSkZJRgABAgEASABIAAD/7QAMQWRvYmVfQ00AAv/uAA5BZG9iZQBkgAAAAAH/2wCEAAwICAgJCAwJCQwRCwoLERUPDAwPFRgTExUTExgRDAwMDAwMEQwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwBDQsLDQ4NEA4OEBQODg4UFA4ODg4UEQwMDAwMEREMDAwMDAwRDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDP/AABEIABQAgAMBIgACEQEDEQH/3QAEAAj/xAE/AAABBQEBAQEBAQAAAAAAAAADAAECBAUGBwgJCgsBAAEFAQEBAQEBAAAAAAAAAAEAAgMEBQYHCAkKCxAAAQQBAwIEAgUHBggFAwwzAQACEQMEIRIxBUFRYRMicYEyBhSRobFCIyQVUsFiMzRygtFDByWSU/Dh8WNzNRaisoMmRJNUZEXCo3Q2F9JV4mXys4TD03Xj80YnlKSFtJXE1OT0pbXF1eX1VmZ2hpamtsbW5vY3R1dnd4eXp7fH1+f3EQACAgECBAQDBAUGBwcGBTUBAAIRAyExEgRBUWFxIhMFMoGRFKGxQiPBUtHwMyRi4XKCkkNTFWNzNPElBhaisoMHJjXC0kSTVKMXZEVVNnRl4vKzhMPTdePzRpSkhbSVxNTk9KW1xdXl9VZmdoaWprbG1ub2JzdHV2d3h5ent8f/2gAMAwEAAhEDEQA/AO4619ZsbByaMHGtrfnvycem3HeHEiu1zPUc3bt9/pP3tT/Vf6y4/WsKkWW1/tE1mzIoqDgGQ7Z/hN/7zP8ACKPXOh5F+TRn4Fl5yhlY7rWC9zKhSxzfX/Q7vT/mm/QS+qvRMjp+FTfnPvPUX1luSyy91rJLt0tbufVu9v5iZ6+Lw/Z/3zCDl9zpw2en6PT/AA3eWD1DO65j591WOBfTOP6TG0+8C03+sBdZfXjvfUzG/wAJ6P8AP/pP8Gt5Y9/VepVdSsqZiPtxXbKqH7HgCwWVV5Ftj2sf+h9PL31+zZ+oZH6X9J+jezNE/WPqTqW2ei6it7aqzfZjvDWXF1bs0ub63qNZRjW2e22quurJxL6/tN30Eh9YOo7L3OjfVj2W47G0wcgt+1+jbTXbcy39M3Gpf6LP3/5707mI7Os9Vvyam/Y7sestZvb6T3S578GXOe6pnpVsZfmM/wBLsouvfWz01cp6vbaR+p3Vhzq2AWVvB/SAO9R0MdspZ7q37/ex9f6RBTXv61l41V1VrNuaytt1NLmSXM32iz+j2Wsttrpp9Syqiz/R/wCl9NNj9dsty6muM1XWuZjtrqcfUr32VsyW2Pe1r6m+nusso9TYz9PYz7PkY9qWT1DqRb022pltdV9L7MoOpeXtcPQ2sexlFrvU9936vsx/W/01Xpo1fWsiwx9iuZLi1pNdndrHscd1bG7fUe+q39J/gklNTI6n1XFy7G32sbi/bDjttNJbtq+zfbhYbLLvTf8Ap3fZt38j/TKZ61nHK9Olous9f0rMQ1PY6pge+tt78rd6P6aprL6t7f0zPfSidS6h1asYl2DU61t1Fhuq9F8te4V/Zrju2Pr9G0/psZ/6b0v+IRbesZDS2ujDussOwTZXYxvvdjt3ueymxntqynWvZ/3Wvr/R+mkpz6PrF1U1NOTiurfZq0sote1m2iu7Iruh25z6n2uvp9P+l1UW4dX61/OH/b1gx8htLhlZLanuwyKntbeWb9z6Q0u9drNv0Kf5/wBP1Mf+eqSb1vqe+q5+DcK3th+O1jyQT9lu3te+mv3VU5OQx9b/AOdtxLK6v0vsWlhZxynuBrtrDWg/pK3sBO6xntdbXX9JrGP/AKj0lOG76wdRZu94tx2OP2fKrx3O+1Eej+rUVuurr9VnqXN9tv616f6r+kx8mpWWdcyfWyBkPFApZLKzS6SP9LAe/IsYz8/0sf0/Yt9JFTXwMkZeIy8SQ4uAJESGucze2C9rq37d9djP0d1f6WtWEkklP//Q9VSXyqkkp+qkl8qpJKfqpJfKqSSn6qSXyqkkp+qkl8qpJKfqpJfKqSSn6qSXyqkkp+qkl8qpJKf/2f/tDBJQaG90b3Nob3AgMy4wADhCSU0EJQAAAAAAEAAAAAAAAAAAAAAAAAAAAAA4QklNA+0AAAAAABACWAAAAAEAAgJYAAAAAQACOEJJTQQmAAAAAAAOAAAAAAAAAAAAAD+AAAA4QklNBA0AAAAAAAQAAAAeOEJJTQQZAAAAAAAEAAAAHjhCSU0D8wAAAAAACQAAAAAAAAAAAQA4QklNBAoAAAAAAAEAADhCSU0nEAAAAAAACgABAAAAAAAAAAI4QklNA/UAAAAAAEgAL2ZmAAEAbGZmAAYAAAAAAAEAL2ZmAAEAoZmaAAYAAAAAAAEAMgAAAAEAWgAAAAYAAAAAAAEANQAAAAEALQAAAAYAAAAAAAE4QklNA/gAAAAAAHAAAP////////////////////////////8D6AAAAAD/////////////////////////////A+gAAAAA/////////////////////////////wPoAAAAAP////////////////////////////8D6AAAOEJJTQQAAAAAAAACAAM4QklNBAIAAAAAAAgAAAAAAAAAADhCSU0ECAAAAAAAEAAAAAEAAAJAAAACQAAAAAA4QklNBB4AAAAAAAQAAAAAOEJJTQQaAAAAAANbAAAABgAAAAAAAAAAAAAAnQAABAAAAAATAEMAbwBtAGIAaQBuAGUAZABDAG8AbgB0AHIAYQBjAHQASgBQAEcAAAABAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAAAABAAAAACdAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAEAAAAAAABudWxsAAAAAgAAAAZib3VuZHNPYmpjAAAAAQAAAAAAAFJjdDEAAAAEAAAAAFRvcCBsb25nAAAAAAAAAABMZWZ0bG9uZwAAAAAAAAAAQnRvbWxvbmcAAACdAAAAAFJnaHRsb25nAAAEAAAAAAZzbGljZXNWbExzAAAAAU9iamMAAAABAAAAAAAFc2xpY2UAAAASAAAAB3NsaWNlSURsb25nAAAAAAAAAAdncm91cElEbG9uZwAAAAAAAAAGb3JpZ2luZW51bQAAAAxFU2xpY2VPcmlnaW4AAAANYXV0b0dlbmVyYXRlZAAAAABUeXBlZW51bQAAAApFU2xpY2VUeXBlAAAAAEltZyAAAAAGYm91bmRzT2JqYwAAAAEAAAAAAABSY3QxAAAABAAAAABUb3AgbG9uZwAAAAAAAAAATGVmdGxvbmcAAAAAAAAAAEJ0b21sb25nAAAAnQAAAABSZ2h0bG9uZwAABAAAAAADdXJsVEVYVAAAAAEAAAAAAABudWxsVEVYVAAAAAEAAAAAAABNc2dlVEVYVAAAAAEAAAAAAAZhbHRUYWdURVhUAAAAAQAAAAAADmNlbGxUZXh0SXNIVE1MYm9vbAEAAAAIY2VsbFRleHRURVhUAAAAAQAAAAAACWhvcnpBbGlnbmVudW0AAAAPRVNsaWNlSG9yekFsaWduAAAAB2RlZmF1bHQAAAAJdmVydEFsaWduZW51bQAAAA9FU2xpY2VWZXJ0QWxpZ24AAAAHZGVmYXVsdAAAAAtiZ0NvbG9yVHlwZWVudW0AAAARRVNsaWNlQkdDb2xvclR5cGUAAAAATm9uZQAAAAl0b3BPdXRzZXRsb25nAAAAAAAAAApsZWZ0T3V0c2V0bG9uZwAAAAAAAAAMYm90dG9tT3V0c2V0bG9uZwAAAAAAAAALcmlnaHRPdXRzZXRsb25nAAAAAAA4QklNBBEAAAAAAAEBADhCSU0EFAAAAAAABAAAAAQ4QklNBAwAAAAABi8AAAABAAAAgAAAABQAAAGAAAAeAAAABhMAGAAB/9j/4AAQSkZJRgABAgEASABIAAD/7QAMQWRvYmVfQ00AAv/uAA5BZG9iZQBkgAAAAAH/2wCEAAwICAgJCAwJCQwRCwoLERUPDAwPFRgTExUTExgRDAwMDAwMEQwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwBDQsLDQ4NEA4OEBQODg4UFA4ODg4UEQwMDAwMEREMDAwMDAwRDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDP/AABEIABQAgAMBIgACEQEDEQH/3QAEAAj/xAE/AAABBQEBAQEBAQAAAAAAAAADAAECBAUGBwgJCgsBAAEFAQEBAQEBAAAAAAAAAAEAAgMEBQYHCAkKCxAAAQQBAwIEAgUHBggFAwwzAQACEQMEIRIxBUFRYRMicYEyBhSRobFCIyQVUsFiMzRygtFDByWSU/Dh8WNzNRaisoMmRJNUZEXCo3Q2F9JV4mXys4TD03Xj80YnlKSFtJXE1OT0pbXF1eX1VmZ2hpamtsbW5vY3R1dnd4eXp7fH1+f3EQACAgECBAQDBAUGBwcGBTUBAAIRAyExEgRBUWFxIhMFMoGRFKGxQiPBUtHwMyRi4XKCkkNTFWNzNPElBhaisoMHJjXC0kSTVKMXZEVVNnRl4vKzhMPTdePzRpSkhbSVxNTk9KW1xdXl9VZmdoaWprbG1ub2JzdHV2d3h5ent8f/2gAMAwEAAhEDEQA/AO4619ZsbByaMHGtrfnvycem3HeHEiu1zPUc3bt9/pP3tT/Vf6y4/WsKkWW1/tE1mzIoqDgGQ7Z/hN/7zP8ACKPXOh5F+TRn4Fl5yhlY7rWC9zKhSxzfX/Q7vT/mm/QS+qvRMjp+FTfnPvPUX1luSyy91rJLt0tbufVu9v5iZ6+Lw/Z/3zCDl9zpw2en6PT/AA3eWD1DO65j591WOBfTOP6TG0+8C03+sBdZfXjvfUzG/wAJ6P8AP/pP8Gt5Y9/VepVdSsqZiPtxXbKqH7HgCwWVV5Ftj2sf+h9PL31+zZ+oZH6X9J+jezNE/WPqTqW2ei6it7aqzfZjvDWXF1bs0ub63qNZRjW2e22quurJxL6/tN30Eh9YOo7L3OjfVj2W47G0wcgt+1+jbTXbcy39M3Gpf6LP3/5707mI7Os9Vvyam/Y7sestZvb6T3S578GXOe6pnpVsZfmM/wBLsouvfWz01cp6vbaR+p3Vhzq2AWVvB/SAO9R0MdspZ7q37/ex9f6RBTXv61l41V1VrNuaytt1NLmSXM32iz+j2Wsttrpp9Syqiz/R/wCl9NNj9dsty6muM1XWuZjtrqcfUr32VsyW2Pe1r6m+nusso9TYz9PYz7PkY9qWT1DqRb022pltdV9L7MoOpeXtcPQ2sexlFrvU9936vsx/W/01Xpo1fWsiwx9iuZLi1pNdndrHscd1bG7fUe+q39J/gklNTI6n1XFy7G32sbi/bDjttNJbtq+zfbhYbLLvTf8Ap3fZt38j/TKZ61nHK9Olous9f0rMQ1PY6pge+tt78rd6P6aprL6t7f0zPfSidS6h1asYl2DU61t1Fhuq9F8te4V/Zrju2Pr9G0/psZ/6b0v+IRbesZDS2ujDussOwTZXYxvvdjt3ueymxntqynWvZ/3Wvr/R+mkpz6PrF1U1NOTiurfZq0sote1m2iu7Iruh25z6n2uvp9P+l1UW4dX61/OH/b1gx8htLhlZLanuwyKntbeWb9z6Q0u9drNv0Kf5/wBP1Mf+eqSb1vqe+q5+DcK3th+O1jyQT9lu3te+mv3VU5OQx9b/AOdtxLK6v0vsWlhZxynuBrtrDWg/pK3sBO6xntdbXX9JrGP/AKj0lOG76wdRZu94tx2OP2fKrx3O+1Eej+rUVuurr9VnqXN9tv616f6r+kx8mpWWdcyfWyBkPFApZLKzS6SP9LAe/IsYz8/0sf0/Yt9JFTXwMkZeIy8SQ4uAJESGucze2C9rq37d9djP0d1f6WtWEkklP//Q9VSXyqkkp+qkl8qpJKfqpJfKqSSn6qSXyqkkp+qkl8qpJKfqpJfKqSSn6qSXyqkkp+qkl8qpJKf/2QA4QklNBCEAAAAAAFUAAAABAQAAAA8AQQBkAG8AYgBlACAAUABoAG8AdABvAHMAaABvAHAAAAATAEEAZABvAGIAZQAgAFAAaABvAHQAbwBzAGgAbwBwACAANwAuADAAAAABADhCSU0EBgAAAAAABwABAAAAAQEA/+ESSGh0dHA6Ly9ucy5hZG9iZS5jb20veGFwLzEuMC8APD94cGFja2V0IGJlZ2luPSfvu78nIGlkPSdXNU0wTXBDZWhpSHpyZVN6TlRjemtjOWQnPz4KPD9hZG9iZS14YXAtZmlsdGVycyBlc2M9IkNSIj8+Cjx4OnhhcG1ldGEgeG1sbnM6eD0nYWRvYmU6bnM6bWV0YS8nIHg6eGFwdGs9J1hNUCB0b29sa2l0IDIuOC4yLTMzLCBmcmFtZXdvcmsgMS41Jz4KPHJkZjpSREYgeG1sbnM6cmRmPSdodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjJyB4bWxuczppWD0naHR0cDovL25zLmFkb2JlLmNvbS9pWC8xLjAvJz4KCiA8cmRmOkRlc2NyaXB0aW9uIGFib3V0PSd1dWlkOjQ1ODFkYzcxLTkzNzctMTFlYi1iZjk5LWM2MjM4YTRmODgzOCcKICB4bWxuczp4YXBNTT0naHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wL21tLyc+CiAgPHhhcE1NOkRvY3VtZW50SUQ+YWRvYmU6ZG9jaWQ6cGhvdG9zaG9wOjQ1ODFkYzZhLTkzNzctMTFlYi1iZjk5LWM2MjM4YTRmODgzODwveGFwTU06RG9jdW1lbnRJRD4KIDwvcmRmOkRlc2NyaXB0aW9uPgoKPC9yZGY6UkRGPgo8L3g6eGFwbWV0YT4KICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIC</t>
+  </si>
+  <si>
+    <t>Request_Get_PledgeForMargin</t>
+  </si>
+  <si>
+    <t>[ { "securities_Code": "531518 ", "securities_Name": "VIKASGRAN", "securities_ISIN": "INE767B01022", "holding_Rate": 2, "holding_Qty": 300, "holding_Value": 600, "hairCut": 24.29, "netValue": 453, "request_Qty": 300, "request_Value": 600 }, { "securities_Code": "542655 ", "securities_Name": "VIKASMCORP", "securities_ISIN": "INE161L01027", "holding_Rate": 3.47, "holding_Qty": 210, "holding_Value": 728.7, "hairCut": 25.15, "netValue": 546, "request_Qty": 210, "request_Value": 728.7 }, { "securities_Code": "519307 ", "securities_Name": "VIKASWSP", "securities_ISIN": "INE706A01022", "holding_Rate": 3.6, "holding_Qty": 100, "holding_Value": 360, "hairCut": 26.34, "netValue": 265, "request_Qty": 100, "request_Value": 360 }, { "securities_Code": "533295 ", "securities_Name": "PSB", "securities_ISIN": "INE608A01012", "holding_Rate": 16, "holding_Qty": 60, "holding_Value": 960, "hairCut": 19.36, "netValue": 774, "request_Qty": 60, "request_Value": 960 }, { "securities_Code": "531307 ", "securities_Name": "RRILLTD", "securities_ISIN": "INE951M01037", "holding_Rate": 13.49, "holding_Qty": 18, "holding_Value": 242.82, "hairCut": 21.98, "netValue": 189.36, "request_Qty": 18, "request_Value": 242.82 }, { "securities_Code": "526371 ", "securities_Name": "NMDC", "securities_ISIN": "INE584A01023", "holding_Rate": 134.9, "holding_Qty": 3, "holding_Value": 404.70000000000005, "hairCut": 17.11, "netValue": 335.46, "request_Qty": 6, "request_Value": 809.4000000000001 }, { "securities_Code": "500288 ", "securities_Name": "MOREPENLAB", "securities_ISIN": "INE083A01026", "holding_Rate": 55.35, "holding_Qty": 6, "holding_Value": 332.1, "hairCut": 25.28, "netValue": 248.16, "request_Qty": 6, "request_Value": 332.1 }, { "securities_Code": "526650 ", "securities_Name": "TFCILTD", "securities_ISIN": "INE305A01015", "holding_Rate": 59.6, "holding_Qty": 3, "holding_Value": 178.8, "hairCut": 19.71, "netValue": 143.55, "request_Qty": 6, "request_Value": 357.6 }, { "securities_Code": "500188 ", "securities_Name": "HINDZINC", "securities_ISIN": "INE267A01025", "holding_Rate": 315.1, "holding_Qty": 3, "holding_Value": 945.3000000000001, "hairCut": 14.8, "netValue": 805.41, "request_Qty": 3, "request_Value": 945.3000000000001 }, { "securities_Code": "534816 ", "securities_Name": "INDUSTOWER", "securities_ISIN": "INE121J01017", "holding_Rate": 253.3, "holding_Qty": 3, "holding_Value": 759.9000000000001, "hairCut": 19.25, "netValue": 613.62, "request_Qty": 3, "request_Value": 759.9000000000001 }, { "securities_Code": "532872 ", "securities_Name": "SPARC", "securities_ISIN": "INE232I01014", "holding_Rate": 250.7, "holding_Qty": 3, "holding_Value": 752.0999999999999, "hairCut": 19.58, "netValue": 604.83, "request_Qty": 3, "request_Value": 752.0999999999999 }, { "securities_Code": "532898 ", "securities_Name": "POWERGRID", "securities_ISIN": "INE752E01010", "holding_Rate": 208.4, "holding_Qty": 3, "holding_Value": 625.2, "hairCut": 11.63, "netValue": 552.48, "request_Qty": 3, "request_Value": 625.2 }, { "securities_Code": "500086 ", "securities_Name": "EXIDEIND", "securities_ISIN": "INE302A01020", "holding_Rate": 164.35, "holding_Qty": 3, "holding_Value": 493.04999999999995, "hairCut": 10.78, "netValue": 439.89, "request_Qty": 3, "request_Value": 493.04999999999995 }, { "securities_Code": "540065 ", "securities_Name": "RBLBANK", "securities_ISIN": "INE976G01028", "holding_Rate": 177.95, "holding_Qty": 3, "holding_Value": 533.8499999999999, "hairCut": 21.51, "netValue": 419.01, "request_Qty": 3, "request_Value": 533.8499999999999 }, { "securities_Code": "511676 ", "securities_Name": "GICHSGFIN", "securities_ISIN": "INE289B01019", "holding_Rate": 145.2, "holding_Qty": 3, "holding_Value": 435.59999999999997, "hairCut": 19.33, "netValue": 351.39, "request_Qty": 3, "request_Value": 435.59999999999997 }, { "securities_Code": "532955 ", "securities_Name": "RECLTD", "securities_ISIN": "INE020B01018", "holding_Rate": 132.55, "holding_Qty": 3, "holding_Value": 397.65000000000003, "hairCut": 13.91, "netValue": 342.33, "request_Qty": 3, "request_Value": 397.65000000000003 }, { "securities_Code": "330179 ", "securities_Name": "AHLADA", "securities_ISIN": "INE00PV01013", "holding_Rate": 127.6, "holding_Qty": 3, "holding_Value": 382.79999999999995, "hairCut": 18.23, "netValue": 313.02, "request_Qty": 3, "request_Value": 382.79999999999995 }, { "securities_Code": "532522 ", "securities_Name": "PETRONET", "securities_ISIN": "INE347G01014", "holding_Rate": 218.7, "holding_Qty": 2, "holding_Value": 437.4, "hairCut": 10.29, "netValue": 392.4, "request_Qty": 2, "request_Value": 437.4 }, { "securities_Code": "500260 ", "securities_Name": "RAMCOCEM", "securities_ISIN": "INE331A01037", "holding_Rate": 997, "holding_Qty": 1, "holding_Value": 997, "hairCut": 11.86, "netValue": 878.76, "request_Qty": 1, "request_Value": 997 }, { "securities_Code": "517385 ", "securities_Name": "SYMPHONY", "securities_ISIN": "INE225D01027", "holding_Rate": 1006.55, "holding_Qty": 1, "holding_Value": 1006.55, "hairCut": 13.78, "netValue": 867.85, "request_Qty": 1, "request_Value": 1006.55 }, { "securities_Code": "500770 ", "securities_Name": "TATACHEM", "securities_ISIN": "INE092A01019", "holding_Rate": 885.45, "holding_Qty": 1, "holding_Value": 885.45, "hairCut": 15.98, "netValue": 743.96, "request_Qty": 1, "request_Value": 885.45 }, { "securities_Code": "500520 ", "securities_Name": "M&amp;M", "securities_ISIN": "INE101A01026", "holding_Rate": 826.65, "holding_Qty": 1, "holding_Value": 826.65, "hairCut": 13.45, "netValue": 715.47, "request_Qty": 1, "request_Value": 826.65 }, { "securities_Code": "532174 ", "securities_Name": "ICICIBANK", "securities_ISIN": "INE090A01021", "holding_Rate": 731, "holding_Qty": 1, "holding_Value": 731, "hairCut": 14.38, "netValue": 625.88, "request_Qty": 1, "request_Value": 731 }, { "securities_Code": "505192 ", "securities_Name": "SMLISUZU", "securities_ISIN": "INE294B01019", "holding_Rate": 646.4, "holding_Qty": 1, "holding_Value": 646.4, "hairCut": 20.13, "netValue": 516.28, "request_Qty": 1, "request_Value": 646.4 }, { "securities_Code": "532967 ", "securities_Name": "KIRIINDUS", "securities_ISIN": "INE415I01015", "holding_Rate": 471.75, "holding_Qty": 1, "holding_Value": 471.75, "hairCut": 20.08, "netValue": 377.02, "request_Qty": 1, "request_Value": 471.75 }, { "securities_Code": "530803 ", "securities_Name": "BHAGERIA", "securities_ISIN": "INE354C01027", "holding_Rate": 249.5, "holding_Qty": 1, "holding_Value": 249.5, "hairCut": 18.98, "netValue": 202.14, "request_Qty": 1, "request_Value": 249.5 }, { "securities_Code": "522205 ", "securities_Name": "PRAJIND", "securities_ISIN": "INE074A01025", "holding_Rate": 307.2, "holding_Qty": 512, "holding_Value": 157286.4, "hairCut": 20.59, "netValue": 124902.4, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "330039 ", "securities_Name": "CDSL", "securities_ISIN": "INE736A01011", "holding_Rate": 1492.9, "holding_Qty": 71, "holding_Value": 105995.90000000001, "hairCut": 17.75, "netValue": 87181.61, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "524558 ", "securities_Name": "NEULANDLAB", "securities_ISIN": "INE794A01010", "holding_Rate": 1587.15, "holding_Qty": 15, "holding_Value": 23807.25, "hairCut": 21.98, "netValue": 18574.35, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "532648 ", "securities_Name": "YESBANK", "securities_ISIN": "INE528G01035", "holding_Rate": 13.58, "holding_Qty": 300, "holding_Value": 4074, "hairCut": 29, "netValue": 2892, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "532822 ", "securities_Name": "IDEA", "securities_ISIN": "INE669E01016", "holding_Rate": 13.79, "holding_Qty": 180, "holding_Value": 2482.2, "hairCut": 38.4, "netValue": 1528.2, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "505537 ", "securities_Name": "ZEEL", "securities_ISIN": "INE256A01028", "holding_Rate": 338.1, "holding_Qty": 6, "holding_Value": 2028.6000000000001, "hairCut": 27.23, "netValue": 1476.24, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500570 ", "securities_Name": "TATAMOTORS", "securities_ISIN": "INE155A01022", "holding_Rate": 472.35, "holding_Qty": 3, "holding_Value": 1417.0500000000002, "hairCut": 21.17, "netValue": 1117.05, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "512573 ", "securities_Name": "AVANTIFEED", "securities_ISIN": "INE871C01038", "holding_Rate": 547.95, "holding_Qty": 2, "holding_Value": 1095.9, "hairCut": 15.1, "netValue": 930.42, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500257 ", "securities_Name": "LUPIN", "securities_ISIN": "INE326A01037", "holding_Rate": 912.25, "holding_Qty": 1, "holding_Value": 912.25, "hairCut": 13.01, "netValue": 793.57, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "533278 ", "securities_Name": "COALINDIA", "securities_ISIN": "INE522F01014", "holding_Rate": 147.7, "holding_Qty": 6, "holding_Value": 886.1999999999999, "hairCut": 13.06, "netValue": 770.46, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "541153 ", "securities_Name": "BANDHANBNK", "securities_ISIN": "INE545U01014", "holding_Rate": 258.9, "holding_Qty": 3, "holding_Value": 776.6999999999999, "hairCut": 20.63, "netValue": 616.47, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500228 ", "securities_Name": "JSWSTEEL", "securities_ISIN": "INE019A01038", "holding_Rate": 649.65, "holding_Qty": 1, "holding_Value": 649.65, "hairCut": 15.86, "netValue": 546.62, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "517334 ", "securities_Name": "MOTHERSUMI", "securities_ISIN": "INE775A01035", "holding_Rate": 214.4, "holding_Qty": 3, "holding_Value": 643.2, "hairCut": 19.16, "netValue": 519.96, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500096 ", "securities_Name": "DABUR", "securities_ISIN": "INE016A01026", "holding_Rate": 569.65, "holding_Qty": 1, "holding_Value": 569.65, "hairCut": 9, "netValue": 518.38, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500850 ", "securities_Name": "INDHOTEL", "securities_ISIN": "INE053A01029", "holding_Rate": 180.45, "holding_Qty": 3, "holding_Value": 541.3499999999999, "hairCut": 18.3, "netValue": 442.29, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500477 ", "securities_Name": "ASHOKLEY", "securities_ISIN": "INE208A01029", "holding_Rate": 125.8, "holding_Qty": 3, "holding_Value": 377.4, "hairCut": 17.79, "netValue": 310.26, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "532461 ", "securities_Name": "PNB", "securities_ISIN": "INE160A01022", "holding_Rate": 38, "holding_Qty": 9, "holding_Value": 342, "hairCut": 17.35, "netValue": 282.69, "request_Qty": 0, "request_Value": 0 } ]</t>
   </si>
 </sst>
 </file>
@@ -1494,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I377"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C148" workbookViewId="0">
-      <selection activeCell="F162" sqref="F162"/>
+    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+      <selection activeCell="E275" sqref="E275"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1526,13 +1526,13 @@
     </row>
     <row r="2" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -1558,13 +1558,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1575,10 +1575,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1598,10 +1598,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1613,7 +1613,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1636,10 +1636,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1659,10 +1659,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1677,13 +1677,13 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1694,10 +1694,10 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1712,7 +1712,7 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D17" s="9"/>
       <c r="E17" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
@@ -1721,7 +1721,7 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D18" s="9"/>
       <c r="E18" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
@@ -1730,7 +1730,7 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D19" s="9"/>
       <c r="E19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -1744,13 +1744,13 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1761,49 +1761,49 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
+        <v>123</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>126</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>127</v>
-      </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="I23" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D24" s="9"/>
       <c r="H24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="I24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="9"/>
       <c r="H25" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="9"/>
       <c r="H26" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="I26" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -1815,10 +1815,10 @@
         <v>9</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -1830,10 +1830,10 @@
         <v>9</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -1844,10 +1844,10 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1859,10 +1859,10 @@
         <v>16</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
@@ -1877,7 +1877,7 @@
         <v>16</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
@@ -1887,49 +1887,49 @@
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D33" s="9"/>
       <c r="E33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F33" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D34" s="9"/>
       <c r="G34" s="20"/>
       <c r="H34" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D35" s="9"/>
       <c r="G35" s="20"/>
       <c r="H35" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D36" s="9"/>
       <c r="G36" s="20"/>
       <c r="H36" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D37" s="9"/>
       <c r="G37" s="20"/>
       <c r="H37" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D38" s="9"/>
       <c r="G38" s="20"/>
       <c r="H38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
@@ -1939,25 +1939,25 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D40" s="9"/>
       <c r="E40" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D41" s="9"/>
       <c r="H41" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D42" s="9"/>
       <c r="H42" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -1968,58 +1968,58 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E44" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D45" s="9"/>
       <c r="I45" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D46" s="9"/>
       <c r="I46" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D47" s="9"/>
       <c r="I47" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D48" s="9"/>
       <c r="I48" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D49" s="9"/>
       <c r="I49" s="19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D50" s="9"/>
       <c r="I50" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2030,22 +2030,22 @@
         <v>46</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H52" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -2073,46 +2073,46 @@
         <v>38</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D56" s="9"/>
       <c r="I56" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D57" s="9"/>
       <c r="I57" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D58" s="9"/>
       <c r="I58" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D59" s="9"/>
       <c r="I59" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D60" s="9"/>
       <c r="I60" s="19" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D61" s="9"/>
       <c r="I61" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
@@ -2126,55 +2126,55 @@
         <v>38</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E63" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I63" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D64" s="9"/>
       <c r="I64" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D65" s="9"/>
       <c r="I65" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D66" s="9"/>
       <c r="I66" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" s="9"/>
       <c r="I67" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D68" s="9"/>
       <c r="I68" s="19" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D69" s="9"/>
       <c r="I69" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
@@ -2188,10 +2188,10 @@
         <v>38</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
@@ -2205,10 +2205,10 @@
         <v>38</v>
       </c>
       <c r="D73" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E73" t="s">
         <v>257</v>
-      </c>
-      <c r="E73" t="s">
-        <v>259</v>
       </c>
       <c r="F73" t="s">
         <v>23</v>
@@ -2217,7 +2217,7 @@
         <v>1202870000086520</v>
       </c>
       <c r="I73" s="26" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
@@ -2231,10 +2231,10 @@
         <v>38</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="E75" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F75" t="s">
         <v>23</v>
@@ -2243,7 +2243,7 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D76" s="9"/>
       <c r="E76" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F76" t="s">
         <v>23</v>
@@ -2260,10 +2260,10 @@
         <v>38</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I78" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
@@ -2324,13 +2324,13 @@
         <v>26</v>
       </c>
       <c r="C84" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
@@ -2341,13 +2341,13 @@
         <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E86" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F86" t="s">
         <v>23</v>
@@ -2356,7 +2356,7 @@
         <v>28</v>
       </c>
       <c r="I86" s="26" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
@@ -2367,7 +2367,7 @@
         <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>29</v>
@@ -2406,22 +2406,22 @@
         <v>26</v>
       </c>
       <c r="C91" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E91" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I91" s="26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
@@ -2433,28 +2433,28 @@
         <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E93" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="I93" s="26" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D94" s="9"/>
       <c r="E94" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>9</v>
@@ -2472,13 +2472,13 @@
         <v>26</v>
       </c>
       <c r="C96" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="E96" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>9</v>
@@ -2488,7 +2488,7 @@
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D97" s="9"/>
       <c r="E97" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>9</v>
@@ -2498,7 +2498,7 @@
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D98" s="9"/>
       <c r="E98" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>9</v>
@@ -2516,13 +2516,13 @@
         <v>26</v>
       </c>
       <c r="C100" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E100" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>9</v>
@@ -2532,7 +2532,7 @@
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D101" s="9"/>
       <c r="E101" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>9</v>
@@ -2548,34 +2548,34 @@
         <v>20</v>
       </c>
       <c r="C103" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E103" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H103" s="30" t="s">
+        <v>287</v>
+      </c>
+      <c r="I103" s="31" t="s">
         <v>289</v>
-      </c>
-      <c r="I103" s="31" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D104" s="9"/>
       <c r="E104" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H104" s="14" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
@@ -2586,13 +2586,13 @@
         <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E106" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>9</v>
@@ -2602,7 +2602,7 @@
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D107" s="9"/>
       <c r="E107" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>9</v>
@@ -2612,7 +2612,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>9</v>
@@ -2622,7 +2622,7 @@
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D109" s="9"/>
       <c r="E109" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>9</v>
@@ -2632,7 +2632,7 @@
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D110" s="9"/>
       <c r="E110" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>9</v>
@@ -2642,7 +2642,7 @@
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D111" s="9"/>
       <c r="E111" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>9</v>
@@ -2657,31 +2657,31 @@
         <v>34</v>
       </c>
       <c r="C113" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F113" t="s">
         <v>9</v>
       </c>
       <c r="H113" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="I113" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D114" s="9"/>
       <c r="H114" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="I114" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
@@ -2693,10 +2693,10 @@
         <v>9</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I115" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
@@ -2708,28 +2708,28 @@
         <v>9</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I116" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D117" s="9"/>
       <c r="I117" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D118" s="9"/>
       <c r="I118" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D119" s="9"/>
       <c r="I119" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
@@ -2740,49 +2740,49 @@
         <v>34</v>
       </c>
       <c r="C121" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F121" t="s">
         <v>9</v>
       </c>
       <c r="H121" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I121" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D122" s="9"/>
       <c r="H122" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I122" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D123" s="9"/>
       <c r="H123" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I123" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D124" s="9"/>
       <c r="H124" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I124" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
@@ -2794,10 +2794,10 @@
         <v>9</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I125" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.3">
@@ -2809,16 +2809,16 @@
         <v>9</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I126" s="19" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D127" s="9"/>
       <c r="I127" s="22" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
@@ -2829,49 +2829,49 @@
         <v>34</v>
       </c>
       <c r="C129" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E129" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F129" t="s">
+        <v>9</v>
+      </c>
+      <c r="H129" t="s">
+        <v>219</v>
+      </c>
+      <c r="I129" s="23" t="s">
         <v>220</v>
-      </c>
-      <c r="F129" t="s">
-        <v>9</v>
-      </c>
-      <c r="H129" t="s">
-        <v>221</v>
-      </c>
-      <c r="I129" s="23" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D130" s="9"/>
       <c r="H130" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D131" s="9"/>
       <c r="H131" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I131" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D132" s="9"/>
       <c r="H132" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I132" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.3">
@@ -2883,10 +2883,10 @@
         <v>9</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I133" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.3">
@@ -2898,22 +2898,22 @@
         <v>9</v>
       </c>
       <c r="H134" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I134" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D135" s="9"/>
       <c r="I135" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D136" s="9"/>
       <c r="I136" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
@@ -2922,49 +2922,49 @@
     <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D138" s="9"/>
       <c r="I138" s="23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D139" s="9"/>
       <c r="I139" s="19" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D140" s="9"/>
       <c r="I140" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D141" s="9"/>
       <c r="I141" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
       <c r="I142" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D143" s="9"/>
       <c r="I143" s="19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D144" s="9"/>
       <c r="I144" s="19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D145" s="9"/>
       <c r="I145" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
@@ -2973,16 +2973,16 @@
     </row>
     <row r="147" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C147" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.3">
@@ -2993,7 +2993,7 @@
         <v>50</v>
       </c>
       <c r="C149" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D149" s="9" t="s">
         <v>51</v>
@@ -3022,22 +3022,22 @@
         <v>50</v>
       </c>
       <c r="C152" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E152" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F152" t="s">
         <v>23</v>
       </c>
       <c r="H152" t="s">
+        <v>204</v>
+      </c>
+      <c r="I152" s="21" t="s">
         <v>206</v>
-      </c>
-      <c r="I152" s="21" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.3">
@@ -3058,13 +3058,13 @@
     <row r="154" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D154" s="9"/>
       <c r="E154" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F154" t="s">
         <v>23</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.3">
@@ -3075,7 +3075,7 @@
         <v>50</v>
       </c>
       <c r="C156" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D156" s="10" t="s">
         <v>56</v>
@@ -3157,10 +3157,10 @@
         <v>50</v>
       </c>
       <c r="C162" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="E162" s="10" t="s">
         <v>52</v>
@@ -3173,7 +3173,7 @@
         <v>53</v>
       </c>
       <c r="I162" s="26" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.3">
@@ -3224,7 +3224,7 @@
         <v>50</v>
       </c>
       <c r="C167" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D167" s="10" t="s">
         <v>60</v>
@@ -3245,20 +3245,20 @@
     </row>
     <row r="170" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B170" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C170" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D170" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
       <c r="H170" s="3"/>
       <c r="I170" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.3">
@@ -3266,26 +3266,26 @@
     </row>
     <row r="172" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B172" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C172" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D172" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E172" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G172" s="1"/>
       <c r="H172" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="I172" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.3">
@@ -3293,14 +3293,14 @@
       <c r="C173" s="1"/>
       <c r="D173" s="10"/>
       <c r="E173" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G173" s="1"/>
       <c r="H173" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I173" s="1"/>
     </row>
@@ -3309,16 +3309,16 @@
     </row>
     <row r="175" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B175" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C175" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>9</v>
@@ -3328,7 +3328,7 @@
         <v>53</v>
       </c>
       <c r="I175" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.3">
@@ -3336,14 +3336,14 @@
       <c r="C176" s="1"/>
       <c r="D176" s="10"/>
       <c r="E176" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G176" s="1"/>
       <c r="H176" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="I176" s="1"/>
     </row>
@@ -3352,7 +3352,7 @@
       <c r="C177" s="1"/>
       <c r="D177" s="10"/>
       <c r="E177" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>9</v>
@@ -3404,13 +3404,13 @@
     </row>
     <row r="181" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B181" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C181" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>32</v>
@@ -3420,10 +3420,10 @@
       </c>
       <c r="G181" s="1"/>
       <c r="H181" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I181" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.3">
@@ -3431,14 +3431,14 @@
       <c r="C182" s="1"/>
       <c r="D182" s="10"/>
       <c r="E182" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G182" s="1"/>
       <c r="H182" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I182" s="1"/>
     </row>
@@ -3481,21 +3481,21 @@
     <row r="185" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D185" s="9"/>
       <c r="F185" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="186" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B186" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C186" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I186" s="26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="187" spans="2:9" x14ac:dyDescent="0.3">
@@ -3503,25 +3503,25 @@
     </row>
     <row r="188" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B188" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C188" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D188" s="10" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E188" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H188" t="s">
         <v>295</v>
       </c>
-      <c r="F188" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H188" t="s">
-        <v>297</v>
-      </c>
       <c r="I188" s="26" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="189" spans="2:9" x14ac:dyDescent="0.3">
@@ -3541,25 +3541,25 @@
     </row>
     <row r="191" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C191" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D191" s="10" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="E191" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H191" t="s">
         <v>295</v>
       </c>
-      <c r="F191" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H191" t="s">
-        <v>297</v>
-      </c>
       <c r="I191" s="26" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.3">
@@ -3568,43 +3568,43 @@
     <row r="193" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D193" s="9"/>
       <c r="H193" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I193" s="26"/>
     </row>
     <row r="194" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C194" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E194" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H194" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I194" s="26" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D195" s="9"/>
       <c r="H195" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="196" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D196" s="9"/>
       <c r="H196" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.3">
@@ -3612,110 +3612,110 @@
     </row>
     <row r="198" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B198" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C198" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D198" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="H198" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="199" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E199" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H199" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H200" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H201" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B203" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C203" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D203" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H203" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E204" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H204" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H205" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H206" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B208" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C208" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D208" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H208" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="209" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D209" s="9"/>
       <c r="E209" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H209" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="210" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D210" s="9"/>
       <c r="H210" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D211" s="9"/>
       <c r="H211" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="212" spans="2:8" x14ac:dyDescent="0.3">
@@ -3723,23 +3723,23 @@
     </row>
     <row r="213" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B213" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D213" s="32" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E213" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F213" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G213" s="8"/>
       <c r="H213" s="18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
     <row r="214" spans="2:8" x14ac:dyDescent="0.3">
@@ -3781,7 +3781,7 @@
       <c r="C216" s="8"/>
       <c r="D216" s="32"/>
       <c r="E216" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F216" s="8" t="s">
         <v>23</v>
@@ -3802,7 +3802,7 @@
     <row r="218" spans="2:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D218" s="9"/>
       <c r="H218" s="18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.3">
@@ -3813,13 +3813,13 @@
     </row>
     <row r="221" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B221" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D221" s="32" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E221" s="33" t="s">
         <v>32</v>
@@ -3829,18 +3829,18 @@
       </c>
       <c r="G221" s="8"/>
       <c r="H221" s="32" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="222" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D222" s="9"/>
       <c r="E222" s="8"/>
       <c r="F222" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G222" s="8"/>
       <c r="H222" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="223" spans="2:8" x14ac:dyDescent="0.3">
@@ -3882,43 +3882,43 @@
     </row>
     <row r="226" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B226" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D226" s="9" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="H226" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I226" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D227" s="9"/>
       <c r="E227" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H227" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D228" s="9"/>
       <c r="H228" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D229" s="9"/>
       <c r="H229" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="230" spans="2:9" x14ac:dyDescent="0.3">
@@ -3930,43 +3930,43 @@
     </row>
     <row r="231" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B231" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="H231" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="I231" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="232" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D232" s="9"/>
       <c r="E232" s="11" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H232" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="233" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D233" s="9"/>
       <c r="H233" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="234" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D234" s="9"/>
       <c r="H234" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="235" spans="2:9" x14ac:dyDescent="0.3">
@@ -3978,26 +3978,26 @@
     </row>
     <row r="236" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
       <c r="B236" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D236" s="34" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="E236" s="8" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="F236" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G236" s="8"/>
       <c r="H236" s="18" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="I236" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.3">
@@ -4033,7 +4033,7 @@
     <row r="239" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D239" s="9"/>
       <c r="E239" s="8" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="F239" s="8" t="s">
         <v>23</v>
@@ -4052,7 +4052,7 @@
     <row r="241" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D241" s="9"/>
       <c r="H241" s="18" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.3">
@@ -4064,13 +4064,13 @@
     </row>
     <row r="243" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B243" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D243" s="32" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="E243" s="33" t="s">
         <v>32</v>
@@ -4080,18 +4080,18 @@
       </c>
       <c r="G243" s="8"/>
       <c r="H243" s="32" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="244" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D244" s="9"/>
       <c r="E244" s="8"/>
       <c r="F244" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="G244" s="8"/>
       <c r="H244" s="18" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="245" spans="2:9" x14ac:dyDescent="0.3">
@@ -4133,13 +4133,13 @@
     </row>
     <row r="248" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B248" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C248" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D248" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E248" t="s">
         <v>15</v>
@@ -4154,7 +4154,7 @@
         <v>20210401</v>
       </c>
       <c r="I248" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="249" spans="2:9" x14ac:dyDescent="0.3">
@@ -4175,7 +4175,7 @@
     <row r="250" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D250" s="9"/>
       <c r="E250" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F250" t="s">
         <v>9</v>
@@ -4190,17 +4190,17 @@
     </row>
     <row r="252" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B252" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C252" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D252" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H252" s="6"/>
       <c r="I252" s="7" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="253" spans="2:9" x14ac:dyDescent="0.3">
@@ -4213,17 +4213,17 @@
     </row>
     <row r="255" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B255" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C255" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D255" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H255" s="6"/>
       <c r="I255" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="256" spans="2:9" x14ac:dyDescent="0.3">
@@ -4236,17 +4236,17 @@
     </row>
     <row r="258" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B258" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C258" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H258" s="6"/>
       <c r="I258" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="259" spans="2:9" x14ac:dyDescent="0.3">
@@ -4259,34 +4259,34 @@
     </row>
     <row r="261" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B261" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C261" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D261" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E261" t="s">
+        <v>116</v>
+      </c>
+      <c r="F261" t="s">
         <v>117</v>
-      </c>
-      <c r="E261" t="s">
-        <v>118</v>
-      </c>
-      <c r="F261" t="s">
-        <v>119</v>
       </c>
       <c r="H261" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I261" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="262" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D262" s="9"/>
       <c r="E262" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F262" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H262" s="6" t="b">
         <v>1</v>
@@ -4298,16 +4298,16 @@
     </row>
     <row r="264" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B264" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C264" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D264" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E264" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F264" t="s">
         <v>21</v>
@@ -4316,7 +4316,7 @@
         <v>3</v>
       </c>
       <c r="I264" s="7" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="265" spans="2:9" x14ac:dyDescent="0.3">
@@ -4327,7 +4327,7 @@
         <v>62</v>
       </c>
       <c r="C266" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D266" s="10" t="s">
         <v>63</v>
@@ -4355,7 +4355,7 @@
         <v>62</v>
       </c>
       <c r="C268" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D268" s="10" t="s">
         <v>65</v>
@@ -4383,23 +4383,23 @@
         <v>62</v>
       </c>
       <c r="C270" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D270" s="10" t="s">
-        <v>66</v>
+        <v>325</v>
       </c>
       <c r="E270" s="11" t="s">
-        <v>67</v>
+        <v>257</v>
       </c>
       <c r="F270" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G270" s="1"/>
       <c r="H270" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="I270" s="7" t="s">
         <v>68</v>
-      </c>
-      <c r="I270" s="7" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="271" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4412,22 +4412,22 @@
       <c r="H271" s="3"/>
       <c r="I271" s="13"/>
     </row>
-    <row r="272" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="272" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B272" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C272" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D272" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E272" s="11"/>
       <c r="F272" s="10"/>
       <c r="G272" s="1"/>
       <c r="H272" s="3"/>
-      <c r="I272" s="7" t="s">
-        <v>71</v>
+      <c r="I272" s="26" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="273" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4445,20 +4445,20 @@
         <v>62</v>
       </c>
       <c r="C274" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D274" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E274" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F274" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G274" s="1"/>
       <c r="H274" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I274" s="7" t="s">
         <v>43</v>
@@ -4469,7 +4469,7 @@
       <c r="C275" s="1"/>
       <c r="D275" s="10"/>
       <c r="E275" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F275" s="10" t="s">
         <v>9</v>
@@ -4485,7 +4485,7 @@
       <c r="C276" s="1"/>
       <c r="D276" s="10"/>
       <c r="E276" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F276" s="10" t="s">
         <v>9</v>
@@ -4517,7 +4517,7 @@
       <c r="C278" s="1"/>
       <c r="D278" s="10"/>
       <c r="E278" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F278" s="10" t="s">
         <v>9</v>
@@ -4536,7 +4536,7 @@
         <v>62</v>
       </c>
       <c r="C280" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D280" s="9" t="s">
         <v>62</v>
@@ -4551,7 +4551,7 @@
         <v>20191101</v>
       </c>
       <c r="I280" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="281" spans="2:9" x14ac:dyDescent="0.3">
@@ -4559,13 +4559,13 @@
     </row>
     <row r="282" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B282" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C282" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D282" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E282" t="s">
         <v>15</v>
@@ -4574,10 +4574,10 @@
         <v>9</v>
       </c>
       <c r="H282" s="35" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I282" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="283" spans="2:9" x14ac:dyDescent="0.3">
@@ -4589,42 +4589,42 @@
         <v>9</v>
       </c>
       <c r="H283" s="35" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I283" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="284" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D284" s="9"/>
       <c r="H284" s="8"/>
       <c r="I284" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="285" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D285" s="9"/>
       <c r="H285" s="8"/>
       <c r="I285" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="286" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D286" s="9"/>
       <c r="I286" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="287" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D287" s="9"/>
       <c r="I287" s="19" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="288" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D288" s="9"/>
       <c r="I288" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.3">
@@ -4635,13 +4635,13 @@
         <v>36</v>
       </c>
       <c r="B290" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C290" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D290" s="10" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E290" s="1" t="s">
         <v>15</v>
@@ -4708,13 +4708,13 @@
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B294" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C294" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D294" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E294" t="s">
         <v>27</v>
@@ -4723,10 +4723,10 @@
         <v>9</v>
       </c>
       <c r="H294" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="I294" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
@@ -4738,10 +4738,10 @@
         <v>9</v>
       </c>
       <c r="H295" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I295" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.3">
@@ -4753,10 +4753,10 @@
         <v>9</v>
       </c>
       <c r="H296" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I296" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.3">
@@ -4768,34 +4768,34 @@
         <v>9</v>
       </c>
       <c r="H297" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I297" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D298" s="9"/>
       <c r="I298" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D299" s="9"/>
       <c r="I299" s="19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D300" s="9"/>
       <c r="I300" s="19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D301" s="9"/>
       <c r="I301" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
@@ -4803,13 +4803,13 @@
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B303" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="C303" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D303" s="9" t="s">
         <v>239</v>
-      </c>
-      <c r="C303" s="1" t="s">
-        <v>245</v>
-      </c>
-      <c r="D303" s="9" t="s">
-        <v>241</v>
       </c>
       <c r="E303" t="s">
         <v>27</v>
@@ -4818,10 +4818,10 @@
         <v>9</v>
       </c>
       <c r="H303" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="I303" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
@@ -4833,10 +4833,10 @@
         <v>9</v>
       </c>
       <c r="H304" s="17" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="I304" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="305" spans="2:9" x14ac:dyDescent="0.3">
@@ -4848,28 +4848,28 @@
         <v>9</v>
       </c>
       <c r="H305" s="17" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="I305" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="306" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D306" s="9"/>
       <c r="I306" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D307" s="9"/>
       <c r="I307" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="308" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D308" s="9"/>
       <c r="I308" s="25" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="309" spans="2:9" x14ac:dyDescent="0.3">
@@ -4877,7 +4877,7 @@
       <c r="E309" s="24"/>
       <c r="H309" s="18"/>
       <c r="I309" s="18" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
@@ -4885,13 +4885,13 @@
     </row>
     <row r="311" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B311" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C311" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D311" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E311" t="s">
         <v>15</v>
@@ -4906,7 +4906,7 @@
         <v>20200401</v>
       </c>
       <c r="I311" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="312" spans="2:9" x14ac:dyDescent="0.3">
@@ -4931,13 +4931,13 @@
     </row>
     <row r="314" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B314" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D314" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E314" t="s">
         <v>15</v>
@@ -4952,7 +4952,7 @@
         <v>20200401</v>
       </c>
       <c r="I314" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="315" spans="2:9" x14ac:dyDescent="0.3">
@@ -4973,49 +4973,49 @@
     <row r="316" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D316" s="9"/>
       <c r="E316" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F316" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H316" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D317" s="9"/>
       <c r="E317" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F317" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H317" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D318" s="9"/>
       <c r="E318" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F318" s="9" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H318" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="319" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D319" s="9"/>
       <c r="E319" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F319" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H319" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="320" spans="2:9" x14ac:dyDescent="0.3">
@@ -5024,13 +5024,13 @@
     </row>
     <row r="321" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B321" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D321" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E321" t="s">
         <v>15</v>
@@ -5045,7 +5045,7 @@
         <v>20200401</v>
       </c>
       <c r="I321" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="322" spans="2:9" x14ac:dyDescent="0.3">
@@ -5066,19 +5066,19 @@
     <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D323" s="9"/>
       <c r="E323" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F323" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H323" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="324" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D324" s="9"/>
       <c r="E324" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F324" s="9" t="s">
         <v>23</v>
@@ -5090,7 +5090,7 @@
     <row r="325" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D325" s="9"/>
       <c r="E325" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="F325" s="9" t="s">
         <v>23</v>
@@ -5105,13 +5105,13 @@
     </row>
     <row r="327" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B327" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D327" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E327" t="s">
         <v>15</v>
@@ -5126,7 +5126,7 @@
         <v>20200401</v>
       </c>
       <c r="I327" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="328" spans="2:9" x14ac:dyDescent="0.3">
@@ -5150,13 +5150,13 @@
     </row>
     <row r="330" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B330" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C330" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D330" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E330" t="s">
         <v>15</v>
@@ -5171,7 +5171,7 @@
         <v>20200401</v>
       </c>
       <c r="I330" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="331" spans="2:9" x14ac:dyDescent="0.3">
@@ -5192,7 +5192,7 @@
     <row r="332" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D332" s="9"/>
       <c r="E332" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F332" s="9" t="s">
         <v>23</v>
@@ -5207,13 +5207,13 @@
     </row>
     <row r="334" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B334" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C334" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D334" s="9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E334" t="s">
         <v>22</v>
@@ -5228,7 +5228,7 @@
         <v>20220228</v>
       </c>
       <c r="I334" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="335" spans="2:9" x14ac:dyDescent="0.3">
@@ -5240,7 +5240,7 @@
         <v>23</v>
       </c>
       <c r="H335" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="336" spans="2:9" x14ac:dyDescent="0.3">
@@ -5264,16 +5264,16 @@
         <v>23</v>
       </c>
       <c r="H337" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="338" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D338" s="9"/>
       <c r="E338" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F338" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H338" s="8">
         <v>4</v>
@@ -5282,10 +5282,10 @@
     <row r="339" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D339" s="9"/>
       <c r="E339" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F339" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H339" s="8">
         <v>48</v>
@@ -5294,10 +5294,10 @@
     <row r="340" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D340" s="9"/>
       <c r="E340" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F340" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H340" s="8">
         <v>1.1000000000000001</v>
@@ -5306,10 +5306,10 @@
     <row r="341" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D341" s="9"/>
       <c r="E341" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F341" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H341" s="8">
         <v>3.2</v>
@@ -5318,10 +5318,10 @@
     <row r="342" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D342" s="9"/>
       <c r="E342" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F342" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H342" s="8">
         <v>0.11</v>
@@ -5330,10 +5330,10 @@
     <row r="343" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D343" s="9"/>
       <c r="E343" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F343" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H343" s="8">
         <v>0.2</v>
@@ -5342,7 +5342,7 @@
     <row r="344" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D344" s="9"/>
       <c r="E344" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F344" s="9" t="s">
         <v>23</v>
@@ -5356,20 +5356,20 @@
     </row>
     <row r="346" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B346" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D346" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E346" s="1"/>
       <c r="F346" s="1"/>
       <c r="G346" s="1"/>
       <c r="H346" s="3"/>
       <c r="I346" s="13" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="347" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5384,26 +5384,26 @@
     </row>
     <row r="348" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B348" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D348" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E348" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F348" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G348" s="1"/>
       <c r="H348" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I348" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="349" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5418,13 +5418,13 @@
     </row>
     <row r="350" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B350" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D350" s="10" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E350" s="1"/>
       <c r="F350" s="1"/>
@@ -5446,26 +5446,26 @@
     </row>
     <row r="352" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B352" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D352" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E352" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F352" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G352" s="1"/>
       <c r="H352" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I352" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="353" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5480,16 +5480,16 @@
     </row>
     <row r="354" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B354" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D354" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F354" s="1" t="s">
         <v>9</v>
@@ -5499,7 +5499,7 @@
         <v>14</v>
       </c>
       <c r="I354" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="355" spans="2:9" x14ac:dyDescent="0.3">
@@ -5507,14 +5507,14 @@
       <c r="C355" s="1"/>
       <c r="D355" s="10"/>
       <c r="E355" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F355" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G355" s="1"/>
       <c r="H355" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I355" s="1"/>
     </row>

</xml_diff>

<commit_message>
Change input parameter in AddPledgeRequest Api
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="324">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -215,25 +215,13 @@
     <t>GetDropdownData</t>
   </si>
   <si>
-    <t>DPIDValue</t>
-  </si>
-  <si>
     <t>"1202870000086521"</t>
   </si>
   <si>
-    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"th_cmcd\": \"MG040\",\r\n \"cm_Name\": \"Testing 5 \",\r\n \"th_MrgShortFall\": 0.0000,\r\n \"th_scripcd\": \"532667 \",\r\n \"ss_Name\": \"SUZLON\",\r\n \"th_qty\": 198.0,\r\n \"th_rate\": 5.55,\r\n \"th_HairCut\": 27.87,\r\n \"th_ISIN\": \"INE040H01021\",\r\n \"th_netValue\": 792.00,\r\n \"Retain\": 198.0,\r\n \"th_DematActNo\": \"1202870000086521\",\r\n \"th_ISIN1\": \"INE040H01021\",\r\n \"th_Value\": 1098.90,\r\n \"th_NetRate\": 4.0000,\r\n \"th_ReqValue\": 792.00\r\n },\r\n {\r\n \"th_cmcd\": \"MG040\",\r\n \"cm_Name\": \"Testing 5 \",\r\n \"th_MrgShortFall\": 0.0000,\r\n \"th_scripcd\": \"532648 \",\r\n \"ss_Name\": \"YESBANK\",\r\n \"th_qty\": 90.0,\r\n \"th_rate\": 16.35,\r\n \"th_HairCut\": 36.97,\r\n \"th_ISIN\": \"INE528G01035\",\r\n \"th_netValue\": 927.90,\r\n \"Retain\": 90.0,\r\n \"th_DematActNo\": \"1202870000086521\",\r\n \"th_ISIN1\": \"INE528G01035\",\r\n \"th_Value\": 1471.50,\r\n \"th_NetRate\": 10.3100,\r\n \"th_ReqValue\": 927.90\r\n },\r\n {\r\n \"th_cmcd\": \"MG040\",\r\n \"cm_Name\": \"Testing 5 \",\r\n \"th_MrgShortFall\": 0.0000,\r\n \"th_scripcd\": \"542655 \",\r\n \"ss_Name\": \"VIKASMCORP\",\r\n \"th_qty\": 90.0,\r\n \"th_rate\": 3.75,\r\n \"th_HairCut\": 26.96,\r\n \"th_ISIN\": \"INE161L01027\",\r\n \"th_netValue\": 246.60,\r\n \"Retain\": 90.0,\r\n \"th_DematActNo\": \"1202870000086521\",\r\n \"th_ISIN1\": \"INE161L01027\",\r\n \"th_Value\": 337.50,\r\n \"th_NetRate\": 2.7400,\r\n \"th_ReqValue\": 246.60\r\n },\r\n {\r\n \"th_cmcd\": \"MG040\",\r\n \"cm_Name\": \"Testing 5 \",\r\n \"th_MrgShortFall\": 0.0000,\r\n \"th_scripcd\": \"532461 \",\r\n \"ss_Name\": \"PNB\",\r\n \"th_qty\": 30.0,\r\n \"th_rate\": 41.70,\r\n \"th_HairCut\": 19.50,\r\n \"th_ISIN\": \"INE160A01022\",\r\n \"th_netValue\": 1007.10,\r\n \"Retain\": 30.0,\r\n \"th_DematActNo\": \"1202870000086521\",\r\n \"th_ISIN1\": \"INE160A01022\",\r\n \"th_Value\": 1251.00,\r\n \"th_NetRate\": 33.5700,\r\n \"th_ReqValue\": 1007.10\r\n },\r\n {\r\n \"th_cmcd\": \"MG040\",\r\n \"cm_Name\": \"Testing 5 \",\r\n \"th_MrgShortFall\": 0.0000,\r\n \"th_scripcd\": \"519307 \",\r\n \"ss_Name\": \"VIKASWSP\",\r\n \"th_qty\": 30.0,\r\n \"th_rate\": 6.45,\r\n \"th_HairCut\": 26.99,\r\n \"th_ISIN\": \"INE706A01022\",\r\n \"th_netValue\": 141.30,\r\n \"Retain\": 30.0,\r\n \"th_DematActNo\": \"1202870000086521\",\r\n \"th_ISIN1\": \"INE706A01022\",\r\n \"th_Value\": 193.50,\r\n \"th_NetRate\": 4.7100,\r\n \"th_ReqValue\": 141.30\r\n },\r\n {\r\n \"th_cmcd\": \"MG040\",\r\n \"cm_Name\": \"Testing 5 \",\r\n \"th_MrgShortFall\": 0.0000,\r\n \"th_scripcd\": \"330039 \",\r\n \"ss_Name\": \"CDSL\",\r\n \"th_qty\": 3.0,\r\n \"th_rate\": 599.90,\r\n \"th_HairCut\": 16.56,\r\n \"th_ISIN\": \"INE736A01011\",\r\n \"th_netValue\": 1501.68,\r\n \"Retain\": 3.0,\r\n \"th_DematActNo\": \"1202870000086521\",\r\n \"th_ISIN1\": \"INE736A01011\",\r\n \"th_Value\": 1799.70,\r\n \"th_NetRate\": 500.5600,\r\n \"th_ReqValue\": 1501.68\r\n },\r\n {\r\n \"th_cmcd\": \"MG040\",\r\n \"cm_Name\": \"Testing 5 \",\r\n \"th_MrgShortFall\": 0.0000,\r\n \"th_scripcd\": \"543227 \",\r\n \"ss_Name\": \"HAPPSTMNDS\",\r\n \"th_qty\": 3.0,\r\n \"th_rate\": 535.55,\r\n \"th_HairCut\": 16.37,\r\n \"th_ISIN\": \"INE419U01012\",\r\n \"th_netValue\": 1343.64,\r\n \"Retain\": 3.0,\r\n \"th_DematActNo\": \"1202870000086521\",\r\n \"th_ISIN1\": \"INE419U01012\",\r\n \"th_Value\": 1606.65,\r\n \"th_NetRate\": 447.8800,\r\n \"th_ReqValue\": 1343.64\r\n },\r\n {\r\n \"th_cmcd\": \"MG040\",\r\n \"cm_Name\": \"Testing 5 \",\r\n \"th_MrgShortFall\": 0.0000,\r\n \"th_scripcd\": \"500188 \",\r\n \"ss_Name\": \"HINDZINC\",\r\n \"th_qty\": 3.0,\r\n \"th_rate\": 311.45,\r\n \"th_HairCut\": 16.21,\r\n \"th_ISIN\": \"INE267A01025\",\r\n \"th_netValue\": 782.88,\r\n \"Retain\": 3.0,\r\n \"th_DematActNo\": \"1202870000086521\",\r\n \"th_ISIN1\": \"INE267A01025\",\r\n \"th_Value\": 934.35,\r\n \"th_NetRate\": 260.9600,\r\n \"th_ReqValue\": 782.88\r\n }\r\n]" }</t>
-  </si>
-  <si>
     <t>GetCurrentPledgeRequest</t>
   </si>
   <si>
     <t>AddPledgeRequest</t>
-  </si>
-  <si>
-    <t>isIdentityOn</t>
-  </si>
-  <si>
-    <t>intcnt</t>
   </si>
   <si>
     <t>quantity</t>
@@ -1024,6 +1012,9 @@
   </si>
   <si>
     <t>[ { "securities_Code": "531518 ", "securities_Name": "VIKASGRAN", "securities_ISIN": "INE767B01022", "holding_Rate": 2, "holding_Qty": 300, "holding_Value": 600, "hairCut": 24.29, "netValue": 453, "request_Qty": 300, "request_Value": 600 }, { "securities_Code": "542655 ", "securities_Name": "VIKASMCORP", "securities_ISIN": "INE161L01027", "holding_Rate": 3.47, "holding_Qty": 210, "holding_Value": 728.7, "hairCut": 25.15, "netValue": 546, "request_Qty": 210, "request_Value": 728.7 }, { "securities_Code": "519307 ", "securities_Name": "VIKASWSP", "securities_ISIN": "INE706A01022", "holding_Rate": 3.6, "holding_Qty": 100, "holding_Value": 360, "hairCut": 26.34, "netValue": 265, "request_Qty": 100, "request_Value": 360 }, { "securities_Code": "533295 ", "securities_Name": "PSB", "securities_ISIN": "INE608A01012", "holding_Rate": 16, "holding_Qty": 60, "holding_Value": 960, "hairCut": 19.36, "netValue": 774, "request_Qty": 60, "request_Value": 960 }, { "securities_Code": "531307 ", "securities_Name": "RRILLTD", "securities_ISIN": "INE951M01037", "holding_Rate": 13.49, "holding_Qty": 18, "holding_Value": 242.82, "hairCut": 21.98, "netValue": 189.36, "request_Qty": 18, "request_Value": 242.82 }, { "securities_Code": "526371 ", "securities_Name": "NMDC", "securities_ISIN": "INE584A01023", "holding_Rate": 134.9, "holding_Qty": 3, "holding_Value": 404.70000000000005, "hairCut": 17.11, "netValue": 335.46, "request_Qty": 6, "request_Value": 809.4000000000001 }, { "securities_Code": "500288 ", "securities_Name": "MOREPENLAB", "securities_ISIN": "INE083A01026", "holding_Rate": 55.35, "holding_Qty": 6, "holding_Value": 332.1, "hairCut": 25.28, "netValue": 248.16, "request_Qty": 6, "request_Value": 332.1 }, { "securities_Code": "526650 ", "securities_Name": "TFCILTD", "securities_ISIN": "INE305A01015", "holding_Rate": 59.6, "holding_Qty": 3, "holding_Value": 178.8, "hairCut": 19.71, "netValue": 143.55, "request_Qty": 6, "request_Value": 357.6 }, { "securities_Code": "500188 ", "securities_Name": "HINDZINC", "securities_ISIN": "INE267A01025", "holding_Rate": 315.1, "holding_Qty": 3, "holding_Value": 945.3000000000001, "hairCut": 14.8, "netValue": 805.41, "request_Qty": 3, "request_Value": 945.3000000000001 }, { "securities_Code": "534816 ", "securities_Name": "INDUSTOWER", "securities_ISIN": "INE121J01017", "holding_Rate": 253.3, "holding_Qty": 3, "holding_Value": 759.9000000000001, "hairCut": 19.25, "netValue": 613.62, "request_Qty": 3, "request_Value": 759.9000000000001 }, { "securities_Code": "532872 ", "securities_Name": "SPARC", "securities_ISIN": "INE232I01014", "holding_Rate": 250.7, "holding_Qty": 3, "holding_Value": 752.0999999999999, "hairCut": 19.58, "netValue": 604.83, "request_Qty": 3, "request_Value": 752.0999999999999 }, { "securities_Code": "532898 ", "securities_Name": "POWERGRID", "securities_ISIN": "INE752E01010", "holding_Rate": 208.4, "holding_Qty": 3, "holding_Value": 625.2, "hairCut": 11.63, "netValue": 552.48, "request_Qty": 3, "request_Value": 625.2 }, { "securities_Code": "500086 ", "securities_Name": "EXIDEIND", "securities_ISIN": "INE302A01020", "holding_Rate": 164.35, "holding_Qty": 3, "holding_Value": 493.04999999999995, "hairCut": 10.78, "netValue": 439.89, "request_Qty": 3, "request_Value": 493.04999999999995 }, { "securities_Code": "540065 ", "securities_Name": "RBLBANK", "securities_ISIN": "INE976G01028", "holding_Rate": 177.95, "holding_Qty": 3, "holding_Value": 533.8499999999999, "hairCut": 21.51, "netValue": 419.01, "request_Qty": 3, "request_Value": 533.8499999999999 }, { "securities_Code": "511676 ", "securities_Name": "GICHSGFIN", "securities_ISIN": "INE289B01019", "holding_Rate": 145.2, "holding_Qty": 3, "holding_Value": 435.59999999999997, "hairCut": 19.33, "netValue": 351.39, "request_Qty": 3, "request_Value": 435.59999999999997 }, { "securities_Code": "532955 ", "securities_Name": "RECLTD", "securities_ISIN": "INE020B01018", "holding_Rate": 132.55, "holding_Qty": 3, "holding_Value": 397.65000000000003, "hairCut": 13.91, "netValue": 342.33, "request_Qty": 3, "request_Value": 397.65000000000003 }, { "securities_Code": "330179 ", "securities_Name": "AHLADA", "securities_ISIN": "INE00PV01013", "holding_Rate": 127.6, "holding_Qty": 3, "holding_Value": 382.79999999999995, "hairCut": 18.23, "netValue": 313.02, "request_Qty": 3, "request_Value": 382.79999999999995 }, { "securities_Code": "532522 ", "securities_Name": "PETRONET", "securities_ISIN": "INE347G01014", "holding_Rate": 218.7, "holding_Qty": 2, "holding_Value": 437.4, "hairCut": 10.29, "netValue": 392.4, "request_Qty": 2, "request_Value": 437.4 }, { "securities_Code": "500260 ", "securities_Name": "RAMCOCEM", "securities_ISIN": "INE331A01037", "holding_Rate": 997, "holding_Qty": 1, "holding_Value": 997, "hairCut": 11.86, "netValue": 878.76, "request_Qty": 1, "request_Value": 997 }, { "securities_Code": "517385 ", "securities_Name": "SYMPHONY", "securities_ISIN": "INE225D01027", "holding_Rate": 1006.55, "holding_Qty": 1, "holding_Value": 1006.55, "hairCut": 13.78, "netValue": 867.85, "request_Qty": 1, "request_Value": 1006.55 }, { "securities_Code": "500770 ", "securities_Name": "TATACHEM", "securities_ISIN": "INE092A01019", "holding_Rate": 885.45, "holding_Qty": 1, "holding_Value": 885.45, "hairCut": 15.98, "netValue": 743.96, "request_Qty": 1, "request_Value": 885.45 }, { "securities_Code": "500520 ", "securities_Name": "M&amp;M", "securities_ISIN": "INE101A01026", "holding_Rate": 826.65, "holding_Qty": 1, "holding_Value": 826.65, "hairCut": 13.45, "netValue": 715.47, "request_Qty": 1, "request_Value": 826.65 }, { "securities_Code": "532174 ", "securities_Name": "ICICIBANK", "securities_ISIN": "INE090A01021", "holding_Rate": 731, "holding_Qty": 1, "holding_Value": 731, "hairCut": 14.38, "netValue": 625.88, "request_Qty": 1, "request_Value": 731 }, { "securities_Code": "505192 ", "securities_Name": "SMLISUZU", "securities_ISIN": "INE294B01019", "holding_Rate": 646.4, "holding_Qty": 1, "holding_Value": 646.4, "hairCut": 20.13, "netValue": 516.28, "request_Qty": 1, "request_Value": 646.4 }, { "securities_Code": "532967 ", "securities_Name": "KIRIINDUS", "securities_ISIN": "INE415I01015", "holding_Rate": 471.75, "holding_Qty": 1, "holding_Value": 471.75, "hairCut": 20.08, "netValue": 377.02, "request_Qty": 1, "request_Value": 471.75 }, { "securities_Code": "530803 ", "securities_Name": "BHAGERIA", "securities_ISIN": "INE354C01027", "holding_Rate": 249.5, "holding_Qty": 1, "holding_Value": 249.5, "hairCut": 18.98, "netValue": 202.14, "request_Qty": 1, "request_Value": 249.5 }, { "securities_Code": "522205 ", "securities_Name": "PRAJIND", "securities_ISIN": "INE074A01025", "holding_Rate": 307.2, "holding_Qty": 512, "holding_Value": 157286.4, "hairCut": 20.59, "netValue": 124902.4, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "330039 ", "securities_Name": "CDSL", "securities_ISIN": "INE736A01011", "holding_Rate": 1492.9, "holding_Qty": 71, "holding_Value": 105995.90000000001, "hairCut": 17.75, "netValue": 87181.61, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "524558 ", "securities_Name": "NEULANDLAB", "securities_ISIN": "INE794A01010", "holding_Rate": 1587.15, "holding_Qty": 15, "holding_Value": 23807.25, "hairCut": 21.98, "netValue": 18574.35, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "532648 ", "securities_Name": "YESBANK", "securities_ISIN": "INE528G01035", "holding_Rate": 13.58, "holding_Qty": 300, "holding_Value": 4074, "hairCut": 29, "netValue": 2892, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "532822 ", "securities_Name": "IDEA", "securities_ISIN": "INE669E01016", "holding_Rate": 13.79, "holding_Qty": 180, "holding_Value": 2482.2, "hairCut": 38.4, "netValue": 1528.2, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "505537 ", "securities_Name": "ZEEL", "securities_ISIN": "INE256A01028", "holding_Rate": 338.1, "holding_Qty": 6, "holding_Value": 2028.6000000000001, "hairCut": 27.23, "netValue": 1476.24, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500570 ", "securities_Name": "TATAMOTORS", "securities_ISIN": "INE155A01022", "holding_Rate": 472.35, "holding_Qty": 3, "holding_Value": 1417.0500000000002, "hairCut": 21.17, "netValue": 1117.05, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "512573 ", "securities_Name": "AVANTIFEED", "securities_ISIN": "INE871C01038", "holding_Rate": 547.95, "holding_Qty": 2, "holding_Value": 1095.9, "hairCut": 15.1, "netValue": 930.42, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500257 ", "securities_Name": "LUPIN", "securities_ISIN": "INE326A01037", "holding_Rate": 912.25, "holding_Qty": 1, "holding_Value": 912.25, "hairCut": 13.01, "netValue": 793.57, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "533278 ", "securities_Name": "COALINDIA", "securities_ISIN": "INE522F01014", "holding_Rate": 147.7, "holding_Qty": 6, "holding_Value": 886.1999999999999, "hairCut": 13.06, "netValue": 770.46, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "541153 ", "securities_Name": "BANDHANBNK", "securities_ISIN": "INE545U01014", "holding_Rate": 258.9, "holding_Qty": 3, "holding_Value": 776.6999999999999, "hairCut": 20.63, "netValue": 616.47, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500228 ", "securities_Name": "JSWSTEEL", "securities_ISIN": "INE019A01038", "holding_Rate": 649.65, "holding_Qty": 1, "holding_Value": 649.65, "hairCut": 15.86, "netValue": 546.62, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "517334 ", "securities_Name": "MOTHERSUMI", "securities_ISIN": "INE775A01035", "holding_Rate": 214.4, "holding_Qty": 3, "holding_Value": 643.2, "hairCut": 19.16, "netValue": 519.96, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500096 ", "securities_Name": "DABUR", "securities_ISIN": "INE016A01026", "holding_Rate": 569.65, "holding_Qty": 1, "holding_Value": 569.65, "hairCut": 9, "netValue": 518.38, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500850 ", "securities_Name": "INDHOTEL", "securities_ISIN": "INE053A01029", "holding_Rate": 180.45, "holding_Qty": 3, "holding_Value": 541.3499999999999, "hairCut": 18.3, "netValue": 442.29, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500477 ", "securities_Name": "ASHOKLEY", "securities_ISIN": "INE208A01029", "holding_Rate": 125.8, "holding_Qty": 3, "holding_Value": 377.4, "hairCut": 17.79, "netValue": 310.26, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "532461 ", "securities_Name": "PNB", "securities_ISIN": "INE160A01022", "holding_Rate": 38, "holding_Qty": 9, "holding_Value": 342, "hairCut": 17.35, "netValue": 282.69, "request_Qty": 0, "request_Value": 0 } ]</t>
+  </si>
+  <si>
+    <t>securities_Code</t>
   </si>
 </sst>
 </file>
@@ -1492,9 +1483,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I377"/>
+  <dimension ref="A1:I375"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A259" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
       <selection activeCell="E275" sqref="E275"/>
     </sheetView>
   </sheetViews>
@@ -1526,13 +1517,13 @@
     </row>
     <row r="2" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -1558,13 +1549,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1575,10 +1566,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1598,10 +1589,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1613,7 +1604,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1636,10 +1627,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1659,10 +1650,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1677,13 +1668,13 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1694,10 +1685,10 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1712,7 +1703,7 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D17" s="9"/>
       <c r="E17" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
@@ -1721,7 +1712,7 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D18" s="9"/>
       <c r="E18" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
@@ -1730,7 +1721,7 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D19" s="9"/>
       <c r="E19" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -1744,13 +1735,13 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1761,49 +1752,49 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="I23" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D24" s="9"/>
       <c r="H24" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="I24" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="9"/>
       <c r="H25" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="I25" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="9"/>
       <c r="H26" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="I26" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -1815,10 +1806,10 @@
         <v>9</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -1830,10 +1821,10 @@
         <v>9</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -1844,10 +1835,10 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1859,10 +1850,10 @@
         <v>16</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
@@ -1877,7 +1868,7 @@
         <v>16</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
@@ -1887,49 +1878,49 @@
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D33" s="9"/>
       <c r="E33" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F33" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D34" s="9"/>
       <c r="G34" s="20"/>
       <c r="H34" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D35" s="9"/>
       <c r="G35" s="20"/>
       <c r="H35" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D36" s="9"/>
       <c r="G36" s="20"/>
       <c r="H36" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D37" s="9"/>
       <c r="G37" s="20"/>
       <c r="H37" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D38" s="9"/>
       <c r="G38" s="20"/>
       <c r="H38" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
@@ -1939,25 +1930,25 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D40" s="9"/>
       <c r="E40" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D41" s="9"/>
       <c r="H41" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D42" s="9"/>
       <c r="H42" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -1968,58 +1959,58 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="E44" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I44" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D45" s="9"/>
       <c r="I45" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D46" s="9"/>
       <c r="I46" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D47" s="9"/>
       <c r="I47" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D48" s="9"/>
       <c r="I48" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D49" s="9"/>
       <c r="I49" s="19" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D50" s="9"/>
       <c r="I50" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2030,22 +2021,22 @@
         <v>46</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H52" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -2073,46 +2064,46 @@
         <v>38</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D56" s="9"/>
       <c r="I56" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D57" s="9"/>
       <c r="I57" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D58" s="9"/>
       <c r="I58" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D59" s="9"/>
       <c r="I59" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D60" s="9"/>
       <c r="I60" s="19" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D61" s="9"/>
       <c r="I61" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
@@ -2126,55 +2117,55 @@
         <v>38</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="E63" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="I63" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D64" s="9"/>
       <c r="I64" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D65" s="9"/>
       <c r="I65" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D66" s="9"/>
       <c r="I66" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" s="9"/>
       <c r="I67" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D68" s="9"/>
       <c r="I68" s="19" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D69" s="9"/>
       <c r="I69" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
@@ -2188,10 +2179,10 @@
         <v>38</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
@@ -2205,10 +2196,10 @@
         <v>38</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E73" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F73" t="s">
         <v>23</v>
@@ -2217,7 +2208,7 @@
         <v>1202870000086520</v>
       </c>
       <c r="I73" s="26" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
@@ -2231,10 +2222,10 @@
         <v>38</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="E75" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F75" t="s">
         <v>23</v>
@@ -2243,7 +2234,7 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D76" s="9"/>
       <c r="E76" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="F76" t="s">
         <v>23</v>
@@ -2260,10 +2251,10 @@
         <v>38</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="I78" s="26" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
@@ -2324,13 +2315,13 @@
         <v>26</v>
       </c>
       <c r="C84" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
@@ -2341,13 +2332,13 @@
         <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="E86" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F86" t="s">
         <v>23</v>
@@ -2356,7 +2347,7 @@
         <v>28</v>
       </c>
       <c r="I86" s="26" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
@@ -2367,7 +2358,7 @@
         <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>29</v>
@@ -2406,22 +2397,22 @@
         <v>26</v>
       </c>
       <c r="C91" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="E91" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I91" s="26" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
@@ -2433,28 +2424,28 @@
         <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E93" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="I93" s="26" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D94" s="9"/>
       <c r="E94" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>9</v>
@@ -2472,13 +2463,13 @@
         <v>26</v>
       </c>
       <c r="C96" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="E96" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>9</v>
@@ -2488,7 +2479,7 @@
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D97" s="9"/>
       <c r="E97" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>9</v>
@@ -2498,7 +2489,7 @@
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D98" s="9"/>
       <c r="E98" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>9</v>
@@ -2516,13 +2507,13 @@
         <v>26</v>
       </c>
       <c r="C100" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="E100" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>9</v>
@@ -2532,7 +2523,7 @@
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D101" s="9"/>
       <c r="E101" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>9</v>
@@ -2548,34 +2539,34 @@
         <v>20</v>
       </c>
       <c r="C103" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E103" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H103" s="30" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I103" s="31" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D104" s="9"/>
       <c r="E104" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H104" s="14" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
@@ -2586,13 +2577,13 @@
         <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="E106" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>9</v>
@@ -2602,7 +2593,7 @@
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D107" s="9"/>
       <c r="E107" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>9</v>
@@ -2612,7 +2603,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>9</v>
@@ -2622,7 +2613,7 @@
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D109" s="9"/>
       <c r="E109" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>9</v>
@@ -2632,7 +2623,7 @@
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D110" s="9"/>
       <c r="E110" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>9</v>
@@ -2642,7 +2633,7 @@
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D111" s="9"/>
       <c r="E111" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>9</v>
@@ -2657,31 +2648,31 @@
         <v>34</v>
       </c>
       <c r="C113" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F113" t="s">
         <v>9</v>
       </c>
       <c r="H113" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="I113" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D114" s="9"/>
       <c r="H114" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="I114" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
@@ -2693,10 +2684,10 @@
         <v>9</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I115" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
@@ -2708,28 +2699,28 @@
         <v>9</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I116" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D117" s="9"/>
       <c r="I117" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D118" s="9"/>
       <c r="I118" s="19" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D119" s="9"/>
       <c r="I119" s="19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
@@ -2740,49 +2731,49 @@
         <v>34</v>
       </c>
       <c r="C121" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="F121" t="s">
         <v>9</v>
       </c>
       <c r="H121" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="I121" s="19" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D122" s="9"/>
       <c r="H122" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="I122" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D123" s="9"/>
       <c r="H123" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="I123" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D124" s="9"/>
       <c r="H124" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="I124" s="19" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
@@ -2794,10 +2785,10 @@
         <v>9</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I125" s="19" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.3">
@@ -2809,16 +2800,16 @@
         <v>9</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I126" s="19" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D127" s="9"/>
       <c r="I127" s="22" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
@@ -2829,49 +2820,49 @@
         <v>34</v>
       </c>
       <c r="C129" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E129" s="11" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="F129" t="s">
         <v>9</v>
       </c>
       <c r="H129" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="I129" s="23" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D130" s="9"/>
       <c r="H130" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D131" s="9"/>
       <c r="H131" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="I131" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D132" s="9"/>
       <c r="H132" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="I132" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.3">
@@ -2883,10 +2874,10 @@
         <v>9</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="I133" s="19" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.3">
@@ -2898,22 +2889,22 @@
         <v>9</v>
       </c>
       <c r="H134" s="17" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I134" s="19" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D135" s="9"/>
       <c r="I135" s="19" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D136" s="9"/>
       <c r="I136" s="19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
@@ -2922,49 +2913,49 @@
     <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D138" s="9"/>
       <c r="I138" s="23" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D139" s="9"/>
       <c r="I139" s="19" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D140" s="9"/>
       <c r="I140" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D141" s="9"/>
       <c r="I141" s="19" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
       <c r="I142" s="19" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D143" s="9"/>
       <c r="I143" s="19" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D144" s="9"/>
       <c r="I144" s="19" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D145" s="9"/>
       <c r="I145" s="19" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
@@ -2973,16 +2964,16 @@
     </row>
     <row r="147" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="C147" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.3">
@@ -2993,7 +2984,7 @@
         <v>50</v>
       </c>
       <c r="C149" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D149" s="9" t="s">
         <v>51</v>
@@ -3022,22 +3013,22 @@
         <v>50</v>
       </c>
       <c r="C152" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="E152" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F152" t="s">
         <v>23</v>
       </c>
       <c r="H152" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I152" s="21" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.3">
@@ -3058,13 +3049,13 @@
     <row r="154" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D154" s="9"/>
       <c r="E154" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="F154" t="s">
         <v>23</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.3">
@@ -3075,7 +3066,7 @@
         <v>50</v>
       </c>
       <c r="C156" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D156" s="10" t="s">
         <v>56</v>
@@ -3157,10 +3148,10 @@
         <v>50</v>
       </c>
       <c r="C162" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="E162" s="10" t="s">
         <v>52</v>
@@ -3173,7 +3164,7 @@
         <v>53</v>
       </c>
       <c r="I162" s="26" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.3">
@@ -3224,7 +3215,7 @@
         <v>50</v>
       </c>
       <c r="C167" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="D167" s="10" t="s">
         <v>60</v>
@@ -3245,20 +3236,20 @@
     </row>
     <row r="170" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B170" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C170" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D170" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
       <c r="H170" s="3"/>
       <c r="I170" s="7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.3">
@@ -3266,26 +3257,26 @@
     </row>
     <row r="172" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B172" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C172" t="s">
+        <v>237</v>
+      </c>
+      <c r="D172" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="E172" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C172" t="s">
-        <v>241</v>
-      </c>
-      <c r="D172" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G172" s="1"/>
       <c r="H172" s="3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I172" s="7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.3">
@@ -3293,14 +3284,14 @@
       <c r="C173" s="1"/>
       <c r="D173" s="10"/>
       <c r="E173" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G173" s="1"/>
       <c r="H173" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I173" s="1"/>
     </row>
@@ -3309,16 +3300,16 @@
     </row>
     <row r="175" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B175" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C175" t="s">
+        <v>237</v>
+      </c>
+      <c r="D175" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E175" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="C175" t="s">
-        <v>241</v>
-      </c>
-      <c r="D175" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>9</v>
@@ -3328,7 +3319,7 @@
         <v>53</v>
       </c>
       <c r="I175" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.3">
@@ -3336,14 +3327,14 @@
       <c r="C176" s="1"/>
       <c r="D176" s="10"/>
       <c r="E176" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G176" s="1"/>
       <c r="H176" s="3" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I176" s="1"/>
     </row>
@@ -3352,7 +3343,7 @@
       <c r="C177" s="1"/>
       <c r="D177" s="10"/>
       <c r="E177" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>9</v>
@@ -3404,13 +3395,13 @@
     </row>
     <row r="181" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B181" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C181" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>32</v>
@@ -3420,10 +3411,10 @@
       </c>
       <c r="G181" s="1"/>
       <c r="H181" s="3" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="I181" s="7" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.3">
@@ -3431,14 +3422,14 @@
       <c r="C182" s="1"/>
       <c r="D182" s="10"/>
       <c r="E182" s="1" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G182" s="1"/>
       <c r="H182" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="I182" s="1"/>
     </row>
@@ -3481,21 +3472,21 @@
     <row r="185" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D185" s="9"/>
       <c r="F185" s="10" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
     </row>
     <row r="186" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B186" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C186" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="I186" s="26" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
     </row>
     <row r="187" spans="2:9" x14ac:dyDescent="0.3">
@@ -3503,25 +3494,25 @@
     </row>
     <row r="188" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B188" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C188" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D188" s="10" t="s">
+        <v>288</v>
+      </c>
+      <c r="E188" s="11" t="s">
+        <v>289</v>
+      </c>
+      <c r="F188" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H188" t="s">
+        <v>291</v>
+      </c>
+      <c r="I188" s="26" t="s">
         <v>292</v>
-      </c>
-      <c r="E188" s="11" t="s">
-        <v>293</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H188" t="s">
-        <v>295</v>
-      </c>
-      <c r="I188" s="26" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="189" spans="2:9" x14ac:dyDescent="0.3">
@@ -3541,25 +3532,25 @@
     </row>
     <row r="191" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C191" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D191" s="10" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="E191" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H191" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="I191" s="26" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.3">
@@ -3568,43 +3559,43 @@
     <row r="193" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D193" s="9"/>
       <c r="H193" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I193" s="26"/>
     </row>
     <row r="194" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C194" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="E194" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H194" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="I194" s="26" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D195" s="9"/>
       <c r="H195" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="196" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D196" s="9"/>
       <c r="H196" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.3">
@@ -3612,110 +3603,110 @@
     </row>
     <row r="198" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B198" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C198" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D198" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H198" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="199" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E199" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H199" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H200" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H201" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B203" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C203" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D203" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="H203" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E204" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H204" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H205" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H206" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B208" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C208" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D208" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="H208" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="209" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D209" s="9"/>
       <c r="E209" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H209" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="210" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D210" s="9"/>
       <c r="H210" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D211" s="9"/>
       <c r="H211" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="212" spans="2:8" x14ac:dyDescent="0.3">
@@ -3723,23 +3714,23 @@
     </row>
     <row r="213" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B213" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D213" s="32" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="E213" s="8" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F213" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G213" s="8"/>
       <c r="H213" s="18" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
     </row>
     <row r="214" spans="2:8" x14ac:dyDescent="0.3">
@@ -3781,7 +3772,7 @@
       <c r="C216" s="8"/>
       <c r="D216" s="32"/>
       <c r="E216" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F216" s="8" t="s">
         <v>23</v>
@@ -3802,7 +3793,7 @@
     <row r="218" spans="2:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D218" s="9"/>
       <c r="H218" s="18" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.3">
@@ -3813,13 +3804,13 @@
     </row>
     <row r="221" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B221" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D221" s="32" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E221" s="33" t="s">
         <v>32</v>
@@ -3829,18 +3820,18 @@
       </c>
       <c r="G221" s="8"/>
       <c r="H221" s="32" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="222" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D222" s="9"/>
       <c r="E222" s="8"/>
       <c r="F222" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G222" s="8"/>
       <c r="H222" s="18" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="223" spans="2:8" x14ac:dyDescent="0.3">
@@ -3882,43 +3873,43 @@
     </row>
     <row r="226" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B226" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D226" s="9" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="H226" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I226" s="7" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D227" s="9"/>
       <c r="E227" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H227" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D228" s="9"/>
       <c r="H228" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D229" s="9"/>
       <c r="H229" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="230" spans="2:9" x14ac:dyDescent="0.3">
@@ -3930,43 +3921,43 @@
     </row>
     <row r="231" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B231" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="H231" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I231" s="7" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
     </row>
     <row r="232" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D232" s="9"/>
       <c r="E232" s="11" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H232" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
     </row>
     <row r="233" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D233" s="9"/>
       <c r="H233" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
     </row>
     <row r="234" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D234" s="9"/>
       <c r="H234" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
     </row>
     <row r="235" spans="2:9" x14ac:dyDescent="0.3">
@@ -3978,26 +3969,26 @@
     </row>
     <row r="236" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
       <c r="B236" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D236" s="34" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E236" s="8" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F236" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G236" s="8"/>
       <c r="H236" s="18" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="I236" s="7" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.3">
@@ -4033,7 +4024,7 @@
     <row r="239" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D239" s="9"/>
       <c r="E239" s="8" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="F239" s="8" t="s">
         <v>23</v>
@@ -4052,7 +4043,7 @@
     <row r="241" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D241" s="9"/>
       <c r="H241" s="18" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.3">
@@ -4064,13 +4055,13 @@
     </row>
     <row r="243" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B243" s="8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D243" s="32" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="E243" s="33" t="s">
         <v>32</v>
@@ -4080,18 +4071,18 @@
       </c>
       <c r="G243" s="8"/>
       <c r="H243" s="32" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="244" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D244" s="9"/>
       <c r="E244" s="8"/>
       <c r="F244" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G244" s="8"/>
       <c r="H244" s="18" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
     </row>
     <row r="245" spans="2:9" x14ac:dyDescent="0.3">
@@ -4133,13 +4124,13 @@
     </row>
     <row r="248" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B248" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C248" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D248" s="9" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E248" t="s">
         <v>15</v>
@@ -4154,7 +4145,7 @@
         <v>20210401</v>
       </c>
       <c r="I248" s="7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="249" spans="2:9" x14ac:dyDescent="0.3">
@@ -4175,7 +4166,7 @@
     <row r="250" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D250" s="9"/>
       <c r="E250" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="F250" t="s">
         <v>9</v>
@@ -4190,17 +4181,17 @@
     </row>
     <row r="252" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B252" t="s">
+        <v>101</v>
+      </c>
+      <c r="C252" t="s">
+        <v>238</v>
+      </c>
+      <c r="D252" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="C252" t="s">
-        <v>242</v>
-      </c>
-      <c r="D252" s="9" t="s">
-        <v>109</v>
       </c>
       <c r="H252" s="6"/>
       <c r="I252" s="7" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="253" spans="2:9" x14ac:dyDescent="0.3">
@@ -4213,17 +4204,17 @@
     </row>
     <row r="255" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B255" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C255" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D255" s="9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H255" s="6"/>
       <c r="I255" s="7" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="256" spans="2:9" x14ac:dyDescent="0.3">
@@ -4236,17 +4227,17 @@
     </row>
     <row r="258" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B258" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C258" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H258" s="6"/>
       <c r="I258" s="7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="259" spans="2:9" x14ac:dyDescent="0.3">
@@ -4259,34 +4250,34 @@
     </row>
     <row r="261" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B261" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C261" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D261" s="9" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E261" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="F261" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H261" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I261" s="7" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="262" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D262" s="9"/>
       <c r="E262" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="F262" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H262" s="6" t="b">
         <v>1</v>
@@ -4298,16 +4289,16 @@
     </row>
     <row r="264" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B264" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C264" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D264" s="9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E264" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="F264" t="s">
         <v>21</v>
@@ -4316,7 +4307,7 @@
         <v>3</v>
       </c>
       <c r="I264" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="265" spans="2:9" x14ac:dyDescent="0.3">
@@ -4327,7 +4318,7 @@
         <v>62</v>
       </c>
       <c r="C266" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D266" s="10" t="s">
         <v>63</v>
@@ -4355,7 +4346,7 @@
         <v>62</v>
       </c>
       <c r="C268" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D268" s="10" t="s">
         <v>65</v>
@@ -4378,28 +4369,28 @@
       <c r="H269" s="3"/>
       <c r="I269" s="13"/>
     </row>
-    <row r="270" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="270" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B270" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C270" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D270" s="10" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="E270" s="11" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="F270" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G270" s="1"/>
       <c r="H270" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="I270" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="I270" s="26" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="271" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4412,25 +4403,22 @@
       <c r="H271" s="3"/>
       <c r="I271" s="13"/>
     </row>
-    <row r="272" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="272" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B272" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C272" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D272" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E272" s="11"/>
       <c r="F272" s="10"/>
       <c r="G272" s="1"/>
       <c r="H272" s="3"/>
-      <c r="I272" s="26" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="273" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="273" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B273" s="1"/>
       <c r="C273" s="1"/>
       <c r="D273" s="10"/>
@@ -4440,290 +4428,288 @@
       <c r="H273" s="3"/>
       <c r="I273" s="13"/>
     </row>
-    <row r="274" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B274" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C274" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="D274" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E274" s="11" t="s">
-        <v>66</v>
+        <v>253</v>
       </c>
       <c r="F274" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G274" s="1"/>
       <c r="H274" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="I274" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="275" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
       <c r="D275" s="10"/>
       <c r="E275" s="11" t="s">
-        <v>71</v>
+        <v>323</v>
       </c>
       <c r="F275" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G275" s="1"/>
-      <c r="H275" s="3" t="b">
-        <v>1</v>
+      <c r="H275" s="3">
+        <v>532667</v>
       </c>
       <c r="I275" s="13"/>
     </row>
-    <row r="276" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B276" s="1"/>
       <c r="C276" s="1"/>
       <c r="D276" s="10"/>
       <c r="E276" s="11" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="F276" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G276" s="1"/>
       <c r="H276" s="3">
-        <v>43590</v>
+        <v>198</v>
       </c>
       <c r="I276" s="13"/>
     </row>
-    <row r="277" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B277" s="1"/>
-      <c r="C277" s="1"/>
-      <c r="D277" s="10"/>
-      <c r="E277" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F277" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G277" s="1"/>
-      <c r="H277" s="3">
-        <v>532667</v>
-      </c>
-      <c r="I277" s="13"/>
-    </row>
-    <row r="278" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B278" s="1"/>
-      <c r="C278" s="1"/>
-      <c r="D278" s="10"/>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D277" s="9"/>
+    </row>
+    <row r="278" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B278" t="s">
+        <v>62</v>
+      </c>
+      <c r="C278" t="s">
+        <v>272</v>
+      </c>
+      <c r="D278" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="E278" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F278" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G278" s="1"/>
-      <c r="H278" s="3">
-        <v>198</v>
-      </c>
-      <c r="I278" s="13"/>
-    </row>
-    <row r="279" spans="2:9" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="F278" t="s">
+        <v>9</v>
+      </c>
+      <c r="H278" s="8">
+        <v>20191101</v>
+      </c>
+      <c r="I278" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D279" s="9"/>
     </row>
-    <row r="280" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B280" t="s">
-        <v>62</v>
-      </c>
-      <c r="C280" t="s">
-        <v>276</v>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B280" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C280" s="1" t="s">
+        <v>239</v>
       </c>
       <c r="D280" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E280" s="11" t="s">
-        <v>22</v>
+        <v>225</v>
+      </c>
+      <c r="E280" t="s">
+        <v>15</v>
       </c>
       <c r="F280" t="s">
         <v>9</v>
       </c>
-      <c r="H280" s="8">
-        <v>20191101</v>
-      </c>
-      <c r="I280" s="7" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="281" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H280" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="I280" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D281" s="9"/>
-    </row>
-    <row r="282" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B282" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C282" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D282" s="9" t="s">
-        <v>229</v>
-      </c>
-      <c r="E282" t="s">
-        <v>15</v>
-      </c>
-      <c r="F282" t="s">
-        <v>9</v>
-      </c>
-      <c r="H282" s="35" t="s">
-        <v>169</v>
-      </c>
+      <c r="E281" t="s">
+        <v>17</v>
+      </c>
+      <c r="F281" t="s">
+        <v>9</v>
+      </c>
+      <c r="H281" s="35" t="s">
+        <v>167</v>
+      </c>
+      <c r="I281" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D282" s="9"/>
+      <c r="H282" s="8"/>
       <c r="I282" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="283" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D283" s="9"/>
-      <c r="E283" t="s">
-        <v>17</v>
-      </c>
-      <c r="F283" t="s">
-        <v>9</v>
-      </c>
-      <c r="H283" s="35" t="s">
-        <v>171</v>
-      </c>
+      <c r="H283" s="8"/>
       <c r="I283" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="284" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D284" s="9"/>
-      <c r="H284" s="8"/>
       <c r="I284" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="285" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D285" s="9"/>
-      <c r="H285" s="8"/>
-      <c r="I285" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="286" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I285" s="19" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D286" s="9"/>
       <c r="I286" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="287" spans="2:9" x14ac:dyDescent="0.3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D287" s="9"/>
-      <c r="I287" s="19" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="288" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D288" s="9"/>
-      <c r="I288" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D289" s="9"/>
+    </row>
+    <row r="288" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A288" s="1">
+        <v>36</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C288" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D288" s="10" t="s">
+        <v>232</v>
+      </c>
+      <c r="E288" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F288" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G288" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H288" s="15">
+        <v>20200401</v>
+      </c>
+      <c r="I288" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A289" s="1"/>
+      <c r="B289" s="1"/>
+      <c r="C289" s="1"/>
+      <c r="D289" s="10"/>
+      <c r="E289" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F289" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G289" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H289" s="6">
+        <v>20210331</v>
+      </c>
+      <c r="I289" s="1"/>
     </row>
     <row r="290" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A290" s="1">
-        <v>36</v>
-      </c>
-      <c r="B290" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C290" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D290" s="10" t="s">
-        <v>236</v>
-      </c>
+      <c r="A290" s="1"/>
+      <c r="B290" s="1"/>
+      <c r="C290" s="1"/>
+      <c r="D290" s="10"/>
       <c r="E290" s="1" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="F290" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G290" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H290" s="15">
-        <v>20200401</v>
-      </c>
-      <c r="I290" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="291" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="G290" s="1"/>
+      <c r="H290" s="3">
+        <v>533271</v>
+      </c>
+      <c r="I290" s="13"/>
+    </row>
+    <row r="291" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A291" s="1"/>
       <c r="B291" s="1"/>
       <c r="C291" s="1"/>
       <c r="D291" s="10"/>
-      <c r="E291" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F291" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G291" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H291" s="6">
-        <v>20210331</v>
-      </c>
-      <c r="I291" s="1"/>
-    </row>
-    <row r="292" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A292" s="1"/>
-      <c r="B292" s="1"/>
-      <c r="C292" s="1"/>
-      <c r="D292" s="10"/>
-      <c r="E292" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F292" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G292" s="1"/>
-      <c r="H292" s="3">
-        <v>533271</v>
-      </c>
-      <c r="I292" s="13"/>
-    </row>
-    <row r="293" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A293" s="1"/>
-      <c r="B293" s="1"/>
-      <c r="C293" s="1"/>
-      <c r="D293" s="10"/>
-      <c r="E293" s="1"/>
-      <c r="F293" s="1"/>
-      <c r="G293" s="1"/>
-      <c r="H293" s="3"/>
-      <c r="I293" s="13"/>
+      <c r="E291" s="1"/>
+      <c r="F291" s="1"/>
+      <c r="G291" s="1"/>
+      <c r="H291" s="3"/>
+      <c r="I291" s="13"/>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B292" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D292" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="E292" t="s">
+        <v>27</v>
+      </c>
+      <c r="F292" t="s">
+        <v>9</v>
+      </c>
+      <c r="H292" t="s">
+        <v>226</v>
+      </c>
+      <c r="I292" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D293" s="9"/>
+      <c r="E293" t="s">
+        <v>48</v>
+      </c>
+      <c r="F293" t="s">
+        <v>9</v>
+      </c>
+      <c r="H293" t="s">
+        <v>227</v>
+      </c>
+      <c r="I293" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B294" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C294" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D294" s="9" t="s">
-        <v>238</v>
-      </c>
+      <c r="D294" s="9"/>
       <c r="E294" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="F294" t="s">
         <v>9</v>
       </c>
-      <c r="H294" t="s">
-        <v>230</v>
+      <c r="H294" s="17" t="s">
+        <v>165</v>
       </c>
       <c r="I294" t="s">
         <v>162</v>
@@ -4732,13 +4718,13 @@
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D295" s="9"/>
       <c r="E295" t="s">
-        <v>48</v>
+        <v>17</v>
       </c>
       <c r="F295" t="s">
         <v>9</v>
       </c>
-      <c r="H295" t="s">
-        <v>231</v>
+      <c r="H295" s="17" t="s">
+        <v>167</v>
       </c>
       <c r="I295" t="s">
         <v>164</v>
@@ -4746,79 +4732,79 @@
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D296" s="9"/>
-      <c r="E296" t="s">
-        <v>15</v>
-      </c>
-      <c r="F296" t="s">
-        <v>9</v>
-      </c>
-      <c r="H296" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="I296" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D297" s="9"/>
-      <c r="E297" t="s">
-        <v>17</v>
-      </c>
-      <c r="F297" t="s">
-        <v>9</v>
-      </c>
-      <c r="H297" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="I297" t="s">
-        <v>168</v>
+      <c r="I297" s="19" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D298" s="9"/>
-      <c r="I298" t="s">
-        <v>170</v>
+      <c r="I298" s="19" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D299" s="9"/>
-      <c r="I299" s="19" t="s">
-        <v>232</v>
+      <c r="I299" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D300" s="9"/>
-      <c r="I300" s="19" t="s">
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B301" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D301" s="9"/>
+      <c r="C301" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D301" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E301" t="s">
+        <v>27</v>
+      </c>
+      <c r="F301" t="s">
+        <v>9</v>
+      </c>
+      <c r="H301" t="s">
+        <v>230</v>
+      </c>
       <c r="I301" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D302" s="9"/>
+      <c r="E302" t="s">
+        <v>15</v>
+      </c>
+      <c r="F302" t="s">
+        <v>9</v>
+      </c>
+      <c r="H302" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="I302" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B303" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="C303" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D303" s="9" t="s">
-        <v>239</v>
-      </c>
+      <c r="D303" s="9"/>
       <c r="E303" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="F303" t="s">
         <v>9</v>
       </c>
-      <c r="H303" t="s">
-        <v>234</v>
+      <c r="H303" s="17" t="s">
+        <v>167</v>
       </c>
       <c r="I303" t="s">
         <v>162</v>
@@ -4826,93 +4812,91 @@
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D304" s="9"/>
-      <c r="E304" t="s">
-        <v>15</v>
-      </c>
-      <c r="F304" t="s">
-        <v>9</v>
-      </c>
-      <c r="H304" s="17" t="s">
-        <v>169</v>
-      </c>
       <c r="I304" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="305" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D305" s="9"/>
-      <c r="E305" t="s">
-        <v>17</v>
-      </c>
-      <c r="F305" t="s">
-        <v>9</v>
-      </c>
-      <c r="H305" s="17" t="s">
-        <v>171</v>
-      </c>
       <c r="I305" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="306" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D306" s="9"/>
-      <c r="I306" t="s">
-        <v>168</v>
+      <c r="I306" s="25" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D307" s="9"/>
-      <c r="I307" t="s">
-        <v>170</v>
+      <c r="E307" s="24"/>
+      <c r="H307" s="18"/>
+      <c r="I307" s="18" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="308" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D308" s="9"/>
-      <c r="I308" s="25" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="309" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D309" s="9"/>
-      <c r="E309" s="24"/>
-      <c r="H309" s="18"/>
-      <c r="I309" s="18" t="s">
-        <v>186</v>
+    </row>
+    <row r="309" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B309" t="s">
+        <v>122</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D309" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E309" t="s">
+        <v>15</v>
+      </c>
+      <c r="F309" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G309" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H309" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I309" s="7" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D310" s="9"/>
-    </row>
-    <row r="311" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B311" t="s">
-        <v>126</v>
-      </c>
-      <c r="C311" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D311" s="9" t="s">
-        <v>127</v>
-      </c>
-      <c r="E311" t="s">
+      <c r="E310" t="s">
+        <v>17</v>
+      </c>
+      <c r="F310" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G310" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H310" s="8">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="311" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D311" s="9"/>
+      <c r="F311" s="9"/>
+      <c r="H311" s="8"/>
+    </row>
+    <row r="312" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B312" t="s">
+        <v>122</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D312" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="E312" t="s">
         <v>15</v>
-      </c>
-      <c r="F311" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G311" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H311" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I311" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="312" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D312" s="9"/>
-      <c r="E312" t="s">
-        <v>17</v>
       </c>
       <c r="F312" s="9" t="s">
         <v>23</v>
@@ -4921,74 +4905,70 @@
         <v>16</v>
       </c>
       <c r="H312" s="8">
-        <v>20210331</v>
+        <v>20200401</v>
+      </c>
+      <c r="I312" s="7" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="313" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D313" s="9"/>
-      <c r="F313" s="9"/>
-      <c r="H313" s="8"/>
-    </row>
-    <row r="314" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B314" t="s">
-        <v>126</v>
-      </c>
-      <c r="C314" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D314" s="9" t="s">
-        <v>129</v>
-      </c>
+      <c r="E313" t="s">
+        <v>17</v>
+      </c>
+      <c r="F313" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G313" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H313" s="8">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="314" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D314" s="9"/>
       <c r="E314" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="F314" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G314" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H314" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I314" s="7" t="s">
-        <v>130</v>
+        <v>113</v>
+      </c>
+      <c r="H314" s="8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="315" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D315" s="9"/>
       <c r="E315" t="s">
-        <v>17</v>
+        <v>129</v>
       </c>
       <c r="F315" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G315" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H315" s="8">
-        <v>20210331</v>
+        <v>113</v>
+      </c>
+      <c r="H315" s="8" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="316" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D316" s="9"/>
       <c r="E316" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F316" s="9" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H316" s="8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D317" s="9"/>
       <c r="E317" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F317" s="9" t="s">
-        <v>117</v>
+        <v>23</v>
       </c>
       <c r="H317" s="8" t="s">
         <v>132</v>
@@ -4996,143 +4976,146 @@
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D318" s="9"/>
-      <c r="E318" t="s">
-        <v>134</v>
-      </c>
-      <c r="F318" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="H318" s="8" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="319" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D319" s="9"/>
+      <c r="H318" s="8"/>
+    </row>
+    <row r="319" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B319" t="s">
+        <v>122</v>
+      </c>
+      <c r="C319" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D319" s="9" t="s">
+        <v>133</v>
+      </c>
       <c r="E319" t="s">
-        <v>135</v>
+        <v>15</v>
       </c>
       <c r="F319" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H319" s="8" t="s">
-        <v>136</v>
+      <c r="G319" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H319" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I319" s="7" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="320" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D320" s="9"/>
-      <c r="H320" s="8"/>
-    </row>
-    <row r="321" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B321" t="s">
-        <v>126</v>
-      </c>
-      <c r="C321" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D321" s="9" t="s">
-        <v>137</v>
-      </c>
+      <c r="E320" t="s">
+        <v>17</v>
+      </c>
+      <c r="F320" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G320" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H320" s="8">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="321" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D321" s="9"/>
       <c r="E321" t="s">
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="F321" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G321" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H321" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I321" s="7" t="s">
-        <v>138</v>
+      <c r="H321" s="8" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="322" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D322" s="9"/>
       <c r="E322" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
       <c r="F322" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G322" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H322" s="8">
-        <v>20210331</v>
+      <c r="H322" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D323" s="9"/>
       <c r="E323" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F323" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H323" s="8" t="s">
-        <v>140</v>
+      <c r="H323" s="8">
+        <v>512573</v>
       </c>
     </row>
     <row r="324" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D324" s="9"/>
-      <c r="E324" t="s">
-        <v>141</v>
-      </c>
-      <c r="F324" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H324" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="325" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D325" s="9"/>
+      <c r="H324" s="8"/>
+    </row>
+    <row r="325" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B325" t="s">
+        <v>122</v>
+      </c>
+      <c r="C325" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D325" s="9" t="s">
+        <v>139</v>
+      </c>
       <c r="E325" t="s">
-        <v>142</v>
+        <v>15</v>
       </c>
       <c r="F325" s="9" t="s">
         <v>23</v>
       </c>
+      <c r="G325" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="H325" s="8">
-        <v>512573</v>
+        <v>20200401</v>
+      </c>
+      <c r="I325" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="326" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D326" s="9"/>
-      <c r="H326" s="8"/>
-    </row>
-    <row r="327" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B327" t="s">
-        <v>126</v>
-      </c>
-      <c r="C327" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D327" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E327" t="s">
+      <c r="E326" t="s">
+        <v>17</v>
+      </c>
+      <c r="F326" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G326" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H326" s="8">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="327" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D327" s="9"/>
+      <c r="H327" s="8"/>
+    </row>
+    <row r="328" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B328" t="s">
+        <v>122</v>
+      </c>
+      <c r="C328" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D328" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E328" t="s">
         <v>15</v>
-      </c>
-      <c r="F327" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G327" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H327" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I327" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="328" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D328" s="9"/>
-      <c r="E328" t="s">
-        <v>17</v>
       </c>
       <c r="F328" s="9" t="s">
         <v>23</v>
@@ -5141,234 +5124,241 @@
         <v>16</v>
       </c>
       <c r="H328" s="8">
-        <v>20210331</v>
+        <v>20200401</v>
+      </c>
+      <c r="I328" s="7" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="329" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D329" s="9"/>
-      <c r="H329" s="8"/>
-    </row>
-    <row r="330" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B330" t="s">
-        <v>126</v>
-      </c>
-      <c r="C330" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D330" s="9" t="s">
-        <v>145</v>
-      </c>
+      <c r="E329" t="s">
+        <v>17</v>
+      </c>
+      <c r="F329" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G329" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H329" s="8">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="330" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D330" s="9"/>
       <c r="E330" t="s">
-        <v>15</v>
+        <v>143</v>
       </c>
       <c r="F330" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G330" s="9" t="s">
-        <v>16</v>
-      </c>
       <c r="H330" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I330" s="7" t="s">
-        <v>146</v>
+        <v>500425</v>
       </c>
     </row>
     <row r="331" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D331" s="9"/>
-      <c r="E331" t="s">
-        <v>17</v>
-      </c>
-      <c r="F331" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G331" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H331" s="8">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="332" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D332" s="9"/>
+      <c r="H331" s="8"/>
+    </row>
+    <row r="332" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B332" t="s">
+        <v>122</v>
+      </c>
+      <c r="C332" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D332" s="9" t="s">
+        <v>144</v>
+      </c>
       <c r="E332" t="s">
-        <v>147</v>
+        <v>22</v>
       </c>
       <c r="F332" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H332" s="8">
-        <v>500425</v>
+      <c r="G332" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H332" s="16">
+        <v>20220228</v>
+      </c>
+      <c r="I332" s="7" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="333" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D333" s="9"/>
-      <c r="H333" s="8"/>
-    </row>
-    <row r="334" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B334" t="s">
-        <v>126</v>
-      </c>
-      <c r="C334" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D334" s="9" t="s">
-        <v>148</v>
-      </c>
+      <c r="E333" t="s">
+        <v>37</v>
+      </c>
+      <c r="F333" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H333" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="334" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D334" s="9"/>
       <c r="E334" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F334" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G334" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H334" s="16">
-        <v>20220228</v>
-      </c>
-      <c r="I334" s="7" t="s">
-        <v>149</v>
+      <c r="H334" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="335" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D335" s="9"/>
       <c r="E335" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F335" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H335" s="8" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="336" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D336" s="9"/>
       <c r="E336" t="s">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="F336" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H336" s="8" t="s">
-        <v>25</v>
+        <v>148</v>
+      </c>
+      <c r="H336" s="8">
+        <v>4</v>
       </c>
     </row>
     <row r="337" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D337" s="9"/>
       <c r="E337" t="s">
-        <v>35</v>
+        <v>149</v>
       </c>
       <c r="F337" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H337" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
+      </c>
+      <c r="H337" s="8">
+        <v>48</v>
       </c>
     </row>
     <row r="338" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D338" s="9"/>
       <c r="E338" t="s">
-        <v>73</v>
+        <v>150</v>
       </c>
       <c r="F338" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H338" s="8">
-        <v>4</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="339" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D339" s="9"/>
       <c r="E339" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F339" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H339" s="8">
-        <v>48</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="340" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D340" s="9"/>
       <c r="E340" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F340" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H340" s="8">
-        <v>1.1000000000000001</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="341" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D341" s="9"/>
       <c r="E341" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F341" s="9" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H341" s="8">
-        <v>3.2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="342" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D342" s="9"/>
       <c r="E342" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="F342" s="9" t="s">
-        <v>152</v>
+        <v>23</v>
       </c>
       <c r="H342" s="8">
-        <v>0.11</v>
+        <v>500820</v>
       </c>
     </row>
     <row r="343" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D343" s="9"/>
-      <c r="E343" t="s">
-        <v>157</v>
-      </c>
-      <c r="F343" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="H343" s="8">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="344" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D344" s="9"/>
-      <c r="E344" t="s">
-        <v>147</v>
-      </c>
-      <c r="F344" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H344" s="8">
-        <v>500820</v>
-      </c>
-    </row>
-    <row r="345" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D345" s="9"/>
+    </row>
+    <row r="344" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B344" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D344" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E344" s="1"/>
+      <c r="F344" s="1"/>
+      <c r="G344" s="1"/>
+      <c r="H344" s="3"/>
+      <c r="I344" s="13" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="345" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B345" s="1"/>
+      <c r="C345" s="1"/>
+      <c r="D345" s="10"/>
+      <c r="E345" s="1"/>
+      <c r="F345" s="1"/>
+      <c r="G345" s="1"/>
+      <c r="H345" s="12"/>
+      <c r="I345" s="13"/>
     </row>
     <row r="346" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B346" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C346" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D346" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E346" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C346" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D346" s="10" t="s">
+      <c r="F346" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G346" s="1"/>
+      <c r="H346" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="E346" s="1"/>
-      <c r="F346" s="1"/>
-      <c r="G346" s="1"/>
-      <c r="H346" s="3"/>
-      <c r="I346" s="13" t="s">
+      <c r="I346" s="7" t="s">
         <v>76</v>
       </c>
     </row>
@@ -5379,31 +5369,25 @@
       <c r="E347" s="1"/>
       <c r="F347" s="1"/>
       <c r="G347" s="1"/>
-      <c r="H347" s="12"/>
+      <c r="H347" s="3"/>
       <c r="I347" s="13"/>
     </row>
     <row r="348" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B348" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D348" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E348" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F348" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="E348" s="1"/>
+      <c r="F348" s="1"/>
       <c r="G348" s="1"/>
-      <c r="H348" s="3" t="s">
-        <v>79</v>
-      </c>
+      <c r="H348" s="3"/>
       <c r="I348" s="7" t="s">
-        <v>80</v>
+        <v>40</v>
       </c>
     </row>
     <row r="349" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5418,20 +5402,26 @@
     </row>
     <row r="350" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B350" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C350" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D350" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E350" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C350" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D350" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="E350" s="1"/>
-      <c r="F350" s="1"/>
+      <c r="F350" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="G350" s="1"/>
-      <c r="H350" s="3"/>
+      <c r="H350" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="I350" s="7" t="s">
-        <v>40</v>
+        <v>76</v>
       </c>
     </row>
     <row r="351" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5446,113 +5436,85 @@
     </row>
     <row r="352" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B352" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="D352" s="10" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E352" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="F352" s="10" t="s">
-        <v>13</v>
+        <v>80</v>
+      </c>
+      <c r="F352" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="G352" s="1"/>
       <c r="H352" s="3" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="I352" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="353" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="353" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B353" s="1"/>
       <c r="C353" s="1"/>
       <c r="D353" s="10"/>
-      <c r="E353" s="1"/>
-      <c r="F353" s="1"/>
+      <c r="E353" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F353" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G353" s="1"/>
-      <c r="H353" s="3"/>
-      <c r="I353" s="13"/>
-    </row>
-    <row r="354" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B354" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C354" s="1" t="s">
-        <v>244</v>
-      </c>
-      <c r="D354" s="10" t="s">
+      <c r="H353" s="3" t="s">
         <v>83</v>
       </c>
+      <c r="I353" s="1"/>
+    </row>
+    <row r="354" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B354" s="1"/>
+      <c r="C354" s="1"/>
+      <c r="D354" s="10"/>
       <c r="E354" s="1" t="s">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="F354" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G354" s="1"/>
+      <c r="G354" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="H354" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I354" s="7" t="s">
-        <v>85</v>
-      </c>
+      <c r="I354" s="1"/>
     </row>
     <row r="355" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B355" s="1"/>
       <c r="C355" s="1"/>
       <c r="D355" s="10"/>
       <c r="E355" s="1" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="F355" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G355" s="1"/>
-      <c r="H355" s="3" t="s">
-        <v>87</v>
+      <c r="G355" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H355" s="3">
+        <v>20200331</v>
       </c>
       <c r="I355" s="1"/>
     </row>
     <row r="356" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B356" s="1"/>
-      <c r="C356" s="1"/>
-      <c r="D356" s="10"/>
-      <c r="E356" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F356" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G356" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H356" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I356" s="1"/>
+      <c r="D356" s="9"/>
     </row>
     <row r="357" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B357" s="1"/>
-      <c r="C357" s="1"/>
-      <c r="D357" s="10"/>
-      <c r="E357" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F357" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G357" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H357" s="3">
-        <v>20200331</v>
-      </c>
-      <c r="I357" s="1"/>
+      <c r="D357" s="9"/>
     </row>
     <row r="358" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D358" s="9"/>
@@ -5607,12 +5569,6 @@
     </row>
     <row r="375" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D375" s="9"/>
-    </row>
-    <row r="376" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D376" s="9"/>
-    </row>
-    <row r="377" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D377" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Change api name AddPledgeRequest to Request_Post_PledgeForMargin
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -219,9 +219,6 @@
   </si>
   <si>
     <t>GetCurrentPledgeRequest</t>
-  </si>
-  <si>
-    <t>AddPledgeRequest</t>
   </si>
   <si>
     <t>quantity</t>
@@ -1014,7 +1011,10 @@
     <t>[ { "securities_Code": "531518 ", "securities_Name": "VIKASGRAN", "securities_ISIN": "INE767B01022", "holding_Rate": 2, "holding_Qty": 300, "holding_Value": 600, "hairCut": 24.29, "netValue": 453, "request_Qty": 300, "request_Value": 600 }, { "securities_Code": "542655 ", "securities_Name": "VIKASMCORP", "securities_ISIN": "INE161L01027", "holding_Rate": 3.47, "holding_Qty": 210, "holding_Value": 728.7, "hairCut": 25.15, "netValue": 546, "request_Qty": 210, "request_Value": 728.7 }, { "securities_Code": "519307 ", "securities_Name": "VIKASWSP", "securities_ISIN": "INE706A01022", "holding_Rate": 3.6, "holding_Qty": 100, "holding_Value": 360, "hairCut": 26.34, "netValue": 265, "request_Qty": 100, "request_Value": 360 }, { "securities_Code": "533295 ", "securities_Name": "PSB", "securities_ISIN": "INE608A01012", "holding_Rate": 16, "holding_Qty": 60, "holding_Value": 960, "hairCut": 19.36, "netValue": 774, "request_Qty": 60, "request_Value": 960 }, { "securities_Code": "531307 ", "securities_Name": "RRILLTD", "securities_ISIN": "INE951M01037", "holding_Rate": 13.49, "holding_Qty": 18, "holding_Value": 242.82, "hairCut": 21.98, "netValue": 189.36, "request_Qty": 18, "request_Value": 242.82 }, { "securities_Code": "526371 ", "securities_Name": "NMDC", "securities_ISIN": "INE584A01023", "holding_Rate": 134.9, "holding_Qty": 3, "holding_Value": 404.70000000000005, "hairCut": 17.11, "netValue": 335.46, "request_Qty": 6, "request_Value": 809.4000000000001 }, { "securities_Code": "500288 ", "securities_Name": "MOREPENLAB", "securities_ISIN": "INE083A01026", "holding_Rate": 55.35, "holding_Qty": 6, "holding_Value": 332.1, "hairCut": 25.28, "netValue": 248.16, "request_Qty": 6, "request_Value": 332.1 }, { "securities_Code": "526650 ", "securities_Name": "TFCILTD", "securities_ISIN": "INE305A01015", "holding_Rate": 59.6, "holding_Qty": 3, "holding_Value": 178.8, "hairCut": 19.71, "netValue": 143.55, "request_Qty": 6, "request_Value": 357.6 }, { "securities_Code": "500188 ", "securities_Name": "HINDZINC", "securities_ISIN": "INE267A01025", "holding_Rate": 315.1, "holding_Qty": 3, "holding_Value": 945.3000000000001, "hairCut": 14.8, "netValue": 805.41, "request_Qty": 3, "request_Value": 945.3000000000001 }, { "securities_Code": "534816 ", "securities_Name": "INDUSTOWER", "securities_ISIN": "INE121J01017", "holding_Rate": 253.3, "holding_Qty": 3, "holding_Value": 759.9000000000001, "hairCut": 19.25, "netValue": 613.62, "request_Qty": 3, "request_Value": 759.9000000000001 }, { "securities_Code": "532872 ", "securities_Name": "SPARC", "securities_ISIN": "INE232I01014", "holding_Rate": 250.7, "holding_Qty": 3, "holding_Value": 752.0999999999999, "hairCut": 19.58, "netValue": 604.83, "request_Qty": 3, "request_Value": 752.0999999999999 }, { "securities_Code": "532898 ", "securities_Name": "POWERGRID", "securities_ISIN": "INE752E01010", "holding_Rate": 208.4, "holding_Qty": 3, "holding_Value": 625.2, "hairCut": 11.63, "netValue": 552.48, "request_Qty": 3, "request_Value": 625.2 }, { "securities_Code": "500086 ", "securities_Name": "EXIDEIND", "securities_ISIN": "INE302A01020", "holding_Rate": 164.35, "holding_Qty": 3, "holding_Value": 493.04999999999995, "hairCut": 10.78, "netValue": 439.89, "request_Qty": 3, "request_Value": 493.04999999999995 }, { "securities_Code": "540065 ", "securities_Name": "RBLBANK", "securities_ISIN": "INE976G01028", "holding_Rate": 177.95, "holding_Qty": 3, "holding_Value": 533.8499999999999, "hairCut": 21.51, "netValue": 419.01, "request_Qty": 3, "request_Value": 533.8499999999999 }, { "securities_Code": "511676 ", "securities_Name": "GICHSGFIN", "securities_ISIN": "INE289B01019", "holding_Rate": 145.2, "holding_Qty": 3, "holding_Value": 435.59999999999997, "hairCut": 19.33, "netValue": 351.39, "request_Qty": 3, "request_Value": 435.59999999999997 }, { "securities_Code": "532955 ", "securities_Name": "RECLTD", "securities_ISIN": "INE020B01018", "holding_Rate": 132.55, "holding_Qty": 3, "holding_Value": 397.65000000000003, "hairCut": 13.91, "netValue": 342.33, "request_Qty": 3, "request_Value": 397.65000000000003 }, { "securities_Code": "330179 ", "securities_Name": "AHLADA", "securities_ISIN": "INE00PV01013", "holding_Rate": 127.6, "holding_Qty": 3, "holding_Value": 382.79999999999995, "hairCut": 18.23, "netValue": 313.02, "request_Qty": 3, "request_Value": 382.79999999999995 }, { "securities_Code": "532522 ", "securities_Name": "PETRONET", "securities_ISIN": "INE347G01014", "holding_Rate": 218.7, "holding_Qty": 2, "holding_Value": 437.4, "hairCut": 10.29, "netValue": 392.4, "request_Qty": 2, "request_Value": 437.4 }, { "securities_Code": "500260 ", "securities_Name": "RAMCOCEM", "securities_ISIN": "INE331A01037", "holding_Rate": 997, "holding_Qty": 1, "holding_Value": 997, "hairCut": 11.86, "netValue": 878.76, "request_Qty": 1, "request_Value": 997 }, { "securities_Code": "517385 ", "securities_Name": "SYMPHONY", "securities_ISIN": "INE225D01027", "holding_Rate": 1006.55, "holding_Qty": 1, "holding_Value": 1006.55, "hairCut": 13.78, "netValue": 867.85, "request_Qty": 1, "request_Value": 1006.55 }, { "securities_Code": "500770 ", "securities_Name": "TATACHEM", "securities_ISIN": "INE092A01019", "holding_Rate": 885.45, "holding_Qty": 1, "holding_Value": 885.45, "hairCut": 15.98, "netValue": 743.96, "request_Qty": 1, "request_Value": 885.45 }, { "securities_Code": "500520 ", "securities_Name": "M&amp;M", "securities_ISIN": "INE101A01026", "holding_Rate": 826.65, "holding_Qty": 1, "holding_Value": 826.65, "hairCut": 13.45, "netValue": 715.47, "request_Qty": 1, "request_Value": 826.65 }, { "securities_Code": "532174 ", "securities_Name": "ICICIBANK", "securities_ISIN": "INE090A01021", "holding_Rate": 731, "holding_Qty": 1, "holding_Value": 731, "hairCut": 14.38, "netValue": 625.88, "request_Qty": 1, "request_Value": 731 }, { "securities_Code": "505192 ", "securities_Name": "SMLISUZU", "securities_ISIN": "INE294B01019", "holding_Rate": 646.4, "holding_Qty": 1, "holding_Value": 646.4, "hairCut": 20.13, "netValue": 516.28, "request_Qty": 1, "request_Value": 646.4 }, { "securities_Code": "532967 ", "securities_Name": "KIRIINDUS", "securities_ISIN": "INE415I01015", "holding_Rate": 471.75, "holding_Qty": 1, "holding_Value": 471.75, "hairCut": 20.08, "netValue": 377.02, "request_Qty": 1, "request_Value": 471.75 }, { "securities_Code": "530803 ", "securities_Name": "BHAGERIA", "securities_ISIN": "INE354C01027", "holding_Rate": 249.5, "holding_Qty": 1, "holding_Value": 249.5, "hairCut": 18.98, "netValue": 202.14, "request_Qty": 1, "request_Value": 249.5 }, { "securities_Code": "522205 ", "securities_Name": "PRAJIND", "securities_ISIN": "INE074A01025", "holding_Rate": 307.2, "holding_Qty": 512, "holding_Value": 157286.4, "hairCut": 20.59, "netValue": 124902.4, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "330039 ", "securities_Name": "CDSL", "securities_ISIN": "INE736A01011", "holding_Rate": 1492.9, "holding_Qty": 71, "holding_Value": 105995.90000000001, "hairCut": 17.75, "netValue": 87181.61, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "524558 ", "securities_Name": "NEULANDLAB", "securities_ISIN": "INE794A01010", "holding_Rate": 1587.15, "holding_Qty": 15, "holding_Value": 23807.25, "hairCut": 21.98, "netValue": 18574.35, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "532648 ", "securities_Name": "YESBANK", "securities_ISIN": "INE528G01035", "holding_Rate": 13.58, "holding_Qty": 300, "holding_Value": 4074, "hairCut": 29, "netValue": 2892, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "532822 ", "securities_Name": "IDEA", "securities_ISIN": "INE669E01016", "holding_Rate": 13.79, "holding_Qty": 180, "holding_Value": 2482.2, "hairCut": 38.4, "netValue": 1528.2, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "505537 ", "securities_Name": "ZEEL", "securities_ISIN": "INE256A01028", "holding_Rate": 338.1, "holding_Qty": 6, "holding_Value": 2028.6000000000001, "hairCut": 27.23, "netValue": 1476.24, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500570 ", "securities_Name": "TATAMOTORS", "securities_ISIN": "INE155A01022", "holding_Rate": 472.35, "holding_Qty": 3, "holding_Value": 1417.0500000000002, "hairCut": 21.17, "netValue": 1117.05, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "512573 ", "securities_Name": "AVANTIFEED", "securities_ISIN": "INE871C01038", "holding_Rate": 547.95, "holding_Qty": 2, "holding_Value": 1095.9, "hairCut": 15.1, "netValue": 930.42, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500257 ", "securities_Name": "LUPIN", "securities_ISIN": "INE326A01037", "holding_Rate": 912.25, "holding_Qty": 1, "holding_Value": 912.25, "hairCut": 13.01, "netValue": 793.57, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "533278 ", "securities_Name": "COALINDIA", "securities_ISIN": "INE522F01014", "holding_Rate": 147.7, "holding_Qty": 6, "holding_Value": 886.1999999999999, "hairCut": 13.06, "netValue": 770.46, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "541153 ", "securities_Name": "BANDHANBNK", "securities_ISIN": "INE545U01014", "holding_Rate": 258.9, "holding_Qty": 3, "holding_Value": 776.6999999999999, "hairCut": 20.63, "netValue": 616.47, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500228 ", "securities_Name": "JSWSTEEL", "securities_ISIN": "INE019A01038", "holding_Rate": 649.65, "holding_Qty": 1, "holding_Value": 649.65, "hairCut": 15.86, "netValue": 546.62, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "517334 ", "securities_Name": "MOTHERSUMI", "securities_ISIN": "INE775A01035", "holding_Rate": 214.4, "holding_Qty": 3, "holding_Value": 643.2, "hairCut": 19.16, "netValue": 519.96, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500096 ", "securities_Name": "DABUR", "securities_ISIN": "INE016A01026", "holding_Rate": 569.65, "holding_Qty": 1, "holding_Value": 569.65, "hairCut": 9, "netValue": 518.38, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500850 ", "securities_Name": "INDHOTEL", "securities_ISIN": "INE053A01029", "holding_Rate": 180.45, "holding_Qty": 3, "holding_Value": 541.3499999999999, "hairCut": 18.3, "netValue": 442.29, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "500477 ", "securities_Name": "ASHOKLEY", "securities_ISIN": "INE208A01029", "holding_Rate": 125.8, "holding_Qty": 3, "holding_Value": 377.4, "hairCut": 17.79, "netValue": 310.26, "request_Qty": 0, "request_Value": 0 }, { "securities_Code": "532461 ", "securities_Name": "PNB", "securities_ISIN": "INE160A01022", "holding_Rate": 38, "holding_Qty": 9, "holding_Value": 342, "hairCut": 17.35, "netValue": 282.69, "request_Qty": 0, "request_Value": 0 } ]</t>
   </si>
   <si>
-    <t>securities_Code</t>
+    <t>Request_Post_PledgeForMargin</t>
+  </si>
+  <si>
+    <t>ScripCode</t>
   </si>
 </sst>
 </file>
@@ -1517,13 +1517,13 @@
     </row>
     <row r="2" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -1549,13 +1549,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1566,10 +1566,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1589,10 +1589,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1604,7 +1604,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1627,10 +1627,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1650,10 +1650,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1668,13 +1668,13 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1685,10 +1685,10 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1703,7 +1703,7 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D17" s="9"/>
       <c r="E17" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
@@ -1712,7 +1712,7 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D18" s="9"/>
       <c r="E18" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
@@ -1721,7 +1721,7 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D19" s="9"/>
       <c r="E19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -1735,13 +1735,13 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>241</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1752,49 +1752,49 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E23" s="11" t="s">
-        <v>121</v>
-      </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
       <c r="H23" t="s">
+        <v>156</v>
+      </c>
+      <c r="I23" t="s">
         <v>157</v>
-      </c>
-      <c r="I23" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D24" s="9"/>
       <c r="H24" t="s">
+        <v>158</v>
+      </c>
+      <c r="I24" t="s">
         <v>159</v>
-      </c>
-      <c r="I24" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="9"/>
       <c r="H25" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25" t="s">
         <v>161</v>
-      </c>
-      <c r="I25" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="9"/>
       <c r="H26" t="s">
+        <v>162</v>
+      </c>
+      <c r="I26" t="s">
         <v>163</v>
-      </c>
-      <c r="I26" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -1806,10 +1806,10 @@
         <v>9</v>
       </c>
       <c r="H27" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I27" s="18" t="s">
         <v>165</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -1821,10 +1821,10 @@
         <v>9</v>
       </c>
       <c r="H28" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="I28" s="19" t="s">
         <v>167</v>
-      </c>
-      <c r="I28" s="19" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -1835,10 +1835,10 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1850,10 +1850,10 @@
         <v>16</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
@@ -1868,7 +1868,7 @@
         <v>16</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
@@ -1878,49 +1878,49 @@
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D33" s="9"/>
       <c r="E33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F33" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D34" s="9"/>
       <c r="G34" s="20"/>
       <c r="H34" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D35" s="9"/>
       <c r="G35" s="20"/>
       <c r="H35" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D36" s="9"/>
       <c r="G36" s="20"/>
       <c r="H36" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D37" s="9"/>
       <c r="G37" s="20"/>
       <c r="H37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D38" s="9"/>
       <c r="G38" s="20"/>
       <c r="H38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
@@ -1930,25 +1930,25 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D40" s="9"/>
       <c r="E40" t="s">
+        <v>174</v>
+      </c>
+      <c r="F40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H40" t="s">
         <v>175</v>
-      </c>
-      <c r="F40" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D41" s="9"/>
       <c r="H41" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D42" s="9"/>
       <c r="H42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -1959,58 +1959,58 @@
         <v>46</v>
       </c>
       <c r="C44" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E44" t="s">
+        <v>178</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="F44" t="s">
-        <v>9</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>180</v>
-      </c>
       <c r="I44" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D45" s="9"/>
       <c r="I45" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D46" s="9"/>
       <c r="I46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D47" s="9"/>
       <c r="I47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D48" s="9"/>
       <c r="I48" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D49" s="9"/>
       <c r="I49" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D50" s="9"/>
       <c r="I50" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2021,22 +2021,22 @@
         <v>46</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D52" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="E52" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="E52" s="9" t="s">
-        <v>185</v>
-      </c>
       <c r="F52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H52" t="s">
+        <v>272</v>
+      </c>
+      <c r="I52" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="I52" s="7" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -2064,46 +2064,46 @@
         <v>38</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D56" s="9"/>
       <c r="I56" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D57" s="9"/>
       <c r="I57" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D58" s="9"/>
       <c r="I58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D59" s="9"/>
       <c r="I59" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D60" s="9"/>
       <c r="I60" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D61" s="9"/>
       <c r="I61" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
@@ -2117,55 +2117,55 @@
         <v>38</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E63" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D64" s="9"/>
       <c r="I64" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D65" s="9"/>
       <c r="I65" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D66" s="9"/>
       <c r="I66" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" s="9"/>
       <c r="I67" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D68" s="9"/>
       <c r="I68" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D69" s="9"/>
       <c r="I69" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
@@ -2179,10 +2179,10 @@
         <v>38</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
@@ -2196,10 +2196,10 @@
         <v>38</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="E73" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F73" t="s">
         <v>23</v>
@@ -2208,7 +2208,7 @@
         <v>1202870000086520</v>
       </c>
       <c r="I73" s="26" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
@@ -2222,10 +2222,10 @@
         <v>38</v>
       </c>
       <c r="D75" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="E75" t="s">
         <v>252</v>
-      </c>
-      <c r="E75" t="s">
-        <v>253</v>
       </c>
       <c r="F75" t="s">
         <v>23</v>
@@ -2234,7 +2234,7 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D76" s="9"/>
       <c r="E76" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F76" t="s">
         <v>23</v>
@@ -2251,10 +2251,10 @@
         <v>38</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I78" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
@@ -2315,13 +2315,13 @@
         <v>26</v>
       </c>
       <c r="C84" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
@@ -2332,13 +2332,13 @@
         <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D86" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="E86" t="s">
         <v>256</v>
-      </c>
-      <c r="E86" t="s">
-        <v>257</v>
       </c>
       <c r="F86" t="s">
         <v>23</v>
@@ -2347,7 +2347,7 @@
         <v>28</v>
       </c>
       <c r="I86" s="26" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
@@ -2358,7 +2358,7 @@
         <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>29</v>
@@ -2397,22 +2397,22 @@
         <v>26</v>
       </c>
       <c r="C91" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D91" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="E91" t="s">
         <v>258</v>
       </c>
-      <c r="E91" t="s">
-        <v>259</v>
-      </c>
       <c r="F91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I91" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
@@ -2424,28 +2424,28 @@
         <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D93" s="9" t="s">
+        <v>259</v>
+      </c>
+      <c r="E93" t="s">
         <v>260</v>
       </c>
-      <c r="E93" t="s">
-        <v>261</v>
-      </c>
       <c r="F93" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I93" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D94" s="9"/>
       <c r="E94" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>9</v>
@@ -2463,13 +2463,13 @@
         <v>26</v>
       </c>
       <c r="C96" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E96" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>9</v>
@@ -2479,7 +2479,7 @@
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D97" s="9"/>
       <c r="E97" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>9</v>
@@ -2489,7 +2489,7 @@
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D98" s="9"/>
       <c r="E98" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>9</v>
@@ -2507,13 +2507,13 @@
         <v>26</v>
       </c>
       <c r="C100" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E100" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>9</v>
@@ -2523,7 +2523,7 @@
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D101" s="9"/>
       <c r="E101" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>9</v>
@@ -2539,34 +2539,34 @@
         <v>20</v>
       </c>
       <c r="C103" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E103" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H103" s="30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="I103" s="31" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D104" s="9"/>
       <c r="E104" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H104" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
@@ -2577,13 +2577,13 @@
         <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E106" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>9</v>
@@ -2593,7 +2593,7 @@
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D107" s="9"/>
       <c r="E107" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>9</v>
@@ -2603,7 +2603,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>9</v>
@@ -2613,7 +2613,7 @@
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D109" s="9"/>
       <c r="E109" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>9</v>
@@ -2623,7 +2623,7 @@
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D110" s="9"/>
       <c r="E110" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>9</v>
@@ -2633,7 +2633,7 @@
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D111" s="9"/>
       <c r="E111" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>9</v>
@@ -2648,31 +2648,31 @@
         <v>34</v>
       </c>
       <c r="C113" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F113" t="s">
         <v>9</v>
       </c>
       <c r="H113" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="I113" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D114" s="9"/>
       <c r="H114" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I114" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
@@ -2684,10 +2684,10 @@
         <v>9</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I115" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
@@ -2699,28 +2699,28 @@
         <v>9</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I116" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D117" s="9"/>
       <c r="I117" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D118" s="9"/>
       <c r="I118" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D119" s="9"/>
       <c r="I119" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
@@ -2731,49 +2731,49 @@
         <v>34</v>
       </c>
       <c r="C121" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F121" t="s">
         <v>9</v>
       </c>
       <c r="H121" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="I121" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D122" s="9"/>
       <c r="H122" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="I122" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D123" s="9"/>
       <c r="H123" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="I123" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D124" s="9"/>
       <c r="H124" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I124" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
@@ -2785,10 +2785,10 @@
         <v>9</v>
       </c>
       <c r="H125" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I125" s="19" t="s">
         <v>165</v>
-      </c>
-      <c r="I125" s="19" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.3">
@@ -2800,16 +2800,16 @@
         <v>9</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I126" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D127" s="9"/>
       <c r="I127" s="22" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
@@ -2820,49 +2820,49 @@
         <v>34</v>
       </c>
       <c r="C129" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E129" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="F129" t="s">
+        <v>9</v>
+      </c>
+      <c r="H129" t="s">
         <v>214</v>
       </c>
-      <c r="F129" t="s">
-        <v>9</v>
-      </c>
-      <c r="H129" t="s">
+      <c r="I129" s="23" t="s">
         <v>215</v>
-      </c>
-      <c r="I129" s="23" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D130" s="9"/>
       <c r="H130" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D131" s="9"/>
       <c r="H131" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I131" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D132" s="9"/>
       <c r="H132" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="I132" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.3">
@@ -2874,10 +2874,10 @@
         <v>9</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I133" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.3">
@@ -2889,22 +2889,22 @@
         <v>9</v>
       </c>
       <c r="H134" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I134" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D135" s="9"/>
       <c r="I135" s="19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D136" s="9"/>
       <c r="I136" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
@@ -2913,49 +2913,49 @@
     <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D138" s="9"/>
       <c r="I138" s="23" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D139" s="9"/>
       <c r="I139" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D140" s="9"/>
       <c r="I140" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D141" s="9"/>
       <c r="I141" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
       <c r="I142" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D143" s="9"/>
       <c r="I143" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D144" s="9"/>
       <c r="I144" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D145" s="9"/>
       <c r="I145" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
@@ -2964,16 +2964,16 @@
     </row>
     <row r="147" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C147" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D147" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="I147" s="7" t="s">
         <v>195</v>
-      </c>
-      <c r="I147" s="7" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.3">
@@ -2984,7 +2984,7 @@
         <v>50</v>
       </c>
       <c r="C149" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D149" s="9" t="s">
         <v>51</v>
@@ -3013,22 +3013,22 @@
         <v>50</v>
       </c>
       <c r="C152" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D152" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="E152" t="s">
         <v>197</v>
-      </c>
-      <c r="E152" t="s">
-        <v>198</v>
       </c>
       <c r="F152" t="s">
         <v>23</v>
       </c>
       <c r="H152" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I152" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.3">
@@ -3049,13 +3049,13 @@
     <row r="154" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D154" s="9"/>
       <c r="E154" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F154" t="s">
         <v>23</v>
       </c>
       <c r="H154" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.3">
@@ -3066,7 +3066,7 @@
         <v>50</v>
       </c>
       <c r="C156" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D156" s="10" t="s">
         <v>56</v>
@@ -3148,10 +3148,10 @@
         <v>50</v>
       </c>
       <c r="C162" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E162" s="10" t="s">
         <v>52</v>
@@ -3164,7 +3164,7 @@
         <v>53</v>
       </c>
       <c r="I162" s="26" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.3">
@@ -3215,7 +3215,7 @@
         <v>50</v>
       </c>
       <c r="C167" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D167" s="10" t="s">
         <v>60</v>
@@ -3236,20 +3236,20 @@
     </row>
     <row r="170" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B170" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C170" t="s">
+        <v>236</v>
+      </c>
+      <c r="D170" s="10" t="s">
         <v>84</v>
-      </c>
-      <c r="C170" t="s">
-        <v>237</v>
-      </c>
-      <c r="D170" s="10" t="s">
-        <v>85</v>
       </c>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
       <c r="G170" s="1"/>
       <c r="H170" s="3"/>
       <c r="I170" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.3">
@@ -3257,26 +3257,26 @@
     </row>
     <row r="172" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B172" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C172" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D172" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E172" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F172" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G172" s="1"/>
       <c r="H172" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I172" s="7" t="s">
         <v>89</v>
-      </c>
-      <c r="I172" s="7" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.3">
@@ -3284,14 +3284,14 @@
       <c r="C173" s="1"/>
       <c r="D173" s="10"/>
       <c r="E173" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F173" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G173" s="1"/>
       <c r="H173" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I173" s="1"/>
     </row>
@@ -3300,16 +3300,16 @@
     </row>
     <row r="175" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B175" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C175" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E175" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F175" s="1" t="s">
         <v>9</v>
@@ -3319,7 +3319,7 @@
         <v>53</v>
       </c>
       <c r="I175" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.3">
@@ -3327,14 +3327,14 @@
       <c r="C176" s="1"/>
       <c r="D176" s="10"/>
       <c r="E176" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G176" s="1"/>
       <c r="H176" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I176" s="1"/>
     </row>
@@ -3343,7 +3343,7 @@
       <c r="C177" s="1"/>
       <c r="D177" s="10"/>
       <c r="E177" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>9</v>
@@ -3395,13 +3395,13 @@
     </row>
     <row r="181" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B181" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C181" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D181" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E181" s="1" t="s">
         <v>32</v>
@@ -3411,10 +3411,10 @@
       </c>
       <c r="G181" s="1"/>
       <c r="H181" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I181" s="7" t="s">
         <v>97</v>
-      </c>
-      <c r="I181" s="7" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.3">
@@ -3422,14 +3422,14 @@
       <c r="C182" s="1"/>
       <c r="D182" s="10"/>
       <c r="E182" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G182" s="1"/>
       <c r="H182" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I182" s="1"/>
     </row>
@@ -3472,21 +3472,21 @@
     <row r="185" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D185" s="9"/>
       <c r="F185" s="10" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="186" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B186" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C186" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D186" s="10" t="s">
+        <v>285</v>
+      </c>
+      <c r="I186" s="26" t="s">
         <v>286</v>
-      </c>
-      <c r="I186" s="26" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="187" spans="2:9" x14ac:dyDescent="0.3">
@@ -3494,25 +3494,25 @@
     </row>
     <row r="188" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B188" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C188" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D188" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="E188" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="E188" s="11" t="s">
-        <v>289</v>
-      </c>
       <c r="F188" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H188" t="s">
+        <v>290</v>
+      </c>
+      <c r="I188" s="26" t="s">
         <v>291</v>
-      </c>
-      <c r="I188" s="26" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="189" spans="2:9" x14ac:dyDescent="0.3">
@@ -3532,25 +3532,25 @@
     </row>
     <row r="191" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B191" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C191" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D191" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E191" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F191" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H191" t="s">
+        <v>290</v>
+      </c>
+      <c r="I191" s="26" t="s">
         <v>291</v>
-      </c>
-      <c r="I191" s="26" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.3">
@@ -3559,43 +3559,43 @@
     <row r="193" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D193" s="9"/>
       <c r="H193" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="I193" s="26"/>
     </row>
     <row r="194" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B194" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C194" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E194" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F194" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H194" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I194" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D195" s="9"/>
       <c r="H195" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="196" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D196" s="9"/>
       <c r="H196" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.3">
@@ -3603,110 +3603,110 @@
     </row>
     <row r="198" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B198" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C198" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D198" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H198" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="199" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E199" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H199" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H200" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H201" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B203" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C203" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D203" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H203" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E204" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H204" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H205" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H206" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B208" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C208" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D208" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H208" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="209" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D209" s="9"/>
       <c r="E209" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H209" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="210" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D210" s="9"/>
       <c r="H210" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D211" s="9"/>
       <c r="H211" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="212" spans="2:8" x14ac:dyDescent="0.3">
@@ -3714,23 +3714,23 @@
     </row>
     <row r="213" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B213" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C213" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D213" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="E213" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="E213" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="F213" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G213" s="8"/>
       <c r="H213" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="214" spans="2:8" x14ac:dyDescent="0.3">
@@ -3772,7 +3772,7 @@
       <c r="C216" s="8"/>
       <c r="D216" s="32"/>
       <c r="E216" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F216" s="8" t="s">
         <v>23</v>
@@ -3793,7 +3793,7 @@
     <row r="218" spans="2:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D218" s="9"/>
       <c r="H218" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.3">
@@ -3804,13 +3804,13 @@
     </row>
     <row r="221" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B221" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D221" s="32" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E221" s="33" t="s">
         <v>32</v>
@@ -3820,18 +3820,18 @@
       </c>
       <c r="G221" s="8"/>
       <c r="H221" s="32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="222" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D222" s="9"/>
       <c r="E222" s="8"/>
       <c r="F222" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G222" s="8"/>
       <c r="H222" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="223" spans="2:8" x14ac:dyDescent="0.3">
@@ -3873,43 +3873,43 @@
     </row>
     <row r="226" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B226" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D226" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="H226" t="s">
+        <v>294</v>
+      </c>
+      <c r="I226" s="7" t="s">
         <v>311</v>
-      </c>
-      <c r="H226" t="s">
-        <v>295</v>
-      </c>
-      <c r="I226" s="7" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D227" s="9"/>
       <c r="E227" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F227" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H227" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D228" s="9"/>
       <c r="H228" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D229" s="9"/>
       <c r="H229" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="230" spans="2:9" x14ac:dyDescent="0.3">
@@ -3921,43 +3921,43 @@
     </row>
     <row r="231" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B231" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D231" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="H231" t="s">
+        <v>294</v>
+      </c>
+      <c r="I231" s="7" t="s">
         <v>313</v>
-      </c>
-      <c r="H231" t="s">
-        <v>295</v>
-      </c>
-      <c r="I231" s="7" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="232" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D232" s="9"/>
       <c r="E232" s="11" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H232" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="233" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D233" s="9"/>
       <c r="H233" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="234" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D234" s="9"/>
       <c r="H234" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="235" spans="2:9" x14ac:dyDescent="0.3">
@@ -3969,26 +3969,26 @@
     </row>
     <row r="236" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
       <c r="B236" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D236" s="34" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E236" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F236" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G236" s="8"/>
       <c r="H236" s="18" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="I236" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.3">
@@ -4024,7 +4024,7 @@
     <row r="239" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D239" s="9"/>
       <c r="E239" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="F239" s="8" t="s">
         <v>23</v>
@@ -4043,7 +4043,7 @@
     <row r="241" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D241" s="9"/>
       <c r="H241" s="18" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.3">
@@ -4055,13 +4055,13 @@
     </row>
     <row r="243" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B243" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C243" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D243" s="32" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E243" s="33" t="s">
         <v>32</v>
@@ -4071,18 +4071,18 @@
       </c>
       <c r="G243" s="8"/>
       <c r="H243" s="32" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="244" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D244" s="9"/>
       <c r="E244" s="8"/>
       <c r="F244" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G244" s="8"/>
       <c r="H244" s="18" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="245" spans="2:9" x14ac:dyDescent="0.3">
@@ -4124,13 +4124,13 @@
     </row>
     <row r="248" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B248" t="s">
+        <v>100</v>
+      </c>
+      <c r="C248" t="s">
+        <v>237</v>
+      </c>
+      <c r="D248" s="9" t="s">
         <v>101</v>
-      </c>
-      <c r="C248" t="s">
-        <v>238</v>
-      </c>
-      <c r="D248" s="9" t="s">
-        <v>102</v>
       </c>
       <c r="E248" t="s">
         <v>15</v>
@@ -4145,7 +4145,7 @@
         <v>20210401</v>
       </c>
       <c r="I248" s="7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="249" spans="2:9" x14ac:dyDescent="0.3">
@@ -4166,7 +4166,7 @@
     <row r="250" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D250" s="9"/>
       <c r="E250" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F250" t="s">
         <v>9</v>
@@ -4181,17 +4181,17 @@
     </row>
     <row r="252" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B252" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C252" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D252" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H252" s="6"/>
       <c r="I252" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="253" spans="2:9" x14ac:dyDescent="0.3">
@@ -4204,17 +4204,17 @@
     </row>
     <row r="255" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B255" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C255" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D255" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H255" s="6"/>
       <c r="I255" s="7" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="256" spans="2:9" x14ac:dyDescent="0.3">
@@ -4227,17 +4227,17 @@
     </row>
     <row r="258" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B258" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C258" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D258" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H258" s="6"/>
       <c r="I258" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="259" spans="2:9" x14ac:dyDescent="0.3">
@@ -4250,34 +4250,34 @@
     </row>
     <row r="261" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B261" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C261" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D261" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E261" t="s">
         <v>111</v>
       </c>
-      <c r="E261" t="s">
+      <c r="F261" t="s">
         <v>112</v>
-      </c>
-      <c r="F261" t="s">
-        <v>113</v>
       </c>
       <c r="H261" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I261" s="7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="262" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D262" s="9"/>
       <c r="E262" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F262" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H262" s="6" t="b">
         <v>1</v>
@@ -4289,16 +4289,16 @@
     </row>
     <row r="264" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B264" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C264" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D264" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E264" t="s">
         <v>116</v>
-      </c>
-      <c r="E264" t="s">
-        <v>117</v>
       </c>
       <c r="F264" t="s">
         <v>21</v>
@@ -4307,7 +4307,7 @@
         <v>3</v>
       </c>
       <c r="I264" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="265" spans="2:9" x14ac:dyDescent="0.3">
@@ -4318,7 +4318,7 @@
         <v>62</v>
       </c>
       <c r="C266" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D266" s="10" t="s">
         <v>63</v>
@@ -4346,7 +4346,7 @@
         <v>62</v>
       </c>
       <c r="C268" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D268" s="10" t="s">
         <v>65</v>
@@ -4374,13 +4374,13 @@
         <v>62</v>
       </c>
       <c r="C270" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D270" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="E270" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F270" s="10" t="s">
         <v>9</v>
@@ -4390,7 +4390,7 @@
         <v>66</v>
       </c>
       <c r="I270" s="26" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="271" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4408,7 +4408,7 @@
         <v>62</v>
       </c>
       <c r="C272" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D272" s="10" t="s">
         <v>67</v>
@@ -4433,13 +4433,13 @@
         <v>62</v>
       </c>
       <c r="C274" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D274" s="10" t="s">
-        <v>68</v>
+        <v>322</v>
       </c>
       <c r="E274" s="11" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F274" s="10" t="s">
         <v>9</v>
@@ -4473,7 +4473,7 @@
       <c r="C276" s="1"/>
       <c r="D276" s="10"/>
       <c r="E276" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F276" s="10" t="s">
         <v>9</v>
@@ -4492,7 +4492,7 @@
         <v>62</v>
       </c>
       <c r="C278" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D278" s="9" t="s">
         <v>62</v>
@@ -4507,7 +4507,7 @@
         <v>20191101</v>
       </c>
       <c r="I278" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
@@ -4515,13 +4515,13 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B280" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D280" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E280" t="s">
         <v>15</v>
@@ -4530,10 +4530,10 @@
         <v>9</v>
       </c>
       <c r="H280" s="35" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I280" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
@@ -4545,42 +4545,42 @@
         <v>9</v>
       </c>
       <c r="H281" s="35" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I281" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D282" s="9"/>
       <c r="H282" s="8"/>
       <c r="I282" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D283" s="9"/>
       <c r="H283" s="8"/>
       <c r="I283" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D284" s="9"/>
       <c r="I284" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D285" s="9"/>
       <c r="I285" s="19" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D286" s="9"/>
       <c r="I286" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.3">
@@ -4591,13 +4591,13 @@
         <v>36</v>
       </c>
       <c r="B288" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D288" s="10" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E288" s="1" t="s">
         <v>15</v>
@@ -4664,13 +4664,13 @@
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B292" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C292" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D292" s="9" t="s">
         <v>233</v>
-      </c>
-      <c r="C292" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D292" s="9" t="s">
-        <v>234</v>
       </c>
       <c r="E292" t="s">
         <v>27</v>
@@ -4679,10 +4679,10 @@
         <v>9</v>
       </c>
       <c r="H292" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="I292" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.3">
@@ -4694,10 +4694,10 @@
         <v>9</v>
       </c>
       <c r="H293" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="I293" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
@@ -4709,10 +4709,10 @@
         <v>9</v>
       </c>
       <c r="H294" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I294" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
@@ -4724,34 +4724,34 @@
         <v>9</v>
       </c>
       <c r="H295" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I295" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="296" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D296" s="9"/>
       <c r="I296" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="297" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D297" s="9"/>
       <c r="I297" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="298" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D298" s="9"/>
       <c r="I298" s="19" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="299" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D299" s="9"/>
       <c r="I299" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.3">
@@ -4759,13 +4759,13 @@
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B301" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C301" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D301" s="9" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E301" t="s">
         <v>27</v>
@@ -4774,10 +4774,10 @@
         <v>9</v>
       </c>
       <c r="H301" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="I301" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
@@ -4789,10 +4789,10 @@
         <v>9</v>
       </c>
       <c r="H302" s="17" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I302" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
@@ -4804,28 +4804,28 @@
         <v>9</v>
       </c>
       <c r="H303" s="17" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="I303" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D304" s="9"/>
       <c r="I304" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="305" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D305" s="9"/>
       <c r="I305" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="306" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D306" s="9"/>
       <c r="I306" s="25" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
@@ -4833,7 +4833,7 @@
       <c r="E307" s="24"/>
       <c r="H307" s="18"/>
       <c r="I307" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="308" spans="2:9" x14ac:dyDescent="0.3">
@@ -4841,13 +4841,13 @@
     </row>
     <row r="309" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B309" t="s">
+        <v>121</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D309" s="9" t="s">
         <v>122</v>
-      </c>
-      <c r="C309" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D309" s="9" t="s">
-        <v>123</v>
       </c>
       <c r="E309" t="s">
         <v>15</v>
@@ -4862,7 +4862,7 @@
         <v>20200401</v>
       </c>
       <c r="I309" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
@@ -4887,13 +4887,13 @@
     </row>
     <row r="312" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B312" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D312" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E312" t="s">
         <v>15</v>
@@ -4908,7 +4908,7 @@
         <v>20200401</v>
       </c>
       <c r="I312" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="313" spans="2:9" x14ac:dyDescent="0.3">
@@ -4929,49 +4929,49 @@
     <row r="314" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D314" s="9"/>
       <c r="E314" t="s">
+        <v>126</v>
+      </c>
+      <c r="F314" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H314" s="8" t="s">
         <v>127</v>
-      </c>
-      <c r="F314" s="9" t="s">
-        <v>113</v>
-      </c>
-      <c r="H314" s="8" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="315" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D315" s="9"/>
       <c r="E315" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F315" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H315" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="316" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D316" s="9"/>
       <c r="E316" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F316" s="9" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H316" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D317" s="9"/>
       <c r="E317" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F317" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H317" s="8" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.3">
@@ -4980,13 +4980,13 @@
     </row>
     <row r="319" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B319" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D319" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E319" t="s">
         <v>15</v>
@@ -5001,7 +5001,7 @@
         <v>20200401</v>
       </c>
       <c r="I319" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="320" spans="2:9" x14ac:dyDescent="0.3">
@@ -5022,19 +5022,19 @@
     <row r="321" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D321" s="9"/>
       <c r="E321" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F321" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H321" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="322" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D322" s="9"/>
       <c r="E322" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F322" s="9" t="s">
         <v>23</v>
@@ -5046,7 +5046,7 @@
     <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D323" s="9"/>
       <c r="E323" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F323" s="9" t="s">
         <v>23</v>
@@ -5061,13 +5061,13 @@
     </row>
     <row r="325" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B325" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C325" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D325" s="9" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E325" t="s">
         <v>15</v>
@@ -5082,7 +5082,7 @@
         <v>20200401</v>
       </c>
       <c r="I325" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="326" spans="2:9" x14ac:dyDescent="0.3">
@@ -5106,13 +5106,13 @@
     </row>
     <row r="328" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B328" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C328" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D328" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E328" t="s">
         <v>15</v>
@@ -5127,7 +5127,7 @@
         <v>20200401</v>
       </c>
       <c r="I328" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="329" spans="2:9" x14ac:dyDescent="0.3">
@@ -5148,7 +5148,7 @@
     <row r="330" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D330" s="9"/>
       <c r="E330" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F330" s="9" t="s">
         <v>23</v>
@@ -5163,13 +5163,13 @@
     </row>
     <row r="332" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B332" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C332" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D332" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E332" t="s">
         <v>22</v>
@@ -5184,7 +5184,7 @@
         <v>20220228</v>
       </c>
       <c r="I332" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="333" spans="2:9" x14ac:dyDescent="0.3">
@@ -5196,7 +5196,7 @@
         <v>23</v>
       </c>
       <c r="H333" s="8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="334" spans="2:9" x14ac:dyDescent="0.3">
@@ -5220,16 +5220,16 @@
         <v>23</v>
       </c>
       <c r="H335" s="8" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="336" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D336" s="9"/>
       <c r="E336" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F336" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H336" s="8">
         <v>4</v>
@@ -5238,10 +5238,10 @@
     <row r="337" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D337" s="9"/>
       <c r="E337" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F337" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H337" s="8">
         <v>48</v>
@@ -5250,10 +5250,10 @@
     <row r="338" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D338" s="9"/>
       <c r="E338" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F338" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H338" s="8">
         <v>1.1000000000000001</v>
@@ -5262,10 +5262,10 @@
     <row r="339" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D339" s="9"/>
       <c r="E339" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F339" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H339" s="8">
         <v>3.2</v>
@@ -5274,10 +5274,10 @@
     <row r="340" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D340" s="9"/>
       <c r="E340" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F340" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H340" s="8">
         <v>0.11</v>
@@ -5286,10 +5286,10 @@
     <row r="341" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D341" s="9"/>
       <c r="E341" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F341" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H341" s="8">
         <v>0.2</v>
@@ -5298,7 +5298,7 @@
     <row r="342" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D342" s="9"/>
       <c r="E342" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F342" s="9" t="s">
         <v>23</v>
@@ -5312,20 +5312,20 @@
     </row>
     <row r="344" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B344" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C344" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D344" s="10" t="s">
         <v>70</v>
-      </c>
-      <c r="C344" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="D344" s="10" t="s">
-        <v>71</v>
       </c>
       <c r="E344" s="1"/>
       <c r="F344" s="1"/>
       <c r="G344" s="1"/>
       <c r="H344" s="3"/>
       <c r="I344" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="345" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5340,26 +5340,26 @@
     </row>
     <row r="346" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B346" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C346" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D346" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="E346" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E346" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F346" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G346" s="1"/>
       <c r="H346" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I346" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="I346" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="347" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5374,13 +5374,13 @@
     </row>
     <row r="348" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B348" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C348" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D348" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E348" s="1"/>
       <c r="F348" s="1"/>
@@ -5402,26 +5402,26 @@
     </row>
     <row r="350" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B350" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D350" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E350" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F350" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G350" s="1"/>
       <c r="H350" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I350" s="7" t="s">
         <v>75</v>
-      </c>
-      <c r="I350" s="7" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="351" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5436,16 +5436,16 @@
     </row>
     <row r="352" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B352" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D352" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E352" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="E352" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="F352" s="1" t="s">
         <v>9</v>
@@ -5455,7 +5455,7 @@
         <v>14</v>
       </c>
       <c r="I352" s="7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="353" spans="2:9" x14ac:dyDescent="0.3">
@@ -5463,14 +5463,14 @@
       <c r="C353" s="1"/>
       <c r="D353" s="10"/>
       <c r="E353" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F353" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G353" s="1"/>
       <c r="H353" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I353" s="1"/>
     </row>

</xml_diff>

<commit_message>
Create api DigitalDocument_List, DigitalDocument_File
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="875" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="333">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -1030,6 +1030,18 @@
   </si>
   <si>
     <t>1528(Any Amount)</t>
+  </si>
+  <si>
+    <t>DigitalDocument_List</t>
+  </si>
+  <si>
+    <t>product</t>
+  </si>
+  <si>
+    <t>DigitalDocument_File</t>
+  </si>
+  <si>
+    <t>53.0'</t>
   </si>
 </sst>
 </file>
@@ -1498,10 +1510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I375"/>
+  <dimension ref="A1:I383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C347" workbookViewId="0">
-      <selection activeCell="I358" sqref="I358"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="H174" sqref="H174"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3225,412 +3237,439 @@
       <c r="F166" s="1"/>
       <c r="H166" s="3"/>
     </row>
-    <row r="167" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
         <v>50</v>
       </c>
       <c r="C167" t="s">
         <v>270</v>
       </c>
-      <c r="D167" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="E167" s="1"/>
-      <c r="F167" s="1"/>
-      <c r="G167" s="1"/>
-      <c r="H167" s="3"/>
-      <c r="I167" s="7" t="s">
-        <v>61</v>
+      <c r="D167" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="E167" s="10" t="s">
+        <v>330</v>
+      </c>
+      <c r="F167" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H167" s="14" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="168" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D168" s="9"/>
+      <c r="E168" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F168" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H168" s="3">
+        <v>20210101</v>
+      </c>
     </row>
     <row r="169" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D169" s="9"/>
-    </row>
-    <row r="170" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B170" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C170" t="s">
-        <v>236</v>
-      </c>
-      <c r="D170" s="10" t="s">
-        <v>84</v>
-      </c>
+      <c r="E169" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F169" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H169" s="3">
+        <v>20210101</v>
+      </c>
+    </row>
+    <row r="170" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D170" s="9"/>
       <c r="E170" s="1"/>
       <c r="F170" s="1"/>
-      <c r="G170" s="1"/>
       <c r="H170" s="3"/>
-      <c r="I170" s="7" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D171" s="9"/>
-    </row>
-    <row r="172" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B172" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C172" t="s">
-        <v>236</v>
-      </c>
-      <c r="D172" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E172" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F172" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G172" s="1"/>
-      <c r="H172" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="I172" s="7" t="s">
-        <v>89</v>
+      <c r="B171" t="s">
+        <v>50</v>
+      </c>
+      <c r="C171" t="s">
+        <v>270</v>
+      </c>
+      <c r="D171" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="E171" t="s">
+        <v>197</v>
+      </c>
+      <c r="F171" t="s">
+        <v>23</v>
+      </c>
+      <c r="H171" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="172" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D172" s="9"/>
+      <c r="E172" t="s">
+        <v>22</v>
+      </c>
+      <c r="F172" t="s">
+        <v>23</v>
+      </c>
+      <c r="G172" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H172">
+        <v>20210101</v>
       </c>
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B173" s="1"/>
-      <c r="C173" s="1"/>
-      <c r="D173" s="10"/>
-      <c r="E173" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F173" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G173" s="1"/>
-      <c r="H173" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I173" s="1"/>
+      <c r="D173" s="9"/>
+      <c r="E173" t="s">
+        <v>198</v>
+      </c>
+      <c r="F173" t="s">
+        <v>23</v>
+      </c>
+      <c r="H173" s="17" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D174" s="9"/>
+      <c r="E174" s="1"/>
+      <c r="F174" s="1"/>
+      <c r="H174" s="3"/>
     </row>
     <row r="175" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B175" s="1" t="s">
+      <c r="B175" t="s">
+        <v>50</v>
+      </c>
+      <c r="C175" t="s">
+        <v>270</v>
+      </c>
+      <c r="D175" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E175" s="1"/>
+      <c r="F175" s="1"/>
+      <c r="G175" s="1"/>
+      <c r="H175" s="3"/>
+      <c r="I175" s="7" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="176" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D176" s="9"/>
+    </row>
+    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D177" s="9"/>
+    </row>
+    <row r="178" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B178" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C175" t="s">
+      <c r="C178" t="s">
         <v>236</v>
       </c>
-      <c r="D175" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="E175" s="1" t="s">
+      <c r="D178" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="E178" s="1"/>
+      <c r="F178" s="1"/>
+      <c r="G178" s="1"/>
+      <c r="H178" s="3"/>
+      <c r="I178" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="179" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D179" s="9"/>
+    </row>
+    <row r="180" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B180" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C180" t="s">
+        <v>236</v>
+      </c>
+      <c r="D180" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="E180" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F175" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G175" s="1"/>
-      <c r="H175" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I175" s="7" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="176" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B176" s="1"/>
-      <c r="C176" s="1"/>
-      <c r="D176" s="10"/>
-      <c r="E176" s="1" t="s">
+      <c r="F180" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G180" s="1"/>
+      <c r="H180" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="I180" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B181" s="1"/>
+      <c r="C181" s="1"/>
+      <c r="D181" s="10"/>
+      <c r="E181" s="1" t="s">
         <v>90</v>
-      </c>
-      <c r="F176" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G176" s="1"/>
-      <c r="H176" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="I176" s="1"/>
-    </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B177" s="1"/>
-      <c r="C177" s="1"/>
-      <c r="D177" s="10"/>
-      <c r="E177" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F177" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G177" s="1"/>
-      <c r="H177" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I177" s="1"/>
-    </row>
-    <row r="178" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B178" s="1"/>
-      <c r="C178" s="1"/>
-      <c r="D178" s="10"/>
-      <c r="E178" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F178" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G178" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H178" s="3">
-        <v>20200401</v>
-      </c>
-      <c r="I178" s="1"/>
-    </row>
-    <row r="179" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B179" s="1"/>
-      <c r="C179" s="1"/>
-      <c r="D179" s="10"/>
-      <c r="E179" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F179" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G179" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H179" s="3">
-        <v>20210331</v>
-      </c>
-      <c r="I179" s="1"/>
-    </row>
-    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D180" s="9"/>
-    </row>
-    <row r="181" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B181" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C181" t="s">
-        <v>236</v>
-      </c>
-      <c r="D181" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G181" s="1"/>
       <c r="H181" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="I181" s="7" t="s">
-        <v>97</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="I181" s="1"/>
     </row>
     <row r="182" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B182" s="1"/>
-      <c r="C182" s="1"/>
-      <c r="D182" s="10"/>
-      <c r="E182" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="F182" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G182" s="1"/>
-      <c r="H182" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I182" s="1"/>
-    </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B183" s="1"/>
-      <c r="C183" s="1"/>
-      <c r="D183" s="10"/>
+      <c r="D182" s="9"/>
+    </row>
+    <row r="183" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B183" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C183" t="s">
+        <v>236</v>
+      </c>
+      <c r="D183" s="10" t="s">
+        <v>92</v>
+      </c>
       <c r="E183" s="1" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G183" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H183" s="3">
-        <v>20200401</v>
-      </c>
-      <c r="I183" s="1"/>
+      <c r="G183" s="1"/>
+      <c r="H183" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I183" s="7" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
       <c r="D184" s="10"/>
       <c r="E184" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F184" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G184" s="1"/>
+      <c r="H184" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I184" s="1"/>
+    </row>
+    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B185" s="1"/>
+      <c r="C185" s="1"/>
+      <c r="D185" s="10"/>
+      <c r="E185" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F185" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G185" s="1"/>
+      <c r="H185" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I185" s="1"/>
+    </row>
+    <row r="186" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B186" s="1"/>
+      <c r="C186" s="1"/>
+      <c r="D186" s="10"/>
+      <c r="E186" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F186" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G186" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H186" s="3">
+        <v>20200401</v>
+      </c>
+      <c r="I186" s="1"/>
+    </row>
+    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B187" s="1"/>
+      <c r="C187" s="1"/>
+      <c r="D187" s="10"/>
+      <c r="E187" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F184" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G184" s="1" t="s">
+      <c r="F187" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G187" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H184" s="3">
+      <c r="H187" s="3">
         <v>20210331</v>
       </c>
-      <c r="I184" s="1"/>
-    </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D185" s="9"/>
-      <c r="F185" s="10" t="s">
+      <c r="I187" s="1"/>
+    </row>
+    <row r="188" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D188" s="9"/>
+    </row>
+    <row r="189" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B189" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C189" t="s">
+        <v>236</v>
+      </c>
+      <c r="D189" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="E189" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F189" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G189" s="1"/>
+      <c r="H189" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="I189" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B190" s="1"/>
+      <c r="C190" s="1"/>
+      <c r="D190" s="10"/>
+      <c r="E190" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F190" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G190" s="1"/>
+      <c r="H190" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I190" s="1"/>
+    </row>
+    <row r="191" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B191" s="1"/>
+      <c r="C191" s="1"/>
+      <c r="D191" s="10"/>
+      <c r="E191" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F191" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G191" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H191" s="3">
+        <v>20200401</v>
+      </c>
+      <c r="I191" s="1"/>
+    </row>
+    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B192" s="1"/>
+      <c r="C192" s="1"/>
+      <c r="D192" s="10"/>
+      <c r="E192" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F192" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G192" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H192" s="3">
+        <v>20210331</v>
+      </c>
+      <c r="I192" s="1"/>
+    </row>
+    <row r="193" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D193" s="9"/>
+      <c r="F193" s="10" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="186" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B186" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C186" t="s">
-        <v>236</v>
-      </c>
-      <c r="D186" s="10" t="s">
-        <v>285</v>
-      </c>
-      <c r="I186" s="26" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D187" s="9"/>
-    </row>
-    <row r="188" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B188" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C188" t="s">
-        <v>236</v>
-      </c>
-      <c r="D188" s="10" t="s">
-        <v>287</v>
-      </c>
-      <c r="E188" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="F188" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H188" t="s">
-        <v>290</v>
-      </c>
-      <c r="I188" s="26" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="189" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D189" s="9"/>
-      <c r="E189" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F189" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H189">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D190" s="9"/>
-    </row>
-    <row r="191" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B191" t="s">
-        <v>83</v>
-      </c>
-      <c r="C191" t="s">
-        <v>236</v>
-      </c>
-      <c r="D191" s="10" t="s">
-        <v>292</v>
-      </c>
-      <c r="E191" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="F191" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H191" t="s">
-        <v>290</v>
-      </c>
-      <c r="I191" s="26" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D192" s="9"/>
-    </row>
-    <row r="193" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="D193" s="9"/>
-      <c r="H193" t="s">
-        <v>294</v>
-      </c>
-      <c r="I193" s="26"/>
-    </row>
     <row r="194" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B194" t="s">
+      <c r="B194" s="1" t="s">
         <v>83</v>
       </c>
       <c r="C194" t="s">
         <v>236</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>298</v>
-      </c>
-      <c r="E194" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="F194" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H194" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="I194" s="26" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D195" s="9"/>
-      <c r="H195" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="196" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D196" s="9"/>
+    </row>
+    <row r="196" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B196" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C196" t="s">
+        <v>236</v>
+      </c>
+      <c r="D196" s="10" t="s">
+        <v>287</v>
+      </c>
+      <c r="E196" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H196" t="s">
-        <v>297</v>
+        <v>290</v>
+      </c>
+      <c r="I196" s="26" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D197" s="9"/>
+      <c r="E197" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F197" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H197">
+        <v>1234</v>
+      </c>
     </row>
     <row r="198" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B198" t="s">
+      <c r="D198" s="9"/>
+    </row>
+    <row r="199" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B199" t="s">
         <v>83</v>
       </c>
-      <c r="C198" t="s">
+      <c r="C199" t="s">
         <v>236</v>
       </c>
-      <c r="D198" t="s">
-        <v>299</v>
-      </c>
-      <c r="H198" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="199" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D199" s="10" t="s">
+        <v>292</v>
+      </c>
       <c r="E199" s="11" t="s">
         <v>288</v>
       </c>
@@ -3638,186 +3677,172 @@
         <v>9</v>
       </c>
       <c r="H199" t="s">
+        <v>290</v>
+      </c>
+      <c r="I199" s="26" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="200" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D200" s="9"/>
+    </row>
+    <row r="201" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D201" s="9"/>
+      <c r="H201" t="s">
+        <v>294</v>
+      </c>
+      <c r="I201" s="26"/>
+    </row>
+    <row r="202" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B202" t="s">
+        <v>83</v>
+      </c>
+      <c r="C202" t="s">
+        <v>236</v>
+      </c>
+      <c r="D202" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="E202" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F202" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H202" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="200" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H200" t="s">
+      <c r="I202" s="26" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="203" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D203" s="9"/>
+      <c r="H203" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="201" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H201" t="s">
+    <row r="204" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D204" s="9"/>
+      <c r="H204" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="203" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B203" t="s">
+    <row r="205" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D205" s="9"/>
+    </row>
+    <row r="206" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B206" t="s">
         <v>83</v>
       </c>
-      <c r="C203" t="s">
+      <c r="C206" t="s">
         <v>236</v>
       </c>
-      <c r="D203" t="s">
+      <c r="D206" t="s">
+        <v>299</v>
+      </c>
+      <c r="H206" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="207" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E207" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F207" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H207" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="208" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H208" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="209" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H209" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="211" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B211" t="s">
+        <v>83</v>
+      </c>
+      <c r="C211" t="s">
+        <v>236</v>
+      </c>
+      <c r="D211" t="s">
         <v>300</v>
       </c>
-      <c r="H203" t="s">
+      <c r="H211" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="204" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E204" s="11" t="s">
+    <row r="212" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="E212" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="F204" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H204" t="s">
+      <c r="F212" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H212" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="205" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H205" t="s">
+    <row r="213" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H213" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="206" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H206" t="s">
+    <row r="214" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H214" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="208" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B208" t="s">
+    <row r="216" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B216" t="s">
         <v>83</v>
       </c>
-      <c r="C208" t="s">
+      <c r="C216" t="s">
         <v>236</v>
       </c>
-      <c r="D208" t="s">
+      <c r="D216" t="s">
         <v>301</v>
       </c>
-      <c r="H208" t="s">
+      <c r="H216" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="209" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D209" s="9"/>
-      <c r="E209" s="11" t="s">
+    <row r="217" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D217" s="9"/>
+      <c r="E217" s="11" t="s">
         <v>288</v>
       </c>
-      <c r="F209" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H209" t="s">
+      <c r="F217" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H217" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="210" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D210" s="9"/>
-      <c r="H210" t="s">
+    <row r="218" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D218" s="9"/>
+      <c r="H218" t="s">
         <v>296</v>
-      </c>
-    </row>
-    <row r="211" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D211" s="9"/>
-      <c r="H211" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="212" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D212" s="9"/>
-    </row>
-    <row r="213" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B213" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C213" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D213" s="32" t="s">
-        <v>302</v>
-      </c>
-      <c r="E213" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="F213" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G213" s="8"/>
-      <c r="H213" s="18" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="214" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B214" s="8"/>
-      <c r="C214" s="8"/>
-      <c r="D214" s="32"/>
-      <c r="E214" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F214" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G214" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H214" s="3">
-        <v>20200401</v>
-      </c>
-    </row>
-    <row r="215" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B215" s="8"/>
-      <c r="C215" s="8"/>
-      <c r="D215" s="32"/>
-      <c r="E215" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F215" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G215" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H215" s="3">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="216" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B216" s="8"/>
-      <c r="C216" s="8"/>
-      <c r="D216" s="32"/>
-      <c r="E216" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="F216" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G216" s="8"/>
-      <c r="H216" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="217" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B217" s="8"/>
-      <c r="C217" s="8"/>
-      <c r="D217" s="32"/>
-      <c r="E217" s="8"/>
-      <c r="F217" s="8"/>
-      <c r="G217" s="8"/>
-    </row>
-    <row r="218" spans="2:8" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="D218" s="9"/>
-      <c r="H218" s="18" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D219" s="9"/>
+      <c r="H219" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="220" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D220" s="9"/>
     </row>
-    <row r="221" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="221" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B221" s="8" t="s">
         <v>83</v>
       </c>
@@ -3825,34 +3850,42 @@
         <v>236</v>
       </c>
       <c r="D221" s="32" t="s">
-        <v>307</v>
-      </c>
-      <c r="E221" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F221" s="32" t="s">
+        <v>302</v>
+      </c>
+      <c r="E221" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="F221" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G221" s="8"/>
-      <c r="H221" s="32" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="222" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D222" s="9"/>
-      <c r="E222" s="8"/>
+      <c r="H221" s="18" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="222" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B222" s="8"/>
+      <c r="C222" s="8"/>
+      <c r="D222" s="32"/>
+      <c r="E222" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="F222" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="G222" s="8"/>
-      <c r="H222" s="18" t="s">
-        <v>309</v>
+        <v>23</v>
+      </c>
+      <c r="G222" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H222" s="3">
+        <v>20200401</v>
       </c>
     </row>
     <row r="223" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D223" s="9"/>
+      <c r="B223" s="8"/>
+      <c r="C223" s="8"/>
+      <c r="D223" s="32"/>
       <c r="E223" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F223" s="8" t="s">
         <v>23</v>
@@ -3861,243 +3894,231 @@
         <v>16</v>
       </c>
       <c r="H223" s="3">
-        <v>20200401</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="224" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D224" s="9"/>
+      <c r="B224" s="8"/>
+      <c r="C224" s="8"/>
+      <c r="D224" s="32"/>
       <c r="E224" s="8" t="s">
-        <v>17</v>
+        <v>304</v>
       </c>
       <c r="F224" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G224" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H224" s="3">
-        <v>20210331</v>
+      <c r="G224" s="8"/>
+      <c r="H224" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="225" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D225" s="9"/>
+      <c r="B225" s="8"/>
+      <c r="C225" s="8"/>
+      <c r="D225" s="32"/>
       <c r="E225" s="8"/>
       <c r="F225" s="8"/>
-      <c r="G225" s="1"/>
-      <c r="H225" s="3"/>
-    </row>
-    <row r="226" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B226" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C226" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D226" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="H226" t="s">
-        <v>294</v>
-      </c>
-      <c r="I226" s="7" t="s">
-        <v>311</v>
+      <c r="G225" s="8"/>
+    </row>
+    <row r="226" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="D226" s="9"/>
+      <c r="H226" s="18" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D227" s="9"/>
-      <c r="E227" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="F227" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H227" t="s">
-        <v>295</v>
-      </c>
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D228" s="9"/>
-      <c r="H228" t="s">
-        <v>296</v>
-      </c>
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D229" s="9"/>
-      <c r="H229" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="230" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B229" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C229" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D229" s="32" t="s">
+        <v>307</v>
+      </c>
+      <c r="E229" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="F229" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G229" s="8"/>
+      <c r="H229" s="32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="230" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D230" s="9"/>
       <c r="E230" s="8"/>
-      <c r="F230" s="8"/>
-      <c r="G230" s="1"/>
-      <c r="H230" s="3"/>
-    </row>
-    <row r="231" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B231" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C231" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D231" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="H231" t="s">
-        <v>294</v>
-      </c>
-      <c r="I231" s="7" t="s">
-        <v>313</v>
+      <c r="F230" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G230" s="8"/>
+      <c r="H230" s="18" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="231" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D231" s="9"/>
+      <c r="E231" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F231" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G231" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H231" s="3">
+        <v>20200401</v>
       </c>
     </row>
     <row r="232" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D232" s="9"/>
-      <c r="E232" s="11" t="s">
-        <v>288</v>
-      </c>
-      <c r="F232" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H232" t="s">
-        <v>295</v>
+      <c r="E232" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F232" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G232" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H232" s="3">
+        <v>20210331</v>
       </c>
     </row>
     <row r="233" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D233" s="9"/>
-      <c r="H233" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="234" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D234" s="9"/>
+      <c r="E233" s="8"/>
+      <c r="F233" s="8"/>
+      <c r="G233" s="1"/>
+      <c r="H233" s="3"/>
+    </row>
+    <row r="234" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B234" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C234" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D234" s="9" t="s">
+        <v>310</v>
+      </c>
       <c r="H234" t="s">
-        <v>297</v>
+        <v>294</v>
+      </c>
+      <c r="I234" s="7" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="235" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D235" s="9"/>
-      <c r="E235" s="8"/>
-      <c r="F235" s="8"/>
-      <c r="G235" s="1"/>
-      <c r="H235" s="3"/>
-    </row>
-    <row r="236" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
-      <c r="B236" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C236" s="8" t="s">
-        <v>236</v>
-      </c>
-      <c r="D236" s="34" t="s">
-        <v>314</v>
-      </c>
-      <c r="E236" s="8" t="s">
-        <v>303</v>
-      </c>
-      <c r="F236" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G236" s="8"/>
-      <c r="H236" s="18" t="s">
-        <v>305</v>
-      </c>
-      <c r="I236" s="7" t="s">
-        <v>315</v>
+      <c r="E235" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F235" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H235" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="236" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D236" s="9"/>
+      <c r="H236" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D237" s="9"/>
-      <c r="E237" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="F237" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G237" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H237" s="3">
-        <v>20200401</v>
+      <c r="H237" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="238" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D238" s="9"/>
-      <c r="E238" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F238" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G238" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H238" s="3">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="239" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D239" s="9"/>
-      <c r="E239" s="8" t="s">
-        <v>304</v>
-      </c>
-      <c r="F239" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G239" s="8"/>
-      <c r="H239" s="8" t="s">
-        <v>10</v>
+      <c r="E238" s="8"/>
+      <c r="F238" s="8"/>
+      <c r="G238" s="1"/>
+      <c r="H238" s="3"/>
+    </row>
+    <row r="239" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B239" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C239" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D239" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="H239" t="s">
+        <v>294</v>
+      </c>
+      <c r="I239" s="7" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="240" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D240" s="9"/>
-      <c r="E240" s="8"/>
-      <c r="F240" s="8"/>
-      <c r="G240" s="8"/>
-    </row>
-    <row r="241" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="E240" s="11" t="s">
+        <v>288</v>
+      </c>
+      <c r="F240" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H240" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="241" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D241" s="9"/>
-      <c r="H241" s="18" t="s">
-        <v>306</v>
+      <c r="H241" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D242" s="9"/>
-      <c r="E242" s="8"/>
-      <c r="F242" s="8"/>
-      <c r="G242" s="1"/>
-      <c r="H242" s="3"/>
+      <c r="H242" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="243" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B243" s="8" t="s">
+      <c r="D243" s="9"/>
+      <c r="E243" s="8"/>
+      <c r="F243" s="8"/>
+      <c r="G243" s="1"/>
+      <c r="H243" s="3"/>
+    </row>
+    <row r="244" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
+      <c r="B244" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C243" s="8" t="s">
+      <c r="C244" s="8" t="s">
         <v>236</v>
       </c>
-      <c r="D243" s="32" t="s">
-        <v>316</v>
-      </c>
-      <c r="E243" s="33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F243" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="G243" s="8"/>
-      <c r="H243" s="32" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="244" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D244" s="9"/>
-      <c r="E244" s="8"/>
+      <c r="D244" s="34" t="s">
+        <v>314</v>
+      </c>
+      <c r="E244" s="8" t="s">
+        <v>303</v>
+      </c>
       <c r="F244" s="8" t="s">
-        <v>120</v>
+        <v>23</v>
       </c>
       <c r="G244" s="8"/>
       <c r="H244" s="18" t="s">
-        <v>309</v>
+        <v>305</v>
+      </c>
+      <c r="I244" s="7" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="245" spans="2:9" x14ac:dyDescent="0.3">
@@ -4132,318 +4153,297 @@
     </row>
     <row r="247" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D247" s="9"/>
-      <c r="E247" s="8"/>
-      <c r="F247" s="8"/>
-      <c r="G247" s="1"/>
-      <c r="H247" s="3"/>
-    </row>
-    <row r="248" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B248" t="s">
-        <v>100</v>
-      </c>
-      <c r="C248" t="s">
-        <v>237</v>
-      </c>
-      <c r="D248" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="E248" t="s">
-        <v>15</v>
-      </c>
-      <c r="F248" t="s">
-        <v>9</v>
-      </c>
-      <c r="G248" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H248" s="6">
-        <v>20210401</v>
-      </c>
-      <c r="I248" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="249" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E247" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="F247" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G247" s="8"/>
+      <c r="H247" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="248" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D248" s="9"/>
+      <c r="E248" s="8"/>
+      <c r="F248" s="8"/>
+      <c r="G248" s="8"/>
+    </row>
+    <row r="249" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D249" s="9"/>
-      <c r="E249" t="s">
-        <v>17</v>
-      </c>
-      <c r="F249" t="s">
-        <v>9</v>
-      </c>
-      <c r="G249" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H249" s="6">
-        <v>20220112</v>
+      <c r="H249" s="18" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="250" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D250" s="9"/>
-      <c r="E250" t="s">
-        <v>103</v>
-      </c>
-      <c r="F250" t="s">
-        <v>9</v>
-      </c>
-      <c r="H250" s="6">
-        <v>0</v>
-      </c>
+      <c r="E250" s="8"/>
+      <c r="F250" s="8"/>
+      <c r="G250" s="1"/>
+      <c r="H250" s="3"/>
     </row>
     <row r="251" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D251" s="9"/>
-      <c r="H251" s="6"/>
-    </row>
-    <row r="252" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B252" t="s">
-        <v>100</v>
-      </c>
-      <c r="C252" t="s">
-        <v>237</v>
-      </c>
-      <c r="D252" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="H252" s="6"/>
-      <c r="I252" s="7" t="s">
-        <v>105</v>
+      <c r="B251" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C251" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="D251" s="32" t="s">
+        <v>316</v>
+      </c>
+      <c r="E251" s="33" t="s">
+        <v>32</v>
+      </c>
+      <c r="F251" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="G251" s="8"/>
+      <c r="H251" s="32" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="252" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D252" s="9"/>
+      <c r="E252" s="8"/>
+      <c r="F252" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G252" s="8"/>
+      <c r="H252" s="18" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="253" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D253" s="9"/>
-      <c r="H253" s="6"/>
+      <c r="E253" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F253" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G253" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H253" s="3">
+        <v>20200401</v>
+      </c>
     </row>
     <row r="254" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D254" s="9"/>
-      <c r="H254" s="6"/>
-    </row>
-    <row r="255" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B255" t="s">
+      <c r="E254" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F254" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G254" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H254" s="3">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="255" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D255" s="9"/>
+      <c r="E255" s="8"/>
+      <c r="F255" s="8"/>
+      <c r="G255" s="1"/>
+      <c r="H255" s="3"/>
+    </row>
+    <row r="256" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B256" t="s">
         <v>100</v>
       </c>
-      <c r="C255" t="s">
+      <c r="C256" t="s">
         <v>237</v>
       </c>
-      <c r="D255" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H255" s="6"/>
-      <c r="I255" s="7" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="256" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D256" s="9"/>
-      <c r="H256" s="6"/>
+      <c r="D256" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E256" t="s">
+        <v>15</v>
+      </c>
+      <c r="F256" t="s">
+        <v>9</v>
+      </c>
+      <c r="G256" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H256" s="6">
+        <v>20210401</v>
+      </c>
+      <c r="I256" s="7" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="257" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D257" s="9"/>
-      <c r="H257" s="6"/>
-    </row>
-    <row r="258" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B258" t="s">
-        <v>100</v>
-      </c>
-      <c r="C258" t="s">
-        <v>237</v>
-      </c>
-      <c r="D258" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="H258" s="6"/>
-      <c r="I258" s="7" t="s">
-        <v>109</v>
+      <c r="E257" t="s">
+        <v>17</v>
+      </c>
+      <c r="F257" t="s">
+        <v>9</v>
+      </c>
+      <c r="G257" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H257" s="6">
+        <v>20220112</v>
+      </c>
+    </row>
+    <row r="258" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D258" s="9"/>
+      <c r="E258" t="s">
+        <v>103</v>
+      </c>
+      <c r="F258" t="s">
+        <v>9</v>
+      </c>
+      <c r="H258" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="259" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D259" s="9"/>
       <c r="H259" s="6"/>
     </row>
-    <row r="260" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D260" s="9"/>
+    <row r="260" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B260" t="s">
+        <v>100</v>
+      </c>
+      <c r="C260" t="s">
+        <v>237</v>
+      </c>
+      <c r="D260" s="9" t="s">
+        <v>104</v>
+      </c>
       <c r="H260" s="6"/>
-    </row>
-    <row r="261" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B261" t="s">
-        <v>100</v>
-      </c>
-      <c r="C261" t="s">
-        <v>237</v>
-      </c>
-      <c r="D261" s="9" t="s">
-        <v>110</v>
-      </c>
-      <c r="E261" t="s">
-        <v>111</v>
-      </c>
-      <c r="F261" t="s">
-        <v>112</v>
-      </c>
-      <c r="H261" s="6" t="b">
-        <v>0</v>
-      </c>
-      <c r="I261" s="7" t="s">
-        <v>113</v>
-      </c>
+      <c r="I260" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="261" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D261" s="9"/>
+      <c r="H261" s="6"/>
     </row>
     <row r="262" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D262" s="9"/>
-      <c r="E262" t="s">
-        <v>114</v>
-      </c>
-      <c r="F262" t="s">
-        <v>112</v>
-      </c>
-      <c r="H262" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="263" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D263" s="9"/>
+      <c r="H262" s="6"/>
+    </row>
+    <row r="263" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B263" t="s">
+        <v>100</v>
+      </c>
+      <c r="C263" t="s">
+        <v>237</v>
+      </c>
+      <c r="D263" s="9" t="s">
+        <v>106</v>
+      </c>
       <c r="H263" s="6"/>
-    </row>
-    <row r="264" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B264" t="s">
-        <v>100</v>
-      </c>
-      <c r="C264" t="s">
-        <v>237</v>
-      </c>
-      <c r="D264" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E264" t="s">
-        <v>116</v>
-      </c>
-      <c r="F264" t="s">
-        <v>21</v>
-      </c>
-      <c r="H264" s="6">
-        <v>3</v>
-      </c>
-      <c r="I264" s="7" t="s">
-        <v>117</v>
-      </c>
+      <c r="I263" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="264" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D264" s="9"/>
+      <c r="H264" s="6"/>
     </row>
     <row r="265" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D265" s="9"/>
+      <c r="H265" s="6"/>
     </row>
     <row r="266" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B266" s="1" t="s">
-        <v>62</v>
+      <c r="B266" t="s">
+        <v>100</v>
       </c>
       <c r="C266" t="s">
-        <v>271</v>
-      </c>
-      <c r="D266" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E266" s="1"/>
-      <c r="F266" s="10"/>
-      <c r="G266" s="1"/>
-      <c r="H266" s="3"/>
+        <v>237</v>
+      </c>
+      <c r="D266" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="H266" s="6"/>
       <c r="I266" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="267" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B267" s="1"/>
-      <c r="C267" s="1"/>
-      <c r="D267" s="10"/>
-      <c r="E267" s="1"/>
-      <c r="F267" s="1"/>
-      <c r="G267" s="1"/>
-      <c r="H267" s="3"/>
-      <c r="I267" s="13"/>
-    </row>
-    <row r="268" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B268" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C268" t="s">
-        <v>271</v>
-      </c>
-      <c r="D268" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E268" s="1"/>
-      <c r="F268" s="10"/>
-      <c r="G268" s="1"/>
-      <c r="H268" s="3"/>
-      <c r="I268" s="7" t="s">
-        <v>39</v>
-      </c>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="267" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D267" s="9"/>
+      <c r="H267" s="6"/>
+    </row>
+    <row r="268" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D268" s="9"/>
+      <c r="H268" s="6"/>
     </row>
     <row r="269" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B269" s="1"/>
-      <c r="C269" s="1"/>
-      <c r="D269" s="10"/>
-      <c r="E269" s="1"/>
-      <c r="F269" s="1"/>
-      <c r="G269" s="1"/>
-      <c r="H269" s="3"/>
-      <c r="I269" s="13"/>
-    </row>
-    <row r="270" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B270" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C270" t="s">
-        <v>271</v>
-      </c>
-      <c r="D270" s="10" t="s">
-        <v>320</v>
-      </c>
-      <c r="E270" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="F270" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G270" s="1"/>
-      <c r="H270" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="I270" s="26" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="271" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B271" s="1"/>
-      <c r="C271" s="1"/>
-      <c r="D271" s="10"/>
-      <c r="E271" s="11"/>
-      <c r="F271" s="10"/>
-      <c r="G271" s="1"/>
-      <c r="H271" s="3"/>
-      <c r="I271" s="13"/>
-    </row>
-    <row r="272" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B272" s="1" t="s">
-        <v>62</v>
+      <c r="B269" t="s">
+        <v>100</v>
+      </c>
+      <c r="C269" t="s">
+        <v>237</v>
+      </c>
+      <c r="D269" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E269" t="s">
+        <v>111</v>
+      </c>
+      <c r="F269" t="s">
+        <v>112</v>
+      </c>
+      <c r="H269" s="6" t="b">
+        <v>0</v>
+      </c>
+      <c r="I269" s="7" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="270" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D270" s="9"/>
+      <c r="E270" t="s">
+        <v>114</v>
+      </c>
+      <c r="F270" t="s">
+        <v>112</v>
+      </c>
+      <c r="H270" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D271" s="9"/>
+      <c r="H271" s="6"/>
+    </row>
+    <row r="272" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B272" t="s">
+        <v>100</v>
       </c>
       <c r="C272" t="s">
-        <v>271</v>
-      </c>
-      <c r="D272" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E272" s="11"/>
-      <c r="F272" s="10"/>
-      <c r="G272" s="1"/>
-      <c r="H272" s="3"/>
-    </row>
-    <row r="273" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B273" s="1"/>
-      <c r="C273" s="1"/>
-      <c r="D273" s="10"/>
-      <c r="E273" s="11"/>
-      <c r="F273" s="10"/>
-      <c r="G273" s="1"/>
-      <c r="H273" s="3"/>
-      <c r="I273" s="13"/>
-    </row>
-    <row r="274" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+      <c r="D272" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E272" t="s">
+        <v>116</v>
+      </c>
+      <c r="F272" t="s">
+        <v>21</v>
+      </c>
+      <c r="H272" s="6">
+        <v>3</v>
+      </c>
+      <c r="I272" s="7" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="273" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D273" s="9"/>
+    </row>
+    <row r="274" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B274" s="1" t="s">
         <v>62</v>
       </c>
@@ -4451,348 +4451,383 @@
         <v>271</v>
       </c>
       <c r="D274" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="E274" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="F274" s="10" t="s">
-        <v>9</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="E274" s="1"/>
+      <c r="F274" s="10"/>
       <c r="G274" s="1"/>
-      <c r="H274" s="3" t="s">
-        <v>66</v>
-      </c>
+      <c r="H274" s="3"/>
       <c r="I274" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="275" spans="1:9" ht="18" x14ac:dyDescent="0.35">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="275" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B275" s="1"/>
       <c r="C275" s="1"/>
       <c r="D275" s="10"/>
-      <c r="E275" s="11" t="s">
-        <v>323</v>
-      </c>
-      <c r="F275" s="10" t="s">
-        <v>9</v>
-      </c>
+      <c r="E275" s="1"/>
+      <c r="F275" s="1"/>
       <c r="G275" s="1"/>
-      <c r="H275" s="3">
-        <v>532667</v>
-      </c>
+      <c r="H275" s="3"/>
       <c r="I275" s="13"/>
     </row>
-    <row r="276" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B276" s="1"/>
-      <c r="C276" s="1"/>
-      <c r="D276" s="10"/>
-      <c r="E276" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F276" s="10" t="s">
-        <v>9</v>
-      </c>
+    <row r="276" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B276" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C276" t="s">
+        <v>271</v>
+      </c>
+      <c r="D276" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="E276" s="1"/>
+      <c r="F276" s="10"/>
       <c r="G276" s="1"/>
-      <c r="H276" s="3">
-        <v>198</v>
-      </c>
-      <c r="I276" s="13"/>
-    </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D277" s="9"/>
-    </row>
-    <row r="278" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B278" t="s">
+      <c r="H276" s="3"/>
+      <c r="I276" s="7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="277" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B277" s="1"/>
+      <c r="C277" s="1"/>
+      <c r="D277" s="10"/>
+      <c r="E277" s="1"/>
+      <c r="F277" s="1"/>
+      <c r="G277" s="1"/>
+      <c r="H277" s="3"/>
+      <c r="I277" s="13"/>
+    </row>
+    <row r="278" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B278" s="1" t="s">
         <v>62</v>
       </c>
       <c r="C278" t="s">
         <v>271</v>
       </c>
-      <c r="D278" s="9" t="s">
+      <c r="D278" s="10" t="s">
+        <v>320</v>
+      </c>
+      <c r="E278" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="F278" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G278" s="1"/>
+      <c r="H278" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I278" s="26" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="279" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B279" s="1"/>
+      <c r="C279" s="1"/>
+      <c r="D279" s="10"/>
+      <c r="E279" s="11"/>
+      <c r="F279" s="10"/>
+      <c r="G279" s="1"/>
+      <c r="H279" s="3"/>
+      <c r="I279" s="13"/>
+    </row>
+    <row r="280" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B280" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E278" s="11" t="s">
+      <c r="C280" t="s">
+        <v>271</v>
+      </c>
+      <c r="D280" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E280" s="11"/>
+      <c r="F280" s="10"/>
+      <c r="G280" s="1"/>
+      <c r="H280" s="3"/>
+    </row>
+    <row r="281" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B281" s="1"/>
+      <c r="C281" s="1"/>
+      <c r="D281" s="10"/>
+      <c r="E281" s="11"/>
+      <c r="F281" s="10"/>
+      <c r="G281" s="1"/>
+      <c r="H281" s="3"/>
+      <c r="I281" s="13"/>
+    </row>
+    <row r="282" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B282" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C282" t="s">
+        <v>271</v>
+      </c>
+      <c r="D282" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="E282" s="11" t="s">
+        <v>252</v>
+      </c>
+      <c r="F282" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G282" s="1"/>
+      <c r="H282" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="I282" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="283" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B283" s="1"/>
+      <c r="C283" s="1"/>
+      <c r="D283" s="10"/>
+      <c r="E283" s="11" t="s">
+        <v>323</v>
+      </c>
+      <c r="F283" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G283" s="1"/>
+      <c r="H283" s="3">
+        <v>532667</v>
+      </c>
+      <c r="I283" s="13"/>
+    </row>
+    <row r="284" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B284" s="1"/>
+      <c r="C284" s="1"/>
+      <c r="D284" s="10"/>
+      <c r="E284" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F284" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G284" s="1"/>
+      <c r="H284" s="3">
+        <v>198</v>
+      </c>
+      <c r="I284" s="13"/>
+    </row>
+    <row r="285" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D285" s="9"/>
+    </row>
+    <row r="286" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B286" t="s">
+        <v>62</v>
+      </c>
+      <c r="C286" t="s">
+        <v>271</v>
+      </c>
+      <c r="D286" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E286" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F278" t="s">
-        <v>9</v>
-      </c>
-      <c r="H278" s="8">
+      <c r="F286" t="s">
+        <v>9</v>
+      </c>
+      <c r="H286" s="8">
         <v>20191101</v>
       </c>
-      <c r="I278" s="7" t="s">
+      <c r="I286" s="7" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D279" s="9"/>
-    </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B280" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C280" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D280" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="E280" t="s">
-        <v>15</v>
-      </c>
-      <c r="F280" t="s">
-        <v>9</v>
-      </c>
-      <c r="H280" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="I280" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D281" s="9"/>
-      <c r="E281" t="s">
-        <v>17</v>
-      </c>
-      <c r="F281" t="s">
-        <v>9</v>
-      </c>
-      <c r="H281" s="35" t="s">
-        <v>166</v>
-      </c>
-      <c r="I281" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D282" s="9"/>
-      <c r="H282" s="8"/>
-      <c r="I282" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D283" s="9"/>
-      <c r="H283" s="8"/>
-      <c r="I283" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D284" s="9"/>
-      <c r="I284" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D285" s="9"/>
-      <c r="I285" s="19" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D286" s="9"/>
-      <c r="I286" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="287" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D287" s="9"/>
     </row>
-    <row r="288" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A288" s="1">
-        <v>36</v>
-      </c>
+    <row r="288" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B288" s="1" t="s">
         <v>232</v>
       </c>
       <c r="C288" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D288" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="E288" s="1" t="s">
+      <c r="D288" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E288" t="s">
         <v>15</v>
       </c>
-      <c r="F288" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G288" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H288" s="15">
-        <v>20200401</v>
-      </c>
-      <c r="I288" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="289" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A289" s="1"/>
-      <c r="B289" s="1"/>
-      <c r="C289" s="1"/>
-      <c r="D289" s="10"/>
-      <c r="E289" s="1" t="s">
+      <c r="F288" t="s">
+        <v>9</v>
+      </c>
+      <c r="H288" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="I288" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D289" s="9"/>
+      <c r="E289" t="s">
         <v>17</v>
       </c>
-      <c r="F289" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G289" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H289" s="6">
-        <v>20210331</v>
-      </c>
-      <c r="I289" s="1"/>
-    </row>
-    <row r="290" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A290" s="1"/>
-      <c r="B290" s="1"/>
-      <c r="C290" s="1"/>
-      <c r="D290" s="10"/>
-      <c r="E290" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F290" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G290" s="1"/>
-      <c r="H290" s="3">
-        <v>533271</v>
-      </c>
-      <c r="I290" s="13"/>
-    </row>
-    <row r="291" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A291" s="1"/>
-      <c r="B291" s="1"/>
-      <c r="C291" s="1"/>
-      <c r="D291" s="10"/>
-      <c r="E291" s="1"/>
-      <c r="F291" s="1"/>
-      <c r="G291" s="1"/>
-      <c r="H291" s="3"/>
-      <c r="I291" s="13"/>
+      <c r="F289" t="s">
+        <v>9</v>
+      </c>
+      <c r="H289" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="I289" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D290" s="9"/>
+      <c r="H290" s="8"/>
+      <c r="I290" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D291" s="9"/>
+      <c r="H291" s="8"/>
+      <c r="I291" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B292" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C292" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D292" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="E292" t="s">
-        <v>27</v>
-      </c>
-      <c r="F292" t="s">
-        <v>9</v>
-      </c>
-      <c r="H292" t="s">
-        <v>225</v>
-      </c>
+      <c r="D292" s="9"/>
       <c r="I292" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D293" s="9"/>
-      <c r="E293" t="s">
-        <v>48</v>
-      </c>
-      <c r="F293" t="s">
-        <v>9</v>
-      </c>
-      <c r="H293" t="s">
-        <v>226</v>
-      </c>
-      <c r="I293" t="s">
-        <v>159</v>
+      <c r="I293" s="19" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D294" s="9"/>
-      <c r="E294" t="s">
-        <v>15</v>
-      </c>
-      <c r="F294" t="s">
-        <v>9</v>
-      </c>
-      <c r="H294" s="17" t="s">
-        <v>164</v>
-      </c>
       <c r="I294" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D295" s="9"/>
-      <c r="E295" t="s">
+    </row>
+    <row r="296" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A296" s="1">
+        <v>36</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C296" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D296" s="10" t="s">
+        <v>231</v>
+      </c>
+      <c r="E296" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F296" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G296" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H296" s="15">
+        <v>20200401</v>
+      </c>
+      <c r="I296" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A297" s="1"/>
+      <c r="B297" s="1"/>
+      <c r="C297" s="1"/>
+      <c r="D297" s="10"/>
+      <c r="E297" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F295" t="s">
-        <v>9</v>
-      </c>
-      <c r="H295" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="I295" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D296" s="9"/>
-      <c r="I296" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D297" s="9"/>
-      <c r="I297" s="19" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D298" s="9"/>
-      <c r="I298" s="19" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D299" s="9"/>
-      <c r="I299" t="s">
-        <v>181</v>
-      </c>
+      <c r="F297" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G297" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H297" s="6">
+        <v>20210331</v>
+      </c>
+      <c r="I297" s="1"/>
+    </row>
+    <row r="298" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A298" s="1"/>
+      <c r="B298" s="1"/>
+      <c r="C298" s="1"/>
+      <c r="D298" s="10"/>
+      <c r="E298" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F298" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G298" s="1"/>
+      <c r="H298" s="3">
+        <v>533271</v>
+      </c>
+      <c r="I298" s="13"/>
+    </row>
+    <row r="299" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A299" s="1"/>
+      <c r="B299" s="1"/>
+      <c r="C299" s="1"/>
+      <c r="D299" s="10"/>
+      <c r="E299" s="1"/>
+      <c r="F299" s="1"/>
+      <c r="G299" s="1"/>
+      <c r="H299" s="3"/>
+      <c r="I299" s="13"/>
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D300" s="9"/>
+      <c r="B300" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C300" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D300" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E300" t="s">
+        <v>27</v>
+      </c>
+      <c r="F300" t="s">
+        <v>9</v>
+      </c>
+      <c r="H300" t="s">
+        <v>225</v>
+      </c>
+      <c r="I300" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B301" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="C301" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D301" s="9" t="s">
-        <v>234</v>
-      </c>
+      <c r="D301" s="9"/>
       <c r="E301" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
       <c r="F301" t="s">
         <v>9</v>
       </c>
       <c r="H301" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="I301" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
@@ -4807,7 +4842,7 @@
         <v>164</v>
       </c>
       <c r="I302" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
@@ -4822,207 +4857,176 @@
         <v>166</v>
       </c>
       <c r="I303" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D304" s="9"/>
       <c r="I304" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="305" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D305" s="9"/>
-      <c r="I305" t="s">
-        <v>165</v>
+      <c r="I305" s="19" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="306" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D306" s="9"/>
-      <c r="I306" s="25" t="s">
-        <v>230</v>
+      <c r="I306" s="19" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D307" s="9"/>
-      <c r="E307" s="24"/>
-      <c r="H307" s="18"/>
-      <c r="I307" s="18" t="s">
+      <c r="I307" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="308" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D308" s="9"/>
     </row>
-    <row r="309" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B309" t="s">
-        <v>121</v>
+    <row r="309" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B309" s="1" t="s">
+        <v>232</v>
       </c>
       <c r="C309" s="1" t="s">
         <v>238</v>
       </c>
       <c r="D309" s="9" t="s">
-        <v>122</v>
+        <v>234</v>
       </c>
       <c r="E309" t="s">
-        <v>15</v>
-      </c>
-      <c r="F309" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G309" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H309" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I309" s="7" t="s">
-        <v>123</v>
+        <v>27</v>
+      </c>
+      <c r="F309" t="s">
+        <v>9</v>
+      </c>
+      <c r="H309" t="s">
+        <v>229</v>
+      </c>
+      <c r="I309" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D310" s="9"/>
       <c r="E310" t="s">
-        <v>17</v>
-      </c>
-      <c r="F310" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G310" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H310" s="8">
-        <v>20210331</v>
+        <v>15</v>
+      </c>
+      <c r="F310" t="s">
+        <v>9</v>
+      </c>
+      <c r="H310" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I310" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="311" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D311" s="9"/>
-      <c r="F311" s="9"/>
-      <c r="H311" s="8"/>
-    </row>
-    <row r="312" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B312" t="s">
-        <v>121</v>
-      </c>
-      <c r="C312" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D312" s="9" t="s">
-        <v>124</v>
-      </c>
-      <c r="E312" t="s">
-        <v>15</v>
-      </c>
-      <c r="F312" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G312" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H312" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I312" s="7" t="s">
-        <v>125</v>
+      <c r="E311" t="s">
+        <v>17</v>
+      </c>
+      <c r="F311" t="s">
+        <v>9</v>
+      </c>
+      <c r="H311" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="I311" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="312" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D312" s="9"/>
+      <c r="I312" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="313" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D313" s="9"/>
-      <c r="E313" t="s">
-        <v>17</v>
-      </c>
-      <c r="F313" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G313" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H313" s="8">
-        <v>20210331</v>
+      <c r="I313" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="314" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D314" s="9"/>
-      <c r="E314" t="s">
-        <v>126</v>
-      </c>
-      <c r="F314" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H314" s="8" t="s">
-        <v>127</v>
+      <c r="I314" s="25" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="315" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D315" s="9"/>
-      <c r="E315" t="s">
-        <v>128</v>
-      </c>
-      <c r="F315" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H315" s="8" t="s">
-        <v>127</v>
+      <c r="E315" s="24"/>
+      <c r="H315" s="18"/>
+      <c r="I315" s="18" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="316" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D316" s="9"/>
-      <c r="E316" t="s">
-        <v>129</v>
-      </c>
-      <c r="F316" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="H316" s="8" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="317" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D317" s="9"/>
+    </row>
+    <row r="317" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B317" t="s">
+        <v>121</v>
+      </c>
+      <c r="C317" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D317" s="9" t="s">
+        <v>122</v>
+      </c>
       <c r="E317" t="s">
-        <v>130</v>
+        <v>15</v>
       </c>
       <c r="F317" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H317" s="8" t="s">
-        <v>131</v>
+      <c r="G317" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H317" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I317" s="7" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D318" s="9"/>
-      <c r="H318" s="8"/>
-    </row>
-    <row r="319" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B319" t="s">
+      <c r="E318" t="s">
+        <v>17</v>
+      </c>
+      <c r="F318" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G318" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H318" s="8">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="319" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D319" s="9"/>
+      <c r="F319" s="9"/>
+      <c r="H319" s="8"/>
+    </row>
+    <row r="320" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B320" t="s">
         <v>121</v>
       </c>
-      <c r="C319" s="1" t="s">
+      <c r="C320" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D319" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="E319" t="s">
+      <c r="D320" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="E320" t="s">
         <v>15</v>
-      </c>
-      <c r="F319" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G319" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H319" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I319" s="7" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="320" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D320" s="9"/>
-      <c r="E320" t="s">
-        <v>17</v>
       </c>
       <c r="F320" s="9" t="s">
         <v>23</v>
@@ -5031,106 +5035,109 @@
         <v>16</v>
       </c>
       <c r="H320" s="8">
-        <v>20210331</v>
+        <v>20200401</v>
+      </c>
+      <c r="I320" s="7" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="321" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D321" s="9"/>
       <c r="E321" t="s">
-        <v>134</v>
+        <v>17</v>
       </c>
       <c r="F321" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H321" s="8" t="s">
-        <v>135</v>
+      <c r="G321" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H321" s="8">
+        <v>20210331</v>
       </c>
     </row>
     <row r="322" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D322" s="9"/>
       <c r="E322" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="F322" s="9" t="s">
-        <v>23</v>
+        <v>112</v>
       </c>
       <c r="H322" s="8" t="s">
-        <v>28</v>
+        <v>127</v>
       </c>
     </row>
     <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D323" s="9"/>
       <c r="E323" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="F323" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H323" s="8">
-        <v>512573</v>
+        <v>112</v>
+      </c>
+      <c r="H323" s="8" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="324" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D324" s="9"/>
-      <c r="H324" s="8"/>
-    </row>
-    <row r="325" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B325" t="s">
-        <v>121</v>
-      </c>
-      <c r="C325" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D325" s="9" t="s">
-        <v>138</v>
-      </c>
+      <c r="E324" t="s">
+        <v>129</v>
+      </c>
+      <c r="F324" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="H324" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="325" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D325" s="9"/>
       <c r="E325" t="s">
-        <v>15</v>
+        <v>130</v>
       </c>
       <c r="F325" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G325" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H325" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I325" s="7" t="s">
-        <v>139</v>
+      <c r="H325" s="8" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="326" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D326" s="9"/>
-      <c r="E326" t="s">
+      <c r="H326" s="8"/>
+    </row>
+    <row r="327" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B327" t="s">
+        <v>121</v>
+      </c>
+      <c r="C327" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D327" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="E327" t="s">
+        <v>15</v>
+      </c>
+      <c r="F327" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G327" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H327" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I327" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="328" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D328" s="9"/>
+      <c r="E328" t="s">
         <v>17</v>
-      </c>
-      <c r="F326" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G326" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H326" s="8">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="327" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D327" s="9"/>
-      <c r="H327" s="8"/>
-    </row>
-    <row r="328" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B328" t="s">
-        <v>121</v>
-      </c>
-      <c r="C328" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D328" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="E328" t="s">
-        <v>15</v>
       </c>
       <c r="F328" s="9" t="s">
         <v>23</v>
@@ -5139,315 +5146,299 @@
         <v>16</v>
       </c>
       <c r="H328" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I328" s="7" t="s">
-        <v>141</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="329" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D329" s="9"/>
       <c r="E329" t="s">
-        <v>17</v>
+        <v>134</v>
       </c>
       <c r="F329" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G329" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="H329" s="8">
-        <v>20210331</v>
+      <c r="H329" s="8" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="330" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D330" s="9"/>
       <c r="E330" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F330" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H330" s="8">
-        <v>500425</v>
+      <c r="H330" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="331" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D331" s="9"/>
-      <c r="H331" s="8"/>
-    </row>
-    <row r="332" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B332" t="s">
+      <c r="E331" t="s">
+        <v>137</v>
+      </c>
+      <c r="F331" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H331" s="8">
+        <v>512573</v>
+      </c>
+    </row>
+    <row r="332" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D332" s="9"/>
+      <c r="H332" s="8"/>
+    </row>
+    <row r="333" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B333" t="s">
         <v>121</v>
       </c>
-      <c r="C332" s="1" t="s">
+      <c r="C333" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D332" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E332" t="s">
-        <v>22</v>
-      </c>
-      <c r="F332" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G332" s="9" t="s">
+      <c r="D333" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E333" t="s">
+        <v>15</v>
+      </c>
+      <c r="F333" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G333" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="H332" s="16">
-        <v>20220228</v>
-      </c>
-      <c r="I332" s="7" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="333" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D333" s="9"/>
-      <c r="E333" t="s">
-        <v>37</v>
-      </c>
-      <c r="F333" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H333" s="8" t="s">
-        <v>145</v>
+      <c r="H333" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I333" s="7" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="334" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D334" s="9"/>
       <c r="E334" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="F334" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H334" s="8" t="s">
-        <v>25</v>
+      <c r="G334" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H334" s="8">
+        <v>20210331</v>
       </c>
     </row>
     <row r="335" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D335" s="9"/>
-      <c r="E335" t="s">
-        <v>35</v>
-      </c>
-      <c r="F335" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H335" s="8" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="336" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D336" s="9"/>
+      <c r="H335" s="8"/>
+    </row>
+    <row r="336" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B336" t="s">
+        <v>121</v>
+      </c>
+      <c r="C336" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D336" s="9" t="s">
+        <v>140</v>
+      </c>
       <c r="E336" t="s">
-        <v>68</v>
+        <v>15</v>
       </c>
       <c r="F336" s="9" t="s">
-        <v>147</v>
+        <v>23</v>
+      </c>
+      <c r="G336" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H336" s="8">
-        <v>4</v>
+        <v>20200401</v>
+      </c>
+      <c r="I336" s="7" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="337" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D337" s="9"/>
       <c r="E337" t="s">
-        <v>148</v>
+        <v>17</v>
       </c>
       <c r="F337" s="9" t="s">
-        <v>147</v>
+        <v>23</v>
+      </c>
+      <c r="G337" s="9" t="s">
+        <v>16</v>
       </c>
       <c r="H337" s="8">
-        <v>48</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="338" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D338" s="9"/>
       <c r="E338" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="F338" s="9" t="s">
-        <v>147</v>
+        <v>23</v>
       </c>
       <c r="H338" s="8">
-        <v>1.1000000000000001</v>
+        <v>500425</v>
       </c>
     </row>
     <row r="339" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D339" s="9"/>
-      <c r="E339" t="s">
-        <v>150</v>
-      </c>
-      <c r="F339" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H339" s="8">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="340" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D340" s="9"/>
+      <c r="H339" s="8"/>
+    </row>
+    <row r="340" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B340" t="s">
+        <v>121</v>
+      </c>
+      <c r="C340" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D340" s="9" t="s">
+        <v>143</v>
+      </c>
       <c r="E340" t="s">
-        <v>151</v>
+        <v>22</v>
       </c>
       <c r="F340" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H340" s="8">
-        <v>0.11</v>
+        <v>23</v>
+      </c>
+      <c r="G340" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H340" s="16">
+        <v>20220228</v>
+      </c>
+      <c r="I340" s="7" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="341" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D341" s="9"/>
       <c r="E341" t="s">
-        <v>152</v>
+        <v>37</v>
       </c>
       <c r="F341" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="H341" s="8">
-        <v>0.2</v>
+        <v>23</v>
+      </c>
+      <c r="H341" s="8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="342" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D342" s="9"/>
       <c r="E342" t="s">
-        <v>142</v>
+        <v>24</v>
       </c>
       <c r="F342" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H342" s="8">
-        <v>500820</v>
+      <c r="H342" s="8" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="343" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D343" s="9"/>
-    </row>
-    <row r="344" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B344" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C344" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D344" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E344" s="1"/>
-      <c r="F344" s="1"/>
-      <c r="G344" s="1"/>
-      <c r="H344" s="3"/>
-      <c r="I344" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="345" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B345" s="1"/>
-      <c r="C345" s="1"/>
-      <c r="D345" s="10"/>
-      <c r="E345" s="1"/>
-      <c r="F345" s="1"/>
-      <c r="G345" s="1"/>
-      <c r="H345" s="12"/>
-      <c r="I345" s="13"/>
-    </row>
-    <row r="346" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B346" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C346" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D346" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E346" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F346" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G346" s="1"/>
-      <c r="H346" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I346" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="347" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B347" s="1"/>
-      <c r="C347" s="1"/>
-      <c r="D347" s="10"/>
-      <c r="E347" s="1"/>
-      <c r="F347" s="1"/>
-      <c r="G347" s="1"/>
-      <c r="H347" s="3"/>
-      <c r="I347" s="13"/>
-    </row>
-    <row r="348" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B348" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C348" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D348" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="E348" s="1"/>
-      <c r="F348" s="1"/>
-      <c r="G348" s="1"/>
-      <c r="H348" s="3"/>
-      <c r="I348" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="349" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B349" s="1"/>
-      <c r="C349" s="1"/>
-      <c r="D349" s="10"/>
-      <c r="E349" s="1"/>
-      <c r="F349" s="1"/>
-      <c r="G349" s="1"/>
-      <c r="H349" s="3"/>
-      <c r="I349" s="13"/>
-    </row>
-    <row r="350" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B350" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C350" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D350" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="E350" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="F350" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G350" s="1"/>
-      <c r="H350" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="I350" s="7" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="351" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B351" s="1"/>
-      <c r="C351" s="1"/>
-      <c r="D351" s="10"/>
-      <c r="E351" s="1"/>
-      <c r="F351" s="1"/>
-      <c r="G351" s="1"/>
-      <c r="H351" s="3"/>
-      <c r="I351" s="13"/>
+      <c r="E343" t="s">
+        <v>35</v>
+      </c>
+      <c r="F343" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H343" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="344" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D344" s="9"/>
+      <c r="E344" t="s">
+        <v>68</v>
+      </c>
+      <c r="F344" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H344" s="8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="345" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D345" s="9"/>
+      <c r="E345" t="s">
+        <v>148</v>
+      </c>
+      <c r="F345" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H345" s="8">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="346" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D346" s="9"/>
+      <c r="E346" t="s">
+        <v>149</v>
+      </c>
+      <c r="F346" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H346" s="8">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="347" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D347" s="9"/>
+      <c r="E347" t="s">
+        <v>150</v>
+      </c>
+      <c r="F347" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H347" s="8">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="348" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D348" s="9"/>
+      <c r="E348" t="s">
+        <v>151</v>
+      </c>
+      <c r="F348" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H348" s="8">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="349" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D349" s="9"/>
+      <c r="E349" t="s">
+        <v>152</v>
+      </c>
+      <c r="F349" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="H349" s="8">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="350" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D350" s="9"/>
+      <c r="E350" t="s">
+        <v>142</v>
+      </c>
+      <c r="F350" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H350" s="8">
+        <v>500820</v>
+      </c>
+    </row>
+    <row r="351" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D351" s="9"/>
     </row>
     <row r="352" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B352" s="1" t="s">
@@ -5457,125 +5448,197 @@
         <v>239</v>
       </c>
       <c r="D352" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E352" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="F352" s="1" t="s">
-        <v>9</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="E352" s="1"/>
+      <c r="F352" s="1"/>
       <c r="G352" s="1"/>
-      <c r="H352" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I352" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="353" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H352" s="3"/>
+      <c r="I352" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="353" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B353" s="1"/>
       <c r="C353" s="1"/>
       <c r="D353" s="10"/>
-      <c r="E353" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="F353" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="E353" s="1"/>
+      <c r="F353" s="1"/>
       <c r="G353" s="1"/>
-      <c r="H353" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="I353" s="1"/>
-    </row>
-    <row r="354" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B354" s="1"/>
-      <c r="C354" s="1"/>
-      <c r="D354" s="10"/>
+      <c r="H353" s="12"/>
+      <c r="I353" s="13"/>
+    </row>
+    <row r="354" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B354" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C354" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D354" s="10" t="s">
+        <v>72</v>
+      </c>
       <c r="E354" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F354" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G354" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F354" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G354" s="1"/>
       <c r="H354" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I354" s="1"/>
-    </row>
-    <row r="355" spans="2:9" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+      <c r="I354" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="355" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B355" s="1"/>
       <c r="C355" s="1"/>
       <c r="D355" s="10"/>
-      <c r="E355" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F355" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G355" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H355" s="3">
-        <v>20200331</v>
-      </c>
-      <c r="I355" s="1"/>
-    </row>
-    <row r="356" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D356" s="9"/>
-    </row>
-    <row r="357" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D357" s="9"/>
-    </row>
-    <row r="358" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E355" s="1"/>
+      <c r="F355" s="1"/>
+      <c r="G355" s="1"/>
+      <c r="H355" s="3"/>
+      <c r="I355" s="13"/>
+    </row>
+    <row r="356" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B356" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C356" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D356" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="E356" s="1"/>
+      <c r="F356" s="1"/>
+      <c r="G356" s="1"/>
+      <c r="H356" s="3"/>
+      <c r="I356" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="357" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B357" s="1"/>
+      <c r="C357" s="1"/>
+      <c r="D357" s="10"/>
+      <c r="E357" s="1"/>
+      <c r="F357" s="1"/>
+      <c r="G357" s="1"/>
+      <c r="H357" s="3"/>
+      <c r="I357" s="13"/>
+    </row>
+    <row r="358" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B358" s="1" t="s">
         <v>69</v>
       </c>
       <c r="C358" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="D358" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="E358" s="8" t="s">
-        <v>326</v>
-      </c>
-      <c r="F358" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G358" s="8"/>
-      <c r="H358" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="359" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D359" s="9"/>
-      <c r="E359" s="8" t="s">
-        <v>325</v>
-      </c>
-      <c r="F359" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G359" s="8"/>
-      <c r="H359" s="18" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="360" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D360" s="9"/>
+      <c r="D358" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E358" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F358" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G358" s="1"/>
+      <c r="H358" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I358" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="359" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B359" s="1"/>
+      <c r="C359" s="1"/>
+      <c r="D359" s="10"/>
+      <c r="E359" s="1"/>
+      <c r="F359" s="1"/>
+      <c r="G359" s="1"/>
+      <c r="H359" s="3"/>
+      <c r="I359" s="13"/>
+    </row>
+    <row r="360" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B360" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C360" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D360" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E360" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F360" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G360" s="1"/>
+      <c r="H360" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I360" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="361" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D361" s="9"/>
+      <c r="B361" s="1"/>
+      <c r="C361" s="1"/>
+      <c r="D361" s="10"/>
+      <c r="E361" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F361" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G361" s="1"/>
+      <c r="H361" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="I361" s="1"/>
     </row>
     <row r="362" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D362" s="9"/>
+      <c r="B362" s="1"/>
+      <c r="C362" s="1"/>
+      <c r="D362" s="10"/>
+      <c r="E362" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F362" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G362" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H362" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I362" s="1"/>
     </row>
     <row r="363" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D363" s="9"/>
+      <c r="B363" s="1"/>
+      <c r="C363" s="1"/>
+      <c r="D363" s="10"/>
+      <c r="E363" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F363" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G363" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H363" s="3">
+        <v>20200331</v>
+      </c>
+      <c r="I363" s="1"/>
     </row>
     <row r="364" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D364" s="9"/>
@@ -5584,10 +5647,38 @@
       <c r="D365" s="9"/>
     </row>
     <row r="366" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D366" s="9"/>
-    </row>
-    <row r="367" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B366" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C366" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D366" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="E366" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="F366" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G366" s="8"/>
+      <c r="H366" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="367" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D367" s="9"/>
+      <c r="E367" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="F367" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G367" s="8"/>
+      <c r="H367" s="18" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="368" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D368" s="9"/>
@@ -5612,6 +5703,30 @@
     </row>
     <row r="375" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D375" s="9"/>
+    </row>
+    <row r="376" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D376" s="9"/>
+    </row>
+    <row r="377" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D377" s="9"/>
+    </row>
+    <row r="378" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D378" s="9"/>
+    </row>
+    <row r="379" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D379" s="9"/>
+    </row>
+    <row r="380" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D380" s="9"/>
+    </row>
+    <row r="381" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D381" s="9"/>
+    </row>
+    <row r="382" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D382" s="9"/>
+    </row>
+    <row r="383" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D383" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
rename api Request_Get_ShareRequest and change its output parameter
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="336">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -137,9 +137,6 @@
     <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"BOId\": \"1202870000086521 \",\r\n \"Name\": \"PNAKMRMTA HF\",\r\n \"da_clientcd\": \"MG040 \"\r\n }\r\n]" }</t>
   </si>
   <si>
-    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": [] }</t>
-  </si>
-  <si>
     <t>AddUnPledgeRequest</t>
   </si>
   <si>
@@ -243,9 +240,6 @@
   </si>
   <si>
     <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "\"success\"" }</t>
-  </si>
-  <si>
-    <t>RdButtonSharesChecked</t>
   </si>
   <si>
     <t>ExecuteRequestReportPageLoad</t>
@@ -1042,6 +1036,21 @@
   </si>
   <si>
     <t>53.0'</t>
+  </si>
+  <si>
+    <t>[ { "srNo": "53", "documentType": "Tplus", "date": "20210101" } ]</t>
+  </si>
+  <si>
+    <t>{ "document": "JVBERi0xLjQKJeLjz9MKMiAwIG9iago8PC9GaWx0ZXIvRmxhdGVEZWNvZGUvTGVuZ3RoIDk2MTg+PnN0cmVhbQp4nO19W3ccR3Lmu87hf8iX9ZGOZ4qV16rEk0kQkrAmQQ0BeX3W9EMLbJLwFAEt0NCK/36zsjIyI6KqC9WAudMPrbFlxzeIvHwRkZeo6Kr/88xKVzXWCVGH/7SycroVRlVWiaaWVWtbcfnl2fPTL5+UeHXz7G/Pvnt58ey75z9eb14KLy4+PvtO+rZqTCucD8rWiIsPz777/vjt2cW7F8cX4uztxYk4/vWNuHjx7+L07N/enh6fiPff//r8Tmgpbj6Kn84vxIvLzfsffhAX//Xsu5PQ+vWz70wdurbCtb7SrRNfnn1nnamMKlAHUJOhQW6T3DDZi0tQ6QfrK9u2pRWAvMit9rKXInec5MsyuoR0CTEZiaLKTRKxzS2oPLKOIY2ABtPUGB+hhfNiiTPhoiUGs7lgRGP8YIdX61V3df1JvP348epyfSR+fiF+PD0R6rk7fiN+fX36k5AXP7599+r16/N3J3/58d1fxJtf37x8cSp+OT0TR6Hb8I8Uv/z89uwkiEo5K2Xti6nKENphCN5VtdN0EEPn4vRVaKKO/0zauvGVbCWxdYKwrROUrRZlxWSzj7ZOI+sYorKt09QYH4Otpej/c/vp2Xe1+InQ5trKNzFEVF1XXpkMdQCVvxpkl+SWyTFEMtT337SllQSBUhlh7reMmM0BsYYnCRQQqSGkpXF1DGkzaWlijI3QwscDSwtYOu8dCryqLO1kQWlkpQws7DfXm9vV5Uac3cQFwchakWgepukx40aZSjtM+ICoMq4o6zJsIkfCM1QIJxAoqUJe6rbwncdWCB+gllmJGdFhzrkzdBwCrZb5k2e8c7ZVHej2hvLdb4+n13/c9Ato4Lt5LrV31tMFNE7UYcrzQlY4z2tdgvJamAZNZbpbFs7pOiuml2WyeOXRIS+PkGGWYobUxNGZQ3QcAi3DfMox0revozYcYxo1+KusalWgDqAmQ4PcJlkz2QxDTlDs35RWALIit5qHnDouQ2YRi5YIHNKqNIlFg9eINLKOITqvETA1ysdoJT3wtI2nJWupCyPX6Vx0cbv6sBavVpu1EP3RSD4P/xNWAVmie8Jd+7mHozO2g2uqRhpihwiV0Q1yU+ZC5GH+ACE7EMiK3CpwCh0jO8Dw8GLfQ8x43LgtMQXzko5DyZE09TPESvHaA13L6Jp3Xt1WcSLIe1+en8z6aZysx8RbGTaHWmHiB6jYYpBtHjeVh2M9QIV4ClmRW4WtDjpGxMPwEPERapm5uDkbwjzzi45D4Dotcy0/4akHwpYSNu+rrala7amzns076zDflnDfq3tCfUSKNQZZF+qJnK6gCULUE8iK3Go+lg39Fubz4NBZLkKO2Yvb02LmuWN0HALfccy32rGrHuhaSNeso1otK9mf97GjvsGOWjSG7IrylfY9yeHooe2gIOI/vx4fPz/urtbXG3F886G/KkhfazvV1NC5bmy4ZLC2ztebTbf+0rfSX++m0jwpxoJ2rRXVPjvrzy51LbdPoJ9pICwcncLBfTgDTfYDfx8uAKrftpDCuxc/vnktTk5Oxbvzuem5yveLCtJEs3u1mZ+dGzZPpFzb8eFs22h1He9AUe/H1z+/+fnXk0mtNFTbW8JStfOTl2GC609Xd+G2vbm6uX7IIOGyY3tqcSOnZ/+7T981zurJlB3MtndDu4sqn7CqK6UGxf959vO7Vy/evJuZr/PhMiyJ1o/3m/vbtfgn8fb3ONklM0XqO050sSafp6yrWrp0/Hn94tXJxcXMPNugZRqqdXx/e7u+vvw6735pnFhxp4Fa76tWyrSivHmR8rjbxxr++0rZhioev+kztjPjbFXFVKQ0qp7qpiHDC8y4Ok3szerz6nZ19zn4+QyXXgafYZrHb17+8sAImzYuU0Tt9Mw6o/zk2tjgZdaG4faHILTM9v/88uJMnL0NK+yLV++aJkJvbn676uKiq/4M/zStnyEBWg9hIH3DWz/5srrqQkur3/7881/6f1WXN38+3FjYcrwfDfVV5CeMKqxmTV2X/yJtFacfYkZeWdkoM5WTt9ZV4b/qN3htTKV7EySoA6j81SC7JDsmN/2GCFDcI50vrcA2KqBR2EWhX7Srsps3uuvjqzmcPIjkPLrqw7g6hji46sPEGBvDxn4NQ/eYJkhNIJoge5FbS3ez3BmRm9GNzvnxjU5MJ1pIOgJGh3gaoIaRy7h3mCpuw45DYOaGuYEf0wW3TkxXuhJjutKtOdOV7geZLiI3o1tFoovcKsT0Bd8Qr2J3YnQVn0xmCW4kZDfsWVPW1tQZECeFrHTtQWTBrQyRBRc3gOCMCr1RuRmdbAey6MlWTN8xFSGLXcrwbXAyhyK4jZDZMFuTxm6ZM0z4Fhy+MV3D1QCzlS4Pma10uchsEbkhVxLEFrm4iOl7DiaLXwzwjWTyGi+4jZDZEFnTxnbMGVpG1ngbD+Fqwl+Z0FebNqQXXSf+bdXdr+/E1bU4vf5wtboW7+5/X6/vqrmzWZ/jtLqtbAuH7qvb529WH1Zf/vKgmmor3bRpkxbPxf9ai8+rP9Zi8/nqTnxYfRUfbq7X4rev4uvN/a24uf2wvhWr6w8inBcjsrq8vLkPu9rm81p8vOm6m//bP/kO54rru9Vlf6y8Q0eFsKKHix/+98QzAStt5QPBwZlkOIy1/XPmBHUA6QwNMmg1TI6PMTKkXCXrprQCkBe51V6WIvc7iGX3S0DZ/BIAO1lqjogN3vzSqDqG5NIDmBbjgj8POHA0yRHc/PlJNqxfzvR/2VaySTHytnflpa45TLYhvDcm3iAx7xFyhfcoN4V3Ig+8A4R4J5AXudXEO/Sbec+Dy8QPiKOm4pa0mHvuEh2HwGsc86pm7KMHshaRtc1Zpe63Bk29NT61Wuyt/azJIqF8XXlH+B+gMqJBbvMMqDw8hAeo8E8hL3KrA5m538J/GluhP5rIU4txgzaEfuYZHYfAeTx1ronl9MDUw0xt9dMwYstX1fP15f3t1ebr81yy8mF9d3l7FTNMS/03ctFIbBZd90s4tsqAlD8a5LJZUDlaJUPFKhTyIrc6cAzdZqPkoWWrDIbz1I7czC22CveXjkPgUp66HGIkO/CBqgVUbfNg5VXVMAd+ef/1+VI/HaZMlg8dDiW+bQn7PVTGN4iykE/kgXyAEPkE8gIaTdxDr5n8PLRM/oAYai5uTXIe427RcQg8xzDPmlhoD1QtoGqbn2qpwuWWOerf7lfXm7DSLnbWSIMhFmjCEBpydRggNMool3MNlQcTAIRMQCAvcquJUOi32AAGV2wQEUXMNjKqJDZg3tFxCBxIMQczE+56IGsJWVsd1uhKRWKQw/50e3N3J96tNovPscPUW2wFI/vEnsRWGKAyzkE2eR5UHgobASpWoJAXudV0eYV+ixVgcMUKEXHUcNyu5CLBHaTjEPiQYz7WTrjsgawlZG112f65U/8wjhwGbm/+vr5dfVrsscPMHTGCaaqmJuexASp/NcjlTE7lwQgAISMQyIvcajIC9FvyMzC4kqCR6bkJths3q8FG4P7RcQhcyDIXc2OPPZC1iKxtHmtkU0meJzhbb3ZaYuPEyfXB+DACS45lA1TOZVF2Zaeg8mACgJAJCORFbjXxCf0WE6SxFQtEK3lqNG5TcgHmztFxCPzHU/+auGkdmHqYqa2uauHogFz1uLu5658V7OSukRlyLrMmQC3Z5Aao5L8HuQQdlaMVMlSsQCEvcqsDp7nfYgUYXDFDRBQxHLerI+cy7iAdh8CHFPOxiUPsgaxFZG1zWlvr+NPB0fp6cbNZdUs9dpg5SYZbG+IGPbjoACp/NcglyUHlwQgAISMQyIvcajIC9JuNkAeXjTAgltqNm5Vsctw/Og6BC1nmYhNPDg5kLSJrq8eGP20dO8O+W3/562Jn7SftyCZn+2f/jtAfkRJSg6zLBIg80A8Qop9AXuRWE5ep28I+DK2wb/GfTJuTJBO5X3QcSq7jqGe5icMA1UOO2o4dtd3iqGOZO6oc+Smb50j8723hSTPZ6qTWV7VuqZOe/LlrkUBtw1kk/m69DUifD05IlxCfkV7szylRVFSM9RmAxMFraCEjRkCDUXQCekwievSdEPTsOyHkSbahosYPv9OoOobk36vDpBgPowKBAz+cn/nfr4Tbf5+wqpv4MGHY6++//La8RCBSYjDxuUKiMJ9rKBKUHxunSVDZjB826/HDZiNovYcrpRnFADC6YoCIKGIzZlFkcuQExQBTfqOoV5mxgx54eoinWUdt26rtM23YUS+uviyvDYBCBMS/MZXSkvAfoTLIQdaFfyIP/AOE+CeQEblV4B86LvzTOglH6jOI1bhVLbYBd4+OQ6oUaBAPa8b+eiBsMWGzjitlOF/EMHj0EjtM3xFTQIEPMgWUAMFAoeIBJkJkM66T0OM6CSNouZIrlUXIFDA8ZIoIWWZAbmBNTME8peMQOJNlzuYmfPdA2FLC5n3XqiEV8OhVN1XVFDvkep9ih1wRlKBc6ZBmQWUzro/Q4/oII2j1kiuFRsgOuObHkVIjYjxu3IaYgXlJxyFVao2wo02cYb85W+Ua+g+tynoKU8RfF5ZTFT6hWKfQmat5EpTLF9KIqGzGRQ96XPRgBK08crlIqPgeLddxpEyIeCz36BY7Hzd2xyFV6oSwvyBWxiVV34ou9Oj/H1lS9SSqZpdL5XXlJVsuz9fd4qRpro1BJoC6HWSDVNgDJoD6BTABkc246kGPqx6MICVIrpQLFY+lhTuOFAwRN+dhQO6z3EE6DqlSMUR8bGK9/OZ0IY/9RxZXPYmqHRbMXOmC+IQqHMQn1OlAn1CMAGMishmXMOhxCYMRtKbIlfIf5ICkEMeRAiDstiOvJvdUbu+OQ6pUABGXmbjTf3vC9qVc6klkzS6aOpwx277IDy+av6xvxa/XV5udK6aKIXIxTjFELtdJUC5KSFOhshmXMuhxKYMRtLTIlSog5LmkHseROiDi7zweyGWV+0nHIVUKgYirtROe+80J25eqqSeRNe+5rYuvTnyS5+bCF2QIKMpBhoCyHTAElCiAIYhsxoUNelzYYAQtMXKlGgglsEldjiP1QMTfeTwY7LncTzoOqVIQRFxt4m7/7Qnbl+qpJ5H1wOsBVXxl6NM8N5XBIDtAgQ6yA5TwwEihTgFmQmQzrm7Q4+oGI2i5kSuVQchxcZGOI7VBxNt5NJC7PfeSjkOqFAdhR5u4XX1ztvakjOopTM37rAurbSuf6LNQBlPMkEt0ihlyEU+CcqlCmgmVzbjAQY8LHIygBUeu1AYhpyVVOo5UB2FX56HgyAmXe0nHIVXKg4ijTZxwvz1h+1JL9SSyHnjGGkzj2Dnh/fcv1x9vbtfi9fqPq/Ud/iLBwsIqZBGo2UEWgaoesAgUKoBFiGzG5Q96XP5gSq0QuDApUnKkWqi4MK3scWI6MMiBgTtMxyFV6oWIz008yPr2hO1LcdWTyJp/e6DRlfSOuvDq9u93O1dYISOkUidkA6iFglFCrRTMgsiGVFghpyWQEbRuywlS2eVIjRXyWUv+aDoQSCqWO0jHIZWrrLCLOTnhsd+arP0oR3sKUfPeavtXvzFvvfw880a6+E4Y4/tu4NMDq9+vNqtOvAlevt6I/8jvm/zP8P+fn4izm9svq+4/0wvO1qvbvqT755v7u/7NbP0fZPD15kMl3n8vzo5fC7zMj98fV4URCNM2VZhAehGkamvlG71dqzXDS+2Jlj+y9sg227WkDH+uqZazYcWYeaOhDAMM68DOXTUhRKSlaserD1fdSvy8XnWbz5erfhu8+nK1WX/Y3o7yYaa8nZf3X7draK0qx6ixE+/Ky3/fV+sb1kP/Vj9NPiIzUotPDRxVk8EB55SMqofvCNC+fGVn1fqXLGlrqJrSvn9D6pyaqyvbMLWzqXfwmdZWyuMlBxC05AAEi8cgayaTJac/AxlP1ucBsnnJGeS8PoNYqugAKVV0gKSSOGiRiLiKDgbWMSS/bh9mxti4nP+aQ3xBbdhNS9EhIKXoEJBUFDWILRU9qqOKXQ/fEcKIh5pDGBp0WEbKxo7YwpODqROJfEIIxtQxJH/nBabEWOAlmQd2GDtk71riVPB4CfGWnj8BAkl5GAOVPU7lI+oIlJ9pARG5170ib5trHTh6ioOlh0eYvPR4KbOXkueZPSJ7nHLH7GGoPLPK9EG/e0XfVhc7sPQUJ4P8DaIPMjwAwbUVBkFljy+7iD4ClbRRPqVAv3tF3zYnO7D0NCdLh0fEHhwvgT04fgJ7RPbk0IrYI0dbMX0S3jPytrrYgaNpBxuVvypftXU/7SbeuoafbP1NbL29itPz07Oj07OTWtYvw/+q/o3t5/1r4PiPZ0fPksNd1RpDu5q6rL5EN0EVzztI4eGbICQZgi1k+vqC1I2TQfHhHANWskfKH029fr+kGGw4eyuiZeqmNfVMNiPnGHbrClIMSOt4dbe5vemGtwnvkF1ATcwnF4Jv9K/6ISOdTRNAdgErKFXVy5ILSKuu9GxPObfAeprXyqkFqqXlsswC0ppOLDgTf3OE1p+E4PUnQXklibJmsiXrT4xlQ9afCKHEAlnVcPSz9QAtQHjBULlFIuLv+MHAOoaUxEKaGWPjcvol2SlIrYses2OUEq3lYYrVhjg1C+J0x84gULHaYyMVt7EsVLGGWhSrZHrLgxWrLY5W3tfCcCWTMsapZfGK1aYD1ppw6yAHhoTggE1QDr0ot1QmP4WPnt94Eq8xGKSYXgVwrLDoQfGKw0vlFrHY4I9xpHF1FCifMIZ5MS4eygMaU5nhC2WQeEoIynQlBNJWUTRUtDjTFbvGv6ccEJdTXWls0GMZKhs8YgvPTuUGiUhWtzSqjiEm05UmxXgYnUEP/HB+Fl5wCnE541SYg5xUQnLGKo2BypbkuQp5FHI50ZWoyN3uF33b3OvA0tOcDDJOiD5ISgF/kLMC/ohsSaYL8UcgV1JdQCB0vF8EbnWzA09Pc7ScdSoE5sRUgnLeKg2CypZkuwqBFHIl3QUHFuh4vwjc5mgHnp7qaOksifiD0ybwB6dR4I/I9M6J+COQE9MH432jb6ubHVja5mSj3KDRVSv7ibuqwanBictsTgvKRr3YLS3YX13rlvSip+53o7QgVnDO60VZQe0qCx/YrevG2HBVfDjhQLT8kVJHdi7FF0bYf4iYqNlaatd4tSDjsGNvkHHAav8ajPKn+Gl123+e926HlANu5IGUQ+hWt1RDzicPIOdAVKSsjF2UcyC8BB9YlHPgfTWTzlVyDmEzkGO1oLUs6YD1ppMOOrhvuKWhtSgheC1KUF5Vouyp3EiyFsWoJktRRFDSgSxweBlgCwNaivDKoXKLRMQrURpWRxHn80qU5sW4mM8RKldpLSFkfRhPPRNFELJEKwSRO5ITn6gdhSxWCyHbeK/aBSG7Y28Qsljt0SGLG1mWJcQayzL6RCPEiFoWsYSWpRHL+7IPRGzKEjI1O78f5IDFatMBq0xVh3BCAZsQHLAJyrEXZcNkRwI2Or8lERshdHggywAOFxZAKGJxhKncIhEtDtk0sI4h5fCQZsbYmA/Z/oVQyuWQdbadS7VDyBKtGER6LkEPIYvVbK200Yvy+qw3XR/puUiHkMVqjw5Z3MiykKWTXBKyWKN/o5dfFrKElqUhS/sKy8OykCWTsk4uLPHFatMhK8PJ1ZI9NiE4ZBOUg6+XHRPpFht9nwRsRJSYXgZwsLDwQQGL40vlFomI4zUNq2NIDtc0K8bEfLjWwbcVLNNStdbNnVMhXIlWCCB1JOdq6yFcsVoI12BRt+Rx+Y69QbhitUeHK25kUT0+VmhmqMzBihX6YG2WPYUjpCwNVt6Xn1WzsqniAQ5PyfcfCHQLQhVrTYdqrStnDQ7VhOBQTVAOuyhbJtPdNTo+3V0j1IjpBQCHCgseFKw4ulRukYhkd00D6xhic7immTE2ZsNVexu/6b1buFKtGEBLdleiFsK1cc2SX9CMetNHVj4crkTtseFKGlkSrkTBzJzbIVyJwvJwpaQsDNdRX4vClU7J98ws2FmJ1mS4aq8rYzwKV0BQuAIEgRdly0RFojX6vSTRGiG0tZI1AEcKix0UrTi4VG6RiBJFKwysYwgEK8yLcTEfrK2trFS7BivRWh6sWM3Wxjqj5qIOgpX1ZtojtSDhRNQeHay4kUXBihUWBStW2CFYCSlLg5X3tSxYyZQWByvWmg7WVse396BgTQgO1gTl6IyyZXKDo3VwfHIQHqBWTC8BOFRY8JRoJdGlcotExCdhGFjHkBKuaWaMjflwDb6ta1iitXa1nTtmQrhiLVkfKRMidkG4YjVbN01rmplDVQ7XHXuDcMVqjw5X3MiimyvRWFSSRufXJ2SXBSwx3dKA5X3Nq8HNlU5KKesW3VyJ2nTINrqqNdlfE4JDNkE5+HrZSCaTDXZwfrLBDpAW0wsBDhcWQChkcYSp3CIRyQabBtYxROaQTTNjbMyHrLNhvdx5hyVay3dYrGZrL03dLnikQ9RCyBp1ZJeELFZ7dMjiRhbtsFhh0Q5LZrd8hyUmWBqwvK9lOyyZ0uIdFmtNh6tTVavx15QAweGaoBx4UXZMpjtsdHzyNGeA0A5LFgEcKix4ULji6FK5RSLixzkwsI4hOdkEM2NszIerNVXr213DlWgtD1esFsK1bWu5ZIfFaiFcrT6ae+SUwxWrPTpccSOLwhUrLApXMrvl4UpMsDRceV/LwpVMaXG4Yq3pcLWBMfwkJwE4WAckR10UJZM1idXo9YrEaoTQ1kpWABwnLHJQrOLQUrlFIiocq2lgHUPK1jpMjDIxH6nGBGPoXSOVaC2PVKyWInVJngmr7RCpWO3RkYobWXYWxhrKzDxuyrFK5rc8VokRlsYq7+uhWE1nYTKpxqr+RLcgWrHadLQaVRlFNteE4HhNUA69KDsmk99nRN9XdHONUPlBJ1kFULDQ6EHRioJL5daISDbWNKiOIWVjTbNiTDzw44x+Q1D4twcJKD89SED6GcEgMRF/6WroNzeQkfxZOBgY9FfGyUaOqMJTU7lBIpKFLY2qY4jKXA1zohzwCsADNZiaZbWlhTMo+i+kpV8FJAB+MwDdU5m8kx7xRqH8fQZgIXe6T8xtcaoDQY92rVTmj5hLPwQA6tLvBDJ1RCZvjcfUEah8eyFzB93uE3fbnOtA0aPdC4r7C3dQ/p8Q+HUA9E9l8qZWxB2FyouP82kEut0n7ra414GiJ7hXOiAW6uAAmaiD8yVQR2R6jUTUEai83pWedfeLuW3OdSBoyrVGP7XQvmr7r35oU5kWkj9i+maaf2vhavVT/1uLevlvLWz8QC3pZrpWr/zaoq8c5CrWqXB9W/B7C636H2vARVQ1tZTtw5WgRCvc6mszny6HHAJWs7Wr21rOvbYVcgg79gY5BKz2+v73q+sdUgdYd1GSDyuoJUk+rOAbv/QhGunngR9m5MQB6at96PccOXFA+jJWu2puZjlxgNWmEwf9ayykw+tPQvAClKC8lkS5YTJ5EVQMZkleBDVAKHGAlzUU/XQ5QMsPWi1Ubo2I+DVQMKiOIU1efdKsGBMPJQ6kjMsPuh4nBN2PEwK33SgqKuJPyg9d40/KD0i5IKexQY9lqGzwiC08O5UbJCJ+GS6MqmNIWazTpBgPo/3swA/nZ+FJqRCXb6uFObjPJiRfd9MYqEw+W4jIo1C5JCcqcrf7Rd829zqw9DQngzsrog+utcAfXHuBPyKTTxNi/giELstAIHS8XwRudbMDT09ztHx7LQTmC26C8gU4DYLK5AtBiEAKoWszHFeg4/0icJujHXh6qqOlkyTiD46awB8cRYE/IpNPFGD+CISu0ORYvG/0bXWzA0vbnGyUanC6alU/8XCBb9KHMk7+JsgNNqcYtHL96xz0zm95Jc1PXev46xyowoO3Qcgv1GE28BaIutG10kvyC1hL6iNpFv04nKg1LtyX5dwQc35horcFP10jau/W3dXq+nLdv3Xj/m5ze7XepVABt7Qo20BGPJdtCFN08dPeWKH/dZhZlm7AeuaBggMjhy+D885spZcVKmA95b3uqykW5Buw2nS+oZaBBZJvSAheiBKUl5Qot0ym+YY+pGuab4hRLqZXN7wGsFUBrUN42YAWiFSTjEMaVseQ/B5JmBfj4oGMg/IyuAh+IA9IuVEDkq7Hg6ipSG7UsWtyo46IzTfqNDa4UZehssEjtvDsVG6QiHjVhlF1DMlvyYVJMR743nbgZ8TPsqMTIg4utYi5dO0FBG7FMAYq07t0IY9CNt+lExX5Lr1f9G1zrwNLT3OydKHF9KU7b+Yv3Ykzf0SmN2nEH4FsuUkDgXCT3i8Ct7rZgaenORpcaBGBcOcFCO7EMAgq05t0IZBCttyk4cACN+n9InCbox14eqqjDWdJzF86bWb+0mE080dkepdG/BGofLuAHoz3jb6tbnZgaZuTjTIOylZS93+vK+dKxmHmTlu+MlPH10nKdtf8A+ls6grL8w9EYXw7ZOGDfKKVlfT424+AoJN6QuBoHsUWiwqd03tetffonB6ZFhPHfnQvuBx5afEEYrhkViz0vSE/iOPpiNwPFxpLk2HzH8XKgRfghUTHEkfKe1hhLO9hCcp7VhoElhXewRBrZJ8T07ui3CfitjnUgZ/HOlbatRBvsGsBb7BLAW9IJr8ox7zhnU1M74P7RNtWtzqw89Be3mfpbdOEv9eVcfCe2/Vm2JbF++9frj/e9F+LW/8RtvP3P4ggDd+K3/qx+YdrD0lnupG6aQOO9uawGViB/z11wnVhQx++Dti/t1Y3GekAkRkaZJVkT+WBZUCaPo/hSyMJSt/ZiI1GWQnoNonI1AlBpgaVZDtoEYktMfYwro4CbX7vbp4X5WIUCweOpjjKETHvZ3HolMQ2BLfShMUIlb8aZFcGg+Vh+IAgFjEUv9ycGgVKoF9EI4wO8Rghw7jntqFUUht3DMleYJiXTLncga5ldIH38dXRWF+1qg9RXdUWluLzk8XrYpy1xwawOkDGYQMMUJuhQfZ5AkQenl4BUgxAoP47qdBoojL3iwwAo0MGiFDDzMbN6ogBqHt0DMkO1DAH8xP+ShSRv7qxv7ot/jqWucPimbotMx3L//2tPGlGC9fLtM7aurKtxntOQvCek6AcPlE2TLajmEvfqySQE9M7GbEJ3QPQpoM3CdQiFvELQGFgHUPy67XzzCgbo535W7G0H1vz41miV6BlGzTiElZ+RCZsDtAl+DeMiMh2HDV2HDWubDkkajTxObb04y1n8sjlBPd1bFhE6aQ7GOYuU773zQnbpz36SYTNXpqMq4cUo1XBfYeN+vjFL2/+9WLnvbpYIu+ZxRJ5W01Q3nbTPKhsyWZdXJdCTkyfACa2MD/eNvi+ygPCEddljtJxyJTdmvian3Ddb07YPp1unkTYrOvauq5cJK247sXbixevw1U/XPvf/zCTia91iJIQsUbFJgbd1Z+r37q1+GPV3a/FzUdxvr794+pyfdenDm5v/r6+XX1ai38Wx59Xt5/6BML29vvvcbta0fa9sVUz8e7aklIISv2yMqeEtt3wf3XTEvdJEHafBGVHiLKnciuJ+0T+ifdEBHkP8UmHLcZ2QbTv4m1S5SaJiLfdNK6OIk25EqeJMTYuJ98a1WdllA9/pVVlTHrn+y+rr6fXz8O/b+434u1v3dWn1ebq5nqmyM8GAznayETKZ1SsVwe1PnX7gB4yra4r2dCVIUHYtAnKVoqyYbIjpo0s0aU0Qo2YdhiHiWVUI9tiW6jcJBHJyTONrGNIOVOlqTE+po1rpAyrTvgrpSqlU9y83Xxe34ZQ/XQ3V6fbv7/VUEWpwpo/Y0wVdPpFa0YHGVL6yjsaownChkxQNkkvN0ykIRoJIWaMiBLTzuEwhYxUZEbMuspNEhFbMY2rY0g2YpoW42JLhHpZqX7xC1zW8M2j4/X15nbViZ/OL8S/CP8/FpgSq7e2kjM/ls6mnNFBpqx91ThDTJkgbMoEZbNE2TK5IbaMvDhizAihmCQO4jCVjFxkTMy+yk0SEb+yGkbWMSS/shqmxvjYZk5XWRs22FrGRFDk9nyz2qx3MSZWXmrMGZ1iTOl9GJ7HxgQIGRMgMEuUHRMVsWUkRRJbRggFJvEQh3lkzCJbYupVbpKI+F3GMLKOIWBKmBhjY/vy6uJ0w/9V6Y2z5ycvT8WPJyfnc1YMNxFD1fqNYM6GQcPpORVkwtbHynlswgRhEyYo2yzKjskkHgc2SDwOUCumHcNhAhmlxYaEc5WbJCKORxhZx5BixDQ1xsd2I2rZz1dWRpZ4/PK7eHW/mfnVBcQiUXzoleIpFud0kCEbX0lL7Dgg2IwDku0RRclkEokDHSQSB0iLad9wmEHGKbIiJl3lJolIIjGNrGNIfvVpmhnlYosNdbCh6mcbtkqZXjJxfnExY7z+GuJaqqGbBz4XGt9zq+aVkPlcG1/qge2XIGzABGVbRNkxuSUW7Lkw5JAzQCgOsVs4xB6lE5kPsa1yc0TEJxwYVceQEoNpWoyLy/kfmEjb9l8HLvnSBKB0aUIg2zOIkska54iGvlGmCSCTs6V5tKnXMlo2fkQYniBqEYv4FUQwsI4hxd/TxAgTPKN8IGhM0LJaWcRcSkoi6lLaEnpI6ZjcP5E1TuJg6ghkci408wDd7hN325zrQNGj3SuvuZm7vCgPSF6zU/9U1mSlL9xRyIjp/cPtF3db3OtA0cG9Du71/9+9xsn+4bmCdP1Vpi11gasvN/fXG/Fufbm++qNP/b///q/vfxDPxS+rr4P4z0F8+VUcd1fr681Mut82lfWG9hAOFL5tJ4/aL3FmWDaL9c5EO/RX2yrWHoYLtoNk9qe1OLs5+iv6pt7/A6nBW9UKZW5kc3RyZWFtCmVuZG9iago1IDAgb2JqCjw8L1R5cGUvRm9udERlc2NyaXB0b3IvRm9udE5hbWUvQXJpYWwvRmxhZ3MgMzIvRm9udEJCb3hbLTI1MCAtMjIxIDExOTAgMTAwMF0vTWlzc2luZ1dpZHRoIDI3Mi9TdGVtViA4MC9TdGVtSCA4MC9JdGFsaWNBbmdsZSAwL0NhcEhlaWdodCA5MDUvWEhlaWdodCA0NTMvQXNjZW50IDkwNS9EZXNjZW50IC0yMTIvTGVhZGluZyAxNTAvTWF4V2lkdGggOTkyL0F2Z1dpZHRoIDQ0MT4+CmVuZG9iago0IDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50Ti9CYXNlRm9udC9BcmlhbC9GaXJzdENoYXIgMzIvTGFzdENoYXIgMjU1L0ZvbnREZXNjcmlwdG9yIDUgMCBSL0VuY29kaW5nL1dpbkFuc2lFbmNvZGluZy9XaWR0aHNbMjc4IDI3OCAzNTUgNTU2IDU1NiA4ODkgNjY3IDE5MSAzMzMgMzMzIDM4OSA1ODQgMjc4IDMzMyAyNzggMjc4IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiAyNzggMjc4IDU4NCA1ODQgNTg0IDU1NiAxMDE1IDY2NyA2NjcgNzIyIDcyMiA2NjcgNjExIDc3OCA3MjIgMjc4IDUwMCA2NjcgNTU2IDgzMyA3MjIgNzc4IDY2NyA3NzggNzIyIDY2NyA2MTEgNzIyIDY2NyA5NDQgNjY3IDY2NyA2MTEgMjc4IDI3OCAyNzggNDY5IDU1NiAzMzMgNTU2IDU1NiA1MDAgNTU2IDU1NiAyNzggNTU2IDU1NiAyMjIgMjIyIDUwMCAyMjIgODMzIDU1NiA1NTYgNTU2IDU1NiAzMzMgNTAwIDI3OCA1NTYgNTAwIDcyMiA1MDAgNTAwIDUwMCAzMzQgMjYwIDMzNCA1ODQgNzUwIDU1NiA3NTAgMjIyIDU1NiAzMzMgMTAwMCA1NTYgNTU2IDMzMyAxMDAwIDY2NyAzMzMgMTAwMCA3NTAgNjExIDc1MCA3NTAgMjIyIDIyMiAzMzMgMzMzIDM1MCA1NTYgMTAwMCAzMzMgMTAwMCA1MDAgMzMzIDk0NCA3NTAgNTAwIDY2NyAyNzggMzMzIDU1NiA1NTYgNTU2IDU1NiAyNjAgNTU2IDMzMyA3MzcgMzcwIDU1NiA1ODQgMzMzIDczNyA1NTIgNDAwIDU0OSAzMzMgMzMzIDMzMyA1NzYgNTM3IDI3OCAzMzMgMzMzIDM2NSA1NTYgODM0IDgzNCA4MzQgNjExIDY2NyA2NjcgNjY3IDY2NyA2NjcgNjY3IDEwMDAgNzIyIDY2NyA2NjcgNjY3IDY2NyAyNzggMjc4IDI3OCAyNzggNzIyIDcyMiA3NzggNzc4IDc3OCA3NzggNzc4IDU4NCA3NzggNzIyIDcyMiA3MjIgNzIyIDY2NyA2NjcgNjExIDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDg4OSA1MDAgNTU2IDU1NiA1NTYgNTU2IDI3OCAyNzggMjc4IDI3OCA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTQ5IDYxMSA1NTYgNTU2IDU1NiA1NTYgNTAwIDU1NiA1MDBdPj4KZW5kb2JqCjcgMCBvYmoKPDwvVHlwZS9Gb250RGVzY3JpcHRvci9Gb250TmFtZS9BcmlhbCxCb2xkL0ZsYWdzIDE2NDE2L0ZvbnRCQm94Wy0yNTAgLTIxMiAxMTIwIDEwMDBdL01pc3NpbmdXaWR0aCAzMTEvU3RlbVYgMTUzL1N0ZW1IIDE1My9JdGFsaWNBbmdsZSAwL0NhcEhlaWdodCA5MDUvWEhlaWdodCA0NTMvQXNjZW50IDkwNS9EZXNjZW50IC0yMTIvTGVhZGluZyAxNTAvTWF4V2lkdGggOTMzL0F2Z1dpZHRoIDQ3OT4+CmVuZG9iago2IDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50Qi9CYXNlRm9udC9BcmlhbCxCb2xkL0ZpcnN0Q2hhciAzMi9MYXN0Q2hhciAyNTUvRm9udERlc2NyaXB0b3IgNyAwIFIvRW5jb2RpbmcvV2luQW5zaUVuY29kaW5nL1dpZHRoc1syNzggMzMzIDQ3NCA1NTYgNTU2IDg4OSA3MjIgMjM4IDMzMyAzMzMgMzg5IDU4NCAyNzggMzMzIDI3OCAyNzggNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDMzMyAzMzMgNTg0IDU4NCA1ODQgNjExIDk3NSA3MjIgNzIyIDcyMiA3MjIgNjY3IDYxMSA3NzggNzIyIDI3OCA1NTYgNzIyIDYxMSA4MzMgNzIyIDc3OCA2NjcgNzc4IDcyMiA2NjcgNjExIDcyMiA2NjcgOTQ0IDY2NyA2NjcgNjExIDMzMyAyNzggMzMzIDU4NCA1NTYgMzMzIDU1NiA2MTEgNTU2IDYxMSA1NTYgMzMzIDYxMSA2MTEgMjc4IDI3OCA1NTYgMjc4IDg4OSA2MTEgNjExIDYxMSA2MTEgMzg5IDU1NiAzMzMgNjExIDU1NiA3NzggNTU2IDU1NiA1MDAgMzg5IDI4MCAzODkgNTg0IDc1MCA1NTYgNzUwIDI3OCA1NTYgNTAwIDEwMDAgNTU2IDU1NiAzMzMgMTAwMCA2NjcgMzMzIDEwMDAgNzUwIDYxMSA3NTAgNzUwIDI3OCAyNzggNTAwIDUwMCAzNTAgNTU2IDEwMDAgMzMzIDEwMDAgNTU2IDMzMyA5NDQgNzUwIDUwMCA2NjcgMjc4IDMzMyA1NTYgNTU2IDU1NiA1NTYgMjgwIDU1NiAzMzMgNzM3IDM3MCA1NTYgNTg0IDMzMyA3MzcgNTUyIDQwMCA1NDkgMzMzIDMzMyAzMzMgNTc2IDU1NiAyNzggMzMzIDMzMyAzNjUgNTU2IDgzNCA4MzQgODM0IDYxMSA3MjIgNzIyIDcyMiA3MjIgNzIyIDcyMiAxMDAwIDcyMiA2NjcgNjY3IDY2NyA2NjcgMjc4IDI3OCAyNzggMjc4IDcyMiA3MjIgNzc4IDc3OCA3NzggNzc4IDc3OCA1ODQgNzc4IDcyMiA3MjIgNzIyIDcyMiA2NjcgNjY3IDYxMSA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA4ODkgNTU2IDU1NiA1NTYgNTU2IDU1NiAyNzggMjc4IDI3OCAyNzggNjExIDYxMSA2MTEgNjExIDYxMSA2MTEgNjExIDU0OSA2MTEgNjExIDYxMSA2MTEgNjExIDU1NiA2MTEgNTU2XT4+CmVuZG9iago5IDAgb2JqCjw8L1R5cGUvRm9udERlc2NyaXB0b3IvRm9udE5hbWUvQ291cmllck5ldyxJdGFsaWMvRmxhZ3MgOTgvRm9udEJCb3hbLTI1MCAtMzAwIDcyMCAxMDAwXS9NaXNzaW5nV2lkdGggNjAwL1N0ZW1WIDEwOS9TdGVtSCAxMDkvSXRhbGljQW5nbGUgLTExL0NhcEhlaWdodCA4MzMvWEhlaWdodCA0MTcvQXNjZW50IDgzMy9EZXNjZW50IC0zMDAvTGVhZGluZyAxMzMvTWF4V2lkdGggNjAwL0F2Z1dpZHRoIDYwMD4+CmVuZG9iago4IDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50MS9CYXNlRm9udC9Db3VyaWVyTmV3LEl0YWxpYy9GaXJzdENoYXIgMzIvTGFzdENoYXIgMjU1L0ZvbnREZXNjcmlwdG9yIDkgMCBSL0VuY29kaW5nL1dpbkFuc2lFbmNvZGluZy9XaWR0aHNbNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMCA2MDAgNjAwIDYwMF0+PgplbmRvYmoKMTEgMCBvYmoKPDwvVHlwZS9Gb250RGVzY3JpcHRvci9Gb250TmFtZS9UaW1lc05ld1JvbWFuL0ZsYWdzIDM0L0ZvbnRCQm94Wy0yNTAgLTIxNiAxMjAwIDEwMDBdL01pc3NpbmdXaWR0aCAzMzMvU3RlbVYgNzMvU3RlbUggNzMvSXRhbGljQW5nbGUgMC9DYXBIZWlnaHQgODkxL1hIZWlnaHQgNDQ2L0FzY2VudCA4OTEvRGVzY2VudCAtMjE2L0xlYWRpbmcgMTQ5L01heFdpZHRoIDEwMDAvQXZnV2lkdGggNDAxPj4KZW5kb2JqCjEwIDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50Mi9CYXNlRm9udC9UaW1lc05ld1JvbWFuL0ZpcnN0Q2hhciAzMi9MYXN0Q2hhciAyNTUvRm9udERlc2NyaXB0b3IgMTEgMCBSL0VuY29kaW5nL1dpbkFuc2lFbmNvZGluZy9XaWR0aHNbMjUwIDMzMyA0MDggNTAwIDUwMCA4MzMgNzc4IDE4MCAzMzMgMzMzIDUwMCA1NjQgMjUwIDMzMyAyNTAgMjc4IDUwMCA1MDAgNTAwIDUwMCA1MDAgNTAwIDUwMCA1MDAgNTAwIDUwMCAyNzggMjc4IDU2NCA1NjQgNTY0IDQ0NCA5MjEgNzIyIDY2NyA2NjcgNzIyIDYxMSA1NTYgNzIyIDcyMiAzMzMgMzg5IDcyMiA2MTEgODg5IDcyMiA3MjIgNTU2IDcyMiA2NjcgNTU2IDYxMSA3MjIgNzIyIDk0NCA3MjIgNzIyIDYxMSAzMzMgMjc4IDMzMyA0NjkgNTAwIDMzMyA0NDQgNTAwIDQ0NCA1MDAgNDQ0IDMzMyA1MDAgNTAwIDI3OCAyNzggNTAwIDI3OCA3NzggNTAwIDUwMCA1MDAgNTAwIDMzMyAzODkgMjc4IDUwMCA1MDAgNzIyIDUwMCA1MDAgNDQ0IDQ4MCAyMDAgNDgwIDU0MSA3NzggNTAwIDc3OCAzMzMgNTAwIDQ0NCAxMDAwIDUwMCA1MDAgMzMzIDEwMDAgNTU2IDMzMyA4ODkgNzc4IDYxMSA3NzggNzc4IDMzMyAzMzMgNDQ0IDQ0NCAzNTAgNTAwIDEwMDAgMzMzIDk4MCAzODkgMzMzIDcyMiA3NzggNDQ0IDcyMiAyNTAgMzMzIDUwMCA1MDAgNTAwIDUwMCAyMDAgNTAwIDMzMyA3NjAgMjc2IDUwMCA1NjQgMzMzIDc2MCA1MDAgNDAwIDU0OSAzMDAgMzAwIDMzMyA1NzYgNDUzIDI1MCAzMzMgMzAwIDMxMCA1MDAgNzUwIDc1MCA3NTAgNDQ0IDcyMiA3MjIgNzIyIDcyMiA3MjIgNzIyIDg4OSA2NjcgNjExIDYxMSA2MTEgNjExIDMzMyAzMzMgMzMzIDMzMyA3MjIgNzIyIDcyMiA3MjIgNzIyIDcyMiA3MjIgNTY0IDcyMiA3MjIgNzIyIDcyMiA3MjIgNzIyIDU1NiA1MDAgNDQ0IDQ0NCA0NDQgNDQ0IDQ0NCA0NDQgNjY3IDQ0NCA0NDQgNDQ0IDQ0NCA0NDQgMjc4IDI3OCAyNzggMjc4IDUwMCA1MDAgNTAwIDUwMCA1MDAgNTAwIDUwMCA1NDkgNTAwIDUwMCA1MDAgNTAwIDUwMCA1MDAgNTAwIDUwMF0+PgplbmRvYmoKMTMgMCBvYmoKPDwvVHlwZS9Gb250RGVzY3JpcHRvci9Gb250TmFtZS9BcmlhbCxCb2xkSXRhbGljL0ZsYWdzIDE2NDgwL0ZvbnRCQm94Wy0yNTAgLTIxMiAxMTIwIDEwMDBdL01pc3NpbmdXaWR0aCAzMTEvU3RlbVYgMTUzL1N0ZW1IIDE1My9JdGFsaWNBbmdsZSAtMTEvQ2FwSGVpZ2h0IDkwNS9YSGVpZ2h0IDQ1My9Bc2NlbnQgOTA1L0Rlc2NlbnQgLTIxMi9MZWFkaW5nIDE1MC9NYXhXaWR0aCA5MzMvQXZnV2lkdGggNDc5Pj4KZW5kb2JqCjEyIDAgb2JqCjw8L1R5cGUvRm9udC9TdWJ0eXBlL1RydWVUeXBlL05hbWUvRm50My9CYXNlRm9udC9BcmlhbCxCb2xkSXRhbGljL0ZpcnN0Q2hhciAzMi9MYXN0Q2hhciAyNTUvRm9udERlc2NyaXB0b3IgMTMgMCBSL0VuY29kaW5nL1dpbkFuc2lFbmNvZGluZy9XaWR0aHNbMjc4IDMzMyA0NzQgNTU2IDU1NiA4ODkgNzIyIDIzOCAzMzMgMzMzIDM4OSA1ODQgMjc4IDMzMyAyNzggMjc4IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgNTU2IDU1NiAzMzMgMzMzIDU4NCA1ODQgNTg0IDYxMSA5NzUgNzIyIDcyMiA3MjIgNzIyIDY2NyA2MTEgNzc4IDcyMiAyNzggNTU2IDcyMiA2MTEgODMzIDcyMiA3NzggNjY3IDc3OCA3MjIgNjY3IDYxMSA3MjIgNjY3IDk0NCA2NjcgNjY3IDYxMSAzMzMgMjc4IDMzMyA1ODQgNTU2IDMzMyA1NTYgNjExIDU1NiA2MTEgNTU2IDMzMyA2MTEgNjExIDI3OCAyNzggNTU2IDI3OCA4ODkgNjExIDYxMSA2MTEgNjExIDM4OSA1NTYgMzMzIDYxMSA1NTYgNzc4IDU1NiA1NTYgNTAwIDM4OSAyODAgMzg5IDU4NCA3NTAgNTU2IDc1MCAyNzggNTU2IDUwMCAxMDAwIDU1NiA1NTYgMzMzIDEwMDAgNjY3IDMzMyAxMDAwIDc1MCA2MTEgNzUwIDc1MCAyNzggMjc4IDUwMCA1MDAgMzUwIDU1NiAxMDAwIDMzMyAxMDAwIDU1NiAzMzMgOTQ0IDc1MCA1MDAgNjY3IDI3OCAzMzMgNTU2IDU1NiA1NTYgNTU2IDI4MCA1NTYgMzMzIDczNyAzNzAgNTU2IDU4NCAzMzMgNzM3IDU1MiA0MDAgNTQ5IDMzMyAzMzMgMzMzIDU3NiA1NTYgMjc4IDMzMyAzMzMgMzY1IDU1NiA4MzQgODM0IDgzNCA2MTEgNzIyIDcyMiA3MjIgNzIyIDcyMiA3MjIgMTAwMCA3MjIgNjY3IDY2NyA2NjcgNjY3IDI3OCAyNzggMjc4IDI3OCA3MjIgNzIyIDc3OCA3NzggNzc4IDc3OCA3NzggNTg0IDc3OCA3MjIgNzIyIDcyMiA3MjIgNjY3IDY2NyA2MTEgNTU2IDU1NiA1NTYgNTU2IDU1NiA1NTYgODg5IDU1NiA1NTYgNTU2IDU1NiA1NTYgMjc4IDI3OCAyNzggMjc4IDYxMSA2MTEgNjExIDYxMSA2MTEgNjExIDYxMSA1NDkgNjExIDYxMSA2MTEgNjExIDYxMSA1NTYgNjExIDU1Nl0+PgplbmRvYmoKMTUgMCBvYmoKPDwvTGVuZ3RoIDQ4Pj5zdHJlYW0KAAAAAAA/AD8AAD8/PwAAPwA/Pz8APz8/wMDAAAD/AP8AAP///wAA/wD///8A////CmVuZHN0cmVhbQplbmRvYmoKMTQgMCBvYmoKPDwvVHlwZS9YT2JqZWN0L1N1YnR5cGUvSW1hZ2UvTmFtZS9JbWcxL1dpZHRoIDg4L0hlaWdodCAxOS9CaXRzUGVyQ29tcG9uZW50IDQvQ29sb3JTcGFjZVsvSW5kZXhlZC9EZXZpY2VSR0IgMTUgMTUgMCBSXS9MZW5ndGggODM2Pj5zdHJlYW0K////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////f///////////////P/////////////////////////////////d4d394P3c/93d39z8//394dz8/+I//////////////////////////////P3c/f3d4eHh3Pz/3P/ePd3h4d3+P//////////////8I//////////////////////////////+P//+P//////////////////////CP///////////////////////////////////////////////wj///P//wjwAAAH/wd3cP93/3D/AHd39wd3D/cHdw/3f/+A//8Hd3j/////CPP/8/+Aj/cGZmD/D//wj3f3D/8I///4//8I+P//CPd//wcP/w////////8AAADz93cP92BgYP8P93D/cHdw/wB3//P3dw/z93d/93/3fwj/B3f//////wj/8PP//wj3ZmYA/w//+P93//D/CP//93//j/eP/4/3f4D/8P8I////////AHcH8/d3D/PwAAD/F3dw/3B3AP8Adwfz93cP8/d3D/d/CP/3jwB3A/j/////////////////93//////////////////////////////////////////////////////////cP////////////////////////////////////////////////////////9w////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////////8KZW5kc3RyZWFtCmVuZG9iagoxNiAwIG9iago8PC9UeXBlL1hPYmplY3QvU3VidHlwZS9JbWFnZS9GaWx0ZXJbL0RDVERlY29kZV0vV2lkdGggMTAyNC9IZWlnaHQgMTU3L0NvbG9yU3BhY2UvRGV2aWNlUkdCL0JpdHNQZXJDb21wb25lbnQgOC9MZW5ndGggMjk5NzcvTmFtZS9JbWcyPj5zdHJlYW0K/9j/4AAQSkZJRgABAgECWAJYAAD/4QdBRXhpZgAATU0AKgAAAAgABwESAAMAAAABAAEAAAEaAAUAAAABAAAAYgEbAAUAAAABAAAAagEoAAMAAAABAAIAAAExAAIAAAAUAAAAcgEyAAIAAAAUAAAAhodpAAQAAAABAAAAnAAAAMgAAAJYAAAAAQAAAlgAAAABQWRvYmUgUGhvdG9zaG9wIDcuMAAyMDIxOjA0OjAyIDExOjI1OjA4AAAAAAOgAQADAAAAAf//AACgAgAEAAAAAQAABACgAwAEAAAAAQAAAJ0AAAAAAAAABgEDAAMAAAABAAYAAAEaAAUAAAABAAABFgEbAAUAAAABAAABHgEoAAMAAAABAAIAAAIBAAQAAAABAAABJgICAAQAAAABAAAGEwAAAAAAAABIAAAAAQAAAEgAAAAB/9j/4AAQSkZJRgABAgEASABIAAD/7QAMQWRvYmVfQ00AAv/uAA5BZG9iZQBkgAAAAAH/2wCEAAwICAgJCAwJCQwRCwoLERUPDAwPFRgTExUTExgRDAwMDAwMEQwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwBDQsLDQ4NEA4OEBQODg4UFA4ODg4UEQwMDAwMEREMDAwMDAwRDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDP/AABEIABQAgAMBIgACEQEDEQH/3QAEAAj/xAE/AAABBQEBAQEBAQAAAAAAAAADAAECBAUGBwgJCgsBAAEFAQEBAQEBAAAAAAAAAAEAAgMEBQYHCAkKCxAAAQQBAwIEAgUHBggFAwwzAQACEQMEIRIxBUFRYRMicYEyBhSRobFCIyQVUsFiMzRygtFDByWSU/Dh8WNzNRaisoMmRJNUZEXCo3Q2F9JV4mXys4TD03Xj80YnlKSFtJXE1OT0pbXF1eX1VmZ2hpamtsbW5vY3R1dnd4eXp7fH1+f3EQACAgECBAQDBAUGBwcGBTUBAAIRAyExEgRBUWFxIhMFMoGRFKGxQiPBUtHwMyRi4XKCkkNTFWNzNPElBhaisoMHJjXC0kSTVKMXZEVVNnRl4vKzhMPTdePzRpSkhbSVxNTk9KW1xdXl9VZmdoaWprbG1ub2JzdHV2d3h5ent8f/2gAMAwEAAhEDEQA/AO4619ZsbByaMHGtrfnvycem3HeHEiu1zPUc3bt9/pP3tT/Vf6y4/WsKkWW1/tE1mzIoqDgGQ7Z/hN/7zP8ACKPXOh5F+TRn4Fl5yhlY7rWC9zKhSxzfX/Q7vT/mm/QS+qvRMjp+FTfnPvPUX1luSyy91rJLt0tbufVu9v5iZ6+Lw/Z/3zCDl9zpw2en6PT/AA3eWD1DO65j591WOBfTOP6TG0+8C03+sBdZfXjvfUzG/wAJ6P8AP/pP8Gt5Y9/VepVdSsqZiPtxXbKqH7HgCwWVV5Ftj2sf+h9PL31+zZ+oZH6X9J+jezNE/WPqTqW2ei6it7aqzfZjvDWXF1bs0ub63qNZRjW2e22quurJxL6/tN30Eh9YOo7L3OjfVj2W47G0wcgt+1+jbTXbcy39M3Gpf6LP3/5707mI7Os9Vvyam/Y7sestZvb6T3S578GXOe6pnpVsZfmM/wBLsouvfWz01cp6vbaR+p3Vhzq2AWVvB/SAO9R0MdspZ7q37/ex9f6RBTXv61l41V1VrNuaytt1NLmSXM32iz+j2Wsttrpp9Syqiz/R/wCl9NNj9dsty6muM1XWuZjtrqcfUr32VsyW2Pe1r6m+nusso9TYz9PYz7PkY9qWT1DqRb022pltdV9L7MoOpeXtcPQ2sexlFrvU9936vsx/W/01Xpo1fWsiwx9iuZLi1pNdndrHscd1bG7fUe+q39J/gklNTI6n1XFy7G32sbi/bDjttNJbtq+zfbhYbLLvTf8Ap3fZt38j/TKZ61nHK9Olous9f0rMQ1PY6pge+tt78rd6P6aprL6t7f0zPfSidS6h1asYl2DU61t1Fhuq9F8te4V/Zrju2Pr9G0/psZ/6b0v+IRbesZDS2ujDussOwTZXYxvvdjt3ueymxntqynWvZ/3Wvr/R+mkpz6PrF1U1NOTiurfZq0sote1m2iu7Iruh25z6n2uvp9P+l1UW4dX61/OH/b1gx8htLhlZLanuwyKntbeWb9z6Q0u9drNv0Kf5/wBP1Mf+eqSb1vqe+q5+DcK3th+O1jyQT9lu3te+mv3VU5OQx9b/AOdtxLK6v0vsWlhZxynuBrtrDWg/pK3sBO6xntdbXX9JrGP/AKj0lOG76wdRZu94tx2OP2fKrx3O+1Eej+rUVuurr9VnqXN9tv616f6r+kx8mpWWdcyfWyBkPFApZLKzS6SP9LAe/IsYz8/0sf0/Yt9JFTXwMkZeIy8SQ4uAJESGucze2C9rq37d9djP0d1f6WtWEkklP//Q9VSXyqkkp+qkl8qpJKfqpJfKqSSn6qSXyqkkp+qkl8qpJKfqpJfKqSSn6qSXyqkkp+qkl8qpJKf/2f/tDBJQaG90b3Nob3AgMy4wADhCSU0EJQAAAAAAEAAAAAAAAAAAAAAAAAAAAAA4QklNA+0AAAAAABACWAAAAAEAAgJYAAAAAQACOEJJTQQmAAAAAAAOAAAAAAAAAAAAAD+AAAA4QklNBA0AAAAAAAQAAAAeOEJJTQQZAAAAAAAEAAAAHjhCSU0D8wAAAAAACQAAAAAAAAAAAQA4QklNBAoAAAAAAAEAADhCSU0nEAAAAAAACgABAAAAAAAAAAI4QklNA/UAAAAAAEgAL2ZmAAEAbGZmAAYAAAAAAAEAL2ZmAAEAoZmaAAYAAAAAAAEAMgAAAAEAWgAAAAYAAAAAAAEANQAAAAEALQAAAAYAAAAAAAE4QklNA/gAAAAAAHAAAP////////////////////////////8D6AAAAAD/////////////////////////////A+gAAAAA/////////////////////////////wPoAAAAAP////////////////////////////8D6AAAOEJJTQQAAAAAAAACAAM4QklNBAIAAAAAAAgAAAAAAAAAADhCSU0ECAAAAAAAEAAAAAEAAAJAAAACQAAAAAA4QklNBB4AAAAAAAQAAAAAOEJJTQQaAAAAAANbAAAABgAAAAAAAAAAAAAAnQAABAAAAAATAEMAbwBtAGIAaQBuAGUAZABDAG8AbgB0AHIAYQBjAHQASgBQAEcAAAABAAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAAAABAAAAACdAAAAAAAAAAAAAAAAAAAAAAEAAAAAAAAAAAAAAAAAAAAAAAAAEAAAAAEAAAAAAABudWxsAAAAAgAAAAZib3VuZHNPYmpjAAAAAQAAAAAAAFJjdDEAAAAEAAAAAFRvcCBsb25nAAAAAAAAAABMZWZ0bG9uZwAAAAAAAAAAQnRvbWxvbmcAAACdAAAAAFJnaHRsb25nAAAEAAAAAAZzbGljZXNWbExzAAAAAU9iamMAAAABAAAAAAAFc2xpY2UAAAASAAAAB3NsaWNlSURsb25nAAAAAAAAAAdncm91cElEbG9uZwAAAAAAAAAGb3JpZ2luZW51bQAAAAxFU2xpY2VPcmlnaW4AAAANYXV0b0dlbmVyYXRlZAAAAABUeXBlZW51bQAAAApFU2xpY2VUeXBlAAAAAEltZyAAAAAGYm91bmRzT2JqYwAAAAEAAAAAAABSY3QxAAAABAAAAABUb3AgbG9uZwAAAAAAAAAATGVmdGxvbmcAAAAAAAAAAEJ0b21sb25nAAAAnQAAAABSZ2h0bG9uZwAABAAAAAADdXJsVEVYVAAAAAEAAAAAAABudWxsVEVYVAAAAAEAAAAAAABNc2dlVEVYVAAAAAEAAAAAAAZhbHRUYWdURVhUAAAAAQAAAAAADmNlbGxUZXh0SXNIVE1MYm9vbAEAAAAIY2VsbFRleHRURVhUAAAAAQAAAAAACWhvcnpBbGlnbmVudW0AAAAPRVNsaWNlSG9yekFsaWduAAAAB2RlZmF1bHQAAAAJdmVydEFsaWduZW51bQAAAA9FU2xpY2VWZXJ0QWxpZ24AAAAHZGVmYXVsdAAAAAtiZ0NvbG9yVHlwZWVudW0AAAARRVNsaWNlQkdDb2xvclR5cGUAAAAATm9uZQAAAAl0b3BPdXRzZXRsb25nAAAAAAAAAApsZWZ0T3V0c2V0bG9uZwAAAAAAAAAMYm90dG9tT3V0c2V0bG9uZwAAAAAAAAALcmlnaHRPdXRzZXRsb25nAAAAAAA4QklNBBEAAAAAAAEBADhCSU0EFAAAAAAABAAAAAQ4QklNBAwAAAAABi8AAAABAAAAgAAAABQAAAGAAAAeAAAABhMAGAAB/9j/4AAQSkZJRgABAgEASABIAAD/7QAMQWRvYmVfQ00AAv/uAA5BZG9iZQBkgAAAAAH/2wCEAAwICAgJCAwJCQwRCwoLERUPDAwPFRgTExUTExgRDAwMDAwMEQwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwBDQsLDQ4NEA4OEBQODg4UFA4ODg4UEQwMDAwMEREMDAwMDAwRDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDAwMDP/AABEIABQAgAMBIgACEQEDEQH/3QAEAAj/xAE/AAABBQEBAQEBAQAAAAAAAAADAAECBAUGBwgJCgsBAAEFAQEBAQEBAAAAAAAAAAEAAgMEBQYHCAkKCxAAAQQBAwIEAgUHBggFAwwzAQACEQMEIRIxBUFRYRMicYEyBhSRobFCIyQVUsFiMzRygtFDByWSU/Dh8WNzNRaisoMmRJNUZEXCo3Q2F9JV4mXys4TD03Xj80YnlKSFtJXE1OT0pbXF1eX1VmZ2hpamtsbW5vY3R1dnd4eXp7fH1+f3EQACAgECBAQDBAUGBwcGBTUBAAIRAyExEgRBUWFxIhMFMoGRFKGxQiPBUtHwMyRi4XKCkkNTFWNzNPElBhaisoMHJjXC0kSTVKMXZEVVNnRl4vKzhMPTdePzRpSkhbSVxNTk9KW1xdXl9VZmdoaWprbG1ub2JzdHV2d3h5ent8f/2gAMAwEAAhEDEQA/AO4619ZsbByaMHGtrfnvycem3HeHEiu1zPUc3bt9/pP3tT/Vf6y4/WsKkWW1/tE1mzIoqDgGQ7Z/hN/7zP8ACKPXOh5F+TRn4Fl5yhlY7rWC9zKhSxzfX/Q7vT/mm/QS+qvRMjp+FTfnPvPUX1luSyy91rJLt0tbufVu9v5iZ6+Lw/Z/3zCDl9zpw2en6PT/AA3eWD1DO65j591WOBfTOP6TG0+8C03+sBdZfXjvfUzG/wAJ6P8AP/pP8Gt5Y9/VepVdSsqZiPtxXbKqH7HgCwWVV5Ftj2sf+h9PL31+zZ+oZH6X9J+jezNE/WPqTqW2ei6it7aqzfZjvDWXF1bs0ub63qNZRjW2e22quurJxL6/tN30Eh9YOo7L3OjfVj2W47G0wcgt+1+jbTXbcy39M3Gpf6LP3/5707mI7Os9Vvyam/Y7sestZvb6T3S578GXOe6pnpVsZfmM/wBLsouvfWz01cp6vbaR+p3Vhzq2AWVvB/SAO9R0MdspZ7q37/ex9f6RBTXv61l41V1VrNuaytt1NLmSXM32iz+j2Wsttrpp9Syqiz/R/wCl9NNj9dsty6muM1XWuZjtrqcfUr32VsyW2Pe1r6m+nusso9TYz9PYz7PkY9qWT1DqRb022pltdV9L7MoOpeXtcPQ2sexlFrvU9936vsx/W/01Xpo1fWsiwx9iuZLi1pNdndrHscd1bG7fUe+q39J/gklNTI6n1XFy7G32sbi/bDjttNJbtq+zfbhYbLLvTf8Ap3fZt38j/TKZ61nHK9Olous9f0rMQ1PY6pge+tt78rd6P6aprL6t7f0zPfSidS6h1asYl2DU61t1Fhuq9F8te4V/Zrju2Pr9G0/psZ/6b0v+IRbesZDS2ujDussOwTZXYxvvdjt3ueymxntqynWvZ/3Wvr/R+mkpz6PrF1U1NOTiurfZq0sote1m2iu7Iruh25z6n2uvp9P+l1UW4dX61/OH/b1gx8htLhlZLanuwyKntbeWb9z6Q0u9drNv0Kf5/wBP1Mf+eqSb1vqe+q5+DcK3th+O1jyQT9lu3te+mv3VU5OQx9b/AOdtxLK6v0vsWlhZxynuBrtrDWg/pK3sBO6xntdbXX9JrGP/AKj0lOG76wdRZu94tx2OP2fKrx3O+1Eej+rUVuurr9VnqXN9tv616f6r+kx8mpWWdcyfWyBkPFApZLKzS6SP9LAe/IsYz8/0sf0/Yt9JFTXwMkZeIy8SQ4uAJESGucze2C9rq37d9djP0d1f6WtWEkklP//Q9VSXyqkkp+qkl8qpJKfqpJfKqSSn6qSXyqkkp+qkl8qpJKfqpJfKqSSn6qSXyqkkp+qkl8qpJKf/2QA4QklNBCEAAAAAAFUAAAABAQAAAA8AQQBkAG8AYgBlACAAUABoAG8AdABvAHMAaABvAHAAAAATAEEAZABvAGIAZQAgAFAAaABvAHQAbwBzAGgAbwBwACAANwAuADAAAAABADhCSU0EBgAAAAAABwABAAAAAQEA/+ESSGh0dHA6Ly9ucy5hZG9iZS5jb20veGFwLzEuMC8APD94cGFja2V0IGJlZ2luPSfvu78nIGlkPSdXNU0wTXBDZWhpSHpyZVN6TlRjemtjOWQnPz4KPD9hZG9iZS14YXAtZmlsdGVycyBlc2M9IkNSIj8+Cjx4OnhhcG1ldGEgeG1sbnM6eD0nYWRvYmU6bnM6bWV0YS8nIHg6eGFwdGs9J1hNUCB0b29sa2l0IDIuOC4yLTMzLCBmcmFtZXdvcmsgMS41Jz4KPHJkZjpSREYgeG1sbnM6cmRmPSdodHRwOi8vd3d3LnczLm9yZy8xOTk5LzAyLzIyLXJkZi1zeW50YXgtbnMjJyB4bWxuczppWD0naHR0cDovL25zLmFkb2JlLmNvbS9pWC8xLjAvJz4KCiA8cmRmOkRlc2NyaXB0aW9uIGFib3V0PSd1dWlkOjQ1ODFkYzcxLTkzNzctMTFlYi1iZjk5LWM2MjM4YTRmODgzOCcKICB4bWxuczp4YXBNTT0naHR0cDovL25zLmFkb2JlLmNvbS94YXAvMS4wL21tLyc+CiAgPHhhcE1NOkRvY3VtZW50SUQ+YWRvYmU6ZG9jaWQ6cGhvdG9zaG9wOjQ1ODFkYzZhLTkzNzctMTFlYi1iZjk5LWM2MjM4YTRmODgzODwveGFwTU06RG9jdW1lbnRJRD4KIDwvcmRmOkRlc2NyaXB0aW9uPgoKPC9yZGY6UkRGPgo8L3g6eGFwbWV0YT4KICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgIAogICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgCiAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAKICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAgICAg</t>
+  </si>
+  <si>
+    <t>Request_Get_ShareRequest</t>
+  </si>
+  <si>
+    <t>(Login with Userid - BN522, Pass - 12345)</t>
+  </si>
+  <si>
+    <t>[ { "scrip_Code": "531733", "scrip_Name": "BAFNASP", "isin": "INE657F01034", "holding_Quantity": 1000, "holding_Value": 70, "request_Quantity": 0, "request_Value": 0.07 } ]</t>
   </si>
 </sst>
 </file>
@@ -1512,8 +1521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="F165" sqref="F165"/>
+    <sheetView tabSelected="1" topLeftCell="A349" workbookViewId="0">
+      <selection activeCell="E356" sqref="E356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1544,13 +1553,13 @@
     </row>
     <row r="2" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -1576,13 +1585,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1593,10 +1602,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1616,10 +1625,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1631,7 +1640,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1654,10 +1663,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1677,10 +1686,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1695,13 +1704,13 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1712,10 +1721,10 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1730,7 +1739,7 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D17" s="9"/>
       <c r="E17" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
@@ -1739,7 +1748,7 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D18" s="9"/>
       <c r="E18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
@@ -1748,7 +1757,7 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D19" s="9"/>
       <c r="E19" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -1762,13 +1771,13 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1779,49 +1788,49 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
+        <v>116</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>120</v>
-      </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I23" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D24" s="9"/>
       <c r="H24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I24" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="9"/>
       <c r="H25" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I25" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="9"/>
       <c r="H26" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -1833,10 +1842,10 @@
         <v>9</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -1848,10 +1857,10 @@
         <v>9</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -1862,10 +1871,10 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1877,10 +1886,10 @@
         <v>16</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
@@ -1895,7 +1904,7 @@
         <v>16</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
@@ -1905,49 +1914,49 @@
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D33" s="9"/>
       <c r="E33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F33" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D34" s="9"/>
       <c r="G34" s="20"/>
       <c r="H34" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D35" s="9"/>
       <c r="G35" s="20"/>
       <c r="H35" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D36" s="9"/>
       <c r="G36" s="20"/>
       <c r="H36" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D37" s="9"/>
       <c r="G37" s="20"/>
       <c r="H37" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D38" s="9"/>
       <c r="G38" s="20"/>
       <c r="H38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
@@ -1957,25 +1966,25 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D40" s="9"/>
       <c r="E40" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D41" s="9"/>
       <c r="H41" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D42" s="9"/>
       <c r="H42" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -1983,61 +1992,61 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E44" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D45" s="9"/>
       <c r="I45" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D46" s="9"/>
       <c r="I46" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D47" s="9"/>
       <c r="I47" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D48" s="9"/>
       <c r="I48" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D49" s="9"/>
       <c r="I49" s="19" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D50" s="9"/>
       <c r="I50" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2045,25 +2054,25 @@
     </row>
     <row r="52" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B52" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H52" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -2071,7 +2080,7 @@
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>9</v>
@@ -2091,46 +2100,46 @@
         <v>38</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D56" s="9"/>
       <c r="I56" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D57" s="9"/>
       <c r="I57" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D58" s="9"/>
       <c r="I58" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D59" s="9"/>
       <c r="I59" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D60" s="9"/>
       <c r="I60" s="19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D61" s="9"/>
       <c r="I61" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
@@ -2144,55 +2153,55 @@
         <v>38</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E63" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I63" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D64" s="9"/>
       <c r="I64" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D65" s="9"/>
       <c r="I65" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D66" s="9"/>
       <c r="I66" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" s="9"/>
       <c r="I67" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D68" s="9"/>
       <c r="I68" s="19" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D69" s="9"/>
       <c r="I69" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
@@ -2206,10 +2215,10 @@
         <v>38</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
@@ -2223,10 +2232,10 @@
         <v>38</v>
       </c>
       <c r="D73" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="E73" t="s">
         <v>250</v>
-      </c>
-      <c r="E73" t="s">
-        <v>252</v>
       </c>
       <c r="F73" t="s">
         <v>23</v>
@@ -2235,7 +2244,7 @@
         <v>1202870000086520</v>
       </c>
       <c r="I73" s="26" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
@@ -2249,10 +2258,10 @@
         <v>38</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E75" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F75" t="s">
         <v>23</v>
@@ -2261,7 +2270,7 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D76" s="9"/>
       <c r="E76" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F76" t="s">
         <v>23</v>
@@ -2278,10 +2287,10 @@
         <v>38</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I78" s="26" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
@@ -2295,10 +2304,10 @@
         <v>38</v>
       </c>
       <c r="D80" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E80" t="s">
         <v>41</v>
-      </c>
-      <c r="E80" t="s">
-        <v>42</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>9</v>
@@ -2307,13 +2316,13 @@
         <v>14</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D81" s="9"/>
       <c r="E81" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>9</v>
@@ -2325,7 +2334,7 @@
     <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D82" s="9"/>
       <c r="E82" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>9</v>
@@ -2342,13 +2351,13 @@
         <v>26</v>
       </c>
       <c r="C84" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
@@ -2359,13 +2368,13 @@
         <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E86" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F86" t="s">
         <v>23</v>
@@ -2374,7 +2383,7 @@
         <v>28</v>
       </c>
       <c r="I86" s="26" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
@@ -2385,7 +2394,7 @@
         <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>29</v>
@@ -2424,22 +2433,22 @@
         <v>26</v>
       </c>
       <c r="C91" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E91" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I91" s="26" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
@@ -2451,28 +2460,28 @@
         <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E93" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="I93" s="26" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D94" s="9"/>
       <c r="E94" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>9</v>
@@ -2490,13 +2499,13 @@
         <v>26</v>
       </c>
       <c r="C96" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="E96" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>9</v>
@@ -2506,7 +2515,7 @@
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D97" s="9"/>
       <c r="E97" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>9</v>
@@ -2516,7 +2525,7 @@
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D98" s="9"/>
       <c r="E98" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>9</v>
@@ -2534,13 +2543,13 @@
         <v>26</v>
       </c>
       <c r="C100" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E100" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>9</v>
@@ -2550,7 +2559,7 @@
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D101" s="9"/>
       <c r="E101" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>9</v>
@@ -2566,34 +2575,34 @@
         <v>20</v>
       </c>
       <c r="C103" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E103" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H103" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="I103" s="31" t="s">
         <v>282</v>
-      </c>
-      <c r="I103" s="31" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D104" s="9"/>
       <c r="E104" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H104" s="14" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
@@ -2604,13 +2613,13 @@
         <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="E106" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>9</v>
@@ -2620,7 +2629,7 @@
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D107" s="9"/>
       <c r="E107" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>9</v>
@@ -2630,7 +2639,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>9</v>
@@ -2640,7 +2649,7 @@
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D109" s="9"/>
       <c r="E109" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>9</v>
@@ -2650,7 +2659,7 @@
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D110" s="9"/>
       <c r="E110" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>9</v>
@@ -2660,7 +2669,7 @@
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D111" s="9"/>
       <c r="E111" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>9</v>
@@ -2675,31 +2684,31 @@
         <v>34</v>
       </c>
       <c r="C113" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F113" t="s">
         <v>9</v>
       </c>
       <c r="H113" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I113" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D114" s="9"/>
       <c r="H114" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="I114" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
@@ -2711,10 +2720,10 @@
         <v>9</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I115" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
@@ -2726,28 +2735,28 @@
         <v>9</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I116" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D117" s="9"/>
       <c r="I117" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D118" s="9"/>
       <c r="I118" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D119" s="9"/>
       <c r="I119" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
@@ -2758,49 +2767,49 @@
         <v>34</v>
       </c>
       <c r="C121" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F121" t="s">
         <v>9</v>
       </c>
       <c r="H121" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I121" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D122" s="9"/>
       <c r="H122" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I122" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D123" s="9"/>
       <c r="H123" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="I123" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D124" s="9"/>
       <c r="H124" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="I124" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
@@ -2812,10 +2821,10 @@
         <v>9</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I125" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.3">
@@ -2827,16 +2836,16 @@
         <v>9</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I126" s="19" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D127" s="9"/>
       <c r="I127" s="22" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
@@ -2847,49 +2856,49 @@
         <v>34</v>
       </c>
       <c r="C129" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E129" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="F129" t="s">
+        <v>9</v>
+      </c>
+      <c r="H129" t="s">
+        <v>212</v>
+      </c>
+      <c r="I129" s="23" t="s">
         <v>213</v>
-      </c>
-      <c r="F129" t="s">
-        <v>9</v>
-      </c>
-      <c r="H129" t="s">
-        <v>214</v>
-      </c>
-      <c r="I129" s="23" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D130" s="9"/>
       <c r="H130" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D131" s="9"/>
       <c r="H131" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="I131" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D132" s="9"/>
       <c r="H132" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I132" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.3">
@@ -2901,10 +2910,10 @@
         <v>9</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I133" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.3">
@@ -2916,22 +2925,22 @@
         <v>9</v>
       </c>
       <c r="H134" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I134" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D135" s="9"/>
       <c r="I135" s="19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D136" s="9"/>
       <c r="I136" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
@@ -2940,49 +2949,49 @@
     <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D138" s="9"/>
       <c r="I138" s="23" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D139" s="9"/>
       <c r="I139" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D140" s="9"/>
       <c r="I140" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D141" s="9"/>
       <c r="I141" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
       <c r="I142" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D143" s="9"/>
       <c r="I143" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D144" s="9"/>
       <c r="I144" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D145" s="9"/>
       <c r="I145" s="19" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
@@ -2991,16 +3000,16 @@
     </row>
     <row r="147" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="C147" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.3">
@@ -3008,16 +3017,16 @@
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
+        <v>49</v>
+      </c>
+      <c r="C149" t="s">
+        <v>268</v>
+      </c>
+      <c r="D149" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C149" t="s">
-        <v>270</v>
-      </c>
-      <c r="D149" s="9" t="s">
+      <c r="E149" t="s">
         <v>51</v>
-      </c>
-      <c r="E149" t="s">
-        <v>52</v>
       </c>
       <c r="F149" t="s">
         <v>23</v>
@@ -3026,7 +3035,7 @@
     <row r="150" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D150" s="9"/>
       <c r="E150" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F150" t="s">
         <v>23</v>
@@ -3037,25 +3046,25 @@
     </row>
     <row r="152" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C152" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E152" t="s">
+        <v>195</v>
+      </c>
+      <c r="F152" t="s">
+        <v>23</v>
+      </c>
+      <c r="H152" t="s">
         <v>197</v>
       </c>
-      <c r="F152" t="s">
-        <v>23</v>
-      </c>
-      <c r="H152" t="s">
+      <c r="I152" s="21" t="s">
         <v>199</v>
-      </c>
-      <c r="I152" s="21" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.3">
@@ -3076,13 +3085,13 @@
     <row r="154" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D154" s="9"/>
       <c r="E154" t="s">
+        <v>196</v>
+      </c>
+      <c r="F154" t="s">
+        <v>23</v>
+      </c>
+      <c r="H154" s="17" t="s">
         <v>198</v>
-      </c>
-      <c r="F154" t="s">
-        <v>23</v>
-      </c>
-      <c r="H154" s="17" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.3">
@@ -3090,51 +3099,51 @@
     </row>
     <row r="156" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C156" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D156" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E156" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G156" s="10"/>
       <c r="H156" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I156" s="7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="157" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D157" s="10"/>
       <c r="E157" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H157" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H157" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="I157" s="1"/>
     </row>
     <row r="158" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D158" s="10"/>
       <c r="E158" t="s">
+        <v>57</v>
+      </c>
+      <c r="F158" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H158" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H158" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="I158" s="13"/>
     </row>
@@ -3172,50 +3181,50 @@
     </row>
     <row r="162" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C162" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D162" s="9" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E162" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G162" s="10"/>
       <c r="H162" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I162" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D163" s="9"/>
       <c r="E163" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F163" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H163" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="F163" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H163" s="14" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="164" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D164" s="9"/>
       <c r="E164" t="s">
+        <v>57</v>
+      </c>
+      <c r="F164" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H164" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="F164" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H164" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.3">
@@ -3237,24 +3246,27 @@
       <c r="F166" s="1"/>
       <c r="H166" s="3"/>
     </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="167" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C167" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D167" s="9" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="E167" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="F167" s="10" t="s">
         <v>23</v>
       </c>
       <c r="H167" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="I167" s="26" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="168" spans="2:9" x14ac:dyDescent="0.3">
@@ -3287,24 +3299,27 @@
       <c r="F170" s="1"/>
       <c r="H170" s="3"/>
     </row>
-    <row r="171" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="171" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B171" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C171" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D171" s="9" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="E171" t="s">
+        <v>195</v>
+      </c>
+      <c r="F171" t="s">
+        <v>23</v>
+      </c>
+      <c r="H171" t="s">
         <v>197</v>
       </c>
-      <c r="F171" t="s">
-        <v>23</v>
-      </c>
-      <c r="H171" t="s">
-        <v>199</v>
+      <c r="I171" s="26" t="s">
+        <v>332</v>
       </c>
     </row>
     <row r="172" spans="2:9" x14ac:dyDescent="0.3">
@@ -3325,13 +3340,13 @@
     <row r="173" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D173" s="9"/>
       <c r="E173" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="F173" t="s">
         <v>23</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.3">
@@ -3342,20 +3357,20 @@
     </row>
     <row r="175" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C175" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
       <c r="H175" s="3"/>
       <c r="I175" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.3">
@@ -3366,20 +3381,20 @@
     </row>
     <row r="178" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B178" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C178" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
       <c r="H178" s="3"/>
       <c r="I178" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.3">
@@ -3387,26 +3402,26 @@
     </row>
     <row r="180" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B180" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C180" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G180" s="1"/>
       <c r="H180" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="I180" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="181" spans="2:9" x14ac:dyDescent="0.3">
@@ -3414,14 +3429,14 @@
       <c r="C181" s="1"/>
       <c r="D181" s="10"/>
       <c r="E181" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G181" s="1"/>
       <c r="H181" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I181" s="1"/>
     </row>
@@ -3430,26 +3445,26 @@
     </row>
     <row r="183" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B183" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C183" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G183" s="1"/>
       <c r="H183" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I183" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.3">
@@ -3457,14 +3472,14 @@
       <c r="C184" s="1"/>
       <c r="D184" s="10"/>
       <c r="E184" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G184" s="1"/>
       <c r="H184" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I184" s="1"/>
     </row>
@@ -3473,7 +3488,7 @@
       <c r="C185" s="1"/>
       <c r="D185" s="10"/>
       <c r="E185" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>9</v>
@@ -3525,13 +3540,13 @@
     </row>
     <row r="189" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B189" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C189" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>32</v>
@@ -3541,10 +3556,10 @@
       </c>
       <c r="G189" s="1"/>
       <c r="H189" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="I189" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.3">
@@ -3552,14 +3567,14 @@
       <c r="C190" s="1"/>
       <c r="D190" s="10"/>
       <c r="E190" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G190" s="1"/>
       <c r="H190" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="I190" s="1"/>
     </row>
@@ -3602,21 +3617,21 @@
     <row r="193" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D193" s="9"/>
       <c r="F193" s="10" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="194" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B194" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C194" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="I194" s="26" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.3">
@@ -3624,25 +3639,25 @@
     </row>
     <row r="196" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B196" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C196" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="E196" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H196" t="s">
         <v>288</v>
       </c>
-      <c r="F196" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H196" t="s">
-        <v>290</v>
-      </c>
       <c r="I196" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.3">
@@ -3662,25 +3677,25 @@
     </row>
     <row r="199" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B199" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C199" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="E199" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H199" t="s">
         <v>288</v>
       </c>
-      <c r="F199" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H199" t="s">
-        <v>290</v>
-      </c>
       <c r="I199" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.3">
@@ -3689,43 +3704,43 @@
     <row r="201" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D201" s="9"/>
       <c r="H201" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I201" s="26"/>
     </row>
     <row r="202" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B202" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C202" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D202" s="10" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="E202" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H202" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I202" s="26" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D203" s="9"/>
       <c r="H203" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D204" s="9"/>
       <c r="H204" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.3">
@@ -3733,110 +3748,110 @@
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B206" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C206" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D206" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H206" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="207" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E207" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H207" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H208" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="209" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H209" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B211" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C211" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D211" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H211" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="212" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E212" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H212" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="213" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H213" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="214" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H214" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="216" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B216" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C216" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D216" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H216" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="217" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D217" s="9"/>
       <c r="E217" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H217" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="218" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D218" s="9"/>
       <c r="H218" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D219" s="9"/>
       <c r="H219" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="220" spans="2:8" x14ac:dyDescent="0.3">
@@ -3844,23 +3859,23 @@
     </row>
     <row r="221" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B221" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D221" s="32" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E221" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F221" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G221" s="8"/>
       <c r="H221" s="18" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="222" spans="2:8" x14ac:dyDescent="0.3">
@@ -3902,7 +3917,7 @@
       <c r="C224" s="8"/>
       <c r="D224" s="32"/>
       <c r="E224" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F224" s="8" t="s">
         <v>23</v>
@@ -3923,7 +3938,7 @@
     <row r="226" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D226" s="9"/>
       <c r="H226" s="18" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.3">
@@ -3934,13 +3949,13 @@
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B229" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C229" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D229" s="32" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E229" s="33" t="s">
         <v>32</v>
@@ -3950,18 +3965,18 @@
       </c>
       <c r="G229" s="8"/>
       <c r="H229" s="32" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="230" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D230" s="9"/>
       <c r="E230" s="8"/>
       <c r="F230" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G230" s="8"/>
       <c r="H230" s="18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="231" spans="2:9" x14ac:dyDescent="0.3">
@@ -4003,43 +4018,43 @@
     </row>
     <row r="234" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B234" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C234" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D234" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H234" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I234" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="235" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D235" s="9"/>
       <c r="E235" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H235" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="236" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D236" s="9"/>
       <c r="H236" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D237" s="9"/>
       <c r="H237" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="238" spans="2:9" x14ac:dyDescent="0.3">
@@ -4051,43 +4066,43 @@
     </row>
     <row r="239" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B239" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D239" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="H239" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="I239" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="240" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D240" s="9"/>
       <c r="E240" s="11" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H240" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="241" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D241" s="9"/>
       <c r="H241" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D242" s="9"/>
       <c r="H242" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="243" spans="2:9" x14ac:dyDescent="0.3">
@@ -4099,26 +4114,26 @@
     </row>
     <row r="244" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
       <c r="B244" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D244" s="34" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E244" s="8" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F244" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G244" s="8"/>
       <c r="H244" s="18" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="I244" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="245" spans="2:9" x14ac:dyDescent="0.3">
@@ -4154,7 +4169,7 @@
     <row r="247" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D247" s="9"/>
       <c r="E247" s="8" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="F247" s="8" t="s">
         <v>23</v>
@@ -4173,7 +4188,7 @@
     <row r="249" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D249" s="9"/>
       <c r="H249" s="18" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="250" spans="2:9" x14ac:dyDescent="0.3">
@@ -4185,13 +4200,13 @@
     </row>
     <row r="251" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B251" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D251" s="32" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E251" s="33" t="s">
         <v>32</v>
@@ -4201,18 +4216,18 @@
       </c>
       <c r="G251" s="8"/>
       <c r="H251" s="32" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="252" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D252" s="9"/>
       <c r="E252" s="8"/>
       <c r="F252" s="8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G252" s="8"/>
       <c r="H252" s="18" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="253" spans="2:9" x14ac:dyDescent="0.3">
@@ -4254,13 +4269,13 @@
     </row>
     <row r="256" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B256" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C256" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D256" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E256" t="s">
         <v>15</v>
@@ -4275,7 +4290,7 @@
         <v>20210401</v>
       </c>
       <c r="I256" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="257" spans="2:9" x14ac:dyDescent="0.3">
@@ -4296,7 +4311,7 @@
     <row r="258" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D258" s="9"/>
       <c r="E258" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F258" t="s">
         <v>9</v>
@@ -4311,17 +4326,17 @@
     </row>
     <row r="260" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B260" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C260" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D260" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H260" s="6"/>
       <c r="I260" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="261" spans="2:9" x14ac:dyDescent="0.3">
@@ -4334,17 +4349,17 @@
     </row>
     <row r="263" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B263" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C263" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H263" s="6"/>
       <c r="I263" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="264" spans="2:9" x14ac:dyDescent="0.3">
@@ -4357,17 +4372,17 @@
     </row>
     <row r="266" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B266" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C266" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D266" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H266" s="6"/>
       <c r="I266" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="267" spans="2:9" x14ac:dyDescent="0.3">
@@ -4380,34 +4395,34 @@
     </row>
     <row r="269" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B269" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C269" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D269" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="E269" t="s">
+        <v>109</v>
+      </c>
+      <c r="F269" t="s">
         <v>110</v>
-      </c>
-      <c r="E269" t="s">
-        <v>111</v>
-      </c>
-      <c r="F269" t="s">
-        <v>112</v>
       </c>
       <c r="H269" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I269" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="270" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D270" s="9"/>
       <c r="E270" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F270" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H270" s="6" t="b">
         <v>1</v>
@@ -4419,16 +4434,16 @@
     </row>
     <row r="272" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B272" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C272" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D272" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E272" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F272" t="s">
         <v>21</v>
@@ -4437,7 +4452,7 @@
         <v>3</v>
       </c>
       <c r="I272" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="273" spans="2:9" x14ac:dyDescent="0.3">
@@ -4445,20 +4460,20 @@
     </row>
     <row r="274" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B274" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C274" t="s">
+        <v>269</v>
+      </c>
+      <c r="D274" s="10" t="s">
         <v>62</v>
-      </c>
-      <c r="C274" t="s">
-        <v>271</v>
-      </c>
-      <c r="D274" s="10" t="s">
-        <v>63</v>
       </c>
       <c r="E274" s="1"/>
       <c r="F274" s="10"/>
       <c r="G274" s="1"/>
       <c r="H274" s="3"/>
       <c r="I274" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="275" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4473,13 +4488,13 @@
     </row>
     <row r="276" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B276" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C276" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D276" s="10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E276" s="1"/>
       <c r="F276" s="10"/>
@@ -4501,26 +4516,26 @@
     </row>
     <row r="278" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B278" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C278" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D278" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E278" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F278" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G278" s="1"/>
       <c r="H278" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I278" s="26" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="279" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4535,13 +4550,13 @@
     </row>
     <row r="280" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B280" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C280" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D280" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E280" s="11"/>
       <c r="F280" s="10"/>
@@ -4560,26 +4575,26 @@
     </row>
     <row r="282" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B282" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C282" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D282" s="10" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="E282" s="11" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="F282" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G282" s="1"/>
       <c r="H282" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I282" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="283" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4587,7 +4602,7 @@
       <c r="C283" s="1"/>
       <c r="D283" s="10"/>
       <c r="E283" s="11" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="F283" s="10" t="s">
         <v>9</v>
@@ -4603,7 +4618,7 @@
       <c r="C284" s="1"/>
       <c r="D284" s="10"/>
       <c r="E284" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F284" s="10" t="s">
         <v>9</v>
@@ -4619,13 +4634,13 @@
     </row>
     <row r="286" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B286" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C286" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D286" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E286" s="11" t="s">
         <v>22</v>
@@ -4637,7 +4652,7 @@
         <v>20191101</v>
       </c>
       <c r="I286" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="287" spans="2:9" x14ac:dyDescent="0.3">
@@ -4645,13 +4660,13 @@
     </row>
     <row r="288" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B288" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D288" s="9" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="E288" t="s">
         <v>15</v>
@@ -4660,10 +4675,10 @@
         <v>9</v>
       </c>
       <c r="H288" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I288" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.3">
@@ -4675,42 +4690,42 @@
         <v>9</v>
       </c>
       <c r="H289" s="35" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I289" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D290" s="9"/>
       <c r="H290" s="8"/>
       <c r="I290" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D291" s="9"/>
       <c r="H291" s="8"/>
       <c r="I291" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D292" s="9"/>
       <c r="I292" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D293" s="9"/>
       <c r="I293" s="19" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D294" s="9"/>
       <c r="I294" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
@@ -4721,13 +4736,13 @@
         <v>36</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D296" s="10" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E296" s="1" t="s">
         <v>15</v>
@@ -4742,7 +4757,7 @@
         <v>20200401</v>
       </c>
       <c r="I296" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="297" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4770,7 +4785,7 @@
       <c r="C298" s="1"/>
       <c r="D298" s="10"/>
       <c r="E298" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F298" s="1" t="s">
         <v>9</v>
@@ -4794,13 +4809,13 @@
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B300" s="1" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D300" s="9" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="E300" t="s">
         <v>27</v>
@@ -4809,25 +4824,25 @@
         <v>9</v>
       </c>
       <c r="H300" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="I300" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D301" s="9"/>
       <c r="E301" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F301" t="s">
         <v>9</v>
       </c>
       <c r="H301" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="I301" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
@@ -4839,10 +4854,10 @@
         <v>9</v>
       </c>
       <c r="H302" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I302" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
@@ -4854,34 +4869,34 @@
         <v>9</v>
       </c>
       <c r="H303" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I303" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D304" s="9"/>
       <c r="I304" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="305" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D305" s="9"/>
       <c r="I305" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="306" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D306" s="9"/>
       <c r="I306" s="19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D307" s="9"/>
       <c r="I307" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="308" spans="2:9" x14ac:dyDescent="0.3">
@@ -4889,13 +4904,13 @@
     </row>
     <row r="309" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B309" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D309" s="9" t="s">
         <v>232</v>
-      </c>
-      <c r="C309" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D309" s="9" t="s">
-        <v>234</v>
       </c>
       <c r="E309" t="s">
         <v>27</v>
@@ -4904,10 +4919,10 @@
         <v>9</v>
       </c>
       <c r="H309" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="I309" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
@@ -4919,10 +4934,10 @@
         <v>9</v>
       </c>
       <c r="H310" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I310" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="311" spans="2:9" x14ac:dyDescent="0.3">
@@ -4934,28 +4949,28 @@
         <v>9</v>
       </c>
       <c r="H311" s="17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="I311" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="312" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D312" s="9"/>
       <c r="I312" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="313" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D313" s="9"/>
       <c r="I313" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="314" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D314" s="9"/>
       <c r="I314" s="25" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="315" spans="2:9" x14ac:dyDescent="0.3">
@@ -4963,7 +4978,7 @@
       <c r="E315" s="24"/>
       <c r="H315" s="18"/>
       <c r="I315" s="18" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="316" spans="2:9" x14ac:dyDescent="0.3">
@@ -4971,13 +4986,13 @@
     </row>
     <row r="317" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B317" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D317" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E317" t="s">
         <v>15</v>
@@ -4992,7 +5007,7 @@
         <v>20200401</v>
       </c>
       <c r="I317" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.3">
@@ -5017,13 +5032,13 @@
     </row>
     <row r="320" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B320" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D320" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E320" t="s">
         <v>15</v>
@@ -5038,7 +5053,7 @@
         <v>20200401</v>
       </c>
       <c r="I320" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="321" spans="2:9" x14ac:dyDescent="0.3">
@@ -5059,49 +5074,49 @@
     <row r="322" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D322" s="9"/>
       <c r="E322" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F322" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H322" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D323" s="9"/>
       <c r="E323" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F323" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H323" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="324" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D324" s="9"/>
       <c r="E324" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F324" s="9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H324" s="8" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="325" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D325" s="9"/>
       <c r="E325" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F325" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H325" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="326" spans="2:9" x14ac:dyDescent="0.3">
@@ -5110,13 +5125,13 @@
     </row>
     <row r="327" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B327" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D327" s="9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E327" t="s">
         <v>15</v>
@@ -5131,7 +5146,7 @@
         <v>20200401</v>
       </c>
       <c r="I327" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="328" spans="2:9" x14ac:dyDescent="0.3">
@@ -5152,19 +5167,19 @@
     <row r="329" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D329" s="9"/>
       <c r="E329" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F329" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H329" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="330" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D330" s="9"/>
       <c r="E330" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F330" s="9" t="s">
         <v>23</v>
@@ -5176,7 +5191,7 @@
     <row r="331" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D331" s="9"/>
       <c r="E331" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F331" s="9" t="s">
         <v>23</v>
@@ -5191,13 +5206,13 @@
     </row>
     <row r="333" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B333" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D333" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E333" t="s">
         <v>15</v>
@@ -5212,7 +5227,7 @@
         <v>20200401</v>
       </c>
       <c r="I333" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="334" spans="2:9" x14ac:dyDescent="0.3">
@@ -5236,13 +5251,13 @@
     </row>
     <row r="336" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B336" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D336" s="9" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E336" t="s">
         <v>15</v>
@@ -5257,7 +5272,7 @@
         <v>20200401</v>
       </c>
       <c r="I336" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="337" spans="2:9" x14ac:dyDescent="0.3">
@@ -5278,7 +5293,7 @@
     <row r="338" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D338" s="9"/>
       <c r="E338" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F338" s="9" t="s">
         <v>23</v>
@@ -5293,13 +5308,13 @@
     </row>
     <row r="340" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B340" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D340" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E340" t="s">
         <v>22</v>
@@ -5314,7 +5329,7 @@
         <v>20220228</v>
       </c>
       <c r="I340" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="341" spans="2:9" x14ac:dyDescent="0.3">
@@ -5326,7 +5341,7 @@
         <v>23</v>
       </c>
       <c r="H341" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="342" spans="2:9" x14ac:dyDescent="0.3">
@@ -5350,16 +5365,16 @@
         <v>23</v>
       </c>
       <c r="H343" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="344" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D344" s="9"/>
       <c r="E344" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F344" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H344" s="8">
         <v>4</v>
@@ -5368,10 +5383,10 @@
     <row r="345" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D345" s="9"/>
       <c r="E345" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F345" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H345" s="8">
         <v>48</v>
@@ -5380,10 +5395,10 @@
     <row r="346" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D346" s="9"/>
       <c r="E346" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F346" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H346" s="8">
         <v>1.1000000000000001</v>
@@ -5392,10 +5407,10 @@
     <row r="347" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D347" s="9"/>
       <c r="E347" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F347" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H347" s="8">
         <v>3.2</v>
@@ -5404,10 +5419,10 @@
     <row r="348" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D348" s="9"/>
       <c r="E348" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F348" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H348" s="8">
         <v>0.11</v>
@@ -5416,10 +5431,10 @@
     <row r="349" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D349" s="9"/>
       <c r="E349" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F349" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H349" s="8">
         <v>0.2</v>
@@ -5428,7 +5443,7 @@
     <row r="350" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D350" s="9"/>
       <c r="E350" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F350" s="9" t="s">
         <v>23</v>
@@ -5442,20 +5457,20 @@
     </row>
     <row r="352" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B352" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C352" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D352" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="C352" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D352" s="10" t="s">
-        <v>70</v>
       </c>
       <c r="E352" s="1"/>
       <c r="F352" s="1"/>
       <c r="G352" s="1"/>
       <c r="H352" s="3"/>
       <c r="I352" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="353" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5470,26 +5485,26 @@
     </row>
     <row r="354" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B354" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D354" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="E354" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="E354" s="1" t="s">
-        <v>73</v>
       </c>
       <c r="F354" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G354" s="1"/>
       <c r="H354" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I354" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="I354" s="7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="355" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5502,22 +5517,24 @@
       <c r="H355" s="3"/>
       <c r="I355" s="13"/>
     </row>
-    <row r="356" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="356" spans="2:9" ht="29.4" x14ac:dyDescent="0.35">
       <c r="B356" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D356" s="10" t="s">
-        <v>76</v>
+        <v>333</v>
       </c>
       <c r="E356" s="1"/>
       <c r="F356" s="1"/>
       <c r="G356" s="1"/>
-      <c r="H356" s="3"/>
+      <c r="H356" s="12" t="s">
+        <v>334</v>
+      </c>
       <c r="I356" s="7" t="s">
-        <v>40</v>
+        <v>335</v>
       </c>
     </row>
     <row r="357" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5532,26 +5549,26 @@
     </row>
     <row r="358" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B358" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D358" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E358" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F358" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G358" s="1"/>
       <c r="H358" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="I358" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="I358" s="7" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="359" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5566,16 +5583,16 @@
     </row>
     <row r="360" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B360" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C360" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D360" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E360" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F360" s="1" t="s">
         <v>9</v>
@@ -5585,7 +5602,7 @@
         <v>14</v>
       </c>
       <c r="I360" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="361" spans="2:9" x14ac:dyDescent="0.3">
@@ -5593,14 +5610,14 @@
       <c r="C361" s="1"/>
       <c r="D361" s="10"/>
       <c r="E361" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="F361" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G361" s="1"/>
       <c r="H361" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="I361" s="1"/>
     </row>
@@ -5648,36 +5665,36 @@
     </row>
     <row r="366" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B366" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C366" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D366" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="E366" s="8" t="s">
         <v>324</v>
-      </c>
-      <c r="E366" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="F366" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G366" s="8"/>
       <c r="H366" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
     </row>
     <row r="367" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D367" s="9"/>
       <c r="E367" s="8" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="F367" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G367" s="8"/>
       <c r="H367" s="18" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
     </row>
     <row r="368" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Change input and output parameter of request module
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="340">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -1015,9 +1015,6 @@
     <t>Request_Post_FundRequest</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
     <t>amount</t>
   </si>
   <si>
@@ -1057,10 +1054,16 @@
     <t>Request_Post_ShareRequest</t>
   </si>
   <si>
-    <t>scripCode</t>
-  </si>
-  <si>
     <t>Success</t>
+  </si>
+  <si>
+    <t>scrip_Code</t>
+  </si>
+  <si>
+    <t>request_Quantity</t>
+  </si>
+  <si>
+    <t>dpId</t>
   </si>
 </sst>
 </file>
@@ -1531,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A349" workbookViewId="0">
-      <selection activeCell="D360" sqref="D360"/>
+    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
+      <selection activeCell="E363" sqref="E363"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3264,10 +3267,10 @@
         <v>268</v>
       </c>
       <c r="D167" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="E167" s="10" t="s">
         <v>327</v>
-      </c>
-      <c r="E167" s="10" t="s">
-        <v>328</v>
       </c>
       <c r="F167" s="10" t="s">
         <v>23</v>
@@ -3276,7 +3279,7 @@
         <v>52</v>
       </c>
       <c r="I167" s="26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="168" spans="2:9" x14ac:dyDescent="0.3">
@@ -3317,7 +3320,7 @@
         <v>268</v>
       </c>
       <c r="D171" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E171" t="s">
         <v>195</v>
@@ -3329,7 +3332,7 @@
         <v>197</v>
       </c>
       <c r="I171" s="26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="172" spans="2:9" x14ac:dyDescent="0.3">
@@ -3356,7 +3359,7 @@
         <v>23</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.3">
@@ -5535,16 +5538,16 @@
         <v>237</v>
       </c>
       <c r="D356" s="10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E356" s="1"/>
       <c r="F356" s="1"/>
       <c r="G356" s="1"/>
       <c r="H356" s="12" t="s">
+        <v>333</v>
+      </c>
+      <c r="I356" s="7" t="s">
         <v>334</v>
-      </c>
-      <c r="I356" s="7" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="357" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5565,7 +5568,7 @@
         <v>237</v>
       </c>
       <c r="D358" s="10" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E358" s="1" t="s">
         <v>337</v>
@@ -5578,7 +5581,7 @@
         <v>531733</v>
       </c>
       <c r="I358" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="359" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5586,7 +5589,7 @@
       <c r="C359" s="1"/>
       <c r="D359" s="10"/>
       <c r="E359" s="1" t="s">
-        <v>67</v>
+        <v>338</v>
       </c>
       <c r="F359" s="1" t="s">
         <v>23</v>
@@ -5734,27 +5737,27 @@
         <v>322</v>
       </c>
       <c r="E369" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F369" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G369" s="8"/>
       <c r="H369" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="370" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D370" s="9"/>
       <c r="E370" s="8" t="s">
-        <v>323</v>
+        <v>339</v>
       </c>
       <c r="F370" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G370" s="8"/>
       <c r="H370" s="18" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="371" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Rename api Holding_Post_UnPledgeRequest and change input parameters.
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -138,9 +137,6 @@
     <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": "[\r\n {\r\n \"BOId\": \"1202870000086521 \",\r\n \"Name\": \"PNAKMRMTA HF\",\r\n \"da_clientcd\": \"MG040 \"\r\n }\r\n]" }</t>
   </si>
   <si>
-    <t>AddUnPledgeRequest</t>
-  </si>
-  <si>
     <t>unPledge</t>
   </si>
   <si>
@@ -148,9 +144,6 @@
   </si>
   <si>
     <t>scripcd</t>
-  </si>
-  <si>
-    <t>reqQty</t>
   </si>
   <si>
     <t>OutStanding</t>
@@ -1009,9 +1002,6 @@
     <t>Request_Post_PledgeForMargin</t>
   </si>
   <si>
-    <t>ScripCode</t>
-  </si>
-  <si>
     <t>Request_Post_FundRequest</t>
   </si>
   <si>
@@ -1064,6 +1054,15 @@
   </si>
   <si>
     <t>dpId</t>
+  </si>
+  <si>
+    <t>Securities_Code</t>
+  </si>
+  <si>
+    <t>Request_Qty</t>
+  </si>
+  <si>
+    <t>Holding_Post_UnPledgeRequest</t>
   </si>
 </sst>
 </file>
@@ -1534,8 +1533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I386"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A350" workbookViewId="0">
-      <selection activeCell="E363" sqref="E363"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="D82" sqref="D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1566,13 +1565,13 @@
     </row>
     <row r="2" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -1598,13 +1597,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1615,10 +1614,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1638,10 +1637,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1653,7 +1652,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1676,10 +1675,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1699,10 +1698,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1717,13 +1716,13 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1734,10 +1733,10 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1752,7 +1751,7 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D17" s="9"/>
       <c r="E17" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
@@ -1761,7 +1760,7 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D18" s="9"/>
       <c r="E18" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
@@ -1770,7 +1769,7 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D19" s="9"/>
       <c r="E19" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -1784,13 +1783,13 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1801,49 +1800,49 @@
         <v>33</v>
       </c>
       <c r="C23" t="s">
+        <v>114</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>118</v>
-      </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="I23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D24" s="9"/>
       <c r="H24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I24" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="9"/>
       <c r="H25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="9"/>
       <c r="H26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="I26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -1855,10 +1854,10 @@
         <v>9</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -1870,10 +1869,10 @@
         <v>9</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -1884,10 +1883,10 @@
         <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1899,10 +1898,10 @@
         <v>16</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I30" s="26" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
@@ -1917,7 +1916,7 @@
         <v>16</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
@@ -1927,49 +1926,49 @@
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D33" s="9"/>
       <c r="E33" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F33" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D34" s="9"/>
       <c r="G34" s="20"/>
       <c r="H34" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D35" s="9"/>
       <c r="G35" s="20"/>
       <c r="H35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D36" s="9"/>
       <c r="G36" s="20"/>
       <c r="H36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D37" s="9"/>
       <c r="G37" s="20"/>
       <c r="H37" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D38" s="9"/>
       <c r="G38" s="20"/>
       <c r="H38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
@@ -1979,25 +1978,25 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D40" s="9"/>
       <c r="E40" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D41" s="9"/>
       <c r="H41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D42" s="9"/>
       <c r="H42" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -2005,61 +2004,61 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E44" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I44" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D45" s="9"/>
       <c r="I45" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D46" s="9"/>
       <c r="I46" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D47" s="9"/>
       <c r="I47" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D48" s="9"/>
       <c r="I48" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D49" s="9"/>
       <c r="I49" s="19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D50" s="9"/>
       <c r="I50" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2067,25 +2066,25 @@
     </row>
     <row r="52" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B52" s="9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H52" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -2093,7 +2092,7 @@
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>9</v>
@@ -2113,46 +2112,46 @@
         <v>38</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D56" s="9"/>
       <c r="I56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D57" s="9"/>
       <c r="I57" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D58" s="9"/>
       <c r="I58" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D59" s="9"/>
       <c r="I59" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D60" s="9"/>
       <c r="I60" s="19" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D61" s="9"/>
       <c r="I61" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
@@ -2166,55 +2165,55 @@
         <v>38</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E63" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="I63" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D64" s="9"/>
       <c r="I64" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D65" s="9"/>
       <c r="I65" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D66" s="9"/>
       <c r="I66" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" s="9"/>
       <c r="I67" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D68" s="9"/>
       <c r="I68" s="19" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D69" s="9"/>
       <c r="I69" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
@@ -2228,10 +2227,10 @@
         <v>38</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
@@ -2245,10 +2244,10 @@
         <v>38</v>
       </c>
       <c r="D73" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="E73" t="s">
         <v>248</v>
-      </c>
-      <c r="E73" t="s">
-        <v>250</v>
       </c>
       <c r="F73" t="s">
         <v>23</v>
@@ -2257,7 +2256,7 @@
         <v>1202870000086520</v>
       </c>
       <c r="I73" s="26" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
@@ -2271,10 +2270,10 @@
         <v>38</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E75" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F75" t="s">
         <v>23</v>
@@ -2283,7 +2282,7 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D76" s="9"/>
       <c r="E76" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F76" t="s">
         <v>23</v>
@@ -2300,10 +2299,10 @@
         <v>38</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="I78" s="26" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
@@ -2317,10 +2316,10 @@
         <v>38</v>
       </c>
       <c r="D80" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="E80" t="s">
         <v>40</v>
-      </c>
-      <c r="E80" t="s">
-        <v>41</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>9</v>
@@ -2329,13 +2328,13 @@
         <v>14</v>
       </c>
       <c r="I80" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="81" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D81" s="9"/>
       <c r="E81" t="s">
-        <v>43</v>
+        <v>337</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>9</v>
@@ -2347,7 +2346,7 @@
     <row r="82" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D82" s="9"/>
       <c r="E82" t="s">
-        <v>44</v>
+        <v>338</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>9</v>
@@ -2364,13 +2363,13 @@
         <v>26</v>
       </c>
       <c r="C84" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D84" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="I84" s="26" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="85" spans="2:9" x14ac:dyDescent="0.3">
@@ -2381,13 +2380,13 @@
         <v>26</v>
       </c>
       <c r="C86" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D86" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E86" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F86" t="s">
         <v>23</v>
@@ -2396,7 +2395,7 @@
         <v>28</v>
       </c>
       <c r="I86" s="26" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="87" spans="2:9" x14ac:dyDescent="0.3">
@@ -2407,7 +2406,7 @@
         <v>26</v>
       </c>
       <c r="C88" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D88" s="10" t="s">
         <v>29</v>
@@ -2446,22 +2445,22 @@
         <v>26</v>
       </c>
       <c r="C91" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D91" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E91" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I91" s="26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="92" spans="2:9" x14ac:dyDescent="0.3">
@@ -2473,28 +2472,28 @@
         <v>26</v>
       </c>
       <c r="C93" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E93" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="I93" s="26" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D94" s="9"/>
       <c r="E94" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>9</v>
@@ -2512,13 +2511,13 @@
         <v>26</v>
       </c>
       <c r="C96" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D96" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E96" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>9</v>
@@ -2528,7 +2527,7 @@
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D97" s="9"/>
       <c r="E97" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>9</v>
@@ -2538,7 +2537,7 @@
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D98" s="9"/>
       <c r="E98" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>9</v>
@@ -2556,13 +2555,13 @@
         <v>26</v>
       </c>
       <c r="C100" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E100" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>9</v>
@@ -2572,7 +2571,7 @@
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D101" s="9"/>
       <c r="E101" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>9</v>
@@ -2588,34 +2587,34 @@
         <v>20</v>
       </c>
       <c r="C103" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D103" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E103" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H103" s="30" t="s">
+        <v>278</v>
+      </c>
+      <c r="I103" s="31" t="s">
         <v>280</v>
-      </c>
-      <c r="I103" s="31" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D104" s="9"/>
       <c r="E104" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H104" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
@@ -2626,13 +2625,13 @@
         <v>20</v>
       </c>
       <c r="C106" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E106" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>9</v>
@@ -2642,7 +2641,7 @@
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D107" s="9"/>
       <c r="E107" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>9</v>
@@ -2652,7 +2651,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>9</v>
@@ -2662,7 +2661,7 @@
     <row r="109" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D109" s="9"/>
       <c r="E109" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="F109" s="1" t="s">
         <v>9</v>
@@ -2672,7 +2671,7 @@
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D110" s="9"/>
       <c r="E110" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F110" s="1" t="s">
         <v>9</v>
@@ -2682,7 +2681,7 @@
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D111" s="9"/>
       <c r="E111" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="F111" s="1" t="s">
         <v>9</v>
@@ -2697,31 +2696,31 @@
         <v>34</v>
       </c>
       <c r="C113" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D113" s="9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E113" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F113" t="s">
         <v>9</v>
       </c>
       <c r="H113" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="I113" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D114" s="9"/>
       <c r="H114" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="I114" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
@@ -2733,10 +2732,10 @@
         <v>9</v>
       </c>
       <c r="H115" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I115" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
@@ -2748,28 +2747,28 @@
         <v>9</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I116" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D117" s="9"/>
       <c r="I117" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D118" s="9"/>
       <c r="I118" s="19" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D119" s="9"/>
       <c r="I119" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
@@ -2780,49 +2779,49 @@
         <v>34</v>
       </c>
       <c r="C121" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D121" s="9" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F121" t="s">
         <v>9</v>
       </c>
       <c r="H121" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="I121" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D122" s="9"/>
       <c r="H122" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I122" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D123" s="9"/>
       <c r="H123" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="I123" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D124" s="9"/>
       <c r="H124" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="I124" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
@@ -2834,10 +2833,10 @@
         <v>9</v>
       </c>
       <c r="H125" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I125" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.3">
@@ -2849,16 +2848,16 @@
         <v>9</v>
       </c>
       <c r="H126" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I126" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D127" s="9"/>
       <c r="I127" s="22" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
@@ -2869,49 +2868,49 @@
         <v>34</v>
       </c>
       <c r="C129" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D129" s="9" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E129" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F129" t="s">
+        <v>9</v>
+      </c>
+      <c r="H129" t="s">
+        <v>210</v>
+      </c>
+      <c r="I129" s="23" t="s">
         <v>211</v>
-      </c>
-      <c r="F129" t="s">
-        <v>9</v>
-      </c>
-      <c r="H129" t="s">
-        <v>212</v>
-      </c>
-      <c r="I129" s="23" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D130" s="9"/>
       <c r="H130" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D131" s="9"/>
       <c r="H131" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="I131" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D132" s="9"/>
       <c r="H132" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="I132" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.3">
@@ -2923,10 +2922,10 @@
         <v>9</v>
       </c>
       <c r="H133" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I133" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.3">
@@ -2938,22 +2937,22 @@
         <v>9</v>
       </c>
       <c r="H134" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I134" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D135" s="9"/>
       <c r="I135" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D136" s="9"/>
       <c r="I136" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
@@ -2962,49 +2961,49 @@
     <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D138" s="9"/>
       <c r="I138" s="23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D139" s="9"/>
       <c r="I139" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D140" s="9"/>
       <c r="I140" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D141" s="9"/>
       <c r="I141" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
       <c r="I142" s="19" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D143" s="9"/>
       <c r="I143" s="19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D144" s="9"/>
       <c r="I144" s="19" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D145" s="9"/>
       <c r="I145" s="19" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
@@ -3013,16 +3012,16 @@
     </row>
     <row r="147" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C147" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D147" s="9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I147" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.3">
@@ -3030,16 +3029,16 @@
     </row>
     <row r="149" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
+        <v>47</v>
+      </c>
+      <c r="C149" t="s">
+        <v>266</v>
+      </c>
+      <c r="D149" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E149" t="s">
         <v>49</v>
-      </c>
-      <c r="C149" t="s">
-        <v>268</v>
-      </c>
-      <c r="D149" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="E149" t="s">
-        <v>51</v>
       </c>
       <c r="F149" t="s">
         <v>23</v>
@@ -3048,7 +3047,7 @@
     <row r="150" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D150" s="9"/>
       <c r="E150" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F150" t="s">
         <v>23</v>
@@ -3059,25 +3058,25 @@
     </row>
     <row r="152" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B152" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C152" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D152" s="9" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E152" t="s">
+        <v>193</v>
+      </c>
+      <c r="F152" t="s">
+        <v>23</v>
+      </c>
+      <c r="H152" t="s">
         <v>195</v>
       </c>
-      <c r="F152" t="s">
-        <v>23</v>
-      </c>
-      <c r="H152" t="s">
+      <c r="I152" s="21" t="s">
         <v>197</v>
-      </c>
-      <c r="I152" s="21" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="153" spans="2:9" x14ac:dyDescent="0.3">
@@ -3098,13 +3097,13 @@
     <row r="154" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D154" s="9"/>
       <c r="E154" t="s">
+        <v>194</v>
+      </c>
+      <c r="F154" t="s">
+        <v>23</v>
+      </c>
+      <c r="H154" s="17" t="s">
         <v>196</v>
-      </c>
-      <c r="F154" t="s">
-        <v>23</v>
-      </c>
-      <c r="H154" s="17" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.3">
@@ -3112,51 +3111,51 @@
     </row>
     <row r="156" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B156" t="s">
+        <v>47</v>
+      </c>
+      <c r="C156" t="s">
+        <v>266</v>
+      </c>
+      <c r="D156" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E156" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C156" t="s">
-        <v>268</v>
-      </c>
-      <c r="D156" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E156" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="F156" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G156" s="10"/>
       <c r="H156" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I156" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="157" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D157" s="10"/>
       <c r="E157" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F157" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H157" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I157" s="1"/>
     </row>
     <row r="158" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D158" s="10"/>
       <c r="E158" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F158" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="I158" s="13"/>
     </row>
@@ -3194,50 +3193,50 @@
     </row>
     <row r="162" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B162" t="s">
+        <v>47</v>
+      </c>
+      <c r="C162" t="s">
+        <v>266</v>
+      </c>
+      <c r="D162" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="E162" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="C162" t="s">
-        <v>268</v>
-      </c>
-      <c r="D162" s="9" t="s">
-        <v>316</v>
-      </c>
-      <c r="E162" s="10" t="s">
-        <v>51</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G162" s="10"/>
       <c r="H162" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I162" s="26" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D163" s="9"/>
       <c r="E163" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H163" s="14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="164" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D164" s="9"/>
       <c r="E164" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F164" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.3">
@@ -3261,25 +3260,25 @@
     </row>
     <row r="167" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B167" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C167" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D167" s="9" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E167" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="F167" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="H167" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="I167" s="26" t="s">
         <v>327</v>
-      </c>
-      <c r="F167" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H167" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="I167" s="26" t="s">
-        <v>330</v>
       </c>
     </row>
     <row r="168" spans="2:9" x14ac:dyDescent="0.3">
@@ -3314,25 +3313,25 @@
     </row>
     <row r="171" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B171" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C171" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D171" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="E171" t="s">
+        <v>193</v>
+      </c>
+      <c r="F171" t="s">
+        <v>23</v>
+      </c>
+      <c r="H171" t="s">
+        <v>195</v>
+      </c>
+      <c r="I171" s="26" t="s">
         <v>328</v>
-      </c>
-      <c r="E171" t="s">
-        <v>195</v>
-      </c>
-      <c r="F171" t="s">
-        <v>23</v>
-      </c>
-      <c r="H171" t="s">
-        <v>197</v>
-      </c>
-      <c r="I171" s="26" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="172" spans="2:9" x14ac:dyDescent="0.3">
@@ -3353,13 +3352,13 @@
     <row r="173" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D173" s="9"/>
       <c r="E173" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F173" t="s">
         <v>23</v>
       </c>
       <c r="H173" s="17" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.3">
@@ -3370,20 +3369,20 @@
     </row>
     <row r="175" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B175" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C175" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
       <c r="H175" s="3"/>
       <c r="I175" s="7" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.3">
@@ -3394,20 +3393,20 @@
     </row>
     <row r="178" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B178" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C178" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E178" s="1"/>
       <c r="F178" s="1"/>
       <c r="G178" s="1"/>
       <c r="H178" s="3"/>
       <c r="I178" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.3">
@@ -3415,26 +3414,26 @@
     </row>
     <row r="180" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B180" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C180" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G180" s="1"/>
       <c r="H180" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I180" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="181" spans="2:9" x14ac:dyDescent="0.3">
@@ -3442,14 +3441,14 @@
       <c r="C181" s="1"/>
       <c r="D181" s="10"/>
       <c r="E181" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G181" s="1"/>
       <c r="H181" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I181" s="1"/>
     </row>
@@ -3458,26 +3457,26 @@
     </row>
     <row r="183" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B183" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C183" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D183" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E183" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F183" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G183" s="1"/>
       <c r="H183" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="I183" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="184" spans="2:9" x14ac:dyDescent="0.3">
@@ -3485,14 +3484,14 @@
       <c r="C184" s="1"/>
       <c r="D184" s="10"/>
       <c r="E184" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F184" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G184" s="1"/>
       <c r="H184" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I184" s="1"/>
     </row>
@@ -3501,7 +3500,7 @@
       <c r="C185" s="1"/>
       <c r="D185" s="10"/>
       <c r="E185" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F185" s="1" t="s">
         <v>9</v>
@@ -3553,13 +3552,13 @@
     </row>
     <row r="189" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B189" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C189" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D189" s="10" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E189" s="1" t="s">
         <v>32</v>
@@ -3569,10 +3568,10 @@
       </c>
       <c r="G189" s="1"/>
       <c r="H189" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I189" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="190" spans="2:9" x14ac:dyDescent="0.3">
@@ -3580,14 +3579,14 @@
       <c r="C190" s="1"/>
       <c r="D190" s="10"/>
       <c r="E190" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F190" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G190" s="1"/>
       <c r="H190" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="I190" s="1"/>
     </row>
@@ -3630,21 +3629,21 @@
     <row r="193" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D193" s="9"/>
       <c r="F193" s="10" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="194" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B194" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C194" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D194" s="10" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="I194" s="26" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="195" spans="2:9" x14ac:dyDescent="0.3">
@@ -3652,25 +3651,25 @@
     </row>
     <row r="196" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B196" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C196" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="E196" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H196" t="s">
         <v>286</v>
       </c>
-      <c r="F196" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H196" t="s">
-        <v>288</v>
-      </c>
       <c r="I196" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.3">
@@ -3690,25 +3689,25 @@
     </row>
     <row r="199" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B199" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C199" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E199" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H199" t="s">
         <v>286</v>
       </c>
-      <c r="F199" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H199" t="s">
-        <v>288</v>
-      </c>
       <c r="I199" s="26" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.3">
@@ -3717,43 +3716,43 @@
     <row r="201" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D201" s="9"/>
       <c r="H201" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I201" s="26"/>
     </row>
     <row r="202" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B202" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C202" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D202" s="10" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E202" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F202" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H202" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="I202" s="26" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D203" s="9"/>
       <c r="H203" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D204" s="9"/>
       <c r="H204" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.3">
@@ -3761,110 +3760,110 @@
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B206" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C206" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D206" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="H206" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="207" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E207" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F207" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H207" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H208" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="209" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H209" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B211" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C211" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D211" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="H211" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="212" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E212" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F212" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H212" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="213" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H213" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="214" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H214" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="216" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B216" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C216" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D216" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="H216" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="217" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D217" s="9"/>
       <c r="E217" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F217" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H217" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="218" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D218" s="9"/>
       <c r="H218" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D219" s="9"/>
       <c r="H219" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="220" spans="2:8" x14ac:dyDescent="0.3">
@@ -3872,23 +3871,23 @@
     </row>
     <row r="221" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B221" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C221" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D221" s="32" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E221" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F221" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G221" s="8"/>
       <c r="H221" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="222" spans="2:8" x14ac:dyDescent="0.3">
@@ -3930,7 +3929,7 @@
       <c r="C224" s="8"/>
       <c r="D224" s="32"/>
       <c r="E224" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F224" s="8" t="s">
         <v>23</v>
@@ -3951,7 +3950,7 @@
     <row r="226" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D226" s="9"/>
       <c r="H226" s="18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="227" spans="2:9" x14ac:dyDescent="0.3">
@@ -3962,13 +3961,13 @@
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B229" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C229" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D229" s="32" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E229" s="33" t="s">
         <v>32</v>
@@ -3978,18 +3977,18 @@
       </c>
       <c r="G229" s="8"/>
       <c r="H229" s="32" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="230" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D230" s="9"/>
       <c r="E230" s="8"/>
       <c r="F230" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G230" s="8"/>
       <c r="H230" s="18" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="231" spans="2:9" x14ac:dyDescent="0.3">
@@ -4031,43 +4030,43 @@
     </row>
     <row r="234" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B234" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C234" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D234" s="9" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H234" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I234" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="235" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D235" s="9"/>
       <c r="E235" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F235" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H235" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="236" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D236" s="9"/>
       <c r="H236" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D237" s="9"/>
       <c r="H237" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="238" spans="2:9" x14ac:dyDescent="0.3">
@@ -4079,43 +4078,43 @@
     </row>
     <row r="239" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B239" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C239" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D239" s="9" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="H239" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="I239" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="240" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D240" s="9"/>
       <c r="E240" s="11" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="F240" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H240" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="241" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D241" s="9"/>
       <c r="H241" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D242" s="9"/>
       <c r="H242" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="243" spans="2:9" x14ac:dyDescent="0.3">
@@ -4127,26 +4126,26 @@
     </row>
     <row r="244" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
       <c r="B244" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C244" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D244" s="34" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E244" s="8" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="F244" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G244" s="8"/>
       <c r="H244" s="18" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="I244" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
     </row>
     <row r="245" spans="2:9" x14ac:dyDescent="0.3">
@@ -4182,7 +4181,7 @@
     <row r="247" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D247" s="9"/>
       <c r="E247" s="8" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="F247" s="8" t="s">
         <v>23</v>
@@ -4201,7 +4200,7 @@
     <row r="249" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D249" s="9"/>
       <c r="H249" s="18" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="250" spans="2:9" x14ac:dyDescent="0.3">
@@ -4213,13 +4212,13 @@
     </row>
     <row r="251" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B251" s="8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C251" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D251" s="32" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E251" s="33" t="s">
         <v>32</v>
@@ -4229,18 +4228,18 @@
       </c>
       <c r="G251" s="8"/>
       <c r="H251" s="32" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="252" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D252" s="9"/>
       <c r="E252" s="8"/>
       <c r="F252" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G252" s="8"/>
       <c r="H252" s="18" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="253" spans="2:9" x14ac:dyDescent="0.3">
@@ -4282,13 +4281,13 @@
     </row>
     <row r="256" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B256" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C256" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D256" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E256" t="s">
         <v>15</v>
@@ -4303,7 +4302,7 @@
         <v>20210401</v>
       </c>
       <c r="I256" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="257" spans="2:9" x14ac:dyDescent="0.3">
@@ -4324,7 +4323,7 @@
     <row r="258" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D258" s="9"/>
       <c r="E258" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F258" t="s">
         <v>9</v>
@@ -4339,17 +4338,17 @@
     </row>
     <row r="260" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B260" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C260" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D260" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H260" s="6"/>
       <c r="I260" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="261" spans="2:9" x14ac:dyDescent="0.3">
@@ -4362,17 +4361,17 @@
     </row>
     <row r="263" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B263" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C263" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H263" s="6"/>
       <c r="I263" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="264" spans="2:9" x14ac:dyDescent="0.3">
@@ -4385,17 +4384,17 @@
     </row>
     <row r="266" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B266" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C266" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D266" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H266" s="6"/>
       <c r="I266" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="267" spans="2:9" x14ac:dyDescent="0.3">
@@ -4408,34 +4407,34 @@
     </row>
     <row r="269" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B269" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C269" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D269" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="E269" t="s">
+        <v>107</v>
+      </c>
+      <c r="F269" t="s">
         <v>108</v>
-      </c>
-      <c r="E269" t="s">
-        <v>109</v>
-      </c>
-      <c r="F269" t="s">
-        <v>110</v>
       </c>
       <c r="H269" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I269" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="270" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D270" s="9"/>
       <c r="E270" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F270" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H270" s="6" t="b">
         <v>1</v>
@@ -4447,16 +4446,16 @@
     </row>
     <row r="272" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B272" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C272" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D272" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E272" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F272" t="s">
         <v>21</v>
@@ -4465,7 +4464,7 @@
         <v>3</v>
       </c>
       <c r="I272" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="273" spans="2:9" x14ac:dyDescent="0.3">
@@ -4473,20 +4472,20 @@
     </row>
     <row r="274" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B274" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C274" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D274" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E274" s="1"/>
       <c r="F274" s="10"/>
       <c r="G274" s="1"/>
       <c r="H274" s="3"/>
       <c r="I274" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="275" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4501,13 +4500,13 @@
     </row>
     <row r="276" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B276" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C276" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D276" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E276" s="1"/>
       <c r="F276" s="10"/>
@@ -4529,26 +4528,26 @@
     </row>
     <row r="278" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B278" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C278" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D278" s="10" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E278" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F278" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G278" s="1"/>
       <c r="H278" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I278" s="26" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="279" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4563,13 +4562,13 @@
     </row>
     <row r="280" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B280" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C280" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D280" s="10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E280" s="11"/>
       <c r="F280" s="10"/>
@@ -4588,26 +4587,26 @@
     </row>
     <row r="282" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B282" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C282" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D282" s="10" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E282" s="11" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="F282" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G282" s="1"/>
       <c r="H282" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="I282" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="283" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4615,7 +4614,7 @@
       <c r="C283" s="1"/>
       <c r="D283" s="10"/>
       <c r="E283" s="11" t="s">
-        <v>321</v>
+        <v>337</v>
       </c>
       <c r="F283" s="10" t="s">
         <v>9</v>
@@ -4631,7 +4630,7 @@
       <c r="C284" s="1"/>
       <c r="D284" s="10"/>
       <c r="E284" s="11" t="s">
-        <v>67</v>
+        <v>338</v>
       </c>
       <c r="F284" s="10" t="s">
         <v>9</v>
@@ -4647,13 +4646,13 @@
     </row>
     <row r="286" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B286" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C286" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D286" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E286" s="11" t="s">
         <v>22</v>
@@ -4665,7 +4664,7 @@
         <v>20191101</v>
       </c>
       <c r="I286" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="287" spans="2:9" x14ac:dyDescent="0.3">
@@ -4673,13 +4672,13 @@
     </row>
     <row r="288" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B288" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C288" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D288" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E288" t="s">
         <v>15</v>
@@ -4688,10 +4687,10 @@
         <v>9</v>
       </c>
       <c r="H288" s="35" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I288" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="289" spans="1:9" x14ac:dyDescent="0.3">
@@ -4703,42 +4702,42 @@
         <v>9</v>
       </c>
       <c r="H289" s="35" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I289" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="290" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D290" s="9"/>
       <c r="H290" s="8"/>
       <c r="I290" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="291" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D291" s="9"/>
       <c r="H291" s="8"/>
       <c r="I291" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="292" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D292" s="9"/>
       <c r="I292" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="293" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D293" s="9"/>
       <c r="I293" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="294" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D294" s="9"/>
       <c r="I294" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="295" spans="1:9" x14ac:dyDescent="0.3">
@@ -4749,13 +4748,13 @@
         <v>36</v>
       </c>
       <c r="B296" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D296" s="10" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E296" s="1" t="s">
         <v>15</v>
@@ -4770,7 +4769,7 @@
         <v>20200401</v>
       </c>
       <c r="I296" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="297" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4798,7 +4797,7 @@
       <c r="C298" s="1"/>
       <c r="D298" s="10"/>
       <c r="E298" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F298" s="1" t="s">
         <v>9</v>
@@ -4822,13 +4821,13 @@
     </row>
     <row r="300" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B300" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C300" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D300" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="E300" t="s">
         <v>27</v>
@@ -4837,25 +4836,25 @@
         <v>9</v>
       </c>
       <c r="H300" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="I300" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="301" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D301" s="9"/>
       <c r="E301" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F301" t="s">
         <v>9</v>
       </c>
       <c r="H301" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="I301" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="302" spans="1:9" x14ac:dyDescent="0.3">
@@ -4867,10 +4866,10 @@
         <v>9</v>
       </c>
       <c r="H302" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I302" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="303" spans="1:9" x14ac:dyDescent="0.3">
@@ -4882,34 +4881,34 @@
         <v>9</v>
       </c>
       <c r="H303" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I303" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="304" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D304" s="9"/>
       <c r="I304" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="305" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D305" s="9"/>
       <c r="I305" s="19" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="306" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D306" s="9"/>
       <c r="I306" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D307" s="9"/>
       <c r="I307" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="308" spans="2:9" x14ac:dyDescent="0.3">
@@ -4917,13 +4916,13 @@
     </row>
     <row r="309" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B309" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C309" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D309" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="C309" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D309" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="E309" t="s">
         <v>27</v>
@@ -4932,10 +4931,10 @@
         <v>9</v>
       </c>
       <c r="H309" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="I309" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
@@ -4947,10 +4946,10 @@
         <v>9</v>
       </c>
       <c r="H310" s="17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="I310" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="311" spans="2:9" x14ac:dyDescent="0.3">
@@ -4962,28 +4961,28 @@
         <v>9</v>
       </c>
       <c r="H311" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="I311" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="312" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D312" s="9"/>
       <c r="I312" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="313" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D313" s="9"/>
       <c r="I313" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="314" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D314" s="9"/>
       <c r="I314" s="25" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="315" spans="2:9" x14ac:dyDescent="0.3">
@@ -4991,7 +4990,7 @@
       <c r="E315" s="24"/>
       <c r="H315" s="18"/>
       <c r="I315" s="18" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="316" spans="2:9" x14ac:dyDescent="0.3">
@@ -4999,13 +4998,13 @@
     </row>
     <row r="317" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B317" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D317" s="9" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E317" t="s">
         <v>15</v>
@@ -5020,7 +5019,7 @@
         <v>20200401</v>
       </c>
       <c r="I317" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.3">
@@ -5045,13 +5044,13 @@
     </row>
     <row r="320" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B320" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C320" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D320" s="9" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E320" t="s">
         <v>15</v>
@@ -5066,7 +5065,7 @@
         <v>20200401</v>
       </c>
       <c r="I320" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="321" spans="2:9" x14ac:dyDescent="0.3">
@@ -5087,49 +5086,49 @@
     <row r="322" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D322" s="9"/>
       <c r="E322" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F322" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H322" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D323" s="9"/>
       <c r="E323" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F323" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H323" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="324" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D324" s="9"/>
       <c r="E324" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="F324" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H324" s="8" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="325" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D325" s="9"/>
       <c r="E325" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="F325" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H325" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="326" spans="2:9" x14ac:dyDescent="0.3">
@@ -5138,13 +5137,13 @@
     </row>
     <row r="327" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B327" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C327" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D327" s="9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E327" t="s">
         <v>15</v>
@@ -5159,7 +5158,7 @@
         <v>20200401</v>
       </c>
       <c r="I327" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="328" spans="2:9" x14ac:dyDescent="0.3">
@@ -5180,19 +5179,19 @@
     <row r="329" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D329" s="9"/>
       <c r="E329" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F329" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H329" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="330" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D330" s="9"/>
       <c r="E330" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F330" s="9" t="s">
         <v>23</v>
@@ -5204,7 +5203,7 @@
     <row r="331" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D331" s="9"/>
       <c r="E331" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F331" s="9" t="s">
         <v>23</v>
@@ -5219,13 +5218,13 @@
     </row>
     <row r="333" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B333" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D333" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E333" t="s">
         <v>15</v>
@@ -5240,7 +5239,7 @@
         <v>20200401</v>
       </c>
       <c r="I333" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="334" spans="2:9" x14ac:dyDescent="0.3">
@@ -5264,13 +5263,13 @@
     </row>
     <row r="336" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B336" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C336" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D336" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E336" t="s">
         <v>15</v>
@@ -5285,7 +5284,7 @@
         <v>20200401</v>
       </c>
       <c r="I336" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="337" spans="2:9" x14ac:dyDescent="0.3">
@@ -5306,7 +5305,7 @@
     <row r="338" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D338" s="9"/>
       <c r="E338" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F338" s="9" t="s">
         <v>23</v>
@@ -5321,13 +5320,13 @@
     </row>
     <row r="340" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B340" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C340" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D340" s="9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E340" t="s">
         <v>22</v>
@@ -5342,7 +5341,7 @@
         <v>20220228</v>
       </c>
       <c r="I340" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="341" spans="2:9" x14ac:dyDescent="0.3">
@@ -5354,7 +5353,7 @@
         <v>23</v>
       </c>
       <c r="H341" s="8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="342" spans="2:9" x14ac:dyDescent="0.3">
@@ -5378,16 +5377,16 @@
         <v>23</v>
       </c>
       <c r="H343" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="344" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D344" s="9"/>
       <c r="E344" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F344" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H344" s="8">
         <v>4</v>
@@ -5396,10 +5395,10 @@
     <row r="345" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D345" s="9"/>
       <c r="E345" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F345" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H345" s="8">
         <v>48</v>
@@ -5408,10 +5407,10 @@
     <row r="346" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D346" s="9"/>
       <c r="E346" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F346" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H346" s="8">
         <v>1.1000000000000001</v>
@@ -5420,10 +5419,10 @@
     <row r="347" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D347" s="9"/>
       <c r="E347" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F347" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H347" s="8">
         <v>3.2</v>
@@ -5432,10 +5431,10 @@
     <row r="348" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D348" s="9"/>
       <c r="E348" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F348" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H348" s="8">
         <v>0.11</v>
@@ -5444,10 +5443,10 @@
     <row r="349" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D349" s="9"/>
       <c r="E349" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F349" s="9" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H349" s="8">
         <v>0.2</v>
@@ -5456,7 +5455,7 @@
     <row r="350" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D350" s="9"/>
       <c r="E350" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="F350" s="9" t="s">
         <v>23</v>
@@ -5470,20 +5469,20 @@
     </row>
     <row r="352" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B352" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C352" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D352" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E352" s="1"/>
       <c r="F352" s="1"/>
       <c r="G352" s="1"/>
       <c r="H352" s="3"/>
       <c r="I352" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="353" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5498,26 +5497,26 @@
     </row>
     <row r="354" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B354" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C354" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D354" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E354" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F354" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G354" s="1"/>
       <c r="H354" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I354" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="355" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5532,22 +5531,22 @@
     </row>
     <row r="356" spans="2:9" ht="29.4" x14ac:dyDescent="0.35">
       <c r="B356" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C356" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D356" s="10" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E356" s="1"/>
       <c r="F356" s="1"/>
       <c r="G356" s="1"/>
       <c r="H356" s="12" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="I356" s="7" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="357" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5562,16 +5561,16 @@
     </row>
     <row r="358" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B358" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C358" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D358" s="10" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E358" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="F358" s="10" t="s">
         <v>23</v>
@@ -5581,7 +5580,7 @@
         <v>531733</v>
       </c>
       <c r="I358" s="7" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="359" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5589,7 +5588,7 @@
       <c r="C359" s="1"/>
       <c r="D359" s="10"/>
       <c r="E359" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="F359" s="1" t="s">
         <v>23</v>
@@ -5612,26 +5611,26 @@
     </row>
     <row r="361" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B361" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C361" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D361" s="10" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E361" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F361" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G361" s="1"/>
       <c r="H361" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="I361" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="362" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5646,16 +5645,16 @@
     </row>
     <row r="363" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B363" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C363" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D363" s="10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E363" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F363" s="1" t="s">
         <v>9</v>
@@ -5665,7 +5664,7 @@
         <v>14</v>
       </c>
       <c r="I363" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="364" spans="2:9" x14ac:dyDescent="0.3">
@@ -5673,14 +5672,14 @@
       <c r="C364" s="1"/>
       <c r="D364" s="10"/>
       <c r="E364" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F364" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G364" s="1"/>
       <c r="H364" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I364" s="1"/>
     </row>
@@ -5728,36 +5727,36 @@
     </row>
     <row r="369" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B369" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C369" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D369" s="9" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="E369" s="8" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="F369" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G369" s="8"/>
       <c r="H369" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
     </row>
     <row r="370" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D370" s="9"/>
       <c r="E370" s="8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="F370" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G370" s="8"/>
       <c r="H370" s="18" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="371" spans="2:8" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
capital gain loss input output parameter change
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="908" uniqueCount="338">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -90,9 +90,6 @@
     <t>string</t>
   </si>
   <si>
-    <t>bsFlag</t>
-  </si>
-  <si>
     <t>S</t>
   </si>
   <si>
@@ -123,9 +120,6 @@
     <t>Transaction</t>
   </si>
   <si>
-    <t>tradeType</t>
-  </si>
-  <si>
     <t>Trades</t>
   </si>
   <si>
@@ -381,9 +375,6 @@
     <t>chkIgnoreSection</t>
   </si>
   <si>
-    <t>trxType</t>
-  </si>
-  <si>
     <t>B</t>
   </si>
   <si>
@@ -399,16 +390,10 @@
     <t>ignore112A</t>
   </si>
   <si>
-    <t>scripCd</t>
-  </si>
-  <si>
     <t>CapitalGainLoss_TradeListingSummary</t>
   </si>
   <si>
     <t>CapitalGainLoss_TradeListingDetail</t>
-  </si>
-  <si>
-    <t>sccdPostBack</t>
   </si>
   <si>
     <t>CapitalGainLoss_TradeInsert</t>
@@ -1067,6 +1052,12 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>scripCode</t>
+  </si>
+  <si>
+    <t>flag</t>
   </si>
 </sst>
 </file>
@@ -1532,8 +1523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I380"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C286" workbookViewId="0">
-      <selection activeCell="G297" sqref="G297"/>
+    <sheetView tabSelected="1" topLeftCell="C310" workbookViewId="0">
+      <selection activeCell="H326" sqref="H326"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1564,13 +1555,13 @@
     </row>
     <row r="2" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -1596,13 +1587,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1613,10 +1604,10 @@
         <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1636,10 +1627,10 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1651,7 +1642,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1674,10 +1665,10 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1697,10 +1688,10 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1715,13 +1706,13 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="9"/>
       <c r="E14" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F14" t="s">
         <v>23</v>
       </c>
       <c r="H14" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1732,10 +1723,10 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1750,7 +1741,7 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D17" s="9"/>
       <c r="E17" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
@@ -1759,7 +1750,7 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D18" s="9"/>
       <c r="E18" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F18" t="s">
         <v>23</v>
@@ -1768,7 +1759,7 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D19" s="9"/>
       <c r="E19" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -1779,16 +1770,16 @@
     </row>
     <row r="21" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="I21" s="7" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1796,52 +1787,52 @@
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>113</v>
-      </c>
       <c r="F23" t="s">
         <v>9</v>
       </c>
       <c r="H23" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="I23" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D24" s="9"/>
       <c r="H24" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="I24" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="9"/>
       <c r="H25" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="I25" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="9"/>
       <c r="H26" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="I26" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -1853,10 +1844,10 @@
         <v>9</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I27" s="18" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -1868,10 +1859,10 @@
         <v>9</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -1879,13 +1870,13 @@
     </row>
     <row r="30" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C30" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E30" t="s">
         <v>15</v>
@@ -1897,10 +1888,10 @@
         <v>16</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
@@ -1915,7 +1906,7 @@
         <v>16</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
@@ -1925,49 +1916,49 @@
     <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D33" s="9"/>
       <c r="E33" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F33" t="s">
         <v>9</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D34" s="9"/>
       <c r="G34" s="20"/>
       <c r="H34" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D35" s="9"/>
       <c r="G35" s="20"/>
       <c r="H35" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D36" s="9"/>
       <c r="G36" s="20"/>
       <c r="H36" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D37" s="9"/>
       <c r="G37" s="20"/>
       <c r="H37" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D38" s="9"/>
       <c r="G38" s="20"/>
       <c r="H38" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
@@ -1977,25 +1968,25 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D40" s="9"/>
       <c r="E40" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D41" s="9"/>
       <c r="H41" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D42" s="9"/>
       <c r="H42" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -2003,61 +1994,61 @@
     </row>
     <row r="44" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E44" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F44" t="s">
         <v>9</v>
       </c>
       <c r="H44" s="17" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="I44" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D45" s="9"/>
       <c r="I45" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D46" s="9"/>
       <c r="I46" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D47" s="9"/>
       <c r="I47" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D48" s="9"/>
       <c r="I48" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D49" s="9"/>
       <c r="I49" s="19" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D50" s="9"/>
       <c r="I50" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2065,25 +2056,25 @@
     </row>
     <row r="52" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B52" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C52" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D52" s="9" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="F52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H52" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -2091,7 +2082,7 @@
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>9</v>
@@ -2105,52 +2096,52 @@
     </row>
     <row r="55" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C55" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D56" s="9"/>
       <c r="I56" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D57" s="9"/>
       <c r="I57" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D58" s="9"/>
       <c r="I58" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D59" s="9"/>
       <c r="I59" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D60" s="9"/>
       <c r="I60" s="19" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D61" s="9"/>
       <c r="I61" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
@@ -2158,61 +2149,61 @@
     </row>
     <row r="63" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C63" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E63" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="I63" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D64" s="9"/>
       <c r="I64" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D65" s="9"/>
       <c r="I65" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D66" s="9"/>
       <c r="I66" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" s="9"/>
       <c r="I67" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D68" s="9"/>
       <c r="I68" s="19" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D69" s="9"/>
       <c r="I69" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
@@ -2220,16 +2211,16 @@
     </row>
     <row r="71" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C71" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
@@ -2237,16 +2228,16 @@
     </row>
     <row r="73" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C73" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E73" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F73" t="s">
         <v>23</v>
@@ -2255,7 +2246,7 @@
         <v>1202870000086520</v>
       </c>
       <c r="I73" s="24" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
@@ -2263,16 +2254,16 @@
     </row>
     <row r="75" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C75" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D75" s="9" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E75" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F75" t="s">
         <v>23</v>
@@ -2281,7 +2272,7 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D76" s="9"/>
       <c r="E76" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="F76" t="s">
         <v>23</v>
@@ -2292,16 +2283,16 @@
     </row>
     <row r="78" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B78" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C78" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="I78" s="24" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
@@ -2312,16 +2303,16 @@
     </row>
     <row r="81" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B81" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C81" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="I81" s="24" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.3">
@@ -2329,25 +2320,25 @@
     </row>
     <row r="83" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B83" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C83" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="E83" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F83" t="s">
         <v>23</v>
       </c>
       <c r="H83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I83" s="24" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.3">
@@ -2355,16 +2346,16 @@
     </row>
     <row r="85" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C85" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D85" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E85" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>9</v>
@@ -2379,7 +2370,7 @@
     <row r="86" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D86" s="10"/>
       <c r="E86" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>9</v>
@@ -2394,25 +2385,25 @@
     </row>
     <row r="88" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B88" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C88" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="E88" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I88" s="24" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
@@ -2421,31 +2412,31 @@
     </row>
     <row r="90" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B90" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C90" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E90" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="I90" s="24" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D91" s="9"/>
       <c r="E91" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>9</v>
@@ -2460,16 +2451,16 @@
     </row>
     <row r="93" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B93" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C93" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E93" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>9</v>
@@ -2479,7 +2470,7 @@
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D94" s="9"/>
       <c r="E94" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>9</v>
@@ -2489,7 +2480,7 @@
     <row r="95" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D95" s="9"/>
       <c r="E95" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>9</v>
@@ -2504,16 +2495,16 @@
     </row>
     <row r="97" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B97" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C97" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E97" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>9</v>
@@ -2523,7 +2514,7 @@
     <row r="98" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D98" s="9"/>
       <c r="E98" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>9</v>
@@ -2539,34 +2530,34 @@
         <v>20</v>
       </c>
       <c r="C100" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>20</v>
       </c>
       <c r="E100" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H100" s="28" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="I100" s="29" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D101" s="9"/>
       <c r="E101" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H101" s="14" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.3">
@@ -2577,13 +2568,13 @@
         <v>20</v>
       </c>
       <c r="C103" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E103" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>9</v>
@@ -2593,7 +2584,7 @@
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D104" s="9"/>
       <c r="E104" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>9</v>
@@ -2603,7 +2594,7 @@
     <row r="105" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D105" s="9"/>
       <c r="E105" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F105" s="1" t="s">
         <v>9</v>
@@ -2613,7 +2604,7 @@
     <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D106" s="9"/>
       <c r="E106" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>9</v>
@@ -2623,7 +2614,7 @@
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D107" s="9"/>
       <c r="E107" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>9</v>
@@ -2633,7 +2624,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>9</v>
@@ -2645,34 +2636,34 @@
     </row>
     <row r="110" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B110" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C110" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E110" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F110" t="s">
         <v>9</v>
       </c>
       <c r="H110" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="I110" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D111" s="9"/>
       <c r="H111" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="I111" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.3">
@@ -2684,10 +2675,10 @@
         <v>9</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I112" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.3">
@@ -2699,28 +2690,28 @@
         <v>9</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I113" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D114" s="9"/>
       <c r="I114" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D115" s="9"/>
       <c r="I115" s="19" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D116" s="9"/>
       <c r="I116" s="19" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
@@ -2728,52 +2719,52 @@
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B118" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C118" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E118" s="11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F118" t="s">
         <v>9</v>
       </c>
       <c r="H118" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="I118" s="19" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D119" s="9"/>
       <c r="H119" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="I119" s="19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D120" s="9"/>
       <c r="H120" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="I120" s="19" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D121" s="9"/>
       <c r="H121" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="I121" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
@@ -2785,10 +2776,10 @@
         <v>9</v>
       </c>
       <c r="H122" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I122" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
@@ -2800,16 +2791,16 @@
         <v>9</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I123" s="19" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D124" s="9"/>
       <c r="I124" s="22" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
@@ -2817,52 +2808,52 @@
     </row>
     <row r="126" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B126" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C126" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E126" s="11" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F126" t="s">
         <v>9</v>
       </c>
       <c r="H126" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="I126" s="23" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D127" s="9"/>
       <c r="H127" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="I127" s="19" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D128" s="9"/>
       <c r="H128" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="I128" s="19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D129" s="9"/>
       <c r="H129" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="I129" s="19" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.3">
@@ -2874,10 +2865,10 @@
         <v>9</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
@@ -2889,22 +2880,22 @@
         <v>9</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="I131" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D132" s="9"/>
       <c r="I132" s="19" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D133" s="9"/>
       <c r="I133" s="19" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.3">
@@ -2913,49 +2904,49 @@
     <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D135" s="9"/>
       <c r="I135" s="23" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D136" s="9"/>
       <c r="I136" s="19" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D137" s="9"/>
       <c r="I137" s="19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D138" s="9"/>
       <c r="I138" s="19" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D139" s="9"/>
       <c r="I139" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D140" s="9"/>
       <c r="I140" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D141" s="9"/>
       <c r="I141" s="19" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
       <c r="I142" s="19" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.3">
@@ -2964,16 +2955,16 @@
     </row>
     <row r="144" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C144" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D144" s="9" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="I144" s="7" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
@@ -2981,16 +2972,16 @@
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B146" t="s">
+        <v>43</v>
+      </c>
+      <c r="C146" t="s">
+        <v>248</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="E146" t="s">
         <v>45</v>
-      </c>
-      <c r="C146" t="s">
-        <v>253</v>
-      </c>
-      <c r="D146" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E146" t="s">
-        <v>47</v>
       </c>
       <c r="F146" t="s">
         <v>23</v>
@@ -2999,7 +2990,7 @@
     <row r="147" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D147" s="9"/>
       <c r="E147" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F147" t="s">
         <v>23</v>
@@ -3010,25 +3001,25 @@
     </row>
     <row r="149" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B149" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C149" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D149" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="E149" t="s">
+        <v>179</v>
+      </c>
+      <c r="F149" t="s">
+        <v>23</v>
+      </c>
+      <c r="H149" t="s">
+        <v>181</v>
+      </c>
+      <c r="I149" s="21" t="s">
         <v>183</v>
-      </c>
-      <c r="E149" t="s">
-        <v>184</v>
-      </c>
-      <c r="F149" t="s">
-        <v>23</v>
-      </c>
-      <c r="H149" t="s">
-        <v>186</v>
-      </c>
-      <c r="I149" s="21" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.3">
@@ -3049,13 +3040,13 @@
     <row r="151" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D151" s="9"/>
       <c r="E151" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F151" t="s">
         <v>23</v>
       </c>
       <c r="H151" s="17" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.3">
@@ -3063,51 +3054,51 @@
     </row>
     <row r="153" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B153" t="s">
+        <v>43</v>
+      </c>
+      <c r="C153" t="s">
+        <v>248</v>
+      </c>
+      <c r="D153" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E153" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="C153" t="s">
-        <v>253</v>
-      </c>
-      <c r="D153" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="E153" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="F153" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G153" s="10"/>
       <c r="H153" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I153" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="154" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D154" s="10"/>
       <c r="E154" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F154" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H154" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I154" s="1"/>
     </row>
     <row r="155" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D155" s="10"/>
       <c r="E155" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F155" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="I155" s="13"/>
     </row>
@@ -3145,50 +3136,50 @@
     </row>
     <row r="159" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B159" t="s">
+        <v>43</v>
+      </c>
+      <c r="C159" t="s">
+        <v>248</v>
+      </c>
+      <c r="D159" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="E159" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="C159" t="s">
-        <v>253</v>
-      </c>
-      <c r="D159" s="9" t="s">
-        <v>301</v>
-      </c>
-      <c r="E159" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="F159" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G159" s="10"/>
       <c r="H159" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I159" s="24" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
     </row>
     <row r="160" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D160" s="9"/>
       <c r="E160" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F160" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H160" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="161" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D161" s="9"/>
       <c r="E161" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F161" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H161" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="162" spans="2:9" x14ac:dyDescent="0.3">
@@ -3212,25 +3203,25 @@
     </row>
     <row r="164" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B164" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C164" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D164" s="9" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E164" s="10" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F164" s="10" t="s">
         <v>23</v>
       </c>
       <c r="H164" s="14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I164" s="24" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.3">
@@ -3265,25 +3256,25 @@
     </row>
     <row r="168" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B168" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C168" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="E168" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="F168" t="s">
         <v>23</v>
       </c>
       <c r="H168" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="I168" s="24" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="169" spans="2:9" x14ac:dyDescent="0.3">
@@ -3304,13 +3295,13 @@
     <row r="170" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D170" s="9"/>
       <c r="E170" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F170" t="s">
         <v>23</v>
       </c>
       <c r="H170" s="17" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.3">
@@ -3321,20 +3312,20 @@
     </row>
     <row r="172" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B172" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C172" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D172" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E172" s="1"/>
       <c r="F172" s="1"/>
       <c r="G172" s="1"/>
       <c r="H172" s="3"/>
       <c r="I172" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.3">
@@ -3345,20 +3336,20 @@
     </row>
     <row r="175" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B175" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C175" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E175" s="1"/>
       <c r="F175" s="1"/>
       <c r="G175" s="1"/>
       <c r="H175" s="3"/>
       <c r="I175" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.3">
@@ -3366,26 +3357,26 @@
     </row>
     <row r="177" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B177" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C177" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D177" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E177" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F177" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G177" s="1"/>
       <c r="H177" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I177" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="178" spans="2:9" x14ac:dyDescent="0.3">
@@ -3393,14 +3384,14 @@
       <c r="C178" s="1"/>
       <c r="D178" s="10"/>
       <c r="E178" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G178" s="1"/>
       <c r="H178" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I178" s="1"/>
     </row>
@@ -3409,26 +3400,26 @@
     </row>
     <row r="180" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B180" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C180" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D180" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E180" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F180" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G180" s="1"/>
       <c r="H180" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I180" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="181" spans="2:9" x14ac:dyDescent="0.3">
@@ -3436,14 +3427,14 @@
       <c r="C181" s="1"/>
       <c r="D181" s="10"/>
       <c r="E181" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G181" s="1"/>
       <c r="H181" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I181" s="1"/>
     </row>
@@ -3452,14 +3443,14 @@
       <c r="C182" s="1"/>
       <c r="D182" s="10"/>
       <c r="E182" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F182" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G182" s="1"/>
       <c r="H182" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I182" s="1"/>
     </row>
@@ -3504,26 +3495,26 @@
     </row>
     <row r="186" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B186" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C186" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D186" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E186" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G186" s="1"/>
       <c r="H186" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I186" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="187" spans="2:9" x14ac:dyDescent="0.3">
@@ -3531,14 +3522,14 @@
       <c r="C187" s="1"/>
       <c r="D187" s="10"/>
       <c r="E187" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F187" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G187" s="1"/>
       <c r="H187" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I187" s="1"/>
     </row>
@@ -3581,21 +3572,21 @@
     <row r="190" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D190" s="9"/>
       <c r="F190" s="10" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
     </row>
     <row r="191" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B191" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C191" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D191" s="10" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="I191" s="24" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.3">
@@ -3603,25 +3594,25 @@
     </row>
     <row r="193" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B193" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C193" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D193" s="10" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="E193" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F193" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H193" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="I193" s="24" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="194" spans="2:9" x14ac:dyDescent="0.3">
@@ -3641,25 +3632,25 @@
     </row>
     <row r="196" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B196" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C196" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="E196" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F196" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H196" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="I196" s="24" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.3">
@@ -3668,43 +3659,43 @@
     <row r="198" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D198" s="9"/>
       <c r="H198" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="I198" s="24"/>
     </row>
     <row r="199" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B199" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C199" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E199" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="F199" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H199" t="s">
+        <v>273</v>
+      </c>
+      <c r="I199" s="24" t="s">
         <v>271</v>
-      </c>
-      <c r="F199" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H199" t="s">
-        <v>278</v>
-      </c>
-      <c r="I199" s="24" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D200" s="9"/>
       <c r="H200" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D201" s="9"/>
       <c r="H201" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="202" spans="2:9" x14ac:dyDescent="0.3">
@@ -3712,110 +3703,110 @@
     </row>
     <row r="203" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B203" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C203" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D203" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="H203" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E204" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H204" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H205" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H206" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B208" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C208" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D208" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="H208" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="209" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E209" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H209" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="210" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H210" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H211" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="213" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B213" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C213" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D213" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="H213" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
     </row>
     <row r="214" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D214" s="9"/>
       <c r="E214" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H214" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="215" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D215" s="9"/>
       <c r="H215" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="216" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D216" s="9"/>
       <c r="H216" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="217" spans="2:8" x14ac:dyDescent="0.3">
@@ -3823,23 +3814,23 @@
     </row>
     <row r="218" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B218" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C218" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D218" s="30" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="E218" s="8" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F218" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G218" s="8"/>
       <c r="H218" s="18" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.3">
@@ -3881,7 +3872,7 @@
       <c r="C221" s="8"/>
       <c r="D221" s="30"/>
       <c r="E221" s="8" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F221" s="8" t="s">
         <v>23</v>
@@ -3902,7 +3893,7 @@
     <row r="223" spans="2:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D223" s="9"/>
       <c r="H223" s="18" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="224" spans="2:8" x14ac:dyDescent="0.3">
@@ -3913,34 +3904,34 @@
     </row>
     <row r="226" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B226" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D226" s="30" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="E226" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F226" s="30" t="s">
         <v>23</v>
       </c>
       <c r="G226" s="8"/>
       <c r="H226" s="30" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="227" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D227" s="9"/>
       <c r="E227" s="8"/>
       <c r="F227" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G227" s="8"/>
       <c r="H227" s="18" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.3">
@@ -3982,43 +3973,43 @@
     </row>
     <row r="231" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B231" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D231" s="9" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="H231" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="I231" s="7" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="232" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D232" s="9"/>
       <c r="E232" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H232" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="233" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D233" s="9"/>
       <c r="H233" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="234" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D234" s="9"/>
       <c r="H234" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="235" spans="2:9" x14ac:dyDescent="0.3">
@@ -4030,43 +4021,43 @@
     </row>
     <row r="236" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B236" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D236" s="9" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="H236" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="I236" s="7" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D237" s="9"/>
       <c r="E237" s="11" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H237" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
     </row>
     <row r="238" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D238" s="9"/>
       <c r="H238" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="239" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D239" s="9"/>
       <c r="H239" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
     </row>
     <row r="240" spans="2:9" x14ac:dyDescent="0.3">
@@ -4078,26 +4069,26 @@
     </row>
     <row r="241" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
       <c r="B241" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C241" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D241" s="32" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="E241" s="8" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="F241" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G241" s="8"/>
       <c r="H241" s="18" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="I241" s="7" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.3">
@@ -4133,7 +4124,7 @@
     <row r="244" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D244" s="9"/>
       <c r="E244" s="8" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="F244" s="8" t="s">
         <v>23</v>
@@ -4152,7 +4143,7 @@
     <row r="246" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D246" s="9"/>
       <c r="H246" s="18" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
     </row>
     <row r="247" spans="2:9" x14ac:dyDescent="0.3">
@@ -4164,34 +4155,34 @@
     </row>
     <row r="248" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B248" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D248" s="30" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E248" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F248" s="30" t="s">
         <v>23</v>
       </c>
       <c r="G248" s="8"/>
       <c r="H248" s="30" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
     </row>
     <row r="249" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D249" s="9"/>
       <c r="E249" s="8"/>
       <c r="F249" s="8" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G249" s="8"/>
       <c r="H249" s="18" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="250" spans="2:9" x14ac:dyDescent="0.3">
@@ -4233,13 +4224,13 @@
     </row>
     <row r="253" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B253" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C253" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D253" s="9" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E253" t="s">
         <v>15</v>
@@ -4254,7 +4245,7 @@
         <v>20210401</v>
       </c>
       <c r="I253" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="254" spans="2:9" x14ac:dyDescent="0.3">
@@ -4275,7 +4266,7 @@
     <row r="255" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D255" s="9"/>
       <c r="E255" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F255" t="s">
         <v>9</v>
@@ -4290,17 +4281,17 @@
     </row>
     <row r="257" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B257" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C257" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D257" s="9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H257" s="6"/>
       <c r="I257" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="258" spans="2:9" x14ac:dyDescent="0.3">
@@ -4313,17 +4304,17 @@
     </row>
     <row r="260" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B260" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C260" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D260" s="9" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H260" s="6"/>
       <c r="I260" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="261" spans="2:9" x14ac:dyDescent="0.3">
@@ -4336,17 +4327,17 @@
     </row>
     <row r="263" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B263" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C263" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H263" s="6"/>
       <c r="I263" s="7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="264" spans="2:9" x14ac:dyDescent="0.3">
@@ -4359,34 +4350,34 @@
     </row>
     <row r="266" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B266" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C266" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D266" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E266" t="s">
+        <v>102</v>
+      </c>
+      <c r="F266" t="s">
         <v>103</v>
-      </c>
-      <c r="E266" t="s">
-        <v>104</v>
-      </c>
-      <c r="F266" t="s">
-        <v>105</v>
       </c>
       <c r="H266" s="6" t="b">
         <v>0</v>
       </c>
       <c r="I266" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="267" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D267" s="9"/>
       <c r="E267" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F267" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H267" s="6" t="b">
         <v>1</v>
@@ -4398,16 +4389,16 @@
     </row>
     <row r="269" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B269" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C269" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D269" s="9" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E269" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F269" t="s">
         <v>21</v>
@@ -4416,7 +4407,7 @@
         <v>3</v>
       </c>
       <c r="I269" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="270" spans="2:9" x14ac:dyDescent="0.3">
@@ -4424,20 +4415,20 @@
     </row>
     <row r="271" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B271" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C271" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D271" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E271" s="1"/>
       <c r="F271" s="10"/>
       <c r="G271" s="1"/>
       <c r="H271" s="3"/>
       <c r="I271" s="7" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="272" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4452,20 +4443,20 @@
     </row>
     <row r="273" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B273" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C273" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D273" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E273" s="1"/>
       <c r="F273" s="10"/>
       <c r="G273" s="1"/>
       <c r="H273" s="3"/>
       <c r="I273" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="274" spans="1:9" ht="18" x14ac:dyDescent="0.35">
@@ -4480,13 +4471,13 @@
     </row>
     <row r="275" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B275" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C275" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D275" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E275" s="11" t="s">
         <v>22</v>
@@ -4498,7 +4489,7 @@
         <v>20191101</v>
       </c>
       <c r="I275" s="7" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.3">
@@ -4506,13 +4497,13 @@
     </row>
     <row r="277" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B277" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C277" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D277" s="9" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E277" t="s">
         <v>15</v>
@@ -4521,10 +4512,10 @@
         <v>9</v>
       </c>
       <c r="H277" s="33" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="I277" s="24" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
@@ -4536,7 +4527,7 @@
         <v>9</v>
       </c>
       <c r="H278" s="33" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
@@ -4547,13 +4538,13 @@
         <v>36</v>
       </c>
       <c r="B280" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C280" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D280" s="10" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E280" s="1" t="s">
         <v>15</v>
@@ -4568,7 +4559,7 @@
         <v>20200401</v>
       </c>
       <c r="I280" s="24" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="281" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4596,7 +4587,7 @@
       <c r="C282" s="1"/>
       <c r="D282" s="10"/>
       <c r="E282" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F282" s="1" t="s">
         <v>9</v>
@@ -4620,37 +4611,37 @@
     </row>
     <row r="284" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B284" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C284" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D284" s="9" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E284" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F284" t="s">
         <v>9</v>
       </c>
       <c r="H284" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="I284" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D285" s="9"/>
       <c r="E285" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F285" t="s">
         <v>9</v>
       </c>
       <c r="H285" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.3">
@@ -4662,7 +4653,7 @@
         <v>9</v>
       </c>
       <c r="H286" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="287" spans="1:9" x14ac:dyDescent="0.3">
@@ -4674,7 +4665,7 @@
         <v>9</v>
       </c>
       <c r="H287" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
@@ -4682,25 +4673,25 @@
     </row>
     <row r="289" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B289" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C289" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D289" s="9" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E289" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F289" t="s">
         <v>9</v>
       </c>
       <c r="H289" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="I289" s="24" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
     </row>
     <row r="290" spans="2:9" x14ac:dyDescent="0.3">
@@ -4712,7 +4703,7 @@
         <v>9</v>
       </c>
       <c r="H290" s="17" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="291" spans="2:9" x14ac:dyDescent="0.3">
@@ -4724,7 +4715,7 @@
         <v>9</v>
       </c>
       <c r="H291" s="17" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="292" spans="2:9" x14ac:dyDescent="0.3">
@@ -4732,13 +4723,13 @@
     </row>
     <row r="293" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B293" s="1" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C293" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D293" s="9" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="E293" s="1" t="s">
         <v>15</v>
@@ -4771,25 +4762,25 @@
     <row r="295" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D295" s="9"/>
       <c r="E295" t="s">
+        <v>26</v>
+      </c>
+      <c r="F295" t="s">
+        <v>9</v>
+      </c>
+      <c r="H295" t="s">
         <v>27</v>
-      </c>
-      <c r="F295" t="s">
-        <v>9</v>
-      </c>
-      <c r="H295" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="296" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D296" s="9"/>
       <c r="E296" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F296" t="s">
         <v>9</v>
       </c>
       <c r="H296" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
     </row>
     <row r="297" spans="2:9" x14ac:dyDescent="0.3">
@@ -4797,13 +4788,13 @@
     </row>
     <row r="298" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B298" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C298" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D298" s="9" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E298" t="s">
         <v>15</v>
@@ -4818,7 +4809,7 @@
         <v>20200401</v>
       </c>
       <c r="I298" s="24" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="299" spans="2:9" x14ac:dyDescent="0.3">
@@ -4843,13 +4834,13 @@
     </row>
     <row r="301" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B301" t="s">
+        <v>112</v>
+      </c>
+      <c r="C301" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D301" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="C301" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="D301" s="9" t="s">
-        <v>116</v>
       </c>
       <c r="E301" t="s">
         <v>15</v>
@@ -4864,7 +4855,7 @@
         <v>20200401</v>
       </c>
       <c r="I301" s="24" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
     </row>
     <row r="302" spans="2:9" x14ac:dyDescent="0.3">
@@ -4885,49 +4876,49 @@
     <row r="303" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D303" s="9"/>
       <c r="E303" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F303" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H303" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="304" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D304" s="9"/>
       <c r="E304" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F304" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H304" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="305" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D305" s="9"/>
       <c r="E305" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F305" s="9" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H305" s="8" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="306" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D306" s="9"/>
       <c r="E306" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="F306" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H306" s="8" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
@@ -4936,13 +4927,13 @@
     </row>
     <row r="308" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B308" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C308" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D308" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E308" t="s">
         <v>15</v>
@@ -4957,7 +4948,7 @@
         <v>20200401</v>
       </c>
       <c r="I308" s="24" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="309" spans="2:9" x14ac:dyDescent="0.3">
@@ -4978,31 +4969,31 @@
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D310" s="9"/>
       <c r="E310" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F310" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H310" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="311" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D311" s="9"/>
       <c r="E311" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F311" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H311" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="312" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D312" s="9"/>
       <c r="E312" t="s">
-        <v>127</v>
+        <v>336</v>
       </c>
       <c r="F312" s="9" t="s">
         <v>23</v>
@@ -5017,13 +5008,13 @@
     </row>
     <row r="314" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B314" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C314" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D314" s="9" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E314" t="s">
         <v>15</v>
@@ -5038,7 +5029,7 @@
         <v>20200401</v>
       </c>
       <c r="I314" s="24" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
     </row>
     <row r="315" spans="2:9" x14ac:dyDescent="0.3">
@@ -5062,13 +5053,13 @@
     </row>
     <row r="317" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B317" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C317" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D317" s="9" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E317" t="s">
         <v>15</v>
@@ -5083,7 +5074,7 @@
         <v>20200401</v>
       </c>
       <c r="I317" s="24" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="318" spans="2:9" x14ac:dyDescent="0.3">
@@ -5104,7 +5095,7 @@
     <row r="319" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D319" s="9"/>
       <c r="E319" t="s">
-        <v>130</v>
+        <v>336</v>
       </c>
       <c r="F319" s="9" t="s">
         <v>23</v>
@@ -5119,13 +5110,13 @@
     </row>
     <row r="321" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B321" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C321" s="1" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="D321" s="9" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="E321" t="s">
         <v>22</v>
@@ -5140,52 +5131,52 @@
         <v>20220228</v>
       </c>
       <c r="I321" s="24" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="322" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D322" s="9"/>
       <c r="E322" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F322" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H322" s="8" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
     </row>
     <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D323" s="9"/>
       <c r="E323" t="s">
+        <v>337</v>
+      </c>
+      <c r="F323" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H323" s="8" t="s">
         <v>24</v>
-      </c>
-      <c r="F323" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H323" s="8" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="324" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D324" s="9"/>
       <c r="E324" t="s">
-        <v>35</v>
+        <v>111</v>
       </c>
       <c r="F324" s="9" t="s">
         <v>23</v>
       </c>
       <c r="H324" s="8" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="325" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D325" s="9"/>
       <c r="E325" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F325" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H325" s="8">
         <v>4</v>
@@ -5194,10 +5185,10 @@
     <row r="326" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D326" s="9"/>
       <c r="E326" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F326" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H326" s="8">
         <v>48</v>
@@ -5206,10 +5197,10 @@
     <row r="327" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D327" s="9"/>
       <c r="E327" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F327" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H327" s="8">
         <v>1.1000000000000001</v>
@@ -5218,10 +5209,10 @@
     <row r="328" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D328" s="9"/>
       <c r="E328" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F328" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H328" s="8">
         <v>3.2</v>
@@ -5230,10 +5221,10 @@
     <row r="329" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D329" s="9"/>
       <c r="E329" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F329" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H329" s="8">
         <v>0.11</v>
@@ -5242,10 +5233,10 @@
     <row r="330" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D330" s="9"/>
       <c r="E330" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F330" s="9" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H330" s="8">
         <v>0.2</v>
@@ -5254,7 +5245,7 @@
     <row r="331" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D331" s="9"/>
       <c r="E331" t="s">
-        <v>130</v>
+        <v>336</v>
       </c>
       <c r="F331" s="9" t="s">
         <v>23</v>
@@ -5268,20 +5259,20 @@
     </row>
     <row r="333" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B333" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D333" s="9" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="E333" s="1"/>
       <c r="F333" s="1"/>
       <c r="G333" s="1"/>
       <c r="H333" s="3"/>
       <c r="I333" s="13" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="334" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5296,26 +5287,26 @@
     </row>
     <row r="335" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B335" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C335" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D335" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C335" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="D335" s="10" t="s">
-        <v>66</v>
-      </c>
       <c r="E335" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F335" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G335" s="1"/>
       <c r="H335" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I335" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="336" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5330,22 +5321,22 @@
     </row>
     <row r="337" spans="2:9" ht="29.4" x14ac:dyDescent="0.35">
       <c r="B337" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C337" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D337" s="10" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="E337" s="1"/>
       <c r="F337" s="1"/>
       <c r="G337" s="1"/>
       <c r="H337" s="12" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="I337" s="7" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="338" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5360,16 +5351,16 @@
     </row>
     <row r="339" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B339" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C339" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D339" s="10" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E339" s="1" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F339" s="10" t="s">
         <v>23</v>
@@ -5379,7 +5370,7 @@
         <v>531733</v>
       </c>
       <c r="I339" s="7" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="340" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5387,7 +5378,7 @@
       <c r="C340" s="1"/>
       <c r="D340" s="10"/>
       <c r="E340" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="F340" s="1" t="s">
         <v>23</v>
@@ -5410,26 +5401,26 @@
     </row>
     <row r="342" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B342" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C342" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D342" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E342" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F342" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G342" s="1"/>
       <c r="H342" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="I342" s="7" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="343" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5444,16 +5435,16 @@
     </row>
     <row r="344" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B344" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C344" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D344" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E344" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F344" s="1" t="s">
         <v>9</v>
@@ -5463,7 +5454,7 @@
         <v>14</v>
       </c>
       <c r="I344" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="345" spans="2:9" x14ac:dyDescent="0.3">
@@ -5471,14 +5462,14 @@
       <c r="C345" s="1"/>
       <c r="D345" s="10"/>
       <c r="E345" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F345" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G345" s="1"/>
       <c r="H345" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I345" s="1"/>
     </row>
@@ -5526,36 +5517,36 @@
     </row>
     <row r="350" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B350" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C350" s="1" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D350" s="9" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="E350" s="8" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F350" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G350" s="8"/>
       <c r="H350" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="351" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D351" s="9"/>
       <c r="E351" s="8" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="F351" s="8" t="s">
         <v>23</v>
       </c>
       <c r="G351" s="8"/>
       <c r="H351" s="18" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
     </row>
     <row r="352" spans="2:9" x14ac:dyDescent="0.3">
@@ -5563,16 +5554,16 @@
     </row>
     <row r="353" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B353" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C353" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D353" s="9" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E353" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F353" s="1" t="s">
         <v>9</v>
@@ -5581,13 +5572,13 @@
         <v>532648</v>
       </c>
       <c r="I353" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="354" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D354" s="9"/>
       <c r="E354" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F354" s="1" t="s">
         <v>9</v>
@@ -5603,16 +5594,16 @@
     </row>
     <row r="356" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B356" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C356" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D356" s="9" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E356" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F356" s="1" t="s">
         <v>9</v>
@@ -5624,7 +5615,7 @@
     <row r="357" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D357" s="9"/>
       <c r="E357" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F357" s="1" t="s">
         <v>9</v>
@@ -5638,26 +5629,26 @@
     </row>
     <row r="359" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B359" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C359" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D359" s="10" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="E359" s="11" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F359" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G359" s="1"/>
       <c r="H359" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I359" s="24" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="360" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5672,13 +5663,13 @@
     </row>
     <row r="361" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B361" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C361" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D361" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E361" s="11"/>
       <c r="F361" s="10"/>
@@ -5697,26 +5688,26 @@
     </row>
     <row r="363" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B363" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C363" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D363" s="10" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="E363" s="11" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="F363" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G363" s="1"/>
       <c r="H363" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I363" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="364" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5724,7 +5715,7 @@
       <c r="C364" s="1"/>
       <c r="D364" s="10"/>
       <c r="E364" s="11" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="F364" s="10" t="s">
         <v>9</v>
@@ -5740,7 +5731,7 @@
       <c r="C365" s="1"/>
       <c r="D365" s="10"/>
       <c r="E365" s="11" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="F365" s="10" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Change column order of CapitalGainLoss_Dividend Api output
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -1466,8 +1466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C262" workbookViewId="0">
-      <selection activeCell="D275" sqref="D275"/>
+    <sheetView tabSelected="1" topLeftCell="C314" workbookViewId="0">
+      <selection activeCell="E331" sqref="E331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5054,124 +5054,142 @@
         <v>313</v>
       </c>
     </row>
-    <row r="320" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="320" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C320" s="1"/>
       <c r="D320" s="9"/>
       <c r="E320" t="s">
-        <v>34</v>
+        <v>316</v>
       </c>
       <c r="F320" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H320" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="321" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H320" s="8">
+        <v>500820</v>
+      </c>
+      <c r="I320" s="24"/>
+    </row>
+    <row r="321" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C321" s="1"/>
       <c r="D321" s="9"/>
       <c r="E321" t="s">
-        <v>317</v>
+        <v>56</v>
       </c>
       <c r="F321" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H321" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="322" spans="2:9" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="H321" s="8">
+        <v>48</v>
+      </c>
+      <c r="I321" s="24"/>
+    </row>
+    <row r="322" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C322" s="1"/>
       <c r="D322" s="9"/>
       <c r="E322" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="F322" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H322" s="8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="323" spans="2:9" x14ac:dyDescent="0.3">
+        <v>114</v>
+      </c>
+      <c r="H322" s="8">
+        <v>4</v>
+      </c>
+      <c r="I322" s="24"/>
+    </row>
+    <row r="323" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C323" s="1"/>
       <c r="D323" s="9"/>
       <c r="E323" t="s">
-        <v>56</v>
+        <v>116</v>
       </c>
       <c r="F323" s="9" t="s">
         <v>114</v>
       </c>
       <c r="H323" s="8">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="324" spans="2:9" x14ac:dyDescent="0.3">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I323" s="24"/>
+    </row>
+    <row r="324" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C324" s="1"/>
       <c r="D324" s="9"/>
       <c r="E324" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F324" s="9" t="s">
         <v>114</v>
       </c>
       <c r="H324" s="8">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="325" spans="2:9" x14ac:dyDescent="0.3">
+        <v>3.2</v>
+      </c>
+      <c r="I324" s="24"/>
+    </row>
+    <row r="325" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C325" s="1"/>
       <c r="D325" s="9"/>
       <c r="E325" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F325" s="9" t="s">
         <v>114</v>
       </c>
       <c r="H325" s="8">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="326" spans="2:9" x14ac:dyDescent="0.3">
+        <v>0.11</v>
+      </c>
+      <c r="I325" s="24"/>
+    </row>
+    <row r="326" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C326" s="1"/>
       <c r="D326" s="9"/>
       <c r="E326" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="F326" s="9" t="s">
         <v>114</v>
       </c>
       <c r="H326" s="8">
-        <v>3.2</v>
-      </c>
-    </row>
-    <row r="327" spans="2:9" x14ac:dyDescent="0.3">
+        <v>0.2</v>
+      </c>
+      <c r="I326" s="24"/>
+    </row>
+    <row r="327" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C327" s="1"/>
       <c r="D327" s="9"/>
       <c r="E327" t="s">
-        <v>118</v>
+        <v>34</v>
       </c>
       <c r="F327" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="H327" s="8">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="328" spans="2:9" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="H327" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="I327" s="24"/>
+    </row>
+    <row r="328" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C328" s="1"/>
       <c r="D328" s="9"/>
       <c r="E328" t="s">
-        <v>119</v>
+        <v>317</v>
       </c>
       <c r="F328" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="H328" s="8">
-        <v>0.2</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H328" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I328" s="24"/>
     </row>
     <row r="329" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D329" s="9"/>
       <c r="E329" t="s">
-        <v>316</v>
+        <v>96</v>
       </c>
       <c r="F329" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H329" s="8">
-        <v>500820</v>
+      <c r="H329" s="8" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="330" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Change output model of capital gain loss
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="318">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -334,9 +334,6 @@
   </si>
   <si>
     <t>CapitalGainLoss_ActualPLDetail</t>
-  </si>
-  <si>
-    <t>reportFor</t>
   </si>
   <si>
     <t>TX</t>
@@ -1466,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C314" workbookViewId="0">
-      <selection activeCell="E331" sqref="E331"/>
+    <sheetView tabSelected="1" topLeftCell="C295" workbookViewId="0">
+      <selection activeCell="E308" sqref="E308"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1498,13 +1495,13 @@
     </row>
     <row r="2" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>2</v>
@@ -1533,10 +1530,10 @@
         <v>94</v>
       </c>
       <c r="D4" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="I4" s="7" t="s">
         <v>121</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1550,7 +1547,7 @@
         <v>94</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E6" t="s">
         <v>12</v>
@@ -1573,7 +1570,7 @@
         <v>94</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E8" t="s">
         <v>12</v>
@@ -1585,7 +1582,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -1611,7 +1608,7 @@
         <v>94</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E11" t="s">
         <v>12</v>
@@ -1634,7 +1631,7 @@
         <v>94</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>
@@ -1649,13 +1646,13 @@
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D14" s="9"/>
       <c r="E14" t="s">
+        <v>204</v>
+      </c>
+      <c r="F14" t="s">
+        <v>22</v>
+      </c>
+      <c r="H14" t="s">
         <v>205</v>
-      </c>
-      <c r="F14" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1669,7 +1666,7 @@
         <v>94</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E16" t="s">
         <v>12</v>
@@ -1684,7 +1681,7 @@
     <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D17" s="9"/>
       <c r="E17" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="F17" t="s">
         <v>22</v>
@@ -1693,7 +1690,7 @@
     <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D18" s="9"/>
       <c r="E18" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
@@ -1702,7 +1699,7 @@
     <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D19" s="9"/>
       <c r="E19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="F19" t="s">
         <v>22</v>
@@ -1719,10 +1716,10 @@
         <v>94</v>
       </c>
       <c r="D21" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>202</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
@@ -1745,37 +1742,37 @@
         <v>9</v>
       </c>
       <c r="H23" t="s">
+        <v>122</v>
+      </c>
+      <c r="I23" t="s">
         <v>123</v>
-      </c>
-      <c r="I23" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D24" s="9"/>
       <c r="H24" t="s">
+        <v>124</v>
+      </c>
+      <c r="I24" t="s">
         <v>125</v>
-      </c>
-      <c r="I24" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D25" s="9"/>
       <c r="H25" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" t="s">
         <v>127</v>
-      </c>
-      <c r="I25" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D26" s="9"/>
       <c r="H26" t="s">
+        <v>128</v>
+      </c>
+      <c r="I26" t="s">
         <v>129</v>
-      </c>
-      <c r="I26" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.3">
@@ -1787,10 +1784,10 @@
         <v>9</v>
       </c>
       <c r="H27" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I27" s="18" t="s">
         <v>131</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.3">
@@ -1802,10 +1799,10 @@
         <v>9</v>
       </c>
       <c r="H28" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="I28" s="19" t="s">
         <v>133</v>
-      </c>
-      <c r="I28" s="19" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.3">
@@ -1819,7 +1816,7 @@
         <v>94</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E30" t="s">
         <v>14</v>
@@ -1831,10 +1828,10 @@
         <v>15</v>
       </c>
       <c r="H30" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
@@ -1849,7 +1846,7 @@
         <v>15</v>
       </c>
       <c r="H31" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.3">
@@ -1866,42 +1863,42 @@
       </c>
       <c r="G33" s="20"/>
       <c r="H33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D34" s="9"/>
       <c r="G34" s="20"/>
       <c r="H34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D35" s="9"/>
       <c r="G35" s="20"/>
       <c r="H35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D36" s="9"/>
       <c r="G36" s="20"/>
       <c r="H36" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D37" s="9"/>
       <c r="G37" s="20"/>
       <c r="H37" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="38" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D38" s="9"/>
       <c r="G38" s="20"/>
       <c r="H38" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="2:9" x14ac:dyDescent="0.3">
@@ -1911,25 +1908,25 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D40" s="9"/>
       <c r="E40" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
       </c>
       <c r="H40" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D41" s="9"/>
       <c r="H41" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D42" s="9"/>
       <c r="H42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.3">
@@ -1943,55 +1940,55 @@
         <v>94</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E44" t="s">
+        <v>143</v>
+      </c>
+      <c r="F44" t="s">
+        <v>9</v>
+      </c>
+      <c r="H44" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="F44" t="s">
-        <v>9</v>
-      </c>
-      <c r="H44" s="17" t="s">
-        <v>145</v>
-      </c>
       <c r="I44" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D45" s="9"/>
       <c r="I45" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D46" s="9"/>
       <c r="I46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D47" s="9"/>
       <c r="I47" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D48" s="9"/>
       <c r="I48" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="49" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D49" s="9"/>
       <c r="I49" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D50" s="9"/>
       <c r="I50" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="51" spans="2:9" x14ac:dyDescent="0.3">
@@ -2005,19 +2002,19 @@
         <v>94</v>
       </c>
       <c r="D52" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="E52" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="E52" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="F52" s="9" t="s">
         <v>9</v>
       </c>
       <c r="H52" t="s">
+        <v>230</v>
+      </c>
+      <c r="I52" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="I52" s="7" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="53" spans="2:9" x14ac:dyDescent="0.3">
@@ -2045,46 +2042,46 @@
         <v>35</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I55" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D56" s="9"/>
       <c r="I56" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D57" s="9"/>
       <c r="I57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D58" s="9"/>
       <c r="I58" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D59" s="9"/>
       <c r="I59" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D60" s="9"/>
       <c r="I60" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D61" s="9"/>
       <c r="I61" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="62" spans="2:9" x14ac:dyDescent="0.3">
@@ -2098,55 +2095,55 @@
         <v>35</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E63" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F63" t="s">
         <v>9</v>
       </c>
       <c r="H63" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="64" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D64" s="9"/>
       <c r="I64" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D65" s="9"/>
       <c r="I65" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="66" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D66" s="9"/>
       <c r="I66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D67" s="9"/>
       <c r="I67" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D68" s="9"/>
       <c r="I68" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="69" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D69" s="9"/>
       <c r="I69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="70" spans="2:9" x14ac:dyDescent="0.3">
@@ -2160,10 +2157,10 @@
         <v>35</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I71" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="72" spans="2:9" x14ac:dyDescent="0.3">
@@ -2177,10 +2174,10 @@
         <v>35</v>
       </c>
       <c r="D73" s="9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E73" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F73" t="s">
         <v>22</v>
@@ -2189,7 +2186,7 @@
         <v>1202870000086520</v>
       </c>
       <c r="I73" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="74" spans="2:9" x14ac:dyDescent="0.3">
@@ -2203,10 +2200,10 @@
         <v>35</v>
       </c>
       <c r="D75" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="E75" t="s">
         <v>213</v>
-      </c>
-      <c r="E75" t="s">
-        <v>214</v>
       </c>
       <c r="F75" t="s">
         <v>22</v>
@@ -2215,7 +2212,7 @@
     <row r="76" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D76" s="9"/>
       <c r="E76" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F76" t="s">
         <v>22</v>
@@ -2232,10 +2229,10 @@
         <v>35</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I78" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="79" spans="2:9" x14ac:dyDescent="0.3">
@@ -2249,13 +2246,13 @@
         <v>24</v>
       </c>
       <c r="C81" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D81" s="9" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="I81" s="24" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="82" spans="2:9" x14ac:dyDescent="0.3">
@@ -2266,10 +2263,10 @@
         <v>24</v>
       </c>
       <c r="C83" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D83" s="9" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E83" t="s">
         <v>25</v>
@@ -2281,7 +2278,7 @@
         <v>26</v>
       </c>
       <c r="I83" s="24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="84" spans="2:9" x14ac:dyDescent="0.3">
@@ -2292,7 +2289,7 @@
         <v>24</v>
       </c>
       <c r="C85" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D85" s="10" t="s">
         <v>27</v>
@@ -2331,10 +2328,10 @@
         <v>24</v>
       </c>
       <c r="C88" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D88" s="9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E88" t="s">
         <v>34</v>
@@ -2343,10 +2340,10 @@
         <v>9</v>
       </c>
       <c r="H88" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I88" s="24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
@@ -2358,22 +2355,22 @@
         <v>24</v>
       </c>
       <c r="C90" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D90" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E90" t="s">
         <v>220</v>
       </c>
-      <c r="E90" t="s">
-        <v>221</v>
-      </c>
       <c r="F90" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="I90" s="24" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
@@ -2397,13 +2394,13 @@
         <v>24</v>
       </c>
       <c r="C93" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E93" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>9</v>
@@ -2413,7 +2410,7 @@
     <row r="94" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D94" s="9"/>
       <c r="E94" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>9</v>
@@ -2441,13 +2438,13 @@
         <v>24</v>
       </c>
       <c r="C97" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E97" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>9</v>
@@ -2473,7 +2470,7 @@
         <v>19</v>
       </c>
       <c r="C100" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D100" s="9" t="s">
         <v>19</v>
@@ -2485,10 +2482,10 @@
         <v>9</v>
       </c>
       <c r="H100" s="28" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="I100" s="29" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
@@ -2500,7 +2497,7 @@
         <v>9</v>
       </c>
       <c r="H101" s="14" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.3">
@@ -2511,13 +2508,13 @@
         <v>19</v>
       </c>
       <c r="C103" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E103" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F103" s="1" t="s">
         <v>9</v>
@@ -2527,7 +2524,7 @@
     <row r="104" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D104" s="9"/>
       <c r="E104" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F104" s="1" t="s">
         <v>9</v>
@@ -2547,7 +2544,7 @@
     <row r="106" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D106" s="9"/>
       <c r="E106" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F106" s="1" t="s">
         <v>9</v>
@@ -2557,7 +2554,7 @@
     <row r="107" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D107" s="9"/>
       <c r="E107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F107" s="1" t="s">
         <v>9</v>
@@ -2567,7 +2564,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>9</v>
@@ -2582,10 +2579,10 @@
         <v>32</v>
       </c>
       <c r="C110" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D110" s="9" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E110" s="11" t="s">
         <v>96</v>
@@ -2594,19 +2591,19 @@
         <v>9</v>
       </c>
       <c r="H110" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I110" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D111" s="9"/>
       <c r="H111" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I111" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="112" spans="2:9" x14ac:dyDescent="0.3">
@@ -2618,10 +2615,10 @@
         <v>9</v>
       </c>
       <c r="H112" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I112" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="113" spans="2:9" x14ac:dyDescent="0.3">
@@ -2633,28 +2630,28 @@
         <v>9</v>
       </c>
       <c r="H113" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I113" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="114" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D114" s="9"/>
       <c r="I114" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="115" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D115" s="9"/>
       <c r="I115" s="19" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D116" s="9"/>
       <c r="I116" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
@@ -2665,10 +2662,10 @@
         <v>32</v>
       </c>
       <c r="C118" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E118" s="11" t="s">
         <v>96</v>
@@ -2677,37 +2674,37 @@
         <v>9</v>
       </c>
       <c r="H118" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="I118" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="119" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D119" s="9"/>
       <c r="H119" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="I119" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="120" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D120" s="9"/>
       <c r="H120" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I120" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="121" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D121" s="9"/>
       <c r="H121" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="I121" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="122" spans="2:9" x14ac:dyDescent="0.3">
@@ -2719,10 +2716,10 @@
         <v>9</v>
       </c>
       <c r="H122" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I122" s="19" t="s">
         <v>131</v>
-      </c>
-      <c r="I122" s="19" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
@@ -2734,16 +2731,16 @@
         <v>9</v>
       </c>
       <c r="H123" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I123" s="19" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="124" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D124" s="9"/>
       <c r="I124" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="125" spans="2:9" x14ac:dyDescent="0.3">
@@ -2754,10 +2751,10 @@
         <v>32</v>
       </c>
       <c r="C126" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D126" s="9" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E126" s="11" t="s">
         <v>40</v>
@@ -2766,37 +2763,37 @@
         <v>9</v>
       </c>
       <c r="H126" t="s">
+        <v>179</v>
+      </c>
+      <c r="I126" s="23" t="s">
         <v>180</v>
-      </c>
-      <c r="I126" s="23" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="127" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D127" s="9"/>
       <c r="H127" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I127" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="128" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D128" s="9"/>
       <c r="H128" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I128" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="129" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D129" s="9"/>
       <c r="H129" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I129" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="2:9" x14ac:dyDescent="0.3">
@@ -2808,10 +2805,10 @@
         <v>9</v>
       </c>
       <c r="H130" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I130" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="131" spans="2:9" x14ac:dyDescent="0.3">
@@ -2823,22 +2820,22 @@
         <v>9</v>
       </c>
       <c r="H131" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I131" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D132" s="9"/>
       <c r="I132" s="19" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="133" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D133" s="9"/>
       <c r="I133" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="134" spans="2:9" x14ac:dyDescent="0.3">
@@ -2847,49 +2844,49 @@
     <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D135" s="9"/>
       <c r="I135" s="23" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="136" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D136" s="9"/>
       <c r="I136" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D137" s="9"/>
       <c r="I137" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="138" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D138" s="9"/>
       <c r="I138" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="139" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D139" s="9"/>
       <c r="I139" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D140" s="9"/>
       <c r="I140" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="141" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D141" s="9"/>
       <c r="I141" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
       <c r="I142" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.3">
@@ -2898,16 +2895,16 @@
     </row>
     <row r="144" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C144" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D144" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I144" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="I144" s="7" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
@@ -2918,7 +2915,7 @@
         <v>41</v>
       </c>
       <c r="C146" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D146" s="9" t="s">
         <v>42</v>
@@ -2947,22 +2944,22 @@
         <v>41</v>
       </c>
       <c r="C149" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D149" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E149" t="s">
         <v>162</v>
       </c>
-      <c r="E149" t="s">
-        <v>163</v>
-      </c>
       <c r="F149" t="s">
         <v>22</v>
       </c>
       <c r="H149" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I149" s="21" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="150" spans="2:9" x14ac:dyDescent="0.3">
@@ -2983,13 +2980,13 @@
     <row r="151" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D151" s="9"/>
       <c r="E151" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F151" t="s">
         <v>22</v>
       </c>
       <c r="H151" s="17" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.3">
@@ -3000,7 +2997,7 @@
         <v>41</v>
       </c>
       <c r="C153" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D153" s="10" t="s">
         <v>47</v>
@@ -3082,10 +3079,10 @@
         <v>41</v>
       </c>
       <c r="C159" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D159" s="9" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E159" s="10" t="s">
         <v>43</v>
@@ -3098,7 +3095,7 @@
         <v>44</v>
       </c>
       <c r="I159" s="24" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="160" spans="2:9" x14ac:dyDescent="0.3">
@@ -3149,13 +3146,13 @@
         <v>41</v>
       </c>
       <c r="C164" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D164" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="E164" s="10" t="s">
         <v>285</v>
-      </c>
-      <c r="E164" s="10" t="s">
-        <v>286</v>
       </c>
       <c r="F164" s="10" t="s">
         <v>22</v>
@@ -3164,7 +3161,7 @@
         <v>44</v>
       </c>
       <c r="I164" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="165" spans="2:9" x14ac:dyDescent="0.3">
@@ -3202,22 +3199,22 @@
         <v>41</v>
       </c>
       <c r="C168" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D168" s="9" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E168" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F168" t="s">
         <v>22</v>
       </c>
       <c r="H168" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="I168" s="24" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="169" spans="2:9" x14ac:dyDescent="0.3">
@@ -3238,13 +3235,13 @@
     <row r="170" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D170" s="9"/>
       <c r="E170" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F170" t="s">
         <v>22</v>
       </c>
       <c r="H170" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.3">
@@ -3258,7 +3255,7 @@
         <v>41</v>
       </c>
       <c r="C172" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D172" s="10" t="s">
         <v>51</v>
@@ -3282,7 +3279,7 @@
         <v>59</v>
       </c>
       <c r="C175" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D175" s="10" t="s">
         <v>60</v>
@@ -3303,7 +3300,7 @@
         <v>59</v>
       </c>
       <c r="C177" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D177" s="10" t="s">
         <v>62</v>
@@ -3346,7 +3343,7 @@
         <v>59</v>
       </c>
       <c r="C180" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D180" s="10" t="s">
         <v>68</v>
@@ -3441,7 +3438,7 @@
         <v>59</v>
       </c>
       <c r="C186" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D186" s="10" t="s">
         <v>71</v>
@@ -3521,13 +3518,13 @@
         <v>59</v>
       </c>
       <c r="C191" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D191" s="10" t="s">
+        <v>243</v>
+      </c>
+      <c r="I191" s="24" t="s">
         <v>244</v>
-      </c>
-      <c r="I191" s="24" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="192" spans="2:9" x14ac:dyDescent="0.3">
@@ -3538,22 +3535,22 @@
         <v>59</v>
       </c>
       <c r="C193" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D193" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E193" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="E193" s="11" t="s">
+      <c r="F193" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H193" t="s">
         <v>247</v>
       </c>
-      <c r="F193" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H193" t="s">
+      <c r="I193" s="24" t="s">
         <v>248</v>
-      </c>
-      <c r="I193" s="24" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="194" spans="2:9" x14ac:dyDescent="0.3">
@@ -3576,22 +3573,22 @@
         <v>59</v>
       </c>
       <c r="C196" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D196" s="10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E196" s="11" t="s">
+        <v>246</v>
+      </c>
+      <c r="F196" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H196" t="s">
         <v>247</v>
       </c>
-      <c r="F196" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H196" t="s">
+      <c r="I196" s="24" t="s">
         <v>248</v>
-      </c>
-      <c r="I196" s="24" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="197" spans="2:9" x14ac:dyDescent="0.3">
@@ -3600,7 +3597,7 @@
     <row r="198" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D198" s="9"/>
       <c r="H198" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I198" s="24"/>
     </row>
@@ -3609,34 +3606,34 @@
         <v>59</v>
       </c>
       <c r="C199" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D199" s="10" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E199" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F199" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H199" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I199" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D200" s="9"/>
       <c r="H200" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="201" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D201" s="9"/>
       <c r="H201" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="202" spans="2:9" x14ac:dyDescent="0.3">
@@ -3647,34 +3644,34 @@
         <v>59</v>
       </c>
       <c r="C203" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D203" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H203" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E204" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H204" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H205" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="H206" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="208" spans="2:9" x14ac:dyDescent="0.3">
@@ -3682,34 +3679,34 @@
         <v>59</v>
       </c>
       <c r="C208" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D208" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H208" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="209" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E209" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H209" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="210" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H210" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="211" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H211" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="213" spans="2:8" x14ac:dyDescent="0.3">
@@ -3717,37 +3714,37 @@
         <v>59</v>
       </c>
       <c r="C213" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D213" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H213" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="214" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D214" s="9"/>
       <c r="E214" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F214" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H214" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="215" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D215" s="9"/>
       <c r="H215" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="216" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D216" s="9"/>
       <c r="H216" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="217" spans="2:8" x14ac:dyDescent="0.3">
@@ -3758,20 +3755,20 @@
         <v>59</v>
       </c>
       <c r="C218" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D218" s="30" t="s">
+        <v>259</v>
+      </c>
+      <c r="E218" s="8" t="s">
         <v>260</v>
-      </c>
-      <c r="E218" s="8" t="s">
-        <v>261</v>
       </c>
       <c r="F218" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G218" s="8"/>
       <c r="H218" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="219" spans="2:8" x14ac:dyDescent="0.3">
@@ -3813,7 +3810,7 @@
       <c r="C221" s="8"/>
       <c r="D221" s="30"/>
       <c r="E221" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F221" s="8" t="s">
         <v>22</v>
@@ -3834,7 +3831,7 @@
     <row r="223" spans="2:8" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D223" s="9"/>
       <c r="H223" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="224" spans="2:8" x14ac:dyDescent="0.3">
@@ -3848,10 +3845,10 @@
         <v>59</v>
       </c>
       <c r="C226" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D226" s="30" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E226" s="31" t="s">
         <v>30</v>
@@ -3861,7 +3858,7 @@
       </c>
       <c r="G226" s="8"/>
       <c r="H226" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="227" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -3872,7 +3869,7 @@
       </c>
       <c r="G227" s="8"/>
       <c r="H227" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="228" spans="2:9" x14ac:dyDescent="0.3">
@@ -3917,40 +3914,40 @@
         <v>59</v>
       </c>
       <c r="C231" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D231" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="H231" t="s">
+        <v>251</v>
+      </c>
+      <c r="I231" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="H231" t="s">
-        <v>252</v>
-      </c>
-      <c r="I231" s="7" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="232" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D232" s="9"/>
       <c r="E232" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F232" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H232" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="233" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D233" s="9"/>
       <c r="H233" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="234" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D234" s="9"/>
       <c r="H234" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="235" spans="2:9" x14ac:dyDescent="0.3">
@@ -3965,40 +3962,40 @@
         <v>59</v>
       </c>
       <c r="C236" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D236" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="H236" t="s">
+        <v>251</v>
+      </c>
+      <c r="I236" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="H236" t="s">
-        <v>252</v>
-      </c>
-      <c r="I236" s="7" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D237" s="9"/>
       <c r="E237" s="11" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F237" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H237" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="238" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D238" s="9"/>
       <c r="H238" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="239" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D239" s="9"/>
       <c r="H239" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="240" spans="2:9" x14ac:dyDescent="0.3">
@@ -4013,23 +4010,23 @@
         <v>59</v>
       </c>
       <c r="C241" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D241" s="32" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E241" s="8" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F241" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G241" s="8"/>
       <c r="H241" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I241" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="242" spans="2:9" x14ac:dyDescent="0.3">
@@ -4065,7 +4062,7 @@
     <row r="244" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D244" s="9"/>
       <c r="E244" s="8" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F244" s="8" t="s">
         <v>22</v>
@@ -4084,7 +4081,7 @@
     <row r="246" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D246" s="9"/>
       <c r="H246" s="18" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="247" spans="2:9" x14ac:dyDescent="0.3">
@@ -4099,10 +4096,10 @@
         <v>59</v>
       </c>
       <c r="C248" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D248" s="30" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E248" s="31" t="s">
         <v>30</v>
@@ -4112,7 +4109,7 @@
       </c>
       <c r="G248" s="8"/>
       <c r="H248" s="30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="249" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -4123,7 +4120,7 @@
       </c>
       <c r="G249" s="8"/>
       <c r="H249" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="250" spans="2:9" x14ac:dyDescent="0.3">
@@ -4168,7 +4165,7 @@
         <v>76</v>
       </c>
       <c r="C253" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D253" s="9" t="s">
         <v>77</v>
@@ -4225,7 +4222,7 @@
         <v>76</v>
       </c>
       <c r="C257" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D257" s="9" t="s">
         <v>80</v>
@@ -4248,7 +4245,7 @@
         <v>76</v>
       </c>
       <c r="C260" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D260" s="9" t="s">
         <v>82</v>
@@ -4271,7 +4268,7 @@
         <v>76</v>
       </c>
       <c r="C263" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D263" s="9" t="s">
         <v>84</v>
@@ -4294,7 +4291,7 @@
         <v>76</v>
       </c>
       <c r="C266" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D266" s="9" t="s">
         <v>86</v>
@@ -4333,7 +4330,7 @@
         <v>76</v>
       </c>
       <c r="C269" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D269" s="9" t="s">
         <v>91</v>
@@ -4366,7 +4363,7 @@
         <v>53</v>
       </c>
       <c r="C271" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D271" s="10" t="s">
         <v>54</v>
@@ -4394,7 +4391,7 @@
         <v>53</v>
       </c>
       <c r="C273" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D273" s="9" t="s">
         <v>53</v>
@@ -4409,7 +4406,7 @@
         <v>20191101</v>
       </c>
       <c r="I273" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.3">
@@ -4417,13 +4414,13 @@
     </row>
     <row r="275" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B275" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C275" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D275" s="9" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E275" t="s">
         <v>14</v>
@@ -4432,10 +4429,10 @@
         <v>9</v>
       </c>
       <c r="H275" s="33" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I275" s="24" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.3">
@@ -4447,7 +4444,7 @@
         <v>9</v>
       </c>
       <c r="H276" s="33" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.3">
@@ -4458,13 +4455,13 @@
         <v>36</v>
       </c>
       <c r="B278" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C278" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D278" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E278" s="1" t="s">
         <v>14</v>
@@ -4479,7 +4476,7 @@
         <v>20200401</v>
       </c>
       <c r="I278" s="24" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="279" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4507,7 +4504,7 @@
       <c r="C280" s="1"/>
       <c r="D280" s="10"/>
       <c r="E280" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F280" s="1" t="s">
         <v>9</v>
@@ -4531,13 +4528,13 @@
     </row>
     <row r="282" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B282" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="C282" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D282" s="9" t="s">
         <v>194</v>
-      </c>
-      <c r="C282" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D282" s="9" t="s">
-        <v>195</v>
       </c>
       <c r="E282" t="s">
         <v>25</v>
@@ -4546,10 +4543,10 @@
         <v>9</v>
       </c>
       <c r="H282" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="I282" s="24" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
@@ -4561,7 +4558,7 @@
         <v>9</v>
       </c>
       <c r="H283" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
@@ -4573,7 +4570,7 @@
         <v>9</v>
       </c>
       <c r="H284" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="285" spans="1:9" x14ac:dyDescent="0.3">
@@ -4585,7 +4582,7 @@
         <v>9</v>
       </c>
       <c r="H285" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="286" spans="1:9" x14ac:dyDescent="0.3">
@@ -4593,13 +4590,13 @@
     </row>
     <row r="287" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B287" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C287" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D287" s="9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E287" t="s">
         <v>25</v>
@@ -4608,10 +4605,10 @@
         <v>9</v>
       </c>
       <c r="H287" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I287" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="288" spans="1:9" x14ac:dyDescent="0.3">
@@ -4623,7 +4620,7 @@
         <v>9</v>
       </c>
       <c r="H288" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="289" spans="2:9" x14ac:dyDescent="0.3">
@@ -4635,7 +4632,7 @@
         <v>9</v>
       </c>
       <c r="H289" s="17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="290" spans="2:9" x14ac:dyDescent="0.3">
@@ -4643,13 +4640,13 @@
     </row>
     <row r="291" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B291" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C291" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D291" s="9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E291" s="1" t="s">
         <v>14</v>
@@ -4700,7 +4697,7 @@
         <v>9</v>
       </c>
       <c r="H294" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="295" spans="2:9" x14ac:dyDescent="0.3">
@@ -4711,7 +4708,7 @@
         <v>97</v>
       </c>
       <c r="C296" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D296" s="9" t="s">
         <v>98</v>
@@ -4729,7 +4726,7 @@
         <v>20200401</v>
       </c>
       <c r="I296" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="297" spans="2:9" x14ac:dyDescent="0.3">
@@ -4757,7 +4754,7 @@
         <v>97</v>
       </c>
       <c r="C299" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D299" s="9" t="s">
         <v>99</v>
@@ -4775,7 +4772,7 @@
         <v>20200401</v>
       </c>
       <c r="I299" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="300" spans="2:9" x14ac:dyDescent="0.3">
@@ -4850,7 +4847,7 @@
         <v>97</v>
       </c>
       <c r="C306" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D306" s="9" t="s">
         <v>105</v>
@@ -4868,7 +4865,7 @@
         <v>20200401</v>
       </c>
       <c r="I306" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="307" spans="2:9" x14ac:dyDescent="0.3">
@@ -4889,19 +4886,19 @@
     <row r="308" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D308" s="9"/>
       <c r="E308" t="s">
+        <v>96</v>
+      </c>
+      <c r="F308" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H308" s="8" t="s">
         <v>106</v>
-      </c>
-      <c r="F308" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H308" s="8" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="309" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D309" s="9"/>
       <c r="E309" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F309" s="9" t="s">
         <v>22</v>
@@ -4913,7 +4910,7 @@
     <row r="310" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D310" s="9"/>
       <c r="E310" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F310" s="9" t="s">
         <v>22</v>
@@ -4931,10 +4928,10 @@
         <v>97</v>
       </c>
       <c r="C312" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D312" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E312" t="s">
         <v>14</v>
@@ -4949,7 +4946,7 @@
         <v>20200401</v>
       </c>
       <c r="I312" s="24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="313" spans="2:9" x14ac:dyDescent="0.3">
@@ -4976,10 +4973,10 @@
         <v>97</v>
       </c>
       <c r="C315" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D315" s="9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E315" t="s">
         <v>14</v>
@@ -4994,7 +4991,7 @@
         <v>20200401</v>
       </c>
       <c r="I315" s="24" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="316" spans="2:9" x14ac:dyDescent="0.3">
@@ -5015,7 +5012,7 @@
     <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D317" s="9"/>
       <c r="E317" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F317" s="9" t="s">
         <v>22</v>
@@ -5033,10 +5030,10 @@
         <v>97</v>
       </c>
       <c r="C319" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D319" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E319" t="s">
         <v>21</v>
@@ -5051,14 +5048,14 @@
         <v>20220228</v>
       </c>
       <c r="I319" s="24" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="320" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C320" s="1"/>
       <c r="D320" s="9"/>
       <c r="E320" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F320" s="9" t="s">
         <v>22</v>
@@ -5075,7 +5072,7 @@
         <v>56</v>
       </c>
       <c r="F321" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H321" s="8">
         <v>48</v>
@@ -5086,10 +5083,10 @@
       <c r="C322" s="1"/>
       <c r="D322" s="9"/>
       <c r="E322" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F322" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H322" s="8">
         <v>4</v>
@@ -5100,10 +5097,10 @@
       <c r="C323" s="1"/>
       <c r="D323" s="9"/>
       <c r="E323" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F323" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H323" s="8">
         <v>1.1000000000000001</v>
@@ -5114,10 +5111,10 @@
       <c r="C324" s="1"/>
       <c r="D324" s="9"/>
       <c r="E324" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F324" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H324" s="8">
         <v>3.2</v>
@@ -5128,10 +5125,10 @@
       <c r="C325" s="1"/>
       <c r="D325" s="9"/>
       <c r="E325" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F325" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H325" s="8">
         <v>0.11</v>
@@ -5142,10 +5139,10 @@
       <c r="C326" s="1"/>
       <c r="D326" s="9"/>
       <c r="E326" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F326" s="9" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H326" s="8">
         <v>0.2</v>
@@ -5162,7 +5159,7 @@
         <v>22</v>
       </c>
       <c r="H327" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="I327" s="24"/>
     </row>
@@ -5170,7 +5167,7 @@
       <c r="C328" s="1"/>
       <c r="D328" s="9"/>
       <c r="E328" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F328" s="9" t="s">
         <v>22</v>
@@ -5189,7 +5186,7 @@
         <v>22</v>
       </c>
       <c r="H329" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="330" spans="2:9" x14ac:dyDescent="0.3">
@@ -5200,10 +5197,10 @@
         <v>57</v>
       </c>
       <c r="C331" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D331" s="9" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E331" s="1"/>
       <c r="F331" s="1"/>
@@ -5228,19 +5225,19 @@
         <v>57</v>
       </c>
       <c r="C333" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D333" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E333" s="1"/>
       <c r="F333" s="1"/>
       <c r="G333" s="1"/>
       <c r="H333" s="12" t="s">
+        <v>291</v>
+      </c>
+      <c r="I333" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="I333" s="7" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="334" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5258,13 +5255,13 @@
         <v>57</v>
       </c>
       <c r="C335" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D335" s="10" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E335" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F335" s="10" t="s">
         <v>22</v>
@@ -5274,7 +5271,7 @@
         <v>531733</v>
       </c>
       <c r="I335" s="7" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="336" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5282,7 +5279,7 @@
       <c r="C336" s="1"/>
       <c r="D336" s="10"/>
       <c r="E336" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F336" s="1" t="s">
         <v>22</v>
@@ -5308,33 +5305,33 @@
         <v>57</v>
       </c>
       <c r="C338" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D338" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="E338" s="8" t="s">
         <v>281</v>
-      </c>
-      <c r="E338" s="8" t="s">
-        <v>282</v>
       </c>
       <c r="F338" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G338" s="8"/>
       <c r="H338" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="339" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D339" s="9"/>
       <c r="E339" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F339" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G339" s="8"/>
       <c r="H339" s="18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="340" spans="2:9" x14ac:dyDescent="0.3">
@@ -5345,13 +5342,13 @@
         <v>57</v>
       </c>
       <c r="C341" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D341" s="9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E341" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F341" s="1" t="s">
         <v>9</v>
@@ -5366,7 +5363,7 @@
     <row r="342" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D342" s="9"/>
       <c r="E342" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F342" s="1" t="s">
         <v>9</v>
@@ -5385,13 +5382,13 @@
         <v>57</v>
       </c>
       <c r="C344" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D344" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E344" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F344" s="1" t="s">
         <v>9</v>
@@ -5403,7 +5400,7 @@
     <row r="345" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D345" s="9"/>
       <c r="E345" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F345" s="1" t="s">
         <v>9</v>
@@ -5420,13 +5417,13 @@
         <v>53</v>
       </c>
       <c r="C347" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D347" s="10" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E347" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F347" s="10" t="s">
         <v>9</v>
@@ -5436,7 +5433,7 @@
         <v>55</v>
       </c>
       <c r="I347" s="24" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="348" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5454,13 +5451,13 @@
         <v>53</v>
       </c>
       <c r="C349" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D349" s="10" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E349" s="11" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="F349" s="10" t="s">
         <v>9</v>
@@ -5478,7 +5475,7 @@
       <c r="C350" s="1"/>
       <c r="D350" s="10"/>
       <c r="E350" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F350" s="10" t="s">
         <v>9</v>
@@ -5494,7 +5491,7 @@
       <c r="C351" s="1"/>
       <c r="D351" s="10"/>
       <c r="E351" s="11" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F351" s="10" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Change output of CapitalGainLoss_TradeListingDetail Api
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -1463,8 +1463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C295" workbookViewId="0">
-      <selection activeCell="E308" sqref="E308"/>
+    <sheetView tabSelected="1" topLeftCell="C297" workbookViewId="0">
+      <selection activeCell="H311" sqref="H311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Change bill module api output
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -11,7 +11,6 @@
     <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1463,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I366"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C297" workbookViewId="0">
-      <selection activeCell="H311" sqref="H311"/>
+    <sheetView tabSelected="1" topLeftCell="C77" workbookViewId="0">
+      <selection activeCell="H80" sqref="H80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Change Famil output json
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="807" uniqueCount="307">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -810,9 +810,6 @@
     <t>Family_TransactionJson</t>
   </si>
   <si>
-    <t>{ "status": true, "status_code": 200, "message": "success", "error_message": null, "data": [ { "familyCode": "SJ007 ", "familyName": "BAWNILLTJI ", "debit": "66551.92", "credit": "399.00" }, { "familyCode": "MG040 ", "familyName": "Testing 5 ", "debit": "307093.28", "credit": "300025.32" } ] }</t>
-  </si>
-  <si>
     <t>Family_Transaction_DetailsJson</t>
   </si>
   <si>
@@ -961,6 +958,12 @@
   </si>
   <si>
     <t>[ { "familyCode": "MG040", "familyName": "MG040_PAKMRMTTAL HUF", "holdingDetails": [ { "isin": "INE002J01027", "isinName": "SRS FINANCE-EQ1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE00PV01013", "isinName": "AHLADA ENGINEERS-EQ", "quantity": "3", "valuation": "265.65" }, { "isin": "INE013A01015", "isinName": "RELIANCE CAPITAL", "quantity": "18", "valuation": "207.18" }, { "isin": "INE016A01026", "isinName": "DABUR INDIA (RE.1/-)", "quantity": "1", "valuation": "502.05" }, { "isin": "INE019A01038", "isinName": "JSW STEEL-EQTY", "quantity": "1", "valuation": "361.85" }, { "isin": "INE020B01018", "isinName": "REC LTD - EQ", "quantity": "3", "valuation": "407.70" }, { "isin": "INE028A01039", "isinName": "BANK OF BARODA-EQ", "quantity": "16", "valuation": "1049.60" }, { "isin": "INE040C01022", "isinName": "CALS REFINER-EQ RE 1", "quantity": "0", "valuation": "0.00" }, { "isin": "INE043F01011", "isinName": "N2N TECH- EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE050M01012", "isinName": "VARDHMAN SPECIAL-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE053A01029", "isinName": "INDIAN HOTEL-EQ RE 1", "quantity": "3", "valuation": "395.85" }, { "isin": "INE064A01026", "isinName": "TIMEX GROUP -RE.1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE074A01025", "isinName": "PRAJ INDUSTRI-EQ RS2", "quantity": "512", "valuation": "54528.00" }, { "isin": "INE083A01026", "isinName": "MOREPEN LAB(RS.2/-)", "quantity": "6", "valuation": "192.90" }, { "isin": "INE090A01021", "isinName": "ICICI BANK-EQ", "quantity": "1", "valuation": "511.30" }, { "isin": "INE092A01019", "isinName": "TATA CHEMICALS EQ", "quantity": "1", "valuation": "510.45" }, { "isin": "INE093B01015", "isinName": "ALPS INDUSTRIES EQTY", "quantity": "200", "valuation": "198.00" }, { "isin": "INE09E501017", "isinName": "RAVINDER HEIGHT - EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE101A01026", "isinName": "MAH &amp; MAH EQ RS 5/-", "quantity": "1", "valuation": "754.85" }, { "isin": "INE121J01017", "isinName": "INDUS TOWERS LTD-EQ", "quantity": "3", "valuation": "739.20" }, { "isin": "INE154A01025", "isinName": "ITC LIMITED -EQ RE.1", "quantity": "0", "valuation": "0.00" }, { "isin": "INE155A01022", "isinName": "TATA MOTORS-EQ RS2/-", "quantity": "3", "valuation": "548.10" }, { "isin": "INE160A01022", "isinName": "PUNJAB NATIO-EQ", "quantity": "9", "valuation": "354.60" }, { "isin": "INE161L01027", "isinName": "VIKAS MULTICORP-EQ", "quantity": "210", "valuation": "1617.00" }, { "isin": "INE166C01025", "isinName": "BELLARY STEEL-EQ RE1", "quantity": "1000", "valuation": "1910.00" }, { "isin": "INE208A01029", "isinName": "ASHOK LEYLAND-RE.1/-", "quantity": "3", "valuation": "286.05" }, { "isin": "INE224E01028", "isinName": "STAMPEDE CAP-EQ", "quantity": "33200", "valuation": "19256.00" }, { "isin": "INE225D01027", "isinName": "SYMPHONY LTD-EQ 2/-", "quantity": "1", "valuation": "906.90" }, { "isin": "INE232I01014", "isinName": "SUN PHARMA ADV - EQ", "quantity": "3", "valuation": "578.70" }, { "isin": "INE249G01020", "isinName": "SURYA PHARMA-RE.1-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE256A01028", "isinName": "ZEE ENTERTAINMENT-EQ", "quantity": "6", "valuation": "1293.30" }, { "isin": "INE267A01025", "isinName": "HIND ZINC EQ-RS 2/-", "quantity": "3", "valuation": "729.00" }, { "isin": "INE289B01019", "isinName": "GIC HOU FINAN", "quantity": "3", "valuation": "349.05" }, { "isin": "INE294B01019", "isinName": "SML ISUZU LTD-EQ", "quantity": "1", "valuation": "489.35" }, { "isin": "INE302A01020", "isinName": "EXIDE - EQ RE 1/-", "quantity": "3", "valuation": "578.25" }, { "isin": "INE305A01015", "isinName": "TOURISM FIN CORP", "quantity": "3", "valuation": "144.75" }, { "isin": "INE305H01028", "isinName": "SUNIL HITECH-EQ", "quantity": "2000", "valuation": "760.00" }, { "isin": "INE312K01010", "isinName": "METROPOLITAN STOC-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE315L01029", "isinName": "JAY ENERGY-EQ-RS-2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE318J01027", "isinName": "NU TEK INDIA - EQ5/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE326A01037", "isinName": "LUPIN LIMITED-EQ2/-", "quantity": "1", "valuation": "950.70" }, { "isin": "INE331A01037", "isinName": "THE RAMCO CEM-EQ", "quantity": "1", "valuation": "870.85" }, { "isin": "INE341L01017", "isinName": "BIRLA PACIFIC MED-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE347D01011", "isinName": "LERTHAI FINANCE-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE347G01014", "isinName": "PETRONET LNG LTD-EQ", "quantity": "2", "valuation": "515.40" }, { "isin": "INE347W01011", "isinName": "MAGADH SUGAR-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE352A01017", "isinName": "VALUE INDUSTRIES EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE354C01027", "isinName": "BHAGERIA INDUSTRI-EQ", "quantity": "1", "valuation": "150.05" }, { "isin": "INE378P01028", "isinName": "OMANSH ENTER-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE385B01031", "isinName": "REI AGRO LTD-EQ RE 1", "quantity": "0", "valuation": "0.00" }, { "isin": "INE391I01018", "isinName": "TELEDATA TECHNO - EQ", "quantity": "25", "valuation": "3.00" }, { "isin": "INE415I01015", "isinName": "KIRI INDUSTRIES-EQ", "quantity": "1", "valuation": "481.85" }, { "isin": "INE430G01026", "isinName": "JVL AGRO IND-EQ 1/-", "quantity": "300", "valuation": "207.00" }, { "isin": "INE438E01016", "isinName": "SIKA INTERPLANT SYS", "quantity": "0", "valuation": "0.00" }, { "isin": "INE442C01012", "isinName": "CHARMS INDUSTRIES", "quantity": "0", "valuation": "0.00" }, { "isin": "INE473I01014", "isinName": "TELEDATE MARINE-EQ", "quantity": "25", "valuation": "7.25" }, { "isin": "INE509A01012", "isinName": "DUNLOP INDIA LTD- EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE510H01015", "isinName": "ROYAL INDIA -EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE512B01022", "isinName": "FCS SOFTWARE SOL-EQ1", "quantity": "0", "valuation": "0.00" }, { "isin": "INE522F01014", "isinName": "COAL INDIA LTD-EQ", "quantity": "6", "valuation": "808.50" }, { "isin": "INE528G01035", "isinName": "YES BANK LTD-EQ2/-", "quantity": "300", "valuation": "5718.00" }, { "isin": "INE545U01014", "isinName": "BANDHAN BANK-EQ", "quantity": "3", "valuation": "1199.70" }, { "isin": "INE584A01023", "isinName": "NMDC LIMITED-EQ RE 1", "quantity": "3", "valuation": "321.30" }, { "isin": "INE606B01022", "isinName": "BLS INFOTEC-EQ RE1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE608A01012", "isinName": "PUNJAB AND SIND - EQ", "quantity": "60", "valuation": "894.00" }, { "isin": "INE619I01012", "isinName": "A2Z INFRA ENGINEE-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE669E01016", "isinName": "VODAFONE IDEA-EQ", "quantity": "180", "valuation": "1776.60" }, { "isin": "INE699C01017", "isinName": "TERRUZZI FERCALX-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE706A01022", "isinName": "VIKAS WSP F.V RE.1/-", "quantity": "100", "valuation": "510.00" }, { "isin": "INE715C01011", "isinName": "UNIPRODUCTS (INDIA)", "quantity": "0", "valuation": "0.00" }, { "isin": "INE736A01011", "isinName": "CDSL EQUITY", "quantity": "71", "valuation": "37321.15" }, { "isin": "INE752E01010", "isinName": "POWER GRID CORP - EQ", "quantity": "3", "valuation": "578.10" }, { "isin": "INE767B01022", "isinName": "VIKAS PROPPANT-EQ1/-", "quantity": "300", "valuation": "996.00" }, { "isin": "INE775A01035", "isinName": "MOTHERSON SUMI-RE1/-", "quantity": "3", "valuation": "472.80" }, { "isin": "INE794A01010", "isinName": "NEULAND LABS EQUITY", "quantity": "15", "valuation": "16718.25" }, { "isin": "INE796A01023", "isinName": "AFTEK LIMITED-RS.2", "quantity": "0", "valuation": "0.00" }, { "isin": "INE806A01020", "isinName": "VIKAS ECOTECH-EQ 1/-", "quantity": "300", "valuation": "1371.00" }, { "isin": "INE810G01011", "isinName": "SHYAM METALICS-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE819B01021", "isinName": "JENSON &amp; NICH-RS.2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE843A01023", "isinName": "PEARL ENG POLY-NEW", "quantity": "0", "valuation": "0.00" }, { "isin": "INE854D01024", "isinName": "UNITED SPIRITS-EQ2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE862A01015", "isinName": "LML LIMITED EQUITY", "quantity": "0", "valuation": "0.00" }, { "isin": "INE871C01038", "isinName": "AVANTI FEEDS-EQ1/-", "quantity": "2", "valuation": "1063.90" }, { "isin": "INE871L01013", "isinName": "TV VISION - EQ", "quantity": "150", "valuation": "291.00" }, { "isin": "INE891D01026", "isinName": "REDINGTON-EQ 2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE928K01013", "isinName": "DR. DATSONS- EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE950G01023", "isinName": "UNIPLY INDUST-EQ2/-", "quantity": "1260", "valuation": "4309.20" }, { "isin": "INE951M01037", "isinName": "RRIL LTD-EQ5/-", "quantity": "18", "valuation": "122.40" }, { "isin": "INE969D01012", "isinName": "IND BANK HOUSING LTD", "quantity": "30", "valuation": "739.50" }, { "isin": "INE976G01028", "isinName": "RBL BNK-EQ RE 10", "quantity": "3", "valuation": "710.25" }, { "isin": "INE989C01012", "isinName": "DIAMOND POWER EQ", "quantity": "445", "valuation": "338.20" }, { "isin": "INE001A01036", "isinName": "HDFC LTD-EQ 2/-", "quantity": "1", "valuation": "2305.20" }, { "isin": "INE002A01018", "isinName": "RELIANCE INDUS-EQ", "quantity": "20", "valuation": "40533.00" }, { "isin": "INE002S01010", "isinName": "MAHANAGAR GAS-EQ", "quantity": "2", "valuation": "2075.10" }, { "isin": "INE009A01021", "isinName": "INFOSYS LTD-EQ 5/-", "quantity": "12", "valuation": "14101.80" }, { "isin": "INE00PV01013", "isinName": "AHLADA ENGINEERS-EQ", "quantity": "3", "valuation": "265.65" }, { "isin": "INE010V01017", "isinName": "L&amp;T TECHNOLOGY-EQ", "quantity": "3", "valuation": "5520.15" }, { "isin": "INE016M01021", "isinName": "DILIGENT MEDIA-EQ", "quantity": "500", "valuation": "220.00" }, { "isin": "INE018A01030", "isinName": "LARSEN &amp; TOUBR-EQ2/-", "quantity": "4", "valuation": "4724.40" }, { "isin": "INE018I01017", "isinName": "MINDTREE LIMITED-EQ", "quantity": "6", "valuation": "8737.80" }, { "isin": "INE022Q01020", "isinName": "INDIAN ENERGY-EQ1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE023M01027", "isinName": "PRAKASH CONST-EQ 1/-", "quantity": "23193", "valuation": "24352.65" }, { "isin": "INE029A01011", "isinName": "BPCL EQUITY", "quantity": "2", "valuation": "790.40" }, { "isin": "INE02A801020", "isinName": "ROSSARI BIOTECH-EQ", "quantity": "1", "valuation": "835.35" }, { "isin": "INE031B01049", "isinName": "AJANTA PHAR-EQ", "quantity": "1", "valuation": "1680.25" }, { "isin": "INE034A01011", "isinName": "ARVIND LIMITED EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE040A01034", "isinName": "HDFC BANK-EQ1/-", "quantity": "1", "valuation": "1405.85" }, { "isin": "INE042A01014", "isinName": "ESCORTS LIMITED EQ", "quantity": "1", "valuation": "1389.25" }, { "isin": "INE043D01016", "isinName": "IDFC LIMITED-EQ", "quantity": "1175", "valuation": "46941.25" }, { "isin": "INE044A01036", "isinName": "SUN PHARMA RE.1/-", "quantity": "3", "valuation": "1708.65" }, { "isin": "INE050A01025", "isinName": "BOMBAY BURMAH EQ 2/-", "quantity": "1", "valuation": "1369.80" }, { "isin": "INE050M01012", "isinName": "VARDHMAN SPECIAL-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE052T01013", "isinName": "BEST AGROLIFE-EQ", "quantity": "24", "valuation": "11479.20" }, { "isin": "INE058D01030", "isinName": "JAIPAN IND -EQ RS 10", "quantity": "0", "valuation": "0.00" }, { "isin": "INE061F01013", "isinName": "FORTIS HEALTHCARE-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE062A01020", "isinName": "SBI - EQ", "quantity": "6", "valuation": "1622.10" }, { "isin": "INE073K01018", "isinName": "SONA BLW PRECIS-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE075A01022", "isinName": "WIPRO EQUITY - RS 2", "quantity": "63", "valuation": "22657.95" }, { "isin": "INE079A01024", "isinName": "AMBUJA CEMENTS EQ", "quantity": "106", "valuation": "26807.40" }, { "isin": "INE07T201019", "isinName": "BURGER KING INDIA-EQ", "quantity": "709", "valuation": "0.00" }, { "isin": "INE092B01025", "isinName": "INDIA NIPPON-EQ5/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE092T01019", "isinName": "IDFC FIRST BANK-EQ", "quantity": "305", "valuation": "11788.25" }, { "isin": "INE093A01033", "isinName": "HEXAWARE TECH RS 2/-", "quantity": "3", "valuation": "1412.25" }, { "isin": "INE094A01015", "isinName": "HPCL EQUITY", "quantity": "8", "valuation": "1746.40" }, { "isin": "INE101D01020", "isinName": "GRANULES INDIA-EQ", "quantity": "15", "valuation": "5872.50" }, { "isin": "INE109A01011", "isinName": "SHIPPING CORPN. EQ", "quantity": "8", "valuation": "590.40" }, { "isin": "INE110A01019", "isinName": "BPL LTD EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE114A01011", "isinName": "SAIL EQUITY SHARES", "quantity": "34", "valuation": "1859.80" }, { "isin": "INE115A01026", "isinName": "LIC HSG FIN RS-2-EQ", "quantity": "15", "valuation": "5356.50" }, { "isin": "INE116G01013", "isinName": "VARDHMAN ACRYLICS-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE118H01025", "isinName": "BSE LIMITED-EQ 2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE123W01016", "isinName": "SBI LIFE INSURANC-EQ", "quantity": "1", "valuation": "857.90" }, { "isin": "INE127D01025", "isinName": "HDFC ASSET-EQ5/-", "quantity": "2", "valuation": "5622.10" }, { "isin": "INE129A01019", "isinName": "GAIL (INDIA) LTD-EQ", "quantity": "9", "valuation": "1102.95" }, { "isin": "INE139A01034", "isinName": "NALCO EQ-RS 5/-", "quantity": "37", "valuation": "1557.70" }, { "isin": "INE140A01024", "isinName": "PIRAMAL ENTER - EQ", "quantity": "2", "valuation": "2931.30" }, { "isin": "INE150G01020", "isinName": "LUX INDUSTRIES-EQ", "quantity": "11", "valuation": "17498.25" }, { "isin": "INE151A01013", "isinName": "TATA COMM EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE154A01025", "isinName": "ITC LIMITED -EQ RE.1", "quantity": "9", "valuation": "1848.15" }, { "isin": "INE155A01022", "isinName": "TATA MOTORS-EQ RS2/-", "quantity": "12", "valuation": "2192.40" }, { "isin": "INE160A01022", "isinName": "PUNJAB NATIO-EQ", "quantity": "2470", "valuation": "97318.00" }, { "isin": "INE161L01027", "isinName": "VIKAS MULTICORP-EQ", "quantity": "390", "valuation": "3003.00" }, { "isin": "INE171Z01018", "isinName": "BHARAT DYNAMICS-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE181G01025", "isinName": "GAMMON INFRA - EQ", "quantity": "27900", "valuation": "26784.00" }, { "isin": "INE192B01031", "isinName": "WELSPUN INDIA-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE192R01011", "isinName": "AVENUE SUPER-EQ", "quantity": "14", "valuation": "36713.60" }, { "isin": "INE195A01028", "isinName": "THE SUPREME IND-EQ", "quantity": "1", "valuation": "1728.60" }, { "isin": "INE200M01013", "isinName": "VARUN BEV-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE203G01027", "isinName": "INDRAPRASTHA-EQ2/-", "quantity": "7", "valuation": "3381.00" }, { "isin": "INE205A01025", "isinName": "VEDANTA LTD-EQ RE1/-", "quantity": "3", "valuation": "430.95" }, { "isin": "INE208A01029", "isinName": "ASHOK LEYLAND-RE.1/-", "quantity": "50", "valuation": "4767.50" }, { "isin": "INE213A01029", "isinName": "ONGC-EQ-RS.5/-", "quantity": "39", "valuation": "3554.85" }, { "isin": "INE214F01026", "isinName": "GRAVISS HOSP-EQ RS 2", "quantity": "0", "valuation": "0.00" }, { "isin": "INE216A01030", "isinName": "BRITANNIA IND-EQ1/-", "quantity": "3", "valuation": "10882.05" }, { "isin": "INE220J01025", "isinName": "FUTURE CONS- EQ 6/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE224A01026", "isinName": "GREAVES COTTONE EQ 2", "quantity": "0", "valuation": "0.00" }, { "isin": "INE224E01036", "isinName": "STAMPEDE CAPITAL-EQ", "quantity": "7347", "valuation": "9991.92" }, { "isin": "INE242A01010", "isinName": "INDIAN OIL CORP EQ", "quantity": "12", "valuation": "1127.40" }, { "isin": "INE250K01012", "isinName": "D-LINK (INDIA) L-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE253A01025", "isinName": "HINDUSTAN MOTORS-EQ5", "quantity": "0", "valuation": "0.00" }, { "isin": "INE257A01026", "isinName": "BHARAT HEAVY - EQ 2", "quantity": "23", "valuation": "840.65" }, { "isin": "INE259A01022", "isinName": "COLGATE PALM-EQ RE 1", "quantity": "1", "valuation": "1567.60" }, { "isin": "INE260D01016", "isinName": "OLECTRA GREENTECH-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE267A01025", "isinName": "HIND ZINC EQ-RS 2/-", "quantity": "6", "valuation": "1458.00" }, { "isin": "INE288B01029", "isinName": "DEEPAK NITR-EQ", "quantity": "2", "valuation": "1719.60" }, { "isin": "INE296A01024", "isinName": "BAJAJ FINANCE-EQ", "quantity": "1", "valuation": "4843.00" }, { "isin": "INE319B01014", "isinName": "THE BYKE HOSP- EQ", "quantity": "300", "valuation": "5514.00" }, { "isin": "INE320J01015", "isinName": "RITES LIMITED - EQ", "quantity": "4", "valuation": "1079.20" }, { "isin": "INE326A01037", "isinName": "LUPIN LIMITED-EQ2/-", "quantity": "3", "valuation": "2852.10" }, { "isin": "INE330H01018", "isinName": "RELIANCE COMMUNI -EQ", "quantity": "2800", "valuation": "6468.00" }, { "isin": "INE347W01011", "isinName": "MAGADH SUGAR-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE353K01014", "isinName": "INDIA TOURISM - EQ", "quantity": "30", "valuation": "8610.00" }, { "isin": "INE378D01032", "isinName": "MADHUCON PROJ EQ 1", "quantity": "2000", "valuation": "8880.00" }, { "isin": "INE398A01010", "isinName": "VENKY S (INDIA) EQTY", "quantity": "5", "valuation": "8541.75" }, { "isin": "INE419U01012", "isinName": "HAPPIEST MINDS TE-EQ", "quantity": "3", "valuation": "968.10" }, { "isin": "INE432A01017", "isinName": "AMBALAL SARABHAI", "quantity": "0", "valuation": "0.00" }, { "isin": "INE437A01024", "isinName": "APOLLO HOSPIT-EQ5/-", "quantity": "1", "valuation": "2441.15" }, { "isin": "INE438E01016", "isinName": "SIKA INTERPLANT SYS", "quantity": "0", "valuation": "0.00" }, { "isin": "INE442H01029", "isinName": "ASHOKA BUILD EQ 5/-", "quantity": "30", "valuation": "2863.50" }, { "isin": "INE450G01024", "isinName": "VIP CLOTHING-EQ2/-", "quantity": "1200", "valuation": "14616.00" }, { "isin": "INE467B01029", "isinName": "TATA CONSULTANCY-1/-", "quantity": "8", "valuation": "22478.40" }, { "isin": "INE476A01014", "isinName": "CANARA BANK-EQ", "quantity": "9", "valuation": "1152.90" }, { "isin": "INE481G01011", "isinName": "ULTRATECH CEMENT LTD", "quantity": "1", "valuation": "5147.95" }, { "isin": "INE498L01015", "isinName": "L&amp;T FINANCE HOLD-EQ", "quantity": "119", "valuation": "10948.00" }, { "isin": "INE500A01029", "isinName": "DCW LTD - EQ RS 2", "quantity": "100", "valuation": "1881.00" }, { "isin": "INE522F01014", "isinName": "COAL INDIA LTD-EQ", "quantity": "15", "valuation": "2021.25" }, { "isin": "INE528G01035", "isinName": "YES BANK LTD-EQ2/-", "quantity": "83995", "valuation": "1600944.70" }, { "isin": "INE545U01014", "isinName": "BANDHAN BANK-EQ", "quantity": "48", "valuation": "19195.20" }, { "isin": "INE565A01014", "isinName": "INDIAN OVERSEAS BANK", "quantity": "200", "valuation": "2340.00" }, { "isin": "INE577L01016", "isinName": "STEL HOLDINGS - EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE584A01023", "isinName": "NMDC LIMITED-EQ RE 1", "quantity": "21", "valuation": "2249.10" }, { "isin": "INE585B01010", "isinName": "MARUTI SUZUKI IND-EQ", "quantity": "1", "valuation": "7707.75" }, { "isin": "INE589A01014", "isinName": "NLC INDIA LIMITED-EQ", "quantity": "1880", "valuation": "102460.00" }, { "isin": "INE589D01018", "isinName": "D &amp; H INDIA LTD - EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE596I01012", "isinName": "COMPUTER AGE MAN-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE602G01020", "isinName": "KITEX GARMEN EQ RE.1", "quantity": "0", "valuation": "0.00" }, { "isin": "INE619I01012", "isinName": "A2Z INFRA ENGINEE-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE623B01027", "isinName": "FUTURE ENT-EQ RS2", "quantity": "0", "valuation": "0.00" }, { "isin": "INE645S01016", "isinName": "ROLEX RINGS-EQ", "quantity": "3", "valuation": "0.00" }, { "isin": "INE669C01036", "isinName": "TECH MAHINDRA-EQ", "quantity": "9", "valuation": "8362.80" }, { "isin": "INE691A01018", "isinName": "UCO BANK-EQ", "quantity": "300", "valuation": "4140.00" }, { "isin": "INE692A01016", "isinName": "UNION BANK OF INDIA", "quantity": "120", "valuation": "4074.00" }, { "isin": "INE706A01022", "isinName": "VIKAS WSP F.V RE.1/-", "quantity": "4000", "valuation": "20400.00" }, { "isin": "INE709A01018", "isinName": "VLS FINANCE LTD - EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE710A01016", "isinName": "VST INDUSTRIES EQ", "quantity": "20", "valuation": "77384.00" }, { "isin": "INE725E01024", "isinName": "ORISSA MINERAL EQ1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE733E01010", "isinName": "NTPC LTD", "quantity": "28", "valuation": "2751.00" }, { "isin": "INE736A01011", "isinName": "CDSL EQUITY", "quantity": "329", "valuation": "172938.85" }, { "isin": "INE748C01020", "isinName": "3I INFOTECH RS 10", "quantity": "1000", "valuation": "4360.00" }, { "isin": "INE752E01010", "isinName": "POWER GRID CORP - EQ", "quantity": "9", "valuation": "1734.30" }, { "isin": "INE763B01013", "isinName": "RAMA VISION LTD-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE767B01022", "isinName": "VIKAS PROPPANT-EQ1/-", "quantity": "12600", "valuation": "41832.00" }, { "isin": "INE774D01024", "isinName": "MAH &amp; MAH FIN EQ 2/-", "quantity": "13", "valuation": "2288.65" }, { "isin": "INE775B01025", "isinName": "KWALITY-EQ 1/-", "quantity": "1500", "valuation": "5025.00" }, { "isin": "INE776C01039", "isinName": "GMR INFRA - EQ RE 1", "quantity": "125", "valuation": "3437.50" }, { "isin": "INE781B01015", "isinName": "NOIDA TOLL BRIDGE CO", "quantity": "0", "valuation": "0.00" }, { "isin": "INE782E01017", "isinName": "HESTER BIOSCIENCES", "quantity": "21", "valuation": "36960.00" }, { "isin": "INE783X01023", "isinName": "CHEMFAB ALKAL-EQ10/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE787D01026", "isinName": "BALKRISHNA IND RS.2", "quantity": "1", "valuation": "1667.10" }, { "isin": "INE810G01011", "isinName": "SHYAM METALICS-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE831A01028", "isinName": "MIRC ELEC-RE.1", "quantity": "0", "valuation": "0.00" }, { "isin": "INE854D01024", "isinName": "UNITED SPIRITS-EQ2/-", "quantity": "3", "valuation": "1751.10" }, { "isin": "INE860A01027", "isinName": "HCL TECH (FV RS.2/-)", "quantity": "6", "valuation": "5223.00" }, { "isin": "INE879A01019", "isinName": "SHREE RAMA M-TECH EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE881D01027", "isinName": "ORACLE FINANC RS.5/-", "quantity": "1", "valuation": "3158.55" }, { "isin": "INE891D01026", "isinName": "REDINGTON-EQ 2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE895B01021", "isinName": "RUPA AND CO LTD-1/", "quantity": "3", "valuation": "691.65" }, { "isin": "INE908D01010", "isinName": "SHAKTI PUMPS (INDIA)", "quantity": "28", "valuation": "8079.40" }, { "isin": "INE922B01023", "isinName": "PANCEA BIOTEC RE1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE924D01017", "isinName": "THE INVESTMENT TR-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE937C01029", "isinName": "NILA INFRASTRU RE 1/", "quantity": "900", "valuation": "5220.00" }, { "isin": "INE939A01011", "isinName": "STRIDES PHARMA-EQ", "quantity": "3", "valuation": "2551.20" }, { "isin": "INE947Q01028", "isinName": "LAURUS LABS-EQ2/-", "quantity": "25", "valuation": "8217.50" }, { "isin": "INE955V01021", "isinName": "ARVIND FASHIONS-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE976G01028", "isinName": "RBL BNK-EQ RE 10", "quantity": "25", "valuation": "5918.75" } ] }, { "familyCode": "SJ007", "familyName": "SJ007_BWNILLT JAIN", "holdingDetails": [ { "isin": "INE002J01027", "isinName": "SRS FINANCE-EQ1/-", "quantity": "1", "valuation": "0.19" }, { "isin": "INE00PV01013", "isinName": "AHLADA ENGINEERS-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE013A01015", "isinName": "RELIANCE CAPITAL", "quantity": "0", "valuation": "0.00" }, { "isin": "INE016A01026", "isinName": "DABUR INDIA (RE.1/-)", "quantity": "0", "valuation": "0.00" }, { "isin": "INE019A01038", "isinName": "JSW STEEL-EQTY", "quantity": "0", "valuation": "0.00" }, { "isin": "INE020B01018", "isinName": "REC LTD - EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE028A01039", "isinName": "BANK OF BARODA-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE040C01022", "isinName": "CALS REFINER-EQ RE 1", "quantity": "5100", "valuation": "510.00" }, { "isin": "INE043F01011", "isinName": "N2N TECH- EQ", "quantity": "597", "valuation": "2447.70" }, { "isin": "INE050M01012", "isinName": "VARDHMAN SPECIAL-EQ", "quantity": "100", "valuation": "11465.00" }, { "isin": "INE053A01029", "isinName": "INDIAN HOTEL-EQ RE 1", "quantity": "0", "valuation": "0.00" }, { "isin": "INE064A01026", "isinName": "TIMEX GROUP -RE.1/-", "quantity": "100", "valuation": "3140.00" }, { "isin": "INE074A01025", "isinName": "PRAJ INDUSTRI-EQ RS2", "quantity": "0", "valuation": "0.00" }, { "isin": "INE083A01026", "isinName": "MOREPEN LAB(RS.2/-)", "quantity": "0", "valuation": "0.00" }, { "isin": "INE090A01021", "isinName": "ICICI BANK-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE092A01019", "isinName": "TATA CHEMICALS EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE093B01015", "isinName": "ALPS INDUSTRIES EQTY", "quantity": "0", "valuation": "0.00" }, { "isin": "INE09E501017", "isinName": "RAVINDER HEIGHT - EQ", "quantity": "10", "valuation": "0.00" }, { "isin": "INE101A01026", "isinName": "MAH &amp; MAH EQ RS 5/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE121J01017", "isinName": "INDUS TOWERS LTD-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE154A01025", "isinName": "ITC LIMITED -EQ RE.1", "quantity": "1", "valuation": "205.35" }, { "isin": "INE155A01022", "isinName": "TATA MOTORS-EQ RS2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE160A01022", "isinName": "PUNJAB NATIO-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE161L01027", "isinName": "VIKAS MULTICORP-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE166C01025", "isinName": "BELLARY STEEL-EQ RE1", "quantity": "0", "valuation": "0.00" }, { "isin": "INE208A01029", "isinName": "ASHOK LEYLAND-RE.1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE224E01028", "isinName": "STAMPEDE CAP-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE225D01027", "isinName": "SYMPHONY LTD-EQ 2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE232I01014", "isinName": "SUN PHARMA ADV - EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE249G01020", "isinName": "SURYA PHARMA-RE.1-EQ", "quantity": "25000", "valuation": "4000.00" }, { "isin": "INE256A01028", "isinName": "ZEE ENTERTAINMENT-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE267A01025", "isinName": "HIND ZINC EQ-RS 2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE289B01019", "isinName": "GIC HOU FINAN", "quantity": "0", "valuation": "0.00" }, { "isin": "INE294B01019", "isinName": "SML ISUZU LTD-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE302A01020", "isinName": "EXIDE - EQ RE 1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE305A01015", "isinName": "TOURISM FIN CORP", "quantity": "0", "valuation": "0.00" }, { "isin": "INE305H01028", "isinName": "SUNIL HITECH-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE312K01010", "isinName": "METROPOLITAN STOC-EQ", "quantity": "86000", "valuation": "0.00" }, { "isin": "INE315L01029", "isinName": "JAY ENERGY-EQ-RS-2/-", "quantity": "5000", "valuation": "1650.00" }, { "isin": "INE318J01027", "isinName": "NU TEK INDIA - EQ5/-", "quantity": "46000", "valuation": "13340.00" }, { "isin": "INE326A01037", "isinName": "LUPIN LIMITED-EQ2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE331A01037", "isinName": "THE RAMCO CEM-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE341L01017", "isinName": "BIRLA PACIFIC MED-EQ", "quantity": "49000", "valuation": "13720.00" }, { "isin": "INE347D01011", "isinName": "LERTHAI FINANCE-EQ", "quantity": "200", "valuation": "54000.00" }, { "isin": "INE347G01014", "isinName": "PETRONET LNG LTD-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE347W01011", "isinName": "MAGADH SUGAR-EQ", "quantity": "500", "valuation": "57950.00" }, { "isin": "INE352A01017", "isinName": "VALUE INDUSTRIES EQ", "quantity": "440", "valuation": "998.80" }, { "isin": "INE354C01027", "isinName": "BHAGERIA INDUSTRI-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE378P01028", "isinName": "OMANSH ENTER-EQ", "quantity": "1459", "valuation": "496.06" }, { "isin": "INE385B01031", "isinName": "REI AGRO LTD-EQ RE 1", "quantity": "1000", "valuation": "240.00" }, { "isin": "INE391I01018", "isinName": "TELEDATA TECHNO - EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE415I01015", "isinName": "KIRI INDUSTRIES-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE430G01026", "isinName": "JVL AGRO IND-EQ 1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE438E01016", "isinName": "SIKA INTERPLANT SYS", "quantity": "200", "valuation": "49430.00" }, { "isin": "INE442C01012", "isinName": "CHARMS INDUSTRIES", "quantity": "1140", "valuation": "2565.00" }, { "isin": "INE473I01014", "isinName": "TELEDATE MARINE-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE509A01012", "isinName": "DUNLOP INDIA LTD- EQ", "quantity": "4500", "valuation": "46845.00" }, { "isin": "INE510H01015", "isinName": "ROYAL INDIA -EQ", "quantity": "11000", "valuation": "10560.00" }, { "isin": "INE512B01022", "isinName": "FCS SOFTWARE SOL-EQ1", "quantity": "20000", "valuation": "12400.00" }, { "isin": "INE522F01014", "isinName": "COAL INDIA LTD-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE528G01035", "isinName": "YES BANK LTD-EQ2/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE545U01014", "isinName": "BANDHAN BANK-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE584A01023", "isinName": "NMDC LIMITED-EQ RE 1", "quantity": "0", "valuation": "0.00" }, { "isin": "INE606B01022", "isinName": "BLS INFOTEC-EQ RE1/-", "quantity": "10000", "valuation": "1900.00" }, { "isin": "INE608A01012", "isinName": "PUNJAB AND SIND - EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE619I01012", "isinName": "A2Z INFRA ENGINEE-EQ", "quantity": "1", "valuation": "4.83" }, { "isin": "INE669E01016", "isinName": "VODAFONE IDEA-EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE699C01017", "isinName": "TERRUZZI FERCALX-EQ", "quantity": "500", "valuation": "4290.00" }, { "isin": "INE706A01022", "isinName": "VIKAS WSP F.V RE.1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE715C01011", "isinName": "UNIPRODUCTS (INDIA)", "quantity": "1000", "valuation": "38750.00" }, { "isin": "INE736A01011", "isinName": "CDSL EQUITY", "quantity": "0", "valuation": "0.00" }, { "isin": "INE752E01010", "isinName": "POWER GRID CORP - EQ", "quantity": "0", "valuation": "0.00" }, { "isin": "INE767B01022", "isinName": "VIKAS PROPPANT-EQ1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE775A01035", "isinName": "MOTHERSON SUMI-RE1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE794A01010", "isinName": "NEULAND LABS EQUITY", "quantity": "0", "valuation": "0.00" }, { "isin": "INE796A01023", "isinName": "AFTEK LIMITED-RS.2", "quantity": "1000", "valuation": "1630.00" }, { "isin": "INE806A01020", "isinName": "VIKAS ECOTECH-EQ 1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE810G01011", "isinName": "SHYAM METALICS-EQ", "quantity": "1", "valuation": "0.00" }, { "isin": "INE819B01021", "isinName": "JENSON &amp; NICH-RS.2/-", "quantity": "1", "valuation": "1.97" }, { "isin": "INE843A01023", "isinName": "PEARL ENG POLY-NEW", "quantity": "1000", "valuation": "1220.00" }, { "isin": "INE854D01024", "isinName": "UNITED SPIRITS-EQ2/-", "quantity": "100", "valuation": "58370.00" }, { "isin": "INE862A01015", "isinName": "LML LIMITED EQUITY", "quantity": "13358", "valuation": "49023.86" }, { "isin": "INE871C01038", "isinName": "AVANTI FEEDS-EQ1/-", "quantity": "0", "valuation": "0.00" }, { "isin": "INE871L01013", "isinName": "TV VISION - EQ", "quantity": "0", "val</t>
+  </si>
+  <si>
+    <t>[ { "familyCode": "SJ007 ", "familyName": "BWNILLT JAIN ", "debit": "67171.92", "credit": "399.00" }, { "familyCode": "MG040 ", "familyName": "PAKMRMTTAL HUF ", "debit": "308353.28", "credit": "300025.32" } ]</t>
+  </si>
+  <si>
+    <t>[ { "refNo": "4876", "date": "09/03/2021", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "1260.00", "credit": "0.00" }, { "refNo": "4595", "date": "25/02/2021", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "439.00", "credit": "0.00" }, { "refNo": "4525", "date": "22/02/2021", "particulars": "NSE F&amp;O Bill for 18/02/21", "debit": "36785.03", "credit": "0.00" }, { "refNo": "4539", "date": "22/02/2021", "particulars": "Dividend @ 3.75 on 5 shares of K.P.R. Mill Limited [532889]", "debit": "0.00", "credit": "18.75" }, { "refNo": "4540", "date": "22/02/2021", "particulars": "TDS on Dividend @ 3.75 on 5 shares of K.P.R. Mill Limited [532889]", "debit": "1.41", "credit": "0.00" }, { "refNo": "4524", "date": "19/02/2021", "particulars": "REVERSAL OF NSE F&amp;O Bill for 18/02/21", "debit": "0.00", "credit": "36785.03" }, { "refNo": "4429", "date": "13/02/2021", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "1657.00", "credit": "0.00" }, { "refNo": "4248", "date": "04/02/2021", "particulars": "None collection of STT recovered Dated 02/02/2021", "debit": "1.00", "credit": "0.00" }, { "refNo": "3615", "date": "10/12/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "1671.00", "credit": "0.00" }, { "refNo": "3356", "date": "23/11/2020", "particulars": "Dividend @ 17 on 12 shares of Ambuja Cements Limited [500425]", "debit": "0.00", "credit": "204.00" }, { "refNo": "3357", "date": "23/11/2020", "particulars": "TDS on Dividend @ 17 on 12 shares of Ambuja Cements Limited [500425]", "debit": "15.30", "credit": "0.00" }, { "refNo": "3265", "date": "17/11/2020", "particulars": "NSE F&amp;O Bill for 13/11/20", "debit": "0.00", "credit": "8724.69" }, { "refNo": "3264", "date": "14/11/2020", "particulars": "REVERSAL OF NSE F&amp;O Bill for 13/11/20", "debit": "8724.69", "credit": "0.00" }, { "refNo": "3231", "date": "12/11/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "949.00", "credit": "0.00" }, { "refNo": "3074", "date": "02/11/2020", "particulars": "NSE F&amp;O BILL DT. 29.10.20", "debit": "0.00", "credit": "154202.34" }, { "refNo": "3073", "date": "30/10/2020", "particulars": "REVERSAL OFF NSE &amp;O BILL DT. 29.10.20", "debit": "154202.34", "credit": "0.00" }, { "refNo": "2752", "date": "09/10/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "513.00", "credit": "0.00" }, { "refNo": "2442", "date": "22/09/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "697.00", "credit": "0.00" }, { "refNo": "2176", "date": "14/09/2020", "particulars": "None collection of STT recovered Dated 10/09/2020", "debit": "1.00", "credit": "0.00" }, { "refNo": "2128", "date": "09/09/2020", "particulars": "None collection of STT recovered Dated 07/09/2020", "debit": "1.00", "credit": "0.00" }, { "refNo": "1953", "date": "26/08/2020", "particulars": "Bal Trfd From NSE/FX", "debit": "0.00", "credit": "27827.46" }, { "refNo": "1952", "date": "26/08/2020", "particulars": "Bal Trfd to NSE/Cash", "debit": "27827.46", "credit": "0.00" }, { "refNo": "1719", "date": "10/08/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "142.00", "credit": "0.00" }, { "refNo": "1174", "date": "09/07/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "712.00", "credit": "0.00" }, { "refNo": "751", "date": "08/06/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "198.00", "credit": "0.00" }, { "refNo": "488", "date": "13/05/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "293.00", "credit": "0.00" }, { "refNo": "427", "date": "08/05/2020", "particulars": "NSE F&amp;O Bill for 06/05/20", "debit": "72263.05", "credit": "0.00" }, { "refNo": "426", "date": "07/05/2020", "particulars": "REVERSAL OF NSE F&amp;O Bill for 06/05/20", "debit": "0.00", "credit": "72263.05" } ]</t>
   </si>
 </sst>
 </file>
@@ -1422,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C202" workbookViewId="0">
-      <selection activeCell="I213" sqref="I213"/>
+    <sheetView tabSelected="1" topLeftCell="C218" workbookViewId="0">
+      <selection activeCell="D221" sqref="D221"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1867,7 +1870,7 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D40" s="9"/>
       <c r="E40" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
@@ -2302,7 +2305,7 @@
         <v>225</v>
       </c>
       <c r="I88" s="22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
@@ -2329,7 +2332,7 @@
         <v>225</v>
       </c>
       <c r="I90" s="22" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
@@ -2444,7 +2447,7 @@
         <v>226</v>
       </c>
       <c r="I100" s="27" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
@@ -2523,7 +2526,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>9</v>
@@ -2553,7 +2556,7 @@
         <v>162</v>
       </c>
       <c r="I110" s="22" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
@@ -2609,7 +2612,7 @@
         <v>164</v>
       </c>
       <c r="I115" s="22" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
@@ -2682,7 +2685,7 @@
         <v>170</v>
       </c>
       <c r="I122" s="22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
@@ -2849,10 +2852,10 @@
         <v>215</v>
       </c>
       <c r="D139" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E139" s="10" t="s">
         <v>265</v>
-      </c>
-      <c r="E139" s="10" t="s">
-        <v>266</v>
       </c>
       <c r="F139" s="10" t="s">
         <v>22</v>
@@ -2861,7 +2864,7 @@
         <v>44</v>
       </c>
       <c r="I139" s="22" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
@@ -2902,7 +2905,7 @@
         <v>215</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E143" t="s">
         <v>155</v>
@@ -2914,7 +2917,7 @@
         <v>157</v>
       </c>
       <c r="I143" s="22" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.3">
@@ -2941,7 +2944,7 @@
         <v>22</v>
       </c>
       <c r="H145" s="17" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
@@ -3596,7 +3599,7 @@
         <v>236</v>
       </c>
       <c r="I203" s="22" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
@@ -3644,7 +3647,7 @@
         <v>236</v>
       </c>
       <c r="I208" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="209" spans="2:9" x14ac:dyDescent="0.3">
@@ -3698,11 +3701,9 @@
       <c r="H213" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="I213" s="7" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="214" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I213" s="7"/>
+    </row>
+    <row r="214" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D214" s="9"/>
       <c r="E214" s="8" t="s">
         <v>14</v>
@@ -3715,6 +3716,9 @@
       </c>
       <c r="H214" s="3">
         <v>20200401</v>
+      </c>
+      <c r="I214" s="7" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="215" spans="2:9" x14ac:dyDescent="0.3">
@@ -3764,15 +3768,15 @@
       <c r="G219" s="1"/>
       <c r="H219" s="3"/>
     </row>
-    <row r="220" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="220" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B220" s="8" t="s">
         <v>52</v>
       </c>
       <c r="C220" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="D220" s="28" t="s">
-        <v>256</v>
+      <c r="D220" s="25" t="s">
+        <v>255</v>
       </c>
       <c r="E220" s="29" t="s">
         <v>30</v>
@@ -3783,6 +3787,9 @@
       <c r="G220" s="8"/>
       <c r="H220" s="28" t="s">
         <v>250</v>
+      </c>
+      <c r="I220" s="7" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="221" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -4079,7 +4086,7 @@
         <v>20191101</v>
       </c>
       <c r="I245" s="7" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.3">
@@ -4105,7 +4112,7 @@
         <v>123</v>
       </c>
       <c r="I247" s="22" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.3">
@@ -4149,7 +4156,7 @@
         <v>20200401</v>
       </c>
       <c r="I250" s="22" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="251" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4177,7 +4184,7 @@
       <c r="C252" s="1"/>
       <c r="D252" s="10"/>
       <c r="E252" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>9</v>
@@ -4219,7 +4226,7 @@
         <v>176</v>
       </c>
       <c r="I254" s="22" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.3">
@@ -4281,7 +4288,7 @@
         <v>178</v>
       </c>
       <c r="I259" s="22" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="260" spans="2:9" x14ac:dyDescent="0.3">
@@ -4319,7 +4326,7 @@
         <v>186</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E263" s="1" t="s">
         <v>14</v>
@@ -4370,7 +4377,7 @@
         <v>9</v>
       </c>
       <c r="H266" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="267" spans="2:9" x14ac:dyDescent="0.3">
@@ -4399,7 +4406,7 @@
         <v>20200401</v>
       </c>
       <c r="I268" s="22" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="269" spans="2:9" x14ac:dyDescent="0.3">
@@ -4445,7 +4452,7 @@
         <v>20200401</v>
       </c>
       <c r="I271" s="22" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="272" spans="2:9" x14ac:dyDescent="0.3">
@@ -4538,7 +4545,7 @@
         <v>20200401</v>
       </c>
       <c r="I278" s="22" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="279" spans="2:9" x14ac:dyDescent="0.3">
@@ -4583,7 +4590,7 @@
     <row r="282" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D282" s="9"/>
       <c r="E282" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F282" s="9" t="s">
         <v>22</v>
@@ -4619,7 +4626,7 @@
         <v>20200401</v>
       </c>
       <c r="I284" s="22" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="285" spans="2:9" x14ac:dyDescent="0.3">
@@ -4664,7 +4671,7 @@
         <v>20200401</v>
       </c>
       <c r="I287" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="288" spans="2:9" x14ac:dyDescent="0.3">
@@ -4685,7 +4692,7 @@
     <row r="289" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D289" s="9"/>
       <c r="E289" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F289" s="9" t="s">
         <v>22</v>
@@ -4721,14 +4728,14 @@
         <v>20220228</v>
       </c>
       <c r="I291" s="22" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="292" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C292" s="1"/>
       <c r="D292" s="9"/>
       <c r="E292" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F292" s="9" t="s">
         <v>22</v>
@@ -4840,7 +4847,7 @@
       <c r="C300" s="1"/>
       <c r="D300" s="9"/>
       <c r="E300" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="F300" s="9" t="s">
         <v>22</v>
@@ -4873,7 +4880,7 @@
         <v>187</v>
       </c>
       <c r="D303" s="9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E303" s="1"/>
       <c r="F303" s="1"/>
@@ -4901,16 +4908,16 @@
         <v>187</v>
       </c>
       <c r="D305" s="10" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E305" s="1"/>
       <c r="F305" s="1"/>
       <c r="G305" s="1"/>
       <c r="H305" s="12" t="s">
+        <v>271</v>
+      </c>
+      <c r="I305" s="7" t="s">
         <v>272</v>
-      </c>
-      <c r="I305" s="7" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="306" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4931,10 +4938,10 @@
         <v>187</v>
       </c>
       <c r="D307" s="10" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E307" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F307" s="10" t="s">
         <v>22</v>
@@ -4944,7 +4951,7 @@
         <v>531733</v>
       </c>
       <c r="I307" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="308" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4952,7 +4959,7 @@
       <c r="C308" s="1"/>
       <c r="D308" s="10"/>
       <c r="E308" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F308" s="1" t="s">
         <v>22</v>
@@ -4981,30 +4988,30 @@
         <v>187</v>
       </c>
       <c r="D310" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="E310" s="8" t="s">
         <v>261</v>
-      </c>
-      <c r="E310" s="8" t="s">
-        <v>262</v>
       </c>
       <c r="F310" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G310" s="8"/>
       <c r="H310" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="311" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D311" s="9"/>
       <c r="E311" s="8" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F311" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G311" s="8"/>
       <c r="H311" s="18" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="312" spans="2:9" x14ac:dyDescent="0.3">
@@ -5018,10 +5025,10 @@
         <v>187</v>
       </c>
       <c r="D313" s="9" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E313" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F313" s="1" t="s">
         <v>9</v>
@@ -5036,7 +5043,7 @@
     <row r="314" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D314" s="9"/>
       <c r="E314" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F314" s="1" t="s">
         <v>9</v>
@@ -5058,10 +5065,10 @@
         <v>187</v>
       </c>
       <c r="D316" s="9" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E316" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F316" s="1" t="s">
         <v>9</v>
@@ -5073,7 +5080,7 @@
     <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D317" s="9"/>
       <c r="E317" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F317" s="1" t="s">
         <v>9</v>
@@ -5093,7 +5100,7 @@
         <v>216</v>
       </c>
       <c r="D319" s="10" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E319" s="11" t="s">
         <v>200</v>
@@ -5106,7 +5113,7 @@
         <v>48</v>
       </c>
       <c r="I319" s="22" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="320" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5127,7 +5134,7 @@
         <v>216</v>
       </c>
       <c r="D321" s="10" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E321" s="11" t="s">
         <v>200</v>
@@ -5148,7 +5155,7 @@
       <c r="C322" s="1"/>
       <c r="D322" s="10"/>
       <c r="E322" s="11" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F322" s="10" t="s">
         <v>9</v>
@@ -5164,7 +5171,7 @@
       <c r="C323" s="1"/>
       <c r="D323" s="10"/>
       <c r="E323" s="11" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F323" s="10" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Solve Bill_Fo api issue
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -730,9 +730,6 @@
     <t>Family_Add</t>
   </si>
   <si>
-    <t>UCC_Code</t>
-  </si>
-  <si>
     <t>SJ009</t>
   </si>
   <si>
@@ -773,9 +770,6 @@
   </si>
   <si>
     <t>selectedValue</t>
-  </si>
-  <si>
-    <t>ucC_Codes</t>
   </si>
   <si>
     <t>Journals                                         Trades                                 Receipts/Payments</t>
@@ -964,6 +958,12 @@
   </si>
   <si>
     <t>[ { "refNo": "4876", "date": "09/03/2021", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "1260.00", "credit": "0.00" }, { "refNo": "4595", "date": "25/02/2021", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "439.00", "credit": "0.00" }, { "refNo": "4525", "date": "22/02/2021", "particulars": "NSE F&amp;O Bill for 18/02/21", "debit": "36785.03", "credit": "0.00" }, { "refNo": "4539", "date": "22/02/2021", "particulars": "Dividend @ 3.75 on 5 shares of K.P.R. Mill Limited [532889]", "debit": "0.00", "credit": "18.75" }, { "refNo": "4540", "date": "22/02/2021", "particulars": "TDS on Dividend @ 3.75 on 5 shares of K.P.R. Mill Limited [532889]", "debit": "1.41", "credit": "0.00" }, { "refNo": "4524", "date": "19/02/2021", "particulars": "REVERSAL OF NSE F&amp;O Bill for 18/02/21", "debit": "0.00", "credit": "36785.03" }, { "refNo": "4429", "date": "13/02/2021", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "1657.00", "credit": "0.00" }, { "refNo": "4248", "date": "04/02/2021", "particulars": "None collection of STT recovered Dated 02/02/2021", "debit": "1.00", "credit": "0.00" }, { "refNo": "3615", "date": "10/12/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "1671.00", "credit": "0.00" }, { "refNo": "3356", "date": "23/11/2020", "particulars": "Dividend @ 17 on 12 shares of Ambuja Cements Limited [500425]", "debit": "0.00", "credit": "204.00" }, { "refNo": "3357", "date": "23/11/2020", "particulars": "TDS on Dividend @ 17 on 12 shares of Ambuja Cements Limited [500425]", "debit": "15.30", "credit": "0.00" }, { "refNo": "3265", "date": "17/11/2020", "particulars": "NSE F&amp;O Bill for 13/11/20", "debit": "0.00", "credit": "8724.69" }, { "refNo": "3264", "date": "14/11/2020", "particulars": "REVERSAL OF NSE F&amp;O Bill for 13/11/20", "debit": "8724.69", "credit": "0.00" }, { "refNo": "3231", "date": "12/11/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "949.00", "credit": "0.00" }, { "refNo": "3074", "date": "02/11/2020", "particulars": "NSE F&amp;O BILL DT. 29.10.20", "debit": "0.00", "credit": "154202.34" }, { "refNo": "3073", "date": "30/10/2020", "particulars": "REVERSAL OFF NSE &amp;O BILL DT. 29.10.20", "debit": "154202.34", "credit": "0.00" }, { "refNo": "2752", "date": "09/10/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "513.00", "credit": "0.00" }, { "refNo": "2442", "date": "22/09/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "697.00", "credit": "0.00" }, { "refNo": "2176", "date": "14/09/2020", "particulars": "None collection of STT recovered Dated 10/09/2020", "debit": "1.00", "credit": "0.00" }, { "refNo": "2128", "date": "09/09/2020", "particulars": "None collection of STT recovered Dated 07/09/2020", "debit": "1.00", "credit": "0.00" }, { "refNo": "1953", "date": "26/08/2020", "particulars": "Bal Trfd From NSE/FX", "debit": "0.00", "credit": "27827.46" }, { "refNo": "1952", "date": "26/08/2020", "particulars": "Bal Trfd to NSE/Cash", "debit": "27827.46", "credit": "0.00" }, { "refNo": "1719", "date": "10/08/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "142.00", "credit": "0.00" }, { "refNo": "1174", "date": "09/07/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "712.00", "credit": "0.00" }, { "refNo": "751", "date": "08/06/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "198.00", "credit": "0.00" }, { "refNo": "488", "date": "13/05/2020", "particulars": "Debit Balance of DP Services (1202870000086521)", "debit": "293.00", "credit": "0.00" }, { "refNo": "427", "date": "08/05/2020", "particulars": "NSE F&amp;O Bill for 06/05/20", "debit": "72263.05", "credit": "0.00" }, { "refNo": "426", "date": "07/05/2020", "particulars": "REVERSAL OF NSE F&amp;O Bill for 06/05/20", "debit": "0.00", "credit": "72263.05" } ]</t>
+  </si>
+  <si>
+    <t>uccCode</t>
+  </si>
+  <si>
+    <t>uccCodes</t>
   </si>
 </sst>
 </file>
@@ -1425,8 +1425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I338"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C218" workbookViewId="0">
-      <selection activeCell="D221" sqref="D221"/>
+    <sheetView tabSelected="1" topLeftCell="C214" workbookViewId="0">
+      <selection activeCell="E230" sqref="E230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1870,7 +1870,7 @@
     <row r="40" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D40" s="9"/>
       <c r="E40" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="F40" t="s">
         <v>9</v>
@@ -2305,7 +2305,7 @@
         <v>225</v>
       </c>
       <c r="I88" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="89" spans="2:9" x14ac:dyDescent="0.3">
@@ -2332,7 +2332,7 @@
         <v>225</v>
       </c>
       <c r="I90" s="22" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="91" spans="2:9" x14ac:dyDescent="0.3">
@@ -2447,7 +2447,7 @@
         <v>226</v>
       </c>
       <c r="I100" s="27" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.3">
@@ -2526,7 +2526,7 @@
     <row r="108" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D108" s="9"/>
       <c r="E108" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F108" s="1" t="s">
         <v>9</v>
@@ -2556,7 +2556,7 @@
         <v>162</v>
       </c>
       <c r="I110" s="22" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="111" spans="2:9" x14ac:dyDescent="0.3">
@@ -2612,7 +2612,7 @@
         <v>164</v>
       </c>
       <c r="I115" s="22" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="116" spans="2:9" x14ac:dyDescent="0.3">
@@ -2685,7 +2685,7 @@
         <v>170</v>
       </c>
       <c r="I122" s="22" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="123" spans="2:9" x14ac:dyDescent="0.3">
@@ -2852,10 +2852,10 @@
         <v>215</v>
       </c>
       <c r="D139" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="E139" s="10" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="F139" s="10" t="s">
         <v>22</v>
@@ -2864,7 +2864,7 @@
         <v>44</v>
       </c>
       <c r="I139" s="22" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
@@ -2905,7 +2905,7 @@
         <v>215</v>
       </c>
       <c r="D143" s="9" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E143" t="s">
         <v>155</v>
@@ -2917,7 +2917,7 @@
         <v>157</v>
       </c>
       <c r="I143" s="22" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="144" spans="2:9" x14ac:dyDescent="0.3">
@@ -2944,7 +2944,7 @@
         <v>22</v>
       </c>
       <c r="H145" s="17" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="146" spans="2:9" x14ac:dyDescent="0.3">
@@ -3217,16 +3217,16 @@
         <v>230</v>
       </c>
       <c r="E165" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="F165" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H165" t="s">
         <v>231</v>
       </c>
-      <c r="F165" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H165" t="s">
+      <c r="I165" s="22" t="s">
         <v>232</v>
-      </c>
-      <c r="I165" s="22" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="166" spans="2:9" x14ac:dyDescent="0.3">
@@ -3252,19 +3252,19 @@
         <v>184</v>
       </c>
       <c r="D168" s="10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E168" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="F168" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H168" t="s">
         <v>231</v>
       </c>
-      <c r="F168" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H168" t="s">
+      <c r="I168" s="22" t="s">
         <v>232</v>
-      </c>
-      <c r="I168" s="22" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="169" spans="2:9" x14ac:dyDescent="0.3">
@@ -3273,7 +3273,7 @@
     <row r="170" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D170" s="9"/>
       <c r="H170" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I170" s="22"/>
     </row>
@@ -3285,31 +3285,31 @@
         <v>184</v>
       </c>
       <c r="D171" s="10" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E171" s="11" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="F171" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H171" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="I171" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="172" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D172" s="9"/>
       <c r="H172" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="173" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D173" s="9"/>
       <c r="H173" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.3">
@@ -3323,31 +3323,31 @@
         <v>184</v>
       </c>
       <c r="D175" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="H175" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.3">
       <c r="E176" s="11" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="F176" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H176" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="177" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H177" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="178" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H178" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="180" spans="2:8" x14ac:dyDescent="0.3">
@@ -3358,31 +3358,31 @@
         <v>184</v>
       </c>
       <c r="D180" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="H180" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="181" spans="2:8" x14ac:dyDescent="0.3">
       <c r="E181" s="11" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="F181" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H181" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="182" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H182" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="183" spans="2:8" x14ac:dyDescent="0.3">
       <c r="H183" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="185" spans="2:8" x14ac:dyDescent="0.3">
@@ -3393,34 +3393,34 @@
         <v>184</v>
       </c>
       <c r="D185" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H185" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="186" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D186" s="9"/>
       <c r="E186" s="11" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="F186" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H186" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="187" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D187" s="9"/>
       <c r="H187" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="188" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D188" s="9"/>
       <c r="H188" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="189" spans="2:8" x14ac:dyDescent="0.3">
@@ -3434,17 +3434,17 @@
         <v>184</v>
       </c>
       <c r="D190" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="E190" s="8" t="s">
         <v>244</v>
-      </c>
-      <c r="E190" s="8" t="s">
-        <v>245</v>
       </c>
       <c r="F190" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G190" s="8"/>
       <c r="H190" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="191" spans="2:8" x14ac:dyDescent="0.3">
@@ -3485,8 +3485,8 @@
       <c r="B193" s="8"/>
       <c r="C193" s="8"/>
       <c r="D193" s="28"/>
-      <c r="E193" s="8" t="s">
-        <v>246</v>
+      <c r="E193" s="11" t="s">
+        <v>306</v>
       </c>
       <c r="F193" s="8" t="s">
         <v>22</v>
@@ -3507,7 +3507,7 @@
     <row r="195" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D195" s="9"/>
       <c r="H195" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="196" spans="2:9" x14ac:dyDescent="0.3">
@@ -3524,7 +3524,7 @@
         <v>184</v>
       </c>
       <c r="D198" s="28" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E198" s="29" t="s">
         <v>30</v>
@@ -3534,7 +3534,7 @@
       </c>
       <c r="G198" s="8"/>
       <c r="H198" s="28" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="199" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -3545,7 +3545,7 @@
       </c>
       <c r="G199" s="8"/>
       <c r="H199" s="18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="200" spans="2:9" x14ac:dyDescent="0.3">
@@ -3593,37 +3593,37 @@
         <v>184</v>
       </c>
       <c r="D203" s="9" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H203" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I203" s="22" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="204" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D204" s="9"/>
       <c r="E204" s="11" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="F204" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H204" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="205" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D205" s="9"/>
       <c r="H205" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="206" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D206" s="9"/>
       <c r="H206" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="207" spans="2:9" x14ac:dyDescent="0.3">
@@ -3641,37 +3641,37 @@
         <v>184</v>
       </c>
       <c r="D208" s="9" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H208" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="I208" s="7" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="209" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D209" s="9"/>
       <c r="E209" s="11" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="F209" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H209" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="210" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D210" s="9"/>
       <c r="H210" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="211" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D211" s="9"/>
       <c r="H211" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="212" spans="2:9" x14ac:dyDescent="0.3">
@@ -3689,17 +3689,17 @@
         <v>184</v>
       </c>
       <c r="D213" s="30" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E213" s="8" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F213" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G213" s="8"/>
       <c r="H213" s="18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="I213" s="7"/>
     </row>
@@ -3718,7 +3718,7 @@
         <v>20200401</v>
       </c>
       <c r="I214" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="215" spans="2:9" x14ac:dyDescent="0.3">
@@ -3738,8 +3738,8 @@
     </row>
     <row r="216" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D216" s="9"/>
-      <c r="E216" s="8" t="s">
-        <v>246</v>
+      <c r="E216" s="11" t="s">
+        <v>306</v>
       </c>
       <c r="F216" s="8" t="s">
         <v>22</v>
@@ -3758,7 +3758,7 @@
     <row r="218" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D218" s="9"/>
       <c r="H218" s="18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="219" spans="2:9" x14ac:dyDescent="0.3">
@@ -3776,7 +3776,7 @@
         <v>184</v>
       </c>
       <c r="D220" s="25" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="E220" s="29" t="s">
         <v>30</v>
@@ -3786,10 +3786,10 @@
       </c>
       <c r="G220" s="8"/>
       <c r="H220" s="28" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="I220" s="7" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="221" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
@@ -3800,7 +3800,7 @@
       </c>
       <c r="G221" s="8"/>
       <c r="H221" s="18" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="222" spans="2:9" x14ac:dyDescent="0.3">
@@ -4086,7 +4086,7 @@
         <v>20191101</v>
       </c>
       <c r="I245" s="7" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="246" spans="1:9" x14ac:dyDescent="0.3">
@@ -4112,7 +4112,7 @@
         <v>123</v>
       </c>
       <c r="I247" s="22" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="248" spans="1:9" x14ac:dyDescent="0.3">
@@ -4156,7 +4156,7 @@
         <v>20200401</v>
       </c>
       <c r="I250" s="22" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="251" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
@@ -4184,7 +4184,7 @@
       <c r="C252" s="1"/>
       <c r="D252" s="10"/>
       <c r="E252" s="1" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F252" s="1" t="s">
         <v>9</v>
@@ -4226,7 +4226,7 @@
         <v>176</v>
       </c>
       <c r="I254" s="22" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="255" spans="1:9" x14ac:dyDescent="0.3">
@@ -4288,7 +4288,7 @@
         <v>178</v>
       </c>
       <c r="I259" s="22" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="260" spans="2:9" x14ac:dyDescent="0.3">
@@ -4326,7 +4326,7 @@
         <v>186</v>
       </c>
       <c r="D263" s="9" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E263" s="1" t="s">
         <v>14</v>
@@ -4377,7 +4377,7 @@
         <v>9</v>
       </c>
       <c r="H266" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="267" spans="2:9" x14ac:dyDescent="0.3">
@@ -4406,7 +4406,7 @@
         <v>20200401</v>
       </c>
       <c r="I268" s="22" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="269" spans="2:9" x14ac:dyDescent="0.3">
@@ -4452,7 +4452,7 @@
         <v>20200401</v>
       </c>
       <c r="I271" s="22" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="272" spans="2:9" x14ac:dyDescent="0.3">
@@ -4545,7 +4545,7 @@
         <v>20200401</v>
       </c>
       <c r="I278" s="22" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="279" spans="2:9" x14ac:dyDescent="0.3">
@@ -4590,7 +4590,7 @@
     <row r="282" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D282" s="9"/>
       <c r="E282" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F282" s="9" t="s">
         <v>22</v>
@@ -4626,7 +4626,7 @@
         <v>20200401</v>
       </c>
       <c r="I284" s="22" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="285" spans="2:9" x14ac:dyDescent="0.3">
@@ -4671,7 +4671,7 @@
         <v>20200401</v>
       </c>
       <c r="I287" s="22" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="288" spans="2:9" x14ac:dyDescent="0.3">
@@ -4692,7 +4692,7 @@
     <row r="289" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D289" s="9"/>
       <c r="E289" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F289" s="9" t="s">
         <v>22</v>
@@ -4728,14 +4728,14 @@
         <v>20220228</v>
       </c>
       <c r="I291" s="22" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="292" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C292" s="1"/>
       <c r="D292" s="9"/>
       <c r="E292" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="F292" s="9" t="s">
         <v>22</v>
@@ -4847,7 +4847,7 @@
       <c r="C300" s="1"/>
       <c r="D300" s="9"/>
       <c r="E300" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="F300" s="9" t="s">
         <v>22</v>
@@ -4880,7 +4880,7 @@
         <v>187</v>
       </c>
       <c r="D303" s="9" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E303" s="1"/>
       <c r="F303" s="1"/>
@@ -4908,16 +4908,16 @@
         <v>187</v>
       </c>
       <c r="D305" s="10" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E305" s="1"/>
       <c r="F305" s="1"/>
       <c r="G305" s="1"/>
       <c r="H305" s="12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="I305" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="306" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4938,10 +4938,10 @@
         <v>187</v>
       </c>
       <c r="D307" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="E307" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="E307" s="1" t="s">
-        <v>275</v>
       </c>
       <c r="F307" s="10" t="s">
         <v>22</v>
@@ -4951,7 +4951,7 @@
         <v>531733</v>
       </c>
       <c r="I307" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="308" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -4959,7 +4959,7 @@
       <c r="C308" s="1"/>
       <c r="D308" s="10"/>
       <c r="E308" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="F308" s="1" t="s">
         <v>22</v>
@@ -4988,30 +4988,30 @@
         <v>187</v>
       </c>
       <c r="D310" s="9" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E310" s="8" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="F310" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G310" s="8"/>
       <c r="H310" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="311" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D311" s="9"/>
       <c r="E311" s="8" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="F311" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G311" s="8"/>
       <c r="H311" s="18" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="312" spans="2:9" x14ac:dyDescent="0.3">
@@ -5025,10 +5025,10 @@
         <v>187</v>
       </c>
       <c r="D313" s="9" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E313" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F313" s="1" t="s">
         <v>9</v>
@@ -5043,7 +5043,7 @@
     <row r="314" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D314" s="9"/>
       <c r="E314" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F314" s="1" t="s">
         <v>9</v>
@@ -5065,10 +5065,10 @@
         <v>187</v>
       </c>
       <c r="D316" s="9" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E316" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F316" s="1" t="s">
         <v>9</v>
@@ -5080,7 +5080,7 @@
     <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D317" s="9"/>
       <c r="E317" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F317" s="1" t="s">
         <v>9</v>
@@ -5100,7 +5100,7 @@
         <v>216</v>
       </c>
       <c r="D319" s="10" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E319" s="11" t="s">
         <v>200</v>
@@ -5113,7 +5113,7 @@
         <v>48</v>
       </c>
       <c r="I319" s="22" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="320" spans="2:9" ht="18" x14ac:dyDescent="0.35">
@@ -5134,7 +5134,7 @@
         <v>216</v>
       </c>
       <c r="D321" s="10" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E321" s="11" t="s">
         <v>200</v>
@@ -5155,7 +5155,7 @@
       <c r="C322" s="1"/>
       <c r="D322" s="10"/>
       <c r="E322" s="11" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="F322" s="10" t="s">
         <v>9</v>
@@ -5171,7 +5171,7 @@
       <c r="C323" s="1"/>
       <c r="D323" s="10"/>
       <c r="E323" s="11" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F323" s="10" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
Change output paramter of Transaction_Summary
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="816" uniqueCount="316">
   <si>
     <t>TradeWebService</t>
   </si>
@@ -985,6 +985,12 @@
   </si>
   <si>
     <t>2 = Deliveries</t>
+  </si>
+  <si>
+    <t>20200401</t>
+  </si>
+  <si>
+    <t>20210331</t>
   </si>
 </sst>
 </file>
@@ -1446,8 +1452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I342"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="H113" sqref="H113"/>
+    <sheetView tabSelected="1" topLeftCell="C105" workbookViewId="0">
+      <selection activeCell="H118" sqref="H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2633,7 +2639,7 @@
         <v>9</v>
       </c>
       <c r="H116" s="17" t="s">
-        <v>123</v>
+        <v>314</v>
       </c>
     </row>
     <row r="117" spans="2:9" x14ac:dyDescent="0.3">
@@ -2645,7 +2651,7 @@
         <v>9</v>
       </c>
       <c r="H117" s="17" t="s">
-        <v>125</v>
+        <v>315</v>
       </c>
     </row>
     <row r="118" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
add parameter dictionary in excell sheet
</commit_message>
<xml_diff>
--- a/Docs/NewTrade Web Api.xlsx
+++ b/Docs/NewTrade Web Api.xlsx
@@ -1462,10 +1462,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I348"/>
+  <dimension ref="A1:I345"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+    <sheetView tabSelected="1" topLeftCell="A278" workbookViewId="0">
+      <selection activeCell="H296" sqref="H296"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2855,41 +2855,55 @@
     </row>
     <row r="135" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D135" s="9"/>
-      <c r="H135" s="17"/>
       <c r="I135" s="19"/>
     </row>
-    <row r="136" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D136" s="9"/>
-      <c r="H136" s="17"/>
-      <c r="I136" s="19"/>
+    <row r="136" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B136" t="s">
+        <v>160</v>
+      </c>
+      <c r="C136" t="s">
+        <v>215</v>
+      </c>
+      <c r="D136" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="I136" s="7" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="137" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D137" s="9"/>
-      <c r="H137" s="17"/>
-      <c r="I137" s="19"/>
     </row>
     <row r="138" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D138" s="9"/>
-      <c r="I138" s="19"/>
-    </row>
-    <row r="139" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B139" t="s">
-        <v>160</v>
-      </c>
-      <c r="C139" t="s">
+      <c r="B138" t="s">
+        <v>41</v>
+      </c>
+      <c r="C138" t="s">
         <v>215</v>
       </c>
-      <c r="D139" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="I139" s="7" t="s">
-        <v>153</v>
+      <c r="D138" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="E138" t="s">
+        <v>43</v>
+      </c>
+      <c r="F138" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="139" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D139" s="9"/>
+      <c r="E139" t="s">
+        <v>45</v>
+      </c>
+      <c r="F139" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="140" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D140" s="9"/>
     </row>
-    <row r="141" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B141" t="s">
         <v>41</v>
       </c>
@@ -2897,209 +2911,223 @@
         <v>215</v>
       </c>
       <c r="D141" s="9" t="s">
-        <v>42</v>
+        <v>154</v>
       </c>
       <c r="E141" t="s">
-        <v>43</v>
+        <v>155</v>
       </c>
       <c r="F141" t="s">
         <v>22</v>
+      </c>
+      <c r="H141" t="s">
+        <v>157</v>
+      </c>
+      <c r="I141" s="21" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="142" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
       <c r="E142" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="F142" t="s">
         <v>22</v>
+      </c>
+      <c r="G142" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H142">
+        <v>20210101</v>
       </c>
     </row>
     <row r="143" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D143" s="9"/>
-    </row>
-    <row r="144" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B144" t="s">
-        <v>41</v>
-      </c>
-      <c r="C144" t="s">
-        <v>215</v>
-      </c>
-      <c r="D144" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="E144" t="s">
-        <v>155</v>
-      </c>
-      <c r="F144" t="s">
-        <v>22</v>
-      </c>
-      <c r="H144" t="s">
-        <v>157</v>
-      </c>
-      <c r="I144" s="21" t="s">
-        <v>159</v>
-      </c>
+      <c r="E143" t="s">
+        <v>156</v>
+      </c>
+      <c r="F143" t="s">
+        <v>22</v>
+      </c>
+      <c r="H143" s="17" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="144" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D144" s="9"/>
     </row>
     <row r="145" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D145" s="9"/>
-      <c r="E145" t="s">
-        <v>21</v>
-      </c>
-      <c r="F145" t="s">
-        <v>22</v>
-      </c>
-      <c r="G145" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H145">
-        <v>20210101</v>
-      </c>
-    </row>
-    <row r="146" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D146" s="9"/>
-      <c r="E146" t="s">
-        <v>156</v>
-      </c>
-      <c r="F146" t="s">
-        <v>22</v>
-      </c>
-      <c r="H146" s="17" t="s">
-        <v>158</v>
+      <c r="E145" s="1"/>
+      <c r="F145" s="1"/>
+      <c r="H145" s="3"/>
+    </row>
+    <row r="146" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B146" t="s">
+        <v>41</v>
+      </c>
+      <c r="C146" t="s">
+        <v>215</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="E146" s="10" t="s">
+        <v>263</v>
+      </c>
+      <c r="F146" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H146" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I146" s="22" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="147" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D147" s="9"/>
+      <c r="E147" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F147" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H147" s="3">
+        <v>20210101</v>
+      </c>
     </row>
     <row r="148" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D148" s="9"/>
-      <c r="E148" s="1"/>
-      <c r="F148" s="1"/>
-      <c r="H148" s="3"/>
-    </row>
-    <row r="149" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B149" t="s">
+      <c r="E148" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F148" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H148" s="3">
+        <v>20210101</v>
+      </c>
+    </row>
+    <row r="149" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D149" s="9"/>
+      <c r="E149" s="1"/>
+      <c r="F149" s="1"/>
+      <c r="H149" s="3"/>
+    </row>
+    <row r="150" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B150" t="s">
         <v>41</v>
       </c>
-      <c r="C149" t="s">
+      <c r="C150" t="s">
         <v>215</v>
       </c>
-      <c r="D149" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="E149" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="F149" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H149" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="I149" s="22" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="150" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D150" s="9"/>
-      <c r="E150" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F150" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H150" s="3">
-        <v>20210101</v>
+      <c r="D150" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="E150" t="s">
+        <v>155</v>
+      </c>
+      <c r="F150" t="s">
+        <v>22</v>
+      </c>
+      <c r="H150" t="s">
+        <v>157</v>
+      </c>
+      <c r="I150" s="22" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="151" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D151" s="9"/>
-      <c r="E151" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F151" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H151" s="3">
+      <c r="E151" t="s">
+        <v>21</v>
+      </c>
+      <c r="F151" t="s">
+        <v>22</v>
+      </c>
+      <c r="G151" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H151">
         <v>20210101</v>
       </c>
     </row>
     <row r="152" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D152" s="9"/>
-      <c r="E152" s="1"/>
-      <c r="F152" s="1"/>
-      <c r="H152" s="3"/>
-    </row>
-    <row r="153" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B153" t="s">
-        <v>41</v>
-      </c>
-      <c r="C153" t="s">
-        <v>215</v>
-      </c>
-      <c r="D153" s="9" t="s">
-        <v>264</v>
-      </c>
-      <c r="E153" t="s">
-        <v>155</v>
-      </c>
-      <c r="F153" t="s">
-        <v>22</v>
-      </c>
-      <c r="H153" t="s">
-        <v>157</v>
-      </c>
-      <c r="I153" s="22" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="154" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D154" s="9"/>
-      <c r="E154" t="s">
-        <v>21</v>
-      </c>
-      <c r="F154" t="s">
-        <v>22</v>
-      </c>
-      <c r="G154" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H154">
-        <v>20210101</v>
+      <c r="E152" t="s">
+        <v>156</v>
+      </c>
+      <c r="F152" t="s">
+        <v>22</v>
+      </c>
+      <c r="H152" s="17" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="153" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D153" s="9"/>
+    </row>
+    <row r="154" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B154" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C154" t="s">
+        <v>184</v>
+      </c>
+      <c r="D154" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="E154" s="1"/>
+      <c r="F154" s="1"/>
+      <c r="G154" s="1"/>
+      <c r="H154" s="3"/>
+      <c r="I154" s="7" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="155" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D155" s="9"/>
-      <c r="E155" t="s">
-        <v>156</v>
-      </c>
-      <c r="F155" t="s">
-        <v>22</v>
-      </c>
-      <c r="H155" s="17" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="156" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D156" s="9"/>
-    </row>
-    <row r="157" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B157" s="1" t="s">
+    </row>
+    <row r="156" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B156" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C157" t="s">
+      <c r="C156" t="s">
         <v>184</v>
       </c>
-      <c r="D157" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E157" s="1"/>
-      <c r="F157" s="1"/>
+      <c r="D156" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F156" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G156" s="1"/>
+      <c r="H156" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I156" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="157" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F157" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="G157" s="1"/>
-      <c r="H157" s="3"/>
-      <c r="I157" s="7" t="s">
-        <v>54</v>
-      </c>
+      <c r="H157" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I157" s="1"/>
     </row>
     <row r="158" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D158" s="9"/>
@@ -3112,7 +3140,7 @@
         <v>184</v>
       </c>
       <c r="D159" s="10" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="E159" s="1" t="s">
         <v>56</v>
@@ -3122,10 +3150,10 @@
       </c>
       <c r="G159" s="1"/>
       <c r="H159" s="3" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="I159" s="7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="160" spans="2:9" x14ac:dyDescent="0.3">
@@ -3145,209 +3173,204 @@
       <c r="I160" s="1"/>
     </row>
     <row r="161" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D161" s="9"/>
-    </row>
-    <row r="162" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B162" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C162" t="s">
-        <v>184</v>
-      </c>
-      <c r="D162" s="10" t="s">
-        <v>61</v>
-      </c>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F161" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G161" s="1"/>
+      <c r="H161" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I161" s="1"/>
+    </row>
+    <row r="162" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B162" s="1"/>
+      <c r="C162" s="1"/>
+      <c r="D162" s="10"/>
       <c r="E162" s="1" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="F162" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G162" s="1"/>
-      <c r="H162" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I162" s="7" t="s">
-        <v>62</v>
-      </c>
+      <c r="G162" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H162" s="3">
+        <v>20200401</v>
+      </c>
+      <c r="I162" s="1"/>
     </row>
     <row r="163" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
       <c r="D163" s="10"/>
       <c r="E163" s="1" t="s">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="F163" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G163" s="1"/>
-      <c r="H163" s="3" t="s">
-        <v>60</v>
+      <c r="G163" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H163" s="3">
+        <v>20210331</v>
       </c>
       <c r="I163" s="1"/>
     </row>
     <row r="164" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B164" s="1"/>
-      <c r="C164" s="1"/>
-      <c r="D164" s="10"/>
-      <c r="E164" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F164" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G164" s="1"/>
-      <c r="H164" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I164" s="1"/>
-    </row>
-    <row r="165" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B165" s="1"/>
-      <c r="C165" s="1"/>
-      <c r="D165" s="10"/>
+      <c r="D164" s="9"/>
+    </row>
+    <row r="165" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B165" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C165" t="s">
+        <v>184</v>
+      </c>
+      <c r="D165" s="10" t="s">
+        <v>64</v>
+      </c>
       <c r="E165" s="1" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="F165" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="G165" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H165" s="3">
-        <v>20200401</v>
-      </c>
-      <c r="I165" s="1"/>
+      <c r="G165" s="1"/>
+      <c r="H165" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="I165" s="7" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="166" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
       <c r="D166" s="10"/>
       <c r="E166" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F166" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G166" s="1"/>
+      <c r="H166" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I166" s="1"/>
+    </row>
+    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B167" s="1"/>
+      <c r="C167" s="1"/>
+      <c r="D167" s="10"/>
+      <c r="E167" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F167" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G167" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H167" s="3">
+        <v>20200401</v>
+      </c>
+      <c r="I167" s="1"/>
+    </row>
+    <row r="168" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B168" s="1"/>
+      <c r="C168" s="1"/>
+      <c r="D168" s="10"/>
+      <c r="E168" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F166" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G166" s="1" t="s">
+      <c r="F168" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G168" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H166" s="3">
+      <c r="H168" s="3">
         <v>20210331</v>
       </c>
-      <c r="I166" s="1"/>
-    </row>
-    <row r="167" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D167" s="9"/>
-    </row>
-    <row r="168" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B168" s="1" t="s">
+      <c r="I168" s="1"/>
+    </row>
+    <row r="169" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D169" s="9"/>
+      <c r="F169" s="10"/>
+    </row>
+    <row r="170" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B170" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C168" t="s">
+      <c r="C170" t="s">
         <v>184</v>
       </c>
-      <c r="D168" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E168" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F168" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G168" s="1"/>
-      <c r="H168" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I168" s="7" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="169" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B169" s="1"/>
-      <c r="C169" s="1"/>
-      <c r="D169" s="10"/>
-      <c r="E169" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F169" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G169" s="1"/>
-      <c r="H169" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="I169" s="1"/>
-    </row>
-    <row r="170" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B170" s="1"/>
-      <c r="C170" s="1"/>
-      <c r="D170" s="10"/>
-      <c r="E170" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F170" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G170" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H170" s="3">
-        <v>20200401</v>
-      </c>
-      <c r="I170" s="1"/>
+      <c r="D170" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="I170" s="22" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="171" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B171" s="1"/>
-      <c r="C171" s="1"/>
-      <c r="D171" s="10"/>
-      <c r="E171" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F171" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G171" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H171" s="3">
-        <v>20210331</v>
-      </c>
-      <c r="I171" s="1"/>
-    </row>
-    <row r="172" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D172" s="9"/>
-      <c r="F172" s="10"/>
-    </row>
-    <row r="173" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B173" s="1" t="s">
+      <c r="D171" s="9"/>
+    </row>
+    <row r="172" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B172" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C173" t="s">
+      <c r="C172" t="s">
         <v>184</v>
       </c>
-      <c r="D173" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="I173" s="22" t="s">
-        <v>229</v>
+      <c r="D172" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="E172" s="11" t="s">
+        <v>305</v>
+      </c>
+      <c r="F172" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H172" t="s">
+        <v>231</v>
+      </c>
+      <c r="I172" s="22" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="173" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D173" s="9"/>
+      <c r="E173" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F173" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H173">
+        <v>1234</v>
       </c>
     </row>
     <row r="174" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D174" s="9"/>
     </row>
     <row r="175" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B175" s="1" t="s">
+      <c r="B175" t="s">
         <v>52</v>
       </c>
       <c r="C175" t="s">
         <v>184</v>
       </c>
       <c r="D175" s="10" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="E175" s="11" t="s">
         <v>305</v>
@@ -3364,18 +3387,13 @@
     </row>
     <row r="176" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D176" s="9"/>
-      <c r="E176" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F176" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H176">
-        <v>1234</v>
-      </c>
-    </row>
-    <row r="177" spans="2:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="177" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D177" s="9"/>
+      <c r="H177" t="s">
+        <v>235</v>
+      </c>
+      <c r="I177" s="22"/>
     </row>
     <row r="178" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B178" t="s">
@@ -3385,646 +3403,636 @@
         <v>184</v>
       </c>
       <c r="D178" s="10" t="s">
-        <v>233</v>
+        <v>239</v>
       </c>
       <c r="E178" s="11" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F178" s="1" t="s">
         <v>9</v>
       </c>
       <c r="H178" t="s">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="I178" s="22" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
     </row>
     <row r="179" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D179" s="9"/>
-    </row>
-    <row r="180" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="H179" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="180" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D180" s="9"/>
       <c r="H180" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D181" s="9"/>
+    </row>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B182" t="s">
+        <v>52</v>
+      </c>
+      <c r="C182" t="s">
+        <v>184</v>
+      </c>
+      <c r="D182" t="s">
+        <v>240</v>
+      </c>
+      <c r="H182" t="s">
         <v>235</v>
       </c>
-      <c r="I180" s="22"/>
-    </row>
-    <row r="181" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B181" t="s">
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E183" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F183" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H183" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="184" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H184" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H185" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B187" t="s">
         <v>52</v>
       </c>
-      <c r="C181" t="s">
+      <c r="C187" t="s">
         <v>184</v>
       </c>
-      <c r="D181" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="E181" s="11" t="s">
+      <c r="D187" t="s">
+        <v>241</v>
+      </c>
+      <c r="H187" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="188" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E188" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="F181" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H181" t="s">
+      <c r="F188" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H188" t="s">
         <v>236</v>
       </c>
-      <c r="I181" s="22" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="182" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D182" s="9"/>
-      <c r="H182" t="s">
+    </row>
+    <row r="189" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H189" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="183" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D183" s="9"/>
-      <c r="H183" t="s">
+    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H190" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="184" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D184" s="9"/>
-    </row>
-    <row r="185" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B185" t="s">
+    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B192" t="s">
         <v>52</v>
       </c>
-      <c r="C185" t="s">
+      <c r="C192" t="s">
         <v>184</v>
       </c>
-      <c r="D185" t="s">
-        <v>240</v>
-      </c>
-      <c r="H185" t="s">
+      <c r="D192" t="s">
+        <v>242</v>
+      </c>
+      <c r="H192" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="186" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E186" s="11" t="s">
+    <row r="193" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D193" s="9"/>
+      <c r="E193" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="F186" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H186" t="s">
+      <c r="F193" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H193" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="187" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H187" t="s">
+    <row r="194" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D194" s="9"/>
+      <c r="H194" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="188" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H188" t="s">
+    <row r="195" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D195" s="9"/>
+      <c r="H195" t="s">
         <v>238</v>
-      </c>
-    </row>
-    <row r="190" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B190" t="s">
-        <v>52</v>
-      </c>
-      <c r="C190" t="s">
-        <v>184</v>
-      </c>
-      <c r="D190" t="s">
-        <v>241</v>
-      </c>
-      <c r="H190" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="191" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E191" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="F191" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H191" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="192" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H192" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="193" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="H193" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="195" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B195" t="s">
-        <v>52</v>
-      </c>
-      <c r="C195" t="s">
-        <v>184</v>
-      </c>
-      <c r="D195" t="s">
-        <v>242</v>
-      </c>
-      <c r="H195" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="196" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D196" s="9"/>
-      <c r="E196" s="11" t="s">
+    </row>
+    <row r="197" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B197" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C197" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D197" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="E197" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="F197" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G197" s="8"/>
+      <c r="H197" s="18" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="198" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B198" s="8"/>
+      <c r="C198" s="8"/>
+      <c r="D198" s="28"/>
+      <c r="E198" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F198" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G198" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H198" s="3">
+        <v>20200401</v>
+      </c>
+    </row>
+    <row r="199" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B199" s="8"/>
+      <c r="C199" s="8"/>
+      <c r="D199" s="28"/>
+      <c r="E199" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F199" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G199" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H199" s="3">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="200" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B200" s="8"/>
+      <c r="C200" s="8"/>
+      <c r="D200" s="28"/>
+      <c r="E200" s="11" t="s">
         <v>306</v>
       </c>
-      <c r="F196" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H196" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="197" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D197" s="9"/>
-      <c r="H197" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="198" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D198" s="9"/>
-      <c r="H198" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="199" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="D199" s="9"/>
-    </row>
-    <row r="200" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B200" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C200" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D200" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="E200" s="8" t="s">
-        <v>244</v>
-      </c>
       <c r="F200" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G200" s="8"/>
-      <c r="H200" s="18" t="s">
-        <v>245</v>
+      <c r="H200" s="8" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B201" s="8"/>
       <c r="C201" s="8"/>
       <c r="D201" s="28"/>
-      <c r="E201" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F201" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G201" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H201" s="3">
-        <v>20200401</v>
-      </c>
-    </row>
-    <row r="202" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B202" s="8"/>
-      <c r="C202" s="8"/>
-      <c r="D202" s="28"/>
-      <c r="E202" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F202" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G202" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H202" s="3">
-        <v>20210331</v>
+      <c r="E201" s="8"/>
+      <c r="F201" s="8"/>
+      <c r="G201" s="8"/>
+    </row>
+    <row r="202" spans="2:8" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="D202" s="9"/>
+      <c r="H202" s="18" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="203" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B203" s="8"/>
-      <c r="C203" s="8"/>
-      <c r="D203" s="28"/>
-      <c r="E203" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="F203" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G203" s="8"/>
-      <c r="H203" s="8" t="s">
-        <v>10</v>
-      </c>
+      <c r="D203" s="9"/>
     </row>
     <row r="204" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B204" s="8"/>
-      <c r="C204" s="8"/>
-      <c r="D204" s="28"/>
-      <c r="E204" s="8"/>
-      <c r="F204" s="8"/>
-      <c r="G204" s="8"/>
-    </row>
-    <row r="205" spans="2:8" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="D205" s="9"/>
-      <c r="H205" s="18" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="206" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D204" s="9"/>
+    </row>
+    <row r="205" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B205" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C205" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D205" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="E205" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F205" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="G205" s="8"/>
+      <c r="H205" s="28" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="206" spans="2:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D206" s="9"/>
+      <c r="E206" s="8"/>
+      <c r="F206" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G206" s="8"/>
+      <c r="H206" s="18" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="207" spans="2:8" x14ac:dyDescent="0.3">
       <c r="D207" s="9"/>
+      <c r="E207" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F207" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G207" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H207" s="3">
+        <v>20200401</v>
+      </c>
     </row>
     <row r="208" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B208" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C208" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D208" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="E208" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="F208" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G208" s="8"/>
-      <c r="H208" s="28" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="209" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D208" s="9"/>
+      <c r="E208" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F208" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G208" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H208" s="3">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="209" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D209" s="9"/>
       <c r="E209" s="8"/>
-      <c r="F209" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G209" s="8"/>
-      <c r="H209" s="18" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="210" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D210" s="9"/>
-      <c r="E210" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F210" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G210" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H210" s="3">
-        <v>20200401</v>
+      <c r="F209" s="8"/>
+      <c r="G209" s="1"/>
+      <c r="H209" s="3"/>
+    </row>
+    <row r="210" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B210" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C210" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D210" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="H210" t="s">
+        <v>235</v>
+      </c>
+      <c r="I210" s="22" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="211" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D211" s="9"/>
-      <c r="E211" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F211" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G211" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H211" s="3">
-        <v>20210331</v>
+      <c r="E211" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F211" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H211" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="212" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D212" s="9"/>
-      <c r="E212" s="8"/>
-      <c r="F212" s="8"/>
-      <c r="G212" s="1"/>
-      <c r="H212" s="3"/>
-    </row>
-    <row r="213" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B213" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C213" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D213" s="9" t="s">
-        <v>250</v>
-      </c>
+      <c r="H212" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="213" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D213" s="9"/>
       <c r="H213" t="s">
-        <v>235</v>
-      </c>
-      <c r="I213" s="22" t="s">
-        <v>301</v>
+        <v>238</v>
       </c>
     </row>
     <row r="214" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D214" s="9"/>
-      <c r="E214" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="F214" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H214" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="215" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D215" s="9"/>
+      <c r="E214" s="8"/>
+      <c r="F214" s="8"/>
+      <c r="G214" s="1"/>
+      <c r="H214" s="3"/>
+    </row>
+    <row r="215" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B215" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C215" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D215" s="9" t="s">
+        <v>251</v>
+      </c>
       <c r="H215" t="s">
-        <v>237</v>
+        <v>235</v>
+      </c>
+      <c r="I215" s="7" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="216" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D216" s="9"/>
+      <c r="E216" s="11" t="s">
+        <v>306</v>
+      </c>
+      <c r="F216" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="H216" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="217" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D217" s="9"/>
-      <c r="E217" s="8"/>
-      <c r="F217" s="8"/>
-      <c r="G217" s="1"/>
-      <c r="H217" s="3"/>
-    </row>
-    <row r="218" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B218" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C218" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D218" s="9" t="s">
-        <v>251</v>
-      </c>
+      <c r="H217" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="218" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D218" s="9"/>
       <c r="H218" t="s">
-        <v>235</v>
-      </c>
-      <c r="I218" s="7" t="s">
-        <v>302</v>
+        <v>238</v>
       </c>
     </row>
     <row r="219" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D219" s="9"/>
-      <c r="E219" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="F219" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H219" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="220" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D220" s="9"/>
-      <c r="H220" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="221" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E219" s="8"/>
+      <c r="F219" s="8"/>
+      <c r="G219" s="1"/>
+      <c r="H219" s="3"/>
+    </row>
+    <row r="220" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
+      <c r="B220" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C220" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D220" s="30" t="s">
+        <v>252</v>
+      </c>
+      <c r="E220" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="F220" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G220" s="8"/>
+      <c r="H220" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="I220" s="7"/>
+    </row>
+    <row r="221" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="D221" s="9"/>
-      <c r="H221" t="s">
-        <v>238</v>
+      <c r="E221" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F221" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G221" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H221" s="3">
+        <v>20200401</v>
+      </c>
+      <c r="I221" s="7" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="222" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D222" s="9"/>
-      <c r="E222" s="8"/>
-      <c r="F222" s="8"/>
-      <c r="G222" s="1"/>
-      <c r="H222" s="3"/>
-    </row>
-    <row r="223" spans="2:9" ht="43.8" x14ac:dyDescent="0.35">
-      <c r="B223" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C223" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D223" s="30" t="s">
-        <v>252</v>
-      </c>
-      <c r="E223" s="8" t="s">
-        <v>244</v>
+      <c r="E222" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F222" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G222" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H222" s="3">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="223" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D223" s="9"/>
+      <c r="E223" s="11" t="s">
+        <v>306</v>
       </c>
       <c r="F223" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G223" s="8"/>
-      <c r="H223" s="18" t="s">
-        <v>245</v>
-      </c>
-      <c r="I223" s="7"/>
-    </row>
-    <row r="224" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="H223" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="224" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D224" s="9"/>
-      <c r="E224" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F224" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G224" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H224" s="3">
-        <v>20200401</v>
-      </c>
-      <c r="I224" s="7" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="225" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E224" s="8"/>
+      <c r="F224" s="8"/>
+      <c r="G224" s="8"/>
+    </row>
+    <row r="225" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
       <c r="D225" s="9"/>
-      <c r="E225" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F225" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G225" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H225" s="3">
-        <v>20210331</v>
+      <c r="H225" s="18" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="226" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D226" s="9"/>
-      <c r="E226" s="11" t="s">
-        <v>306</v>
-      </c>
-      <c r="F226" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G226" s="8"/>
-      <c r="H226" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="227" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D227" s="9"/>
-      <c r="E227" s="8"/>
-      <c r="F227" s="8"/>
+      <c r="E226" s="8"/>
+      <c r="F226" s="8"/>
+      <c r="G226" s="1"/>
+      <c r="H226" s="3"/>
+    </row>
+    <row r="227" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B227" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C227" s="8" t="s">
+        <v>184</v>
+      </c>
+      <c r="D227" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="E227" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F227" s="28" t="s">
+        <v>22</v>
+      </c>
       <c r="G227" s="8"/>
-    </row>
-    <row r="228" spans="2:9" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="H227" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="I227" s="7" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="228" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="D228" s="9"/>
+      <c r="E228" s="8"/>
+      <c r="F228" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="G228" s="8"/>
       <c r="H228" s="18" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
     </row>
     <row r="229" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D229" s="9"/>
-      <c r="E229" s="8"/>
-      <c r="F229" s="8"/>
-      <c r="G229" s="1"/>
-      <c r="H229" s="3"/>
-    </row>
-    <row r="230" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B230" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C230" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D230" s="25" t="s">
-        <v>253</v>
-      </c>
-      <c r="E230" s="29" t="s">
-        <v>30</v>
-      </c>
-      <c r="F230" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="G230" s="8"/>
-      <c r="H230" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="I230" s="7" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="231" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E229" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F229" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G229" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H229" s="3">
+        <v>20200401</v>
+      </c>
+    </row>
+    <row r="230" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D230" s="9"/>
+      <c r="E230" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F230" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G230" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H230" s="3">
+        <v>20210331</v>
+      </c>
+    </row>
+    <row r="231" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D231" s="9"/>
       <c r="E231" s="8"/>
-      <c r="F231" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="G231" s="8"/>
-      <c r="H231" s="18" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="232" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D232" s="9"/>
-      <c r="E232" s="8" t="s">
+      <c r="F231" s="8"/>
+      <c r="G231" s="1"/>
+      <c r="H231" s="3"/>
+    </row>
+    <row r="232" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B232" t="s">
+        <v>69</v>
+      </c>
+      <c r="C232" t="s">
+        <v>185</v>
+      </c>
+      <c r="D232" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E232" t="s">
         <v>14</v>
       </c>
-      <c r="F232" s="8" t="s">
-        <v>22</v>
+      <c r="F232" t="s">
+        <v>9</v>
       </c>
       <c r="G232" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H232" s="3">
-        <v>20200401</v>
+      <c r="H232" s="6">
+        <v>20210401</v>
+      </c>
+      <c r="I232" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="233" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D233" s="9"/>
-      <c r="E233" s="8" t="s">
+      <c r="E233" t="s">
         <v>16</v>
       </c>
-      <c r="F233" s="8" t="s">
-        <v>22</v>
+      <c r="F233" t="s">
+        <v>9</v>
       </c>
       <c r="G233" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H233" s="3">
-        <v>20210331</v>
+      <c r="H233" s="6">
+        <v>20220112</v>
       </c>
     </row>
     <row r="234" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D234" s="9"/>
-      <c r="E234" s="8"/>
-      <c r="F234" s="8"/>
-      <c r="G234" s="1"/>
-      <c r="H234" s="3"/>
-    </row>
-    <row r="235" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B235" t="s">
+      <c r="E234" t="s">
+        <v>72</v>
+      </c>
+      <c r="F234" t="s">
+        <v>9</v>
+      </c>
+      <c r="H234" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D235" s="9"/>
+      <c r="H235" s="6"/>
+    </row>
+    <row r="236" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B236" t="s">
         <v>69</v>
       </c>
-      <c r="C235" t="s">
+      <c r="C236" t="s">
         <v>185</v>
       </c>
-      <c r="D235" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E235" t="s">
-        <v>14</v>
-      </c>
-      <c r="F235" t="s">
-        <v>9</v>
-      </c>
-      <c r="G235" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H235" s="6">
-        <v>20210401</v>
-      </c>
-      <c r="I235" s="7" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="236" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D236" s="9"/>
-      <c r="E236" t="s">
-        <v>16</v>
-      </c>
-      <c r="F236" t="s">
-        <v>9</v>
-      </c>
-      <c r="G236" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H236" s="6">
-        <v>20220112</v>
+      <c r="D236" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="H236" s="6"/>
+      <c r="I236" s="7" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="237" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D237" s="9"/>
-      <c r="E237" t="s">
-        <v>72</v>
-      </c>
-      <c r="F237" t="s">
-        <v>9</v>
-      </c>
-      <c r="H237" s="6">
-        <v>0</v>
-      </c>
+      <c r="H237" s="6"/>
     </row>
     <row r="238" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D238" s="9"/>
@@ -4038,11 +4046,11 @@
         <v>185</v>
       </c>
       <c r="D239" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H239" s="6"/>
       <c r="I239" s="7" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="240" spans="2:9" x14ac:dyDescent="0.3">
@@ -4061,11 +4069,11 @@
         <v>185</v>
       </c>
       <c r="D242" s="9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H242" s="6"/>
       <c r="I242" s="7" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="243" spans="2:9" x14ac:dyDescent="0.3">
@@ -4084,16 +4092,32 @@
         <v>185</v>
       </c>
       <c r="D245" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="H245" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="E245" t="s">
+        <v>80</v>
+      </c>
+      <c r="F245" t="s">
+        <v>81</v>
+      </c>
+      <c r="H245" s="6" t="b">
+        <v>0</v>
+      </c>
       <c r="I245" s="7" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
     </row>
     <row r="246" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D246" s="9"/>
-      <c r="H246" s="6"/>
+      <c r="E246" t="s">
+        <v>83</v>
+      </c>
+      <c r="F246" t="s">
+        <v>81</v>
+      </c>
+      <c r="H246" s="6" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="247" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D247" s="9"/>
@@ -4107,414 +4131,421 @@
         <v>185</v>
       </c>
       <c r="D248" s="9" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E248" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F248" t="s">
-        <v>81</v>
-      </c>
-      <c r="H248" s="6" t="b">
-        <v>0</v>
+        <v>20</v>
+      </c>
+      <c r="H248" s="6">
+        <v>3</v>
       </c>
       <c r="I248" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="249" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D249" s="9"/>
-      <c r="E249" t="s">
-        <v>83</v>
-      </c>
-      <c r="F249" t="s">
-        <v>81</v>
-      </c>
-      <c r="H249" s="6" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D250" s="9"/>
-      <c r="H250" s="6"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="249" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B249" s="1"/>
+      <c r="C249" s="1"/>
+      <c r="D249" s="10"/>
+      <c r="E249" s="1"/>
+      <c r="F249" s="1"/>
+      <c r="G249" s="1"/>
+      <c r="H249" s="3"/>
+      <c r="I249" s="13"/>
+    </row>
+    <row r="250" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B250" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C250" t="s">
+        <v>216</v>
+      </c>
+      <c r="D250" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E250" s="1"/>
+      <c r="F250" s="10"/>
+      <c r="G250" s="1"/>
+      <c r="H250" s="3"/>
+      <c r="I250" s="7" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="251" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B251" t="s">
-        <v>69</v>
-      </c>
-      <c r="C251" t="s">
-        <v>185</v>
-      </c>
-      <c r="D251" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="E251" t="s">
-        <v>85</v>
-      </c>
-      <c r="F251" t="s">
-        <v>20</v>
-      </c>
-      <c r="H251" s="6">
-        <v>3</v>
-      </c>
-      <c r="I251" s="7" t="s">
-        <v>86</v>
-      </c>
+      <c r="B251" s="1"/>
+      <c r="C251" s="1"/>
+      <c r="D251" s="10"/>
+      <c r="E251" s="1"/>
+      <c r="F251" s="1"/>
+      <c r="G251" s="1"/>
+      <c r="H251" s="3"/>
+      <c r="I251" s="13"/>
     </row>
     <row r="252" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B252" s="1"/>
-      <c r="C252" s="1"/>
-      <c r="D252" s="10"/>
-      <c r="E252" s="1"/>
-      <c r="F252" s="1"/>
-      <c r="G252" s="1"/>
-      <c r="H252" s="3"/>
-      <c r="I252" s="13"/>
-    </row>
-    <row r="253" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B253" s="1" t="s">
+      <c r="B252" t="s">
         <v>46</v>
       </c>
-      <c r="C253" t="s">
+      <c r="C252" t="s">
         <v>216</v>
       </c>
-      <c r="D253" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E253" s="1"/>
-      <c r="F253" s="10"/>
-      <c r="G253" s="1"/>
-      <c r="H253" s="3"/>
-      <c r="I253" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="254" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B254" s="1"/>
-      <c r="C254" s="1"/>
-      <c r="D254" s="10"/>
-      <c r="E254" s="1"/>
-      <c r="F254" s="1"/>
-      <c r="G254" s="1"/>
-      <c r="H254" s="3"/>
-      <c r="I254" s="13"/>
-    </row>
-    <row r="255" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B255" t="s">
+      <c r="D252" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C255" t="s">
-        <v>216</v>
-      </c>
-      <c r="D255" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E255" s="11" t="s">
+      <c r="E252" s="11" t="s">
         <v>21</v>
       </c>
+      <c r="F252" t="s">
+        <v>9</v>
+      </c>
+      <c r="H252" s="8">
+        <v>20191101</v>
+      </c>
+      <c r="I252" s="7" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="253" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D253" s="9"/>
+    </row>
+    <row r="254" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B254" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C254" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D254" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E254" t="s">
+        <v>14</v>
+      </c>
+      <c r="F254" t="s">
+        <v>9</v>
+      </c>
+      <c r="H254" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="I254" s="22" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="255" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D255" s="9"/>
+      <c r="E255" t="s">
+        <v>16</v>
+      </c>
       <c r="F255" t="s">
         <v>9</v>
       </c>
-      <c r="H255" s="8">
-        <v>20191101</v>
-      </c>
-      <c r="I255" s="7" t="s">
-        <v>254</v>
+      <c r="H255" s="31" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="256" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D256" s="9"/>
     </row>
-    <row r="257" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A257" s="1">
+        <v>36</v>
+      </c>
       <c r="B257" s="1" t="s">
         <v>180</v>
       </c>
       <c r="C257" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D257" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E257" t="s">
+      <c r="D257" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="E257" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F257" t="s">
-        <v>9</v>
-      </c>
-      <c r="H257" s="31" t="s">
+      <c r="F257" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G257" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H257" s="15">
+        <v>20200401</v>
+      </c>
+      <c r="I257" s="22" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A258" s="1"/>
+      <c r="B258" s="1"/>
+      <c r="C258" s="1"/>
+      <c r="D258" s="10"/>
+      <c r="E258" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F258" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G258" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H258" s="6">
+        <v>20210331</v>
+      </c>
+      <c r="I258" s="1"/>
+    </row>
+    <row r="259" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A259" s="1"/>
+      <c r="B259" s="1"/>
+      <c r="C259" s="1"/>
+      <c r="D259" s="10"/>
+      <c r="E259" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="F259" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G259" s="1"/>
+      <c r="H259" s="3">
+        <v>533271</v>
+      </c>
+      <c r="I259" s="13"/>
+    </row>
+    <row r="260" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A260" s="1"/>
+      <c r="B260" s="1"/>
+      <c r="C260" s="1"/>
+      <c r="D260" s="10"/>
+      <c r="E260" s="1"/>
+      <c r="F260" s="1"/>
+      <c r="G260" s="1"/>
+      <c r="H260" s="3"/>
+      <c r="I260" s="13"/>
+    </row>
+    <row r="261" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B261" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C261" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D261" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E261" t="s">
+        <v>25</v>
+      </c>
+      <c r="F261" t="s">
+        <v>9</v>
+      </c>
+      <c r="H261" t="s">
+        <v>176</v>
+      </c>
+      <c r="I261" s="22" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D262" s="9"/>
+      <c r="E262" t="s">
+        <v>40</v>
+      </c>
+      <c r="F262" t="s">
+        <v>9</v>
+      </c>
+      <c r="H262" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D263" s="9"/>
+      <c r="E263" t="s">
+        <v>14</v>
+      </c>
+      <c r="F263" t="s">
+        <v>9</v>
+      </c>
+      <c r="H263" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="I257" s="22" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D258" s="9"/>
-      <c r="E258" t="s">
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D264" s="9"/>
+      <c r="E264" t="s">
         <v>16</v>
       </c>
-      <c r="F258" t="s">
-        <v>9</v>
-      </c>
-      <c r="H258" s="31" t="s">
+      <c r="F264" t="s">
+        <v>9</v>
+      </c>
+      <c r="H264" s="17" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D259" s="9"/>
-    </row>
-    <row r="260" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A260" s="1">
-        <v>36</v>
-      </c>
-      <c r="B260" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C260" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D260" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F260" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G260" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H260" s="15">
-        <v>20200401</v>
-      </c>
-      <c r="I260" s="22" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="261" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A261" s="1"/>
-      <c r="B261" s="1"/>
-      <c r="C261" s="1"/>
-      <c r="D261" s="10"/>
-      <c r="E261" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F261" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G261" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H261" s="6">
-        <v>20210331</v>
-      </c>
-      <c r="I261" s="1"/>
-    </row>
-    <row r="262" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A262" s="1"/>
-      <c r="B262" s="1"/>
-      <c r="C262" s="1"/>
-      <c r="D262" s="10"/>
-      <c r="E262" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F262" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G262" s="1"/>
-      <c r="H262" s="3">
-        <v>533271</v>
-      </c>
-      <c r="I262" s="13"/>
-    </row>
-    <row r="263" spans="1:9" ht="19.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A263" s="1"/>
-      <c r="B263" s="1"/>
-      <c r="C263" s="1"/>
-      <c r="D263" s="10"/>
-      <c r="E263" s="1"/>
-      <c r="F263" s="1"/>
-      <c r="G263" s="1"/>
-      <c r="H263" s="3"/>
-      <c r="I263" s="13"/>
-    </row>
-    <row r="264" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B264" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C264" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D264" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="E264" t="s">
-        <v>25</v>
-      </c>
-      <c r="F264" t="s">
-        <v>9</v>
-      </c>
-      <c r="H264" t="s">
-        <v>176</v>
-      </c>
-      <c r="I264" s="22" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D265" s="9"/>
-      <c r="E265" t="s">
-        <v>40</v>
-      </c>
-      <c r="F265" t="s">
-        <v>9</v>
-      </c>
-      <c r="H265" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D266" s="9"/>
+    </row>
+    <row r="266" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B266" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C266" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D266" s="9" t="s">
+        <v>182</v>
+      </c>
       <c r="E266" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="F266" t="s">
         <v>9</v>
       </c>
-      <c r="H266" s="17" t="s">
-        <v>123</v>
+      <c r="H266" t="s">
+        <v>178</v>
+      </c>
+      <c r="I266" s="22" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D267" s="9"/>
       <c r="E267" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="F267" t="s">
         <v>9</v>
       </c>
       <c r="H267" s="17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D268" s="9"/>
-    </row>
-    <row r="269" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B269" s="1" t="s">
+      <c r="E268" t="s">
+        <v>16</v>
+      </c>
+      <c r="F268" t="s">
+        <v>9</v>
+      </c>
+      <c r="H268" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D269" s="9"/>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B270" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="C269" s="1" t="s">
+      <c r="C270" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D269" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="E269" t="s">
-        <v>25</v>
-      </c>
-      <c r="F269" t="s">
-        <v>9</v>
-      </c>
-      <c r="H269" t="s">
-        <v>178</v>
-      </c>
-      <c r="I269" s="22" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="D270" s="9"/>
-      <c r="E270" t="s">
+      <c r="D270" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="E270" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F270" t="s">
-        <v>9</v>
-      </c>
-      <c r="H270" s="17" t="s">
-        <v>123</v>
+      <c r="F270" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G270" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H270" s="15">
+        <v>20200401</v>
       </c>
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D271" s="9"/>
-      <c r="E271" t="s">
+      <c r="E271" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F271" t="s">
-        <v>9</v>
-      </c>
-      <c r="H271" s="17" t="s">
-        <v>125</v>
+      <c r="F271" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G271" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H271" s="6">
+        <v>20210331</v>
       </c>
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.3">
       <c r="D272" s="9"/>
+      <c r="E272" t="s">
+        <v>25</v>
+      </c>
+      <c r="F272" t="s">
+        <v>9</v>
+      </c>
+      <c r="H272" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="273" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B273" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="C273" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D273" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="E273" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F273" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G273" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H273" s="15">
-        <v>20200401</v>
+      <c r="D273" s="9"/>
+      <c r="E273" t="s">
+        <v>40</v>
+      </c>
+      <c r="F273" t="s">
+        <v>9</v>
+      </c>
+      <c r="H273" t="s">
+        <v>292</v>
       </c>
     </row>
     <row r="274" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D274" s="9"/>
-      <c r="E274" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F274" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G274" s="1" t="s">
+    </row>
+    <row r="275" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B275" t="s">
+        <v>90</v>
+      </c>
+      <c r="C275" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D275" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E275" t="s">
+        <v>14</v>
+      </c>
+      <c r="F275" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G275" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H274" s="6">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="275" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D275" s="9"/>
-      <c r="E275" t="s">
-        <v>25</v>
-      </c>
-      <c r="F275" t="s">
-        <v>9</v>
-      </c>
-      <c r="H275" t="s">
-        <v>26</v>
+      <c r="H275" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I275" s="22" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="276" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D276" s="9"/>
       <c r="E276" t="s">
-        <v>40</v>
-      </c>
-      <c r="F276" t="s">
-        <v>9</v>
-      </c>
-      <c r="H276" t="s">
-        <v>292</v>
+        <v>16</v>
+      </c>
+      <c r="F276" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G276" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H276" s="8">
+        <v>20210331</v>
       </c>
     </row>
     <row r="277" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D277" s="9"/>
+      <c r="F277" s="9"/>
+      <c r="H277" s="8"/>
     </row>
     <row r="278" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B278" t="s">
@@ -4524,7 +4555,7 @@
         <v>186</v>
       </c>
       <c r="D278" s="9" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E278" t="s">
         <v>14</v>
@@ -4539,7 +4570,7 @@
         <v>20200401</v>
       </c>
       <c r="I278" s="22" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="279" spans="2:9" x14ac:dyDescent="0.3">
@@ -4559,177 +4590,176 @@
     </row>
     <row r="280" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D280" s="9"/>
-      <c r="F280" s="9"/>
-      <c r="H280" s="8"/>
-    </row>
-    <row r="281" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B281" t="s">
-        <v>90</v>
-      </c>
-      <c r="C281" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D281" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="E280" t="s">
+        <v>93</v>
+      </c>
+      <c r="F280" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="H280" s="8" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="281" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D281" s="9"/>
       <c r="E281" t="s">
-        <v>14</v>
+        <v>95</v>
       </c>
       <c r="F281" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G281" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H281" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I281" s="22" t="s">
-        <v>286</v>
+        <v>81</v>
+      </c>
+      <c r="H281" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="282" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D282" s="9"/>
       <c r="E282" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="F282" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G282" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H282" s="8">
-        <v>20210331</v>
+        <v>81</v>
+      </c>
+      <c r="H282" s="8" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="283" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D283" s="9"/>
       <c r="E283" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="F283" s="9" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="H283" s="8" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="284" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D284" s="9"/>
-      <c r="E284" t="s">
-        <v>95</v>
-      </c>
-      <c r="F284" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H284" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="285" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D285" s="9"/>
+      <c r="H284" s="8"/>
+    </row>
+    <row r="285" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B285" t="s">
+        <v>90</v>
+      </c>
+      <c r="C285" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D285" s="9" t="s">
+        <v>98</v>
+      </c>
       <c r="E285" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="F285" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="H285" s="8" t="s">
-        <v>94</v>
+        <v>22</v>
+      </c>
+      <c r="G285" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H285" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I285" s="22" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="286" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D286" s="9"/>
       <c r="E286" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="F286" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H286" s="8" t="s">
-        <v>97</v>
+      <c r="G286" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H286" s="8">
+        <v>20210331</v>
       </c>
     </row>
     <row r="287" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D287" s="9"/>
-      <c r="H287" s="8"/>
-    </row>
-    <row r="288" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B288" t="s">
-        <v>90</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D288" s="9" t="s">
-        <v>98</v>
-      </c>
+      <c r="E287" t="s">
+        <v>89</v>
+      </c>
+      <c r="F287" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H287" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="288" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D288" s="9"/>
       <c r="E288" t="s">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="F288" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G288" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H288" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I288" s="22" t="s">
-        <v>287</v>
+      <c r="H288" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="289" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D289" s="9"/>
       <c r="E289" t="s">
-        <v>16</v>
+        <v>293</v>
       </c>
       <c r="F289" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G289" s="9" t="s">
-        <v>15</v>
-      </c>
       <c r="H289" s="8">
-        <v>20210331</v>
+        <v>512573</v>
       </c>
     </row>
     <row r="290" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D290" s="9"/>
-      <c r="E290" t="s">
-        <v>89</v>
-      </c>
-      <c r="F290" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H290" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="291" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D291" s="9"/>
+      <c r="H290" s="8"/>
+    </row>
+    <row r="291" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B291" t="s">
+        <v>90</v>
+      </c>
+      <c r="C291" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D291" s="9" t="s">
+        <v>101</v>
+      </c>
       <c r="E291" t="s">
-        <v>100</v>
+        <v>14</v>
       </c>
       <c r="F291" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H291" s="8" t="s">
-        <v>26</v>
+      <c r="G291" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H291" s="8">
+        <v>20200401</v>
+      </c>
+      <c r="I291" s="22" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="292" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D292" s="9"/>
       <c r="E292" t="s">
-        <v>293</v>
+        <v>16</v>
       </c>
       <c r="F292" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="G292" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="H292" s="8">
-        <v>512573</v>
+        <v>20210331</v>
       </c>
     </row>
     <row r="293" spans="2:9" x14ac:dyDescent="0.3">
@@ -4744,7 +4774,7 @@
         <v>186</v>
       </c>
       <c r="D294" s="9" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E294" t="s">
         <v>14</v>
@@ -4759,7 +4789,7 @@
         <v>20200401</v>
       </c>
       <c r="I294" s="22" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="295" spans="2:9" x14ac:dyDescent="0.3">
@@ -4779,38 +4809,32 @@
     </row>
     <row r="296" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D296" s="9"/>
-      <c r="H296" s="8"/>
-    </row>
-    <row r="297" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B297" t="s">
+      <c r="E296" t="s">
+        <v>293</v>
+      </c>
+      <c r="F296" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H296" s="8">
+        <v>500425</v>
+      </c>
+    </row>
+    <row r="297" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D297" s="9"/>
+      <c r="H297" s="8"/>
+    </row>
+    <row r="298" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B298" t="s">
         <v>90</v>
       </c>
-      <c r="C297" s="1" t="s">
+      <c r="C298" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="D297" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="E297" t="s">
-        <v>14</v>
-      </c>
-      <c r="F297" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G297" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H297" s="8">
-        <v>20200401</v>
-      </c>
-      <c r="I297" s="22" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="298" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D298" s="9"/>
+      <c r="D298" s="9" t="s">
+        <v>103</v>
+      </c>
       <c r="E298" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F298" s="9" t="s">
         <v>22</v>
@@ -4818,11 +4842,15 @@
       <c r="G298" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="H298" s="8">
-        <v>20210331</v>
-      </c>
-    </row>
-    <row r="299" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H298" s="16">
+        <v>20220228</v>
+      </c>
+      <c r="I298" s="22" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="299" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C299" s="1"/>
       <c r="D299" s="9"/>
       <c r="E299" t="s">
         <v>293</v>
@@ -4831,50 +4859,49 @@
         <v>22</v>
       </c>
       <c r="H299" s="8">
-        <v>500425</v>
-      </c>
-    </row>
-    <row r="300" spans="2:9" x14ac:dyDescent="0.3">
+        <v>500820</v>
+      </c>
+      <c r="I299" s="22"/>
+    </row>
+    <row r="300" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C300" s="1"/>
       <c r="D300" s="9"/>
-      <c r="H300" s="8"/>
+      <c r="E300" t="s">
+        <v>49</v>
+      </c>
+      <c r="F300" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="H300" s="8">
+        <v>48</v>
+      </c>
+      <c r="I300" s="22"/>
     </row>
     <row r="301" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B301" t="s">
-        <v>90</v>
-      </c>
-      <c r="C301" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="D301" s="9" t="s">
-        <v>103</v>
-      </c>
+      <c r="C301" s="1"/>
+      <c r="D301" s="9"/>
       <c r="E301" t="s">
-        <v>21</v>
+        <v>107</v>
       </c>
       <c r="F301" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G301" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="H301" s="16">
-        <v>20220228</v>
-      </c>
-      <c r="I301" s="22" t="s">
-        <v>290</v>
-      </c>
+        <v>106</v>
+      </c>
+      <c r="H301" s="8">
+        <v>4</v>
+      </c>
+      <c r="I301" s="22"/>
     </row>
     <row r="302" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C302" s="1"/>
       <c r="D302" s="9"/>
       <c r="E302" t="s">
-        <v>293</v>
+        <v>108</v>
       </c>
       <c r="F302" s="9" t="s">
-        <v>22</v>
+        <v>106</v>
       </c>
       <c r="H302" s="8">
-        <v>500820</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I302" s="22"/>
     </row>
@@ -4882,13 +4909,13 @@
       <c r="C303" s="1"/>
       <c r="D303" s="9"/>
       <c r="E303" t="s">
-        <v>49</v>
+        <v>109</v>
       </c>
       <c r="F303" s="9" t="s">
         <v>106</v>
       </c>
       <c r="H303" s="8">
-        <v>48</v>
+        <v>3.2</v>
       </c>
       <c r="I303" s="22"/>
     </row>
@@ -4896,13 +4923,13 @@
       <c r="C304" s="1"/>
       <c r="D304" s="9"/>
       <c r="E304" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F304" s="9" t="s">
         <v>106</v>
       </c>
       <c r="H304" s="8">
-        <v>4</v>
+        <v>0.11</v>
       </c>
       <c r="I304" s="22"/>
     </row>
@@ -4910,13 +4937,13 @@
       <c r="C305" s="1"/>
       <c r="D305" s="9"/>
       <c r="E305" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="F305" s="9" t="s">
         <v>106</v>
       </c>
       <c r="H305" s="8">
-        <v>1.1000000000000001</v>
+        <v>0.2</v>
       </c>
       <c r="I305" s="22"/>
     </row>
@@ -4924,13 +4951,13 @@
       <c r="C306" s="1"/>
       <c r="D306" s="9"/>
       <c r="E306" t="s">
-        <v>109</v>
+        <v>34</v>
       </c>
       <c r="F306" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H306" s="8">
-        <v>3.2</v>
+        <v>22</v>
+      </c>
+      <c r="H306" s="8" t="s">
+        <v>104</v>
       </c>
       <c r="I306" s="22"/>
     </row>
@@ -4938,120 +4965,128 @@
       <c r="C307" s="1"/>
       <c r="D307" s="9"/>
       <c r="E307" t="s">
-        <v>110</v>
+        <v>294</v>
       </c>
       <c r="F307" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H307" s="8">
-        <v>0.11</v>
+        <v>22</v>
+      </c>
+      <c r="H307" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="I307" s="22"/>
     </row>
-    <row r="308" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C308" s="1"/>
+    <row r="308" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D308" s="9"/>
       <c r="E308" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="F308" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H308" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="I308" s="22"/>
-    </row>
-    <row r="309" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C309" s="1"/>
+        <v>22</v>
+      </c>
+      <c r="H308" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="309" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D309" s="9"/>
-      <c r="E309" t="s">
-        <v>34</v>
-      </c>
-      <c r="F309" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H309" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="I309" s="22"/>
-    </row>
-    <row r="310" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C310" s="1"/>
-      <c r="D310" s="9"/>
-      <c r="E310" t="s">
-        <v>294</v>
-      </c>
-      <c r="F310" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H310" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="I310" s="22"/>
-    </row>
-    <row r="311" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D311" s="9"/>
-      <c r="E311" t="s">
-        <v>89</v>
-      </c>
-      <c r="F311" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H311" s="8" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="312" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D312" s="9"/>
+    </row>
+    <row r="310" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B310" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C310" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D310" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="E310" s="1"/>
+      <c r="F310" s="1"/>
+      <c r="G310" s="1"/>
+      <c r="H310" s="3"/>
+      <c r="I310" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="311" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B311" s="1"/>
+      <c r="C311" s="1"/>
+      <c r="D311" s="10"/>
+      <c r="E311" s="1"/>
+      <c r="F311" s="1"/>
+      <c r="G311" s="1"/>
+      <c r="H311" s="12"/>
+      <c r="I311" s="13"/>
+    </row>
+    <row r="312" spans="2:9" ht="29.4" x14ac:dyDescent="0.35">
+      <c r="B312" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C312" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D312" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="E312" s="1"/>
+      <c r="F312" s="1"/>
+      <c r="G312" s="1"/>
+      <c r="H312" s="12" t="s">
+        <v>269</v>
+      </c>
+      <c r="I312" s="7" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="313" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B313" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C313" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D313" s="9" t="s">
-        <v>280</v>
-      </c>
+      <c r="B313" s="1"/>
+      <c r="C313" s="1"/>
+      <c r="D313" s="10"/>
       <c r="E313" s="1"/>
       <c r="F313" s="1"/>
       <c r="G313" s="1"/>
       <c r="H313" s="3"/>
-      <c r="I313" s="13" t="s">
-        <v>51</v>
-      </c>
+      <c r="I313" s="13"/>
     </row>
     <row r="314" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B314" s="1"/>
-      <c r="C314" s="1"/>
-      <c r="D314" s="10"/>
-      <c r="E314" s="1"/>
-      <c r="F314" s="1"/>
+      <c r="B314" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C314" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D314" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="E314" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F314" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="G314" s="1"/>
-      <c r="H314" s="12"/>
-      <c r="I314" s="13"/>
-    </row>
-    <row r="315" spans="2:9" ht="29.4" x14ac:dyDescent="0.35">
-      <c r="B315" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C315" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D315" s="10" t="s">
-        <v>268</v>
-      </c>
-      <c r="E315" s="1"/>
-      <c r="F315" s="1"/>
+      <c r="H314" s="3">
+        <v>531733</v>
+      </c>
+      <c r="I314" s="7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="315" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B315" s="1"/>
+      <c r="C315" s="1"/>
+      <c r="D315" s="10"/>
+      <c r="E315" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="F315" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="G315" s="1"/>
-      <c r="H315" s="12" t="s">
-        <v>269</v>
-      </c>
-      <c r="I315" s="7" t="s">
-        <v>270</v>
-      </c>
+      <c r="H315" s="3">
+        <v>25</v>
+      </c>
+      <c r="I315" s="13"/>
     </row>
     <row r="316" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B316" s="1"/>
@@ -5063,94 +5098,84 @@
       <c r="H316" s="3"/>
       <c r="I316" s="13"/>
     </row>
-    <row r="317" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="317" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B317" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C317" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D317" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="E317" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F317" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="G317" s="1"/>
-      <c r="H317" s="3">
-        <v>531733</v>
-      </c>
-      <c r="I317" s="7" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="318" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B318" s="1"/>
-      <c r="C318" s="1"/>
-      <c r="D318" s="10"/>
-      <c r="E318" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="F318" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G318" s="1"/>
-      <c r="H318" s="3">
-        <v>25</v>
-      </c>
-      <c r="I318" s="13"/>
-    </row>
-    <row r="319" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B319" s="1"/>
-      <c r="C319" s="1"/>
-      <c r="D319" s="10"/>
-      <c r="E319" s="1"/>
-      <c r="F319" s="1"/>
-      <c r="G319" s="1"/>
-      <c r="H319" s="3"/>
-      <c r="I319" s="13"/>
-    </row>
-    <row r="320" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B320" s="1" t="s">
+      <c r="D317" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="E317" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="F317" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G317" s="8"/>
+      <c r="H317" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="318" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D318" s="9"/>
+      <c r="E318" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="F318" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G318" s="8"/>
+      <c r="H318" s="18" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="319" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D319" s="9"/>
+    </row>
+    <row r="320" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B320" t="s">
         <v>50</v>
       </c>
-      <c r="C320" s="1" t="s">
+      <c r="C320" t="s">
         <v>187</v>
       </c>
       <c r="D320" s="9" t="s">
-        <v>258</v>
-      </c>
-      <c r="E320" s="8" t="s">
-        <v>259</v>
-      </c>
-      <c r="F320" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G320" s="8"/>
-      <c r="H320" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="321" spans="2:9" ht="43.2" x14ac:dyDescent="0.3">
+        <v>278</v>
+      </c>
+      <c r="E320" t="s">
+        <v>276</v>
+      </c>
+      <c r="F320" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H320" s="32">
+        <v>532648</v>
+      </c>
+      <c r="I320" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="321" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D321" s="9"/>
-      <c r="E321" s="8" t="s">
-        <v>275</v>
-      </c>
-      <c r="F321" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G321" s="8"/>
-      <c r="H321" s="18" t="s">
-        <v>260</v>
+      <c r="E321" t="s">
+        <v>277</v>
+      </c>
+      <c r="F321" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H321" s="32">
+        <v>8</v>
       </c>
     </row>
     <row r="322" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D322" s="9"/>
-    </row>
-    <row r="323" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="F322" s="1"/>
+      <c r="H322" s="32"/>
+    </row>
+    <row r="323" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B323" t="s">
         <v>50</v>
       </c>
@@ -5158,7 +5183,7 @@
         <v>187</v>
       </c>
       <c r="D323" s="9" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="E323" t="s">
         <v>276</v>
@@ -5168,9 +5193,6 @@
       </c>
       <c r="H323" s="32">
         <v>532648</v>
-      </c>
-      <c r="I323" s="7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="324" spans="2:9" x14ac:dyDescent="0.3">
@@ -5187,133 +5209,105 @@
     </row>
     <row r="325" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D325" s="9"/>
-      <c r="F325" s="1"/>
-      <c r="H325" s="32"/>
-    </row>
-    <row r="326" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B326" t="s">
-        <v>50</v>
+    </row>
+    <row r="326" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B326" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C326" t="s">
-        <v>187</v>
-      </c>
-      <c r="D326" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="E326" t="s">
+        <v>216</v>
+      </c>
+      <c r="D326" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="E326" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F326" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G326" s="1"/>
+      <c r="H326" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I326" s="22" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="327" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B327" s="1"/>
+      <c r="C327" s="1"/>
+      <c r="D327" s="10"/>
+      <c r="E327" s="11"/>
+      <c r="F327" s="10"/>
+      <c r="G327" s="1"/>
+      <c r="H327" s="3"/>
+      <c r="I327" s="13"/>
+    </row>
+    <row r="328" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B328" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C328" t="s">
+        <v>216</v>
+      </c>
+      <c r="D328" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="E328" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F328" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G328" s="1"/>
+      <c r="H328" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I328" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="329" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+      <c r="B329" s="1"/>
+      <c r="C329" s="1"/>
+      <c r="D329" s="10"/>
+      <c r="E329" s="11" t="s">
         <v>276</v>
       </c>
-      <c r="F326" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H326" s="32">
-        <v>532648</v>
-      </c>
-    </row>
-    <row r="327" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D327" s="9"/>
-      <c r="E327" t="s">
-        <v>277</v>
-      </c>
-      <c r="F327" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="H327" s="32">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="328" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="D328" s="9"/>
-    </row>
-    <row r="329" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B329" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C329" t="s">
-        <v>216</v>
-      </c>
-      <c r="D329" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="E329" s="11" t="s">
-        <v>200</v>
-      </c>
       <c r="F329" s="10" t="s">
         <v>9</v>
       </c>
       <c r="G329" s="1"/>
-      <c r="H329" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I329" s="22" t="s">
-        <v>256</v>
-      </c>
+      <c r="H329" s="3">
+        <v>532667</v>
+      </c>
+      <c r="I329" s="13"/>
     </row>
     <row r="330" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B330" s="1"/>
       <c r="C330" s="1"/>
       <c r="D330" s="10"/>
-      <c r="E330" s="11"/>
-      <c r="F330" s="10"/>
+      <c r="E330" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="F330" s="10" t="s">
+        <v>9</v>
+      </c>
       <c r="G330" s="1"/>
-      <c r="H330" s="3"/>
+      <c r="H330" s="3">
+        <v>198</v>
+      </c>
       <c r="I330" s="13"/>
     </row>
-    <row r="331" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B331" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C331" t="s">
-        <v>216</v>
-      </c>
-      <c r="D331" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="E331" s="11" t="s">
-        <v>200</v>
-      </c>
-      <c r="F331" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G331" s="1"/>
-      <c r="H331" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I331" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="332" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B332" s="1"/>
-      <c r="C332" s="1"/>
-      <c r="D332" s="10"/>
-      <c r="E332" s="11" t="s">
-        <v>276</v>
-      </c>
-      <c r="F332" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G332" s="1"/>
-      <c r="H332" s="3">
-        <v>532667</v>
-      </c>
-      <c r="I332" s="13"/>
-    </row>
-    <row r="333" spans="2:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="B333" s="1"/>
-      <c r="C333" s="1"/>
-      <c r="D333" s="10"/>
-      <c r="E333" s="11" t="s">
-        <v>277</v>
-      </c>
-      <c r="F333" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G333" s="1"/>
-      <c r="H333" s="3">
-        <v>198</v>
-      </c>
-      <c r="I333" s="13"/>
+    <row r="331" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D331" s="9"/>
+    </row>
+    <row r="332" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D332" s="9"/>
+    </row>
+    <row r="333" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D333" s="9"/>
     </row>
     <row r="334" spans="2:9" x14ac:dyDescent="0.3">
       <c r="D334" s="9"/>
@@ -5350,15 +5344,6 @@
     </row>
     <row r="345" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D345" s="9"/>
-    </row>
-    <row r="346" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D346" s="9"/>
-    </row>
-    <row r="347" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D347" s="9"/>
-    </row>
-    <row r="348" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D348" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>